<commit_message>
chore: update output notebook and data
</commit_message>
<xml_diff>
--- a/notebooks/Cleaned_Topic_Headlines.xlsx
+++ b/notebooks/Cleaned_Topic_Headlines.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -512,14 +512,10 @@
       <c r="H2" t="n">
         <v>0</v>
       </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>ignitex sponsor taiwan blockchain hackathon empowering next generation of web innovator is the rule unattainable in typical u household need to spend of income to afford the medianpriced home b rfg advisory launch suite of active etf free settlement money from att who qualifies and when you can file your claim cnet what house and senate republican cant agree on in trump tax bill pony ai the next trillion robotaxi play fcps look toward next decade of school construction enrollment growth tri pointe home inc announces second quarter earnings release and conference call date growth stock that turned investment year ago into over million today the everglades foundation name shannon estenoz a it first chief policy officer santech holding announces unaudited financial result for the first half of fiscal year b bleakley add advisor coach ray sclafani to board of director air canada completes million substantial issuer bid acting on it commitment to balanced longterm capital allocation zapp ev report financial result for the six month ended march and provides operational update ufe doesnt remove fibroidsheres what woman arent being told quincy data precision time exchange service recognized a best time stamping measurement system by tradingtech insight award santech holding announces unaudited financial result for the first half of fiscal year a regulation fade a nonprofit push voluntary standard is the rule unattainable in typical u household need to spend of income to afford the medianpriced home improvement to make playground more accessible underway east texas bbb warns of major data breach chainlink whale diversifying into bitcoin solaris before it inevitable price explosion first quantum provides notice of second quarter result the everglades foundation name shannon estenoz a it first chief policy officer first patient enrolled in aclarions groundbreaking clarity trial pure property management named to inc best workplace hidden cost of homeownership now exceed a year kalmar and cagliari roro terminal continue collaboration with new order for terminal tractor no one expected oil price to crash this much first quantum provides notice of second quarter result sweden riksbank see some probability for further rate cut amid murky outlook buy now pay later plan will soon impact your credit scorewhat you need to know well fargo hike microsoft price target say ai business could reach billion in revenue cd rate today june take home up to teenage sprint sensation gout gout break his own m australian record in first race abroad china and india cut import of lowerquality coal from indonesia fueling ai data center behind the meter solution cherry bekaert appoints dan wheadon a cfo advisory leader is apa stock underperforming the dow bitget head to milan a sponsor at ethmilan watch fed chair jerome powell testify live before senate banking panel could berkshire hathaway stock double by even without warren buffett could berkshire hathaway stock double by even without warren buffett trimble tdks advanced navigation solution to enhance automotive positioning drone maker aerovironment share pop on earnings beat american in line to pocket up to k from m data breach settlement exact date to note down sp future muted with focus on powell testimony finding a mentor can be key to your success expert tip for finding one it going to get you place qdoba restaurant expands with th location in florida skelton big state budget question linger about crime medical delta tunnel former circuit clinical colleague join force again to form health care startup where will coreweave stock be in year how social security privatization could change the role of ira in your portfolio wayfair is selling a lounge chair for just and shopper say it will turn your patio into a little oasis how tariff might impact u car price by brand exclusive uber and palantir alum raise m to disrupt corporate recruitment with ai fortune amazon is selling a stunning citizen ecodrive watch for and buyer call it an eyecatcher amazon prime day start date early deal and shopping tip share in wr berkley corporation nysewrb purchased by kentucky retirement system insurance trust fund kentucky retirement system insurance trust fund make new investment in eversource energy nysees state of alaska department of revenue buy share of hyatt hotel corporation nyseh new york city is closer to electing a democratic socialist mayor business have mixed feeling why blackberry share are trading higher by around here are stock moving premarket kentucky retirement system insurance trust fund invests in citizen financial group inc nysecfg williamssonoma inc nysewsm share bought by janney montgomery scott llc kentucky retirement system insurance trust fund ha stock holding in tyson food inc nysetsn jfs wealth advisor llc purchase share of johnson control international plc nysejci omnicom group inc nyseomc stake reduced by continuum advisory llc xml financial llc ha holding in eaton corporation plc nyseetn exchange traded concept llc raise stock holding in allegion plc nysealle exchange traded concept llc ha stock holding in air product and chemical inc nyseapd gm inc nysegms share sold by state of alaska department of revenue williamssonoma inc nysewsm share acquired by janney montgomery scott llc trump advisor stephen miller reportedly hold stake worth million in ice contractor palantir he could easilyhave a direct and predictable impact micron face earnings test after share price doubled since april nba owner unanimously approve b sale of wolf wnbas lynx from taylor to lorerodriguez group first female reporter at kpnx in phoenix diane kalas dy bitcoin price rise the crypto is being boosted by these factor today verizon team up with nokia to bring hightech g boost to busy british port verizon team up with nokia to bring hightech g boost to busy british port usdinr inch up a market weighs middle east ceasefire amid fed and rbi action jadwa investment buy majority stake in saudi retailer makhazen alenaya why are some people calling for a mcdonalds boycott alexandria real estate equity inc nyseare share purchased by flagship harbor advisor llc kentucky retirement system insurance trust fund acquires new position in synchrony financial nysesyf kentucky retirement system insurance trust fund cut position in darden restaurant inc nysedri flagship harbor advisor llc purchase share of dexcom inc nasdaqdxcm how private capital could be the key to rebuilding america is palantir stock outperforming the dow is palantir stock outperforming the dow retirement system of alabama ha million stock position in firstenergy corporation nysefe retirement system of alabama sell share of cm energy corporation nysecms retirement system of alabama reduces position in kellanova nysek pfg investment llc decrease stake in ishares msci emerging market etf nysearcaeem today quordle hint and answer for june detroit station to open coffee shop in hope of connecting to the community trump medium stock edge higher premarket after nyse file to list truth social bitcoin and ethereum etf share flagship harbor advisor llc ha stake in edward lifesciences corporation nyseew retirement system of alabama lower position in devon energy corporation nysedvn wealth enhancement advisory service llc increase position in public service enterprise group incorporated nysepeg despite promise to remove worst of the worst ice ha arrested only of known immigrant murderer what to do when success make you lose touch with your identity beef price at record high trump attack on iran pushed diplomacy with kim jong un further out of reach more than idaho airman are deployed in the middle east are they safe impactful bill that passed in idaho legislative session this year childrens hospital los angeles threw trans kid overboard teenage sprint sensation gout gout break his own m australian record in first race abroad the longest battle in world war i occurred around which french city the federalist society isnt going anywhere the federalist society isnt going anywhere trump united surveillance state of america how will your data be deployed glen alpine alderman step down cite board behavior highschoollike squabble in resignation orangeburg county council reject homeowner request to close road sioux city resident express concern to staff of sen joni ernst about federal budget cut new york city is closer to electing a democratic socialist mayor business have mixed feeling reader view dont doubt those protesting the powerful reader view beautiful bill could cut service we need editorial cartoon for june rubio hegseth slam medium over iran strike leak professional stabber undermining u victory upper township renews liquor license for the deauville inn on one condition bamberg county sheriff office detention center honor employee behind the curtain ai urgency call for a modern marshall plan gop leader accused of pressuring lobbyist to drop gaming client in ugly pa budget fight a whirlwind hour how trump israeliran ceasefire agreement came together letter let not lose more of bidwells legacy letter let not lose more of bidwells legacy a tremendous victory for everybody trump on iran strike from cable to vision pro how luxshare is replacing foxconn in apple ecosystem trump hoping for comprehensive peace agreement with iran witkoff court order trump administration to return another wrongly deported man overdoses are down in iredell county a more proactive approach may be helping letter eliminating fluoridation carry health risk letter eliminating fluoridation carry health risk a whirlwind hour how trump israeliran ceasefire agreement came together a whirlwind hour how trump israeliran ceasefire agreement came together kennedyappointed cdc vaccine panel say it will scrutinize the childhood vaccine schedule letter trust our president and pray for our country letter trust our president and pray for our country ice will see you now everyday ethic what if you had only one day to live everyday ethic what if you had only one day to live a columbia trustee view higher education is at a crossroad let choose builder over destroyer im a veteran and former democratic congressman here why the gop ought to think hard about iran big beautiful bill should not include sale of public land opinion big beautiful bill should not include sale of public land opinion rare earth startup say without subsidy and support u cant shake china control asra nomani iran ideological foot soldier wage proxy war in america death from heart attack are way down here whats killing u instead trump lawyer and doj enforcer face confirmation hearing for federal judgeship our opinion berkshire carousel horse ride again can they carry this downtown destination to sustainability the normalization of american indecency iran strategic blunder paved the way for humiliating defeat expert say want happier healthier kid let them play a decade after obergefell lgbtq right remain under threat exclusive thune urge light touch on ai regulation when everything go wrong trump pick for appeal judge seen a illsuited to lifetime appointment skinnytok rebranded eating disorder dangerously fast scoop trump admin cut contract with scientific publishing giant how to contact cayuga county federal state and county elected official iranian royalty fed local rumor mill year ago letter bomb and peace dont work well together letter bomb and peace dont work well together u marine sentenced to year over sexual assault in japan letter not feeling represented by district congressman letter not feeling represented by district congressman nato summit yield a big win on defense spending for trump but key question over the alliance remain trump isnt ready for a ceasefire with massie zambian president burial halted just a it wa to begin despite promise to remove worst of the worst ice ha arrested only of known immigrant murderer super coral and supplement inside the lab trying to save the great barrier reef food hygiene rating handed to two doncaster establishment trump did the right thing israeli intelligence see significant damage to iran nuclear facility official say after a halfcentury of legal logjam will killer of coast banker wife face execution june during patriotic season searching for the right america public forum bill threatens mental health care aging entrepreneur face new policy hurdle here how to help highyielding dividend stock to buy for the long haul trump triumph nato bow to u pressure with defense pledge rep mike quigley tell trump to put your ego in your pocket rep mike quigley on intel suggesting limited damage to iran nuclear program a criminal justice expert on the implication of the karen read verdict morning brief nato commits to defense spike nyc pick a socialist expert push transing kid trump pick for appeal judge draw controversy zohran mamdani set to defeat cuomo in nyc mayoral primary upset today in history june korean war begin australian outback transformed by water rubio dont believe report of only modest damage in iran pell grant cut would be a blow to maine economic future opinion pell grant cut would be a blow to maine economic future opinion the supreme court blessed samesex marriage year ago is a backlash brewing franklin board modifies some district policy after discussion astronomical society to hold public night saturday editorial minnesota shooting shatter trust faith bridge builder announces first recipient of technical career investment grant year ago june state issue warning on fake inheritance scam column pursue smarter choice on the northern border scatec asa subscription for the employee share purchase programme exclusive shell in early talk to acquire rival bp wsj palantir stock hit alltime high whats going on vimergy brings mouth of america campaign to washington dc to expose a system that profit while american get sicker cpsc urge firework safety ahead of july th holiday metas insane technology give user something no screen today can deliver say mark zuckerberg in the future ill just beam in is charles river laboratory stock underperforming the sp is charles river laboratory stock underperforming the sp national survey find american favor a federal budget completely different from the one congress is developing bumble to cut of workforce a online dating apps aim to improve user experience wsj why aerovironment stock is soaring today why aerovironment stock is soaring today nvidia stock soar near record high whats driving the rally forget crossfit this million fitness event is taking over how teacher are using chatgptand getting their time back how seattle won over fifas club world cup skeptic bitcoin rise nyse battle for trump etf and crypto may be coming to mortgage next ai for impact day explores the potential for ai to improve decisionmaking and increase efficiency across critical national security operation should you buy slide insurance stock after the slde ipo should you buy slide insurance stock after the slde ipo carnival booking surge ha wall street talking already solstad renews partnership with marlink for it next stage of digital transformation forester financial welcome new leadership to it board of director trump megabill and economic agenda would spur growth and reduce national debt according to white house report here how much invested in oracle year ago would be worth today amazon is selling a espresso machine for and shopper say it make great coffee just like starbucks another huge retail chain liquidating after chapter bankruptcy duck return to a long island farm that lost it entire flock to the bird flu duck return to a long island farm that lost it entire flock to the bird flu duck return to a long island farm that lost it entire flock to the bird flu duck return to a long island farm that lost it entire flock to the bird flu siili solution plc share repurchase duck return to a long island farm that lost it entire flock to the bird flu aigenerated scam claim more victim yearoveryear despite declining consumer concern new sift report reveals duck return to a long island farm that lost it entire flock to the bird flu duck return to a long island farm that lost it entire flock to the bird flu duck return to a long island farm that lost it entire flock to the bird flu duck return to a long island farm that lost it entire flock to the bird flu russia to boost export of china favorite russian crude in july duck return to a long island farm that lost it entire flock to the bird flu how data analytics power and governs nextgen digital twin duck return to a long island farm that lost it entire flock to the bird flu shiba inu to be left in pepe dollar tokenomics attract institutional investor over shiba inus massive dilution risk intrinsic therapeutic announces the first implantation of the barricaid annular closure device via endoscopic approach happy city holding limited announces closing of initial public offering duck return to a long island farm that lost it entire flock to the bird flu duck return to a long island farm that lost it entire flock to the bird flu duck return to a long island farm that lost it entire flock to the bird flu duck return to a long island farm that lost it entire flock to the bird flu fed chair powell the crypto industry is maturing becoming more mainstream duck return to a long island farm that lost it entire flock to the bird flu invent inventor develops temporary replacement for windshield wiper mho duck return to a long island farm that lost it entire flock to the bird flu duck return to a long island farm that lost it entire flock to the bird flu duck return to a long island farm that lost it entire flock to the bird flu nostalgic pepsi brand from the s roll out new flavor week after rival coke launch it version pictory introduces one of the world first ai video mcp server pictory introduces one of the world first ai video mcp server rosen a trusted and leading law firm encourages rocket pharmaceutical inc investor to secure counsel before important deadline in security class action rckt have the wheel fallen off the corn market have the wheel fallen off the corn market senate minority leader schumer treated for dehydration at area hospital his office say study find trump most favored nation drug proposal could still raise outofpocket cost without pbm reform study find trump most favored nation drug proposal could still raise outofpocket cost without pbm reform valuesinaction foundation honor leadership from across the u valuesinaction foundation honor leadership from across the u new home sale plummet more than expected a high mortgage rate sink demand bi claim stablecoins fail a money call for strict limit on their role tidy up your patio in second get off the aerobroom in cordless leaf blower broom is skin cancer linked to climate change hims hers health ceo say compounding novo weightloss drug will continue report himsnyse seeking alpha ahold delhaize usa tap food lion executive a cfo paychex stock take a hit a margin squeeze overshadows outlook spotify stock hit record high get pricetarget hike american became millionaire in way your neigbors are getting rich and how to keep up pacific life introduces new variable universal life insurance product now available through state farm ulta beauty cfo paula oyibo quits pick insider for interim role u state to roll out huge bottle change in new july law and the ban target all of your shower supply you are cordially invited to critique jeff bezos and lauren sanchez wedding invitation robinhood ceo highlight retail investor interest in nvidia tesla despite middle east tension barely a blip hot weather safety trick for your pet hot weather safety advice for your pet mark walter and lakers say sale of the team is expected to close later this year clever carnivore announces scalable costcompetitive and delicious cultivated pork clever carnivore announces scalable costcompetitive and delicious cultivated pork medium advisory federal government to make housing announcement in cape breton stock see support a reduced middle east tension spark riskon stock see support a reduced middle east tension spark riskon piston raise m for cardless fuel payment solution piston raise m for cardless fuel payment solution tsa say these common childrens toy may not be allowed on plane why share of tesla are sinking today navigating the complexity of crossborder freight invent inventor develops new shoe cleaning device mho overture map launch gers a global standard for interoperable geospatial id to drive data interoperability big gain start small best new meme coin to join this month before they moon kandal m venture limited announces pricing of initial public offering and listing on nasdaq woodside close stake sale in louisiana lng project kandal m venture limited announces pricing of initial public offering and listing on nasdaq ap business summarybrief at am edt wary of washington europe fret it will be left behind on an ai battlefield senate prepares for vote on big beautiful bill trump say u will meet with iran next week trump megabill and economic agenda would spur growth and reduce national debt according to white house report fox news racist smear against zohran mamdani fail in new york mayoral race un official say agency cant locate iran uranium after u strike yakima start work on water and wastewater connection in several neighborhood trump israel say u airstrike destroyed crucial nuclear facility and set iran back year denver judge to decide fate of ice subpoena a state employee sue gov polis to halt compliance reader opinion preparing the landscape trump label nycs mamdani a communist lunatic senate gop leader make opening offer on hospital fund california found in violation of title ix in clash with trump official over transgender athlete man indicted on hate crime charge in attack on boulder demonstration for israeli hostage house republican inch closer to answer a former biden advisor lose executive privilege shield you are cordially invited to critique jeff bezos and lauren sanchez wedding invitation man get stuck in chimney while trying to rescue dog trapped in building san francisco mayor daniel lurie unveils family zoning plan to boost homebuilding trump denies iranian moved nuclear material before u strike trump denies iranian moved nuclear material before u strike donald trump should be ashamed of betraying our afghan ally opinion trump denies iranian moved nuclear material before u strike kennedy new vaccine adviser meet for first time kennedy new vaccine adviser meet for first time kennedy new vaccine adviser meet for first time kennedy new vaccine adviser meet for first time kennedy new vaccine adviser meet for first time kennedy new vaccine adviser meet for first time cayuga county budget reality raise tax or cut deeper trump denies iranian moved nuclear material before u strike trump denies iranian moved nuclear material before u strike trump denies iranian moved nuclear material before u strike trump hegseth seethe at fake news medium for doubting u strike obliterated iranian nuclear site scum maverick select cooper flagg no overall in nba draft early u intelligence report suggests u strike only set back iran nuclear program by month trump attack on iran pushed diplomacy with kim jong un further out of reach tracking every firstround pick in the nba draft trump affirms his commitment to nato article pledge for mutual defense he like me trump on nato chief mark rutte calling him daddy unanimous wisconsin supreme court curtails governor partial veto power unanimous wisconsin supreme court curtails governor partial veto power dead congressman social medium account resurrected to boost former chief of staff congressional bid schumer hospitalized for dehydration a dc nears degree the myth of iran invincibility ha been broken and the fallout could be farreaching pope leo xiv urge all side in iranisrael war to reject bullying and arrogance and talk peace new york man arrested in maine on drug trafficking charge longlasting insulin take another step forward with latest clinical trial result tony abbott tell advance supporter bequeathing money to rightwing group will protect australian value excessive social medium found to harm teenager mental health but expert say moderation may be key cruel joke tax concession drive donation to australia richest private school and must stop critic argue trump lay into spain over nato defense spending trump lay into spain over nato defense spending trump lay into spain over nato defense spending we may not agree on climate but we all feel the heat past public policy make today crisis more costly past public policy make today crisis more costly past public policy make today crisis more costly hood our lawmaker arent deadlocked on regulation toyota tlmoda and the salvation army team up to distribute backpack and school supply to student nationwide can i partner with a different attorney on my appeal appeal lawyer wichita wa donald trump decision to strike iran legal trump lay into spain over nato defense spending trump lay into spain over nato defense spending trump lay into spain over nato defense spending shasti conrad leader of the wa democratic party win dnc vice chair race durbin tee off on bove a judiciary hearing kick off trump say assessment of iran nuclear facility damage wa not a complete report zohran mamdani ha nycs business community terrified lawless act of defiance doj say biden judge is refusing to follow supreme court order how chatgpt and other ai tool are changing the teaching profession microsoft sued by author over use of book in ai training democrat primary voter reward first prosecutor to indict trump senator air concern about doj budget proposal billionaire ackman and musk rebuke zohran mamdanis win in nyc mayoral primary senate bill a sensible cure for ada abuse senate bill a sensible cure for ada abuse senate bill a sensible cure for ada abuse senate bill a sensible cure for ada abuse former democrat staffer arrested for abducting assaulting woman on the loose after posting bond baumgartner northwest republican ask rfk jr to reopen niosh worker safety office in spokane thing to know about senate bill navigating new noncompete restriction for healthcare practitioner in texas trump say u will meet with iran next week israel and iran both claim win a trumpbrokered truce hold carlisle vote to sell fire engine address upcoming project gop leader back florida ag uthmeier at u supreme court on immigration trump state visit to the uk to take place this year say buckingham palace u stock hang near their record a wall street take a breath following two big day hamas is preparing attack on american contractor helping distribute aid in gaza bezos arrives in venice a protester say his starstudded wedding highlight growing inequality new dogsized dinosaur specie discovered tax collection tumble again in latest washington budget forecast trump white house clear way for biden aide to tell all i am sweating badly new yorkers and visitor cope with extreme heat no social security tax cut in trump new bill what retiree need to know jerald mcnair while school are out our youth need to continue to read jeff bezos italian wedding by the number the senate majority run through moderate america eric dane and jensen ackles in countdown youre not dreaming score dozen of early th of july deal on mattress vulnerable long island dem warns mamdani too extreme for nyc after primary upset not just alligator alcatraz desantis float building another immigration detention center federal judge order u labor department to keep job corp running during lawsuit federal judge order u labor department to keep job corp running during lawsuit federal judge order u labor department to keep job corp running during lawsuit federal judge order u labor department to keep job corp running during lawsuit federal judge order u labor department to keep job corp running during lawsuit eric adam ha a real chance to stop mamdani but andrew cuomo need to announce he dropping out trump admin sue every federal judge in maryland over immigration order faith leader and family sue to block texas new ten commandment in school law faith leader and family sue to block texas new ten commandment in school law faith leader and family sue to block texas new ten commandment in school law faith leader and family sue to block texas new ten commandment in school law faith leader and family sue to block texas new ten commandment in school law faith leader and family sue to block texas new ten commandment in school law</t>
-        </is>
-      </c>
+      <c r="I2" t="inlineStr"/>
       <c r="J2" t="inlineStr">
         <is>
-          <t>ignitex sponsor taiwan blockchain hackathon empowering next generation web innovator rule unattainable typical household spend income afford medianpriced b rfg advisory launch suite active free settlement money att qualifies file claim cnet house senate republican cant agree trump tax bill pony ai next trillion robotaxi play fcps look next decade school construction enrollment growth tri pointe announces quarter earnings release conference call date growth stock turned investment ago million everglades foundation name shannon estenoz chief policy officer santech announces unaudited financial half fiscal b bleakley add advisor coach ray sclafani board director air canada completes million substantial issuer bid acting commitment balanced longterm allocation zapp ev report financial six month ended march provides operational update ufe doesnt remove fibroidsheres woman arent quincy data precision exchange service recognized best stamping measurement system tradingtech insight award santech announces unaudited financial half fiscal regulation fade nonprofit push voluntary rule unattainable typical household spend income afford medianpriced improvement playground accessible underway east texas bbb warns major data breach chainlink whale diversifying bitcoin solaris inevitable price explosion quantum provides notice quarter everglades foundation name shannon estenoz chief policy officer patient enrolled aclarions groundbreaking clarity trial pure property named best workplace hidden cost homeownership exceed kalmar cagliari roro terminal continue collaboration new order terminal tractor expected oil price crash quantum provides notice quarter sweden riksbank probability rate cut amid murky outlook buy pay later plan soon impact credit scorewhat fargo hike microsoft price target ai business reach billion revenue cd rate take teenage sprint sensation gout gout break australian record race abroad china india cut import lowerquality coal indonesia fueling ai data center behind meter solution cherry bekaert appoints dan wheadon cfo advisory apa stock underperforming dow bitget head milan sponsor ethmilan watch fed chair jerome powell testify senate banking panel berkshire hathaway stock double without warren buffett berkshire hathaway stock double without warren buffett trimble tdks advanced navigation solution enhance automotive positioning drone maker aerovironment share pop earnings beat american line pocket k data breach settlement exact date note sp future muted focus powell testimony finding mentor success expert tip finding place qdoba restaurant expands location florida skelton budget linger crime medical delta tunnel circuit clinical colleague join force form health care startup coreweave stock social security privatization change role ira portfolio wayfair selling lounge chair shopper turn patio little oasis tariff impact car price brand exclusive uber palantir alum raise disrupt corporate recruitment ai fortune amazon selling stunning citizen ecodrive watch buyer call eyecatcher amazon prime start date early deal shopping tip share wr berkley corporation nysewrb purchased kentucky retirement system insurance trust fund kentucky retirement system insurance trust fund new investment eversource energy nysees alaska department revenue buy share hyatt hotel corporation nyseh new york closer electing democratic socialist mayor business mixed feeling blackberry share trading higher around stock moving premarket kentucky retirement system insurance trust fund invests citizen financial nysecfg williamssonoma nysewsm share bought janney montgomery scott kentucky retirement system insurance trust fund stock tyson nysetsn jfs wealth advisor purchase share johnson control international plc nysejci omnicom nyseomc stake reduced continuum advisory xml financial eaton corporation plc nyseetn exchange traded concept raise stock allegion plc nysealle exchange traded concept stock air product chemical nyseapd gm nysegms share alaska department revenue williamssonoma nysewsm share acquired janney montgomery scott trump advisor stephen miller reportedly stake worth million contractor palantir easilyhave direct predictable impact micron face earnings test share price doubled since april nba owner unanimously approve b sale wolf wnbas lynx taylor lorerodriguez female reporter kpnx phoenix diane kalas dy bitcoin price rise crypto boosted factor verizon team nokia hightech g boost busy british port verizon team nokia hightech g boost busy british port usdinr inch market weighs middle east ceasefire amid fed rbi action jadwa investment buy majority stake saudi retailer makhazen alenaya people calling mcdonalds boycott alexandria real estate equity nyseare share purchased flagship harbor advisor kentucky retirement system insurance trust fund acquires new synchrony financial nysesyf kentucky retirement system insurance trust fund cut darden restaurant nysedri flagship harbor advisor purchase share dexcom nasdaqdxcm private rebuilding america palantir stock outperforming dow palantir stock outperforming dow retirement system alabama million stock firstenergy corporation nysefe retirement system alabama sell share cm energy corporation nysecms retirement system alabama reduces kellanova nysek pfg investment decrease stake ishares msci emerging market nysearcaeem quordle hint answer detroit station open coffee shop connecting community trump medium stock edge higher premarket nyse file list truth social bitcoin ethereum share flagship harbor advisor stake edward lifesciences corporation nyseew retirement system alabama lower devon energy corporation nysedvn wealth enhancement advisory service increase public service enterprise incorporated nysepeg promise remove worst worst arrested known immigrant murderer success lose touch identity beef price record high trump attack iran pushed diplomacy kim jong un reach idaho airman deployed middle east safe impactful bill passed idaho legislative session childrens hospital los angeles threw trans kid overboard teenage sprint sensation gout gout break australian record race abroad longest battle world war occurred around french federalist society isnt anywhere federalist society isnt anywhere trump united surveillance america data deployed glen alpine alderman step cite board behavior highschoollike squabble resignation orangeburg county council reject homeowner request close road sioux resident express concern staff sen joni ernst federal budget cut new york closer electing democratic socialist mayor business mixed feeling reader view dont doubt protesting powerful reader view bill cut service editorial cartoon rubio hegseth slam medium iran strike leak professional stabber undermining victory upper township renews liquor license deauville inn condition bamberg county sheriff office detention center honor employee behind curtain ai urgency call modern marshall plan gop accused pressuring lobbyist drop gaming client ugly pa budget fight whirlwind hour trump israeliran ceasefire agreement came together lose bidwells legacy lose bidwells legacy tremendous victory everybody trump iran strike cable vision pro luxshare replacing foxconn apple ecosystem trump hoping comprehensive peace agreement iran witkoff order trump administration another wrongly deported man overdoses iredell county proactive approach helping eliminating fluoridation carry health risk eliminating fluoridation carry health risk whirlwind hour trump israeliran ceasefire agreement came together whirlwind hour trump israeliran ceasefire agreement came together kennedyappointed cdc vaccine panel scrutinize childhood vaccine schedule trust president pray country trust president pray country everyday ethic everyday ethic columbia trustee view higher education crossroad choose builder destroyer im veteran democratic congressman gop ought hard iran bill include sale public land opinion bill include sale public land opinion rare earth startup without subsidy support cant shake china control asra nomani iran ideological foot soldier wage proxy war america death heart attack whats killing instead trump lawyer doj enforcer face confirmation hearing federal judgeship opinion berkshire carousel horse ride carry downtown destination sustainability normalization american indecency iran strategic blunder paved humiliating defeat expert happier healthier kid play decade obergefell lgbtq threat exclusive thune urge light touch ai regulation everything trump pick appeal judge seen illsuited lifetime appointment skinnytok rebranded eating disorder dangerously fast scoop trump admin cut contract scientific publishing giant contact cayuga county federal county elected iranian royalty fed local rumor mill ago bomb peace dont work together bomb peace dont work together marine sentenced sexual assault japan feeling represented district congressman feeling represented district congressman nato summit yield defense spending trump alliance trump isnt ready ceasefire massie zambian president burial halted begin promise remove worst worst arrested known immigrant murderer super coral supplement inside lab save great barrier reef hygiene rating handed doncaster establishment trump israeli intelligence significant damage iran nuclear facility halfcentury legal logjam killer coast banker wife face execution patriotic season searching america public forum bill threatens mental health care aging entrepreneur face new policy hurdle help highyielding dividend stock buy haul trump triumph nato bow pressure defense pledge rep mike quigley trump put ego pocket rep mike quigley intel suggesting limited damage iran nuclear program criminal justice expert implication karen verdict morning brief nato commits defense spike nyc pick socialist expert push transing kid trump pick appeal judge draw controversy zohran mamdani set defeat cuomo nyc mayoral primary upset history korean war begin australian outback transformed water rubio dont believe report modest damage iran pell grant cut blow maine economic future opinion pell grant cut blow maine economic future opinion supreme blessed samesex marriage ago backlash brewing franklin board modifies district policy discussion astronomical society public night saturday editorial minnesota shooting shatter trust faith bridge builder announces recipient technical career investment grant ago issue warning fake inheritance scam column pursue smarter choice northern border scatec asa subscription employee share purchase programme exclusive shell early acquire rival bp wsj palantir stock hit alltime high whats vimergy brings mouth america campaign washington dc expose system profit american sicker cpsc urge firework safety ahead holiday metas insane technology give user something screen deliver mark zuckerberg future ill beam charles river laboratory stock underperforming sp charles river laboratory stock underperforming sp national survey find american favor federal budget completely different congress developing bumble cut workforce online dating apps aim improve user experience wsj aerovironment stock soaring aerovironment stock soaring nvidia stock soar near record high whats driving rally forget crossfit million fitness event taking teacher chatgptand getting seattle fifas club world cup skeptic bitcoin rise nyse battle trump crypto coming mortgage next ai impact explores potential ai improve decisionmaking increase efficiency across critical national security operation buy slide insurance stock slde ipo buy slide insurance stock slde ipo carnival booking surge wall street talking solstad renews partnership marlink next stage digital transformation forester financial welcome new leadership board director trump megabill economic agenda spur growth reduce national debt according white house report invested oracle ago worth amazon selling espresso machine shopper great coffee starbucks another retail chain liquidating chapter bankruptcy island flu island flu island flu island flu siili solution plc share repurchase island flu aigenerated scam claim victim yearoveryear declining consumer concern new sift report reveals island flu island flu island flu island flu russia boost export china favorite russian crude island flu data analytics power governs nextgen digital twin island flu shiba inu left pepe dollar tokenomics attract institutional investor shiba inus massive dilution risk intrinsic therapeutic announces implantation barricaid annular closure device via endoscopic approach happy limited announces closing initial public offering island flu island flu island flu island flu fed chair powell crypto industry maturing becoming mainstream island flu invent inventor develops temporary replacement windshield wiper mho island flu island flu island flu nostalgic pepsi brand roll new flavor rival coke launch version pictory introduces world ai video mcp server pictory introduces world ai video mcp server rosen trusted leading firm encourages rocket pharmaceutical investor secure counsel important deadline security class action rckt wheel fallen corn market wheel fallen corn market senate minority schumer treated dehydration area hospital office study find trump favored nation drug proposal raise outofpocket cost without pbm reform study find trump favored nation drug proposal raise outofpocket cost without pbm reform valuesinaction foundation honor leadership across valuesinaction foundation honor leadership across new sale plummet expected high mortgage rate sink demand bi claim stablecoins fail money call strict limit role tidy patio aerobroom cordless leaf blower broom skin cancer linked climate change hims health ceo compounding novo weightloss drug continue report himsnyse seeking alpha ahold delhaize usa tap lion executive cfo paychex stock take hit margin squeeze overshadows outlook spotify stock hit record high pricetarget hike american became millionaire neigbors getting rich pacific life introduces new variable universal life insurance product available ulta beauty cfo paula oyibo quits pick insider interim role roll bottle change new ban target shower supply cordially invited critique jeff bezos lauren sanchez wedding invitation robinhood ceo highlight retail investor interest nvidia tesla middle east tension barely blip hot weather safety trick pet hot weather safety advice pet mark walter lakers sale team expected close later clever carnivore announces scalable costcompetitive delicious cultivated pork clever carnivore announces scalable costcompetitive delicious cultivated pork medium advisory federal government housing announcement cape breton stock support reduced middle east tension spark riskon stock support reduced middle east tension spark riskon piston raise cardless fuel payment solution piston raise cardless fuel payment solution tsa common childrens toy allowed plane share tesla sinking navigating complexity crossborder freight invent inventor develops new shoe cleaning device mho overture map launch gers global interoperable geospatial id drive data interoperability gain start small best new meme coin join month moon kandal venture limited announces pricing initial public offering listing nasdaq woodside close stake sale louisiana lng project kandal venture limited announces pricing initial public offering listing nasdaq business wary washington europe fret left behind ai battlefield senate prepares vote bill trump meet iran next trump megabill economic agenda spur growth reduce national debt according white house report fox racist smear zohran mamdani fail new york mayoral race un agency cant locate iran uranium strike yakima start work water wastewater connection several neighborhood trump israel airstrike destroyed crucial nuclear facility set iran denver judge decide fate subpoena employee sue gov polis halt compliance reader opinion preparing landscape trump label nycs mamdani communist lunatic senate gop opening offer hospital fund california found violation title ix clash trump transgender athlete man indicted hate crime charge attack boulder demonstration israeli hostage house republican inch closer answer biden advisor lose executive privilege shield cordially invited critique jeff bezos lauren sanchez wedding invitation man stuck chimney rescue dog trapped building san francisco mayor daniel lurie unveils family zoning plan boost homebuilding trump denies iranian moved nuclear material strike trump denies iranian moved nuclear material strike donald trump ashamed betraying afghan ally opinion trump denies iranian moved nuclear material strike kennedy new vaccine adviser meet kennedy new vaccine adviser meet kennedy new vaccine adviser meet kennedy new vaccine adviser meet kennedy new vaccine adviser meet kennedy new vaccine adviser meet cayuga county budget reality raise tax cut deeper trump denies iranian moved nuclear material strike trump denies iranian moved nuclear material strike trump denies iranian moved nuclear material strike trump hegseth seethe fake medium doubting strike obliterated iranian nuclear site scum maverick select cooper flagg overall nba draft early intelligence report suggests strike set iran nuclear program month trump attack iran pushed diplomacy kim jong un reach tracking firstround pick nba draft trump affirms commitment nato article pledge mutual defense trump nato chief mark rutte calling daddy unanimous wisconsin supreme curtails governor partial veto power unanimous wisconsin supreme curtails governor partial veto power dead congressman social medium account resurrected boost chief staff congressional bid schumer hospitalized dehydration dc nears degree myth iran invincibility broken fallout farreaching pope leo xiv urge iranisrael war reject bullying arrogance peace new york man arrested maine drug trafficking charge longlasting insulin take another step forward latest clinical trial tony abbott advance supporter bequeathing money rightwing protect australian value excessive social medium found harm teenager mental health expert moderation cruel joke tax concession drive donation australia richest private school must stop critic argue trump lay spain nato defense spending trump lay spain nato defense spending trump lay spain nato defense spending agree climate feel heat past public policy crisis costly past public policy crisis costly past public policy crisis costly hood lawmaker arent deadlocked regulation toyota tlmoda salvation army team distribute backpack school supply student nationwide partner different attorney appeal appeal lawyer wichita donald trump decision strike iran legal trump lay spain nato defense spending trump lay spain nato defense spending trump lay spain nato defense spending shasti conrad democratic party dnc vice chair race durbin tee bove judiciary hearing kick trump assessment iran nuclear facility damage complete report zohran mamdani nycs business community terrified lawless act defiance doj biden judge refusing follow supreme order chatgpt ai tool changing teaching profession microsoft sued author book ai training democrat primary voter reward prosecutor indict trump senator air concern doj budget proposal billionaire ackman musk rebuke zohran mamdanis nyc mayoral primary senate bill sensible cure ada abuse senate bill sensible cure ada abuse senate bill sensible cure ada abuse senate bill sensible cure ada abuse democrat staffer arrested abducting assaulting woman loose posting bond baumgartner northwest republican rfk jr reopen niosh worker safety office spokane senate bill navigating new noncompete restriction healthcare practitioner texas trump meet iran next israel iran claim trumpbrokered truce carlisle vote sell fire engine address upcoming project gop florida ag uthmeier supreme immigration trump visit uk take place buckingham palace stock hang near record wall street take breath following hamas preparing attack american contractor helping distribute aid gaza bezos arrives venice protester starstudded wedding highlight growing inequality new dogsized dinosaur specie discovered tax collection tumble latest washington budget forecast trump white house biden aide sweating badly new yorkers visitor cope extreme heat social security tax cut trump new bill retiree jerald mcnair school youth continue jeff bezos italian wedding senate majority run moderate america eric dane jensen ackles countdown youre dreaming score dozen early deal mattress vulnerable island dem warns mamdani extreme nyc primary upset alligator alcatraz desantis float building another immigration detention center federal judge order labor department job corp running lawsuit federal judge order labor department job corp running lawsuit federal judge order labor department job corp running lawsuit federal judge order labor department job corp running lawsuit federal judge order labor department job corp running lawsuit eric adam real chance stop mamdani andrew cuomo announce dropping trump admin sue federal judge maryland immigration order faith family sue block texas new ten commandment school faith family sue block texas new ten commandment school faith family sue block texas new ten commandment school faith family sue block texas new ten commandment school faith family sue block texas new ten commandment school faith family sue block texas new ten commandment school</t>
+          <t>nan</t>
         </is>
       </c>
     </row>
@@ -550,12 +546,12 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>jeff bezos and blue origin engaged with trump administration for government contract amid elon musk rift with the president report best smart glass with camera to buy in iran confirms nuclear site damaged a trump promise a meeting next week sitime corporation announces pricing of followon public offering analysisinvestors shore up defence against another august market rout kroger parent company of ralphs plan to close dozen of grocery store investor shore up defence against another august market rout reuters city council committee back minimum wage for hospitality worker who winning the innovation race new year analysis point to what matter most avermedia unveils two new hdmi capture device for creator at every level who winning the innovation race new year analysis point to what matter most why trump need the world to believe iran nuclear program is obliterated how japan and alaska pioneered the global market for lng the alaska town at the center of trump billion lng push ai reasoning problem why thinking model may not actually be smarter bik data analysis indicates including bnpl transaction data in credit history could help almost every second thinfile customer improve their creditworthiness north korea opening a tourist site on it east coast next week thats key to it tourism hope eu rule out production aid in blow to battery cleantech industry hong kong home price little changed in may electricity use for commercial computing could surpass space cooling ventilation tim draper say this will be the fate of bitcoin and the dollar in year billionaire highlight apps built on btc that matter california raise the bar with two three starred restaurant joining selection storage project planned for laurel oak ranch veteran analyst drop bold new call on nvidia stock yahoo finance buyer emerge for northvolt carlsbad newly opened lilo restaurant crowned with a michelin star fujitsus uvance wayfinders consulting empowers customer to evolve business foundation leveraging data and ai strongest naruto character ranked oxford cambridge fall in global college ranking expert say it a red flag for uk innovation trump familybacked world liberty financial plan to launch a new app that will make it easy for lay investor to use crypto at least reason why trump should reject a nobel peace prize china fintech giant ant double down on health care with new ai app and it want it to go global top meme coin to buy for with real narrative and epic roadmaps beijing ramp up stimulus a uschina trade tension threaten recovery kratos defense security solution inc price public offering of common stock asia fx firm dollar hit yr low a trump call for rate cut amid powell feud is this the most political fashion item ever south korea central bank adjusts open market operation to boost money supply mark zuckerbergs meta beat lawsuit over ai training on book judge find no meaningful evidence on market dilution analysis trump claim the press is demeaning the military but questioning power is patriotic colorado native nique clifford selected with no overall pick in nba draft wall street panic a socialist set to take over new york reit tumble at the idiocy of it all enthusiast gaming announces annual general meeting top desktop deal for june alienware lenovo hp and more enthusiast gaming announces annual general meeting colorado proposal seek to double income tax rate for taxpayer who earn at least million bitcoin top this key level a institution pile on ethereum dogecoin rangebound analyst say buying btc now is like buying it for in blacklisted by the u and backed by beijing this chinese ai startup ha caught openais attention vietnam to remove death penalty for embezzlement sparing tycoon life why trump strike on iran will leave north korea more determined than ever to keep it nuke acen and upc renewables break ground on over mw of new renewable energy project in india firm outline audit into iedc operation over past year rove pest control join force with greenix pest control optiva inc announces result of annual meeting mar acquisition of pringles maker trigger eu alarm dw isisinspired drone war plan leaked from u national security council china will take forceful step to boost consumption premier li say fema is not a replacement for insurance coverage risk management expert say here why cnbc daily open funny how the sp is teasing a new high amid uncertainty top poco phone under r first nordic announces annual general meeting voting result judge reject author claim that meta ai training violated copyright variety trump organization scrap made in the usa tag for it gold t smartphone asian stock hesitant dollar slide on trump attack on powell australia job vacancy bounce in may quarter ab data show hm share jump a it flag summer shopping pickup why not an islamic bomb how israel planned failed to stop pakistan going nuclear asos shopper say they were banned for making too many return sembrando vida and mexinol establish the first publicprivate partnership in sinaloa to build local capacity tesla begin rolling out self driving service in texas flexiview lending close million fixandflip loan in montpelier vermont how daddy talk and trump and ruttes bromance stole the nato spotlight htc partner with ntt com to forge a new model for immersive entertainment in japan murata push capacitor design with world first fvdc mlcc in inch size for automotive application bay miner launch aipowered cloud mining supporting bitcoin ethereum sol xrp litecoin and dogecoin jefferson capital announces pricing of initial public offering jefferson capital announces pricing of initial public offering it not my responsibility working with autonomyrestricting algorithm facilitates unethical behavior and displacement of responsibility new covidwave scarecampaign a massive flop the secret out top meme coin to buy that are taking over crypto influencer portfolio best malayalam cop thriller on ott you cant miss craft telemedicine launch to redefine specialty care with humancentered my bos lead the right way understanding how and when the institutionalization of ethic impact supervisor leadership style michael novogratzs galaxy and invesco file to launch solana etf what you should know about qsol trump judicial nominee bove denies advising justice department lawyer to ignore court order treasury yield fall a concern grow over trump criticism of powell inplay oil corp announces annual meeting voting result for election of director trump admin move to let borrower use crypto in mortgage application alaska commissioner of revenue adam crum and prospr aligned announce launch of the frontier economic fund nyse akaf getchell gold corp announces total debenture conversion walmart is selling an easy to assemble gaming chair for and shopper say it quality is excellent cathie wood double down on shopify buy the dip dump million worth of robinhood stock at peak tariff cost boost demand for efficiency in reverse logistics ap technology summarybrief at pm edt ap technology summarybrief at pm edt how chatgpt and other ai tool are changing the teaching profession modernday monopoly gop senator sound alarm on mega corporation hijacking u beef supply hims investor alert robbins geller rudman dowd llp announces that hims hers health inc investor with substantial loss have opportunity to lead the hims hers class action lawsuit denis villeneuve to direct next james bond film international paper to release secondquarter earnings on july trump latest rejection of intelligence assessment reflects a long distrust of spy agency editorial stay up to date on status of water recreation option trump official to give first classified briefing to congress on iran strike iran confirms nuclear site damaged a trump promise a meeting next week republican congresswoman office evacuated after proabortion activist send chilling threat cal thomas make america clean again john hood nc lawmaker arent deadlocked on regulation bull take yearold noa essengue at no for central division lone firstround pick eu leader meet to discus tougher russia sanction u tariff and middle east conflict trump official to give first classified briefing to congress on iran strike trump official to give first classified briefing to congress on iran strike trump latest rejection of intelligence assessment reflects a long distrust of spy agency trump latest rejection of intelligence assessment reflects a long distrust of spy agency senior are the fastestgrowing age group in the bay area and nationwide dear neighbor it because of my value my turn were running out of caregiver im scared for the future larry efird an uncommon spirit why trump need the world to believe iran nuclear program is obliterated how a california psychology student exposed the dark side of therapy education my turn usa bombed iran now the electrical grid and your network are in the crosshairs letter to the editor watt need your support editorial baltimore sun trump entry into iran war left congress mia letter to the editor thanks to city public work steven borne absentee ballot and access help people vote keith kuenning new hampshire budget betrays it child trump announces iran nuclear talk following u strike that severely damaged iranian nuclear program little league serra mesa tierrasanta septum set to vote on budget proposal thursday this is a real doomsday scenario jonah goldberg u right to bomb iran with or without nuclear specter ted talley tinkering trump creates problem where none exist kratos defense security solution inc price public offering of common stock is this the most political fashion item ever analysis trump claim the press is demeaning the military but questioning power is patriotic vietnam to remove death penalty for embezzlement sparing tycoon life mamdani say listening making city affordable key part of campaign trump considering several candidate for next federal reserve chair florida rep kat cammack say her office wa evacuated due to death threat florida rep kat cammack say her office wa evacuated due to death threat why trump strike on iran will leave north korea more determined than ever to keep it nuke miranda devine trumpderangement syndrome drive deep state leaker cnn to treasonous length to deny prez a victory live update hegseth will hold new conference to respond to intelligence report on iran strike nato survives another day sf resident to see a hike in trash fee sembrando vida and mexinol establish the first publicprivate partnership in sinaloa to build local capacity minnesota solar energy advocate mourn the loss of champion rep melissa hortman author of law boosting industry htc partner with ntt com to forge a new model for immersive entertainment in japan citrix release emergency patch for actively exploited cve in netscaler adc cooper flagg is the new face of maine cooper flagg is the new face of maine donation to local organization get matching boost this week where is our mexican vacation refund weve been waiting for month after more than a year on the run gang leader recaptured florida alligator alcatraz what to know minnesota face federal lawsuit for offering illegal immigrant college tuition benefit denied to american gloversvilles antonucci surprised self with mayoral primary win honduras u discus immigration security after tense start to relation under trump administration feeling gutted msnbcs nicolle wallace is sad tren de aragua gang member were deported to cecot exclusive leading house conservative call senate bluff on trump beautiful bill la immigration detention facility a ticking time bomb immigration lawyer say expert warns senate tax cut plan could add far more to the deficit than expected trump administration sue all maryland federal judge over order blocking removal of immigrant the trump administration is suing minnesota over break in higher education for immigrant student young cuban girl asks trump to lift travel ban stopping her from joining mom in u why the fed is keeping rate steady for now rental impact fee discussed a obstacle to college station affordable housing breaking down whistleblower claim against trump judicial pick denver judge say ice subpoena doesnt comply with state law but doesnt prohibit polis from responding the u also ha a bombproof bunker in a mountain analysis a battered iran face an uncertain future after it grinding war with israel sabrina carpenter release alternate album cover after online backlash approved by god federal judge block trump admin from ending collective bargaining for some federal worker independence day drone show spark council debate lt cmdr nathan ouellette retires after year of service veteran from deerfield named nyu truman scholar yearold billing boy remembered a stepfather is sentenced for his murder armed immigration officer arent even telling local police at time about their raid leak are a problem congress feud over trump limit on sharing intel duke phenom cooper flagg go to dallas maverick with no overall pick in nba draft cia say it ha evidence iran nuclear program wa severely damaged a assessment of u strike impact continue little league north park cholla lake mar pending acquisition of kellanova clear ftc antitrust review oklahoma supreme court begin oral argument on state question trump spy chief say new intel show iran nuclear facility were destroyed meta win artificial intelligence copyright case in blow to author republican suddenly realize voter hate their health care cut editorial class of youve earned your place this is your time trump drop made in the usa label for new phone and a debate ensues how to define made trump drop made in the usa label for new phone and a debate ensues how to define made trump drop made in the usa label for new phone and a debate ensues how to define made trump drop made in the usa label for new phone and a debate ensues how to define made trump win over lifelong democrat autoworker with big beautiful bill vehicle loan tax benefit oregon house pass bipartisan bill to combat chronic absenteeism in school republican candidate who ran against maxine water admits to misusing campaign donation scoop protrump group unleashes first tv ad against massie trump administration to investigate university of california hiring practice ltte noise at the uv pilot site</t>
+          <t>ignitex sponsor taiwan blockchain hackathon empowering next generation of web innovator is the rule unattainable in typical u household need to spend of income to afford the medianpriced home b rfg advisory launch suite of active etf free settlement money from att who qualifies and when you can file your claim cnet what house and senate republican cant agree on in trump tax bill pony ai the next trillion robotaxi play fcps look toward next decade of school construction enrollment growth tri pointe home inc announces second quarter earnings release and conference call date growth stock that turned investment year ago into over million today the everglades foundation name shannon estenoz a it first chief policy officer santech holding announces unaudited financial result for the first half of fiscal year b bleakley add advisor coach ray sclafani to board of director air canada completes million substantial issuer bid acting on it commitment to balanced longterm capital allocation zapp ev report financial result for the six month ended march and provides operational update ufe doesnt remove fibroidsheres what woman arent being told quincy data precision time exchange service recognized a best time stamping measurement system by tradingtech insight award santech holding announces unaudited financial result for the first half of fiscal year a regulation fade a nonprofit push voluntary standard is the rule unattainable in typical u household need to spend of income to afford the medianpriced home improvement to make playground more accessible underway east texas bbb warns of major data breach chainlink whale diversifying into bitcoin solaris before it inevitable price explosion first quantum provides notice of second quarter result the everglades foundation name shannon estenoz a it first chief policy officer first patient enrolled in aclarions groundbreaking clarity trial pure property management named to inc best workplace hidden cost of homeownership now exceed a year kalmar and cagliari roro terminal continue collaboration with new order for terminal tractor no one expected oil price to crash this much first quantum provides notice of second quarter result sweden riksbank see some probability for further rate cut amid murky outlook buy now pay later plan will soon impact your credit scorewhat you need to know well fargo hike microsoft price target say ai business could reach billion in revenue cd rate today june take home up to teenage sprint sensation gout gout break his own m australian record in first race abroad china and india cut import of lowerquality coal from indonesia fueling ai data center behind the meter solution cherry bekaert appoints dan wheadon a cfo advisory leader is apa stock underperforming the dow bitget head to milan a sponsor at ethmilan watch fed chair jerome powell testify live before senate banking panel could berkshire hathaway stock double by even without warren buffett could berkshire hathaway stock double by even without warren buffett trimble tdks advanced navigation solution to enhance automotive positioning drone maker aerovironment share pop on earnings beat american in line to pocket up to k from m data breach settlement exact date to note down sp future muted with focus on powell testimony finding a mentor can be key to your success expert tip for finding one it going to get you place qdoba restaurant expands with th location in florida skelton big state budget question linger about crime medical delta tunnel former circuit clinical colleague join force again to form health care startup where will coreweave stock be in year how social security privatization could change the role of ira in your portfolio wayfair is selling a lounge chair for just and shopper say it will turn your patio into a little oasis how tariff might impact u car price by brand exclusive uber and palantir alum raise m to disrupt corporate recruitment with ai fortune amazon is selling a stunning citizen ecodrive watch for and buyer call it an eyecatcher amazon prime day start date early deal and shopping tip share in wr berkley corporation nysewrb purchased by kentucky retirement system insurance trust fund kentucky retirement system insurance trust fund make new investment in eversource energy nysees state of alaska department of revenue buy share of hyatt hotel corporation nyseh new york city is closer to electing a democratic socialist mayor business have mixed feeling why blackberry share are trading higher by around here are stock moving premarket kentucky retirement system insurance trust fund invests in citizen financial group inc nysecfg williamssonoma inc nysewsm share bought by janney montgomery scott llc kentucky retirement system insurance trust fund ha stock holding in tyson food inc nysetsn jfs wealth advisor llc purchase share of johnson control international plc nysejci omnicom group inc nyseomc stake reduced by continuum advisory llc xml financial llc ha holding in eaton corporation plc nyseetn exchange traded concept llc raise stock holding in allegion plc nysealle exchange traded concept llc ha stock holding in air product and chemical inc nyseapd gm inc nysegms share sold by state of alaska department of revenue williamssonoma inc nysewsm share acquired by janney montgomery scott llc trump advisor stephen miller reportedly hold stake worth million in ice contractor palantir he could easilyhave a direct and predictable impact micron face earnings test after share price doubled since april nba owner unanimously approve b sale of wolf wnbas lynx from taylor to lorerodriguez group first female reporter at kpnx in phoenix diane kalas dy bitcoin price rise the crypto is being boosted by these factor today verizon team up with nokia to bring hightech g boost to busy british port verizon team up with nokia to bring hightech g boost to busy british port usdinr inch up a market weighs middle east ceasefire amid fed and rbi action jadwa investment buy majority stake in saudi retailer makhazen alenaya why are some people calling for a mcdonalds boycott alexandria real estate equity inc nyseare share purchased by flagship harbor advisor llc kentucky retirement system insurance trust fund acquires new position in synchrony financial nysesyf kentucky retirement system insurance trust fund cut position in darden restaurant inc nysedri flagship harbor advisor llc purchase share of dexcom inc nasdaqdxcm how private capital could be the key to rebuilding america is palantir stock outperforming the dow is palantir stock outperforming the dow retirement system of alabama ha million stock position in firstenergy corporation nysefe retirement system of alabama sell share of cm energy corporation nysecms retirement system of alabama reduces position in kellanova nysek pfg investment llc decrease stake in ishares msci emerging market etf nysearcaeem today quordle hint and answer for june detroit station to open coffee shop in hope of connecting to the community trump medium stock edge higher premarket after nyse file to list truth social bitcoin and ethereum etf share flagship harbor advisor llc ha stake in edward lifesciences corporation nyseew retirement system of alabama lower position in devon energy corporation nysedvn wealth enhancement advisory service llc increase position in public service enterprise group incorporated nysepeg despite promise to remove worst of the worst ice ha arrested only of known immigrant murderer what to do when success make you lose touch with your identity beef price at record high trump attack on iran pushed diplomacy with kim jong un further out of reach more than idaho airman are deployed in the middle east are they safe impactful bill that passed in idaho legislative session this year childrens hospital los angeles threw trans kid overboard teenage sprint sensation gout gout break his own m australian record in first race abroad the longest battle in world war i occurred around which french city the federalist society isnt going anywhere the federalist society isnt going anywhere trump united surveillance state of america how will your data be deployed glen alpine alderman step down cite board behavior highschoollike squabble in resignation orangeburg county council reject homeowner request to close road sioux city resident express concern to staff of sen joni ernst about federal budget cut new york city is closer to electing a democratic socialist mayor business have mixed feeling reader view dont doubt those protesting the powerful reader view beautiful bill could cut service we need editorial cartoon for june rubio hegseth slam medium over iran strike leak professional stabber undermining u victory upper township renews liquor license for the deauville inn on one condition bamberg county sheriff office detention center honor employee behind the curtain ai urgency call for a modern marshall plan gop leader accused of pressuring lobbyist to drop gaming client in ugly pa budget fight a whirlwind hour how trump israeliran ceasefire agreement came together letter let not lose more of bidwells legacy letter let not lose more of bidwells legacy a tremendous victory for everybody trump on iran strike from cable to vision pro how luxshare is replacing foxconn in apple ecosystem trump hoping for comprehensive peace agreement with iran witkoff court order trump administration to return another wrongly deported man overdoses are down in iredell county a more proactive approach may be helping letter eliminating fluoridation carry health risk letter eliminating fluoridation carry health risk a whirlwind hour how trump israeliran ceasefire agreement came together a whirlwind hour how trump israeliran ceasefire agreement came together kennedyappointed cdc vaccine panel say it will scrutinize the childhood vaccine schedule letter trust our president and pray for our country letter trust our president and pray for our country ice will see you now everyday ethic what if you had only one day to live everyday ethic what if you had only one day to live a columbia trustee view higher education is at a crossroad let choose builder over destroyer im a veteran and former democratic congressman here why the gop ought to think hard about iran big beautiful bill should not include sale of public land opinion big beautiful bill should not include sale of public land opinion rare earth startup say without subsidy and support u cant shake china control asra nomani iran ideological foot soldier wage proxy war in america death from heart attack are way down here whats killing u instead trump lawyer and doj enforcer face confirmation hearing for federal judgeship our opinion berkshire carousel horse ride again can they carry this downtown destination to sustainability the normalization of american indecency iran strategic blunder paved the way for humiliating defeat expert say want happier healthier kid let them play a decade after obergefell lgbtq right remain under threat exclusive thune urge light touch on ai regulation when everything go wrong trump pick for appeal judge seen a illsuited to lifetime appointment skinnytok rebranded eating disorder dangerously fast scoop trump admin cut contract with scientific publishing giant how to contact cayuga county federal state and county elected official iranian royalty fed local rumor mill year ago letter bomb and peace dont work well together letter bomb and peace dont work well together u marine sentenced to year over sexual assault in japan letter not feeling represented by district congressman letter not feeling represented by district congressman nato summit yield a big win on defense spending for trump but key question over the alliance remain trump isnt ready for a ceasefire with massie zambian president burial halted just a it wa to begin despite promise to remove worst of the worst ice ha arrested only of known immigrant murderer super coral and supplement inside the lab trying to save the great barrier reef food hygiene rating handed to two doncaster establishment trump did the right thing israeli intelligence see significant damage to iran nuclear facility official say after a halfcentury of legal logjam will killer of coast banker wife face execution june during patriotic season searching for the right america public forum bill threatens mental health care aging entrepreneur face new policy hurdle here how to help highyielding dividend stock to buy for the long haul trump triumph nato bow to u pressure with defense pledge rep mike quigley tell trump to put your ego in your pocket rep mike quigley on intel suggesting limited damage to iran nuclear program a criminal justice expert on the implication of the karen read verdict morning brief nato commits to defense spike nyc pick a socialist expert push transing kid trump pick for appeal judge draw controversy zohran mamdani set to defeat cuomo in nyc mayoral primary upset today in history june korean war begin australian outback transformed by water rubio dont believe report of only modest damage in iran pell grant cut would be a blow to maine economic future opinion pell grant cut would be a blow to maine economic future opinion the supreme court blessed samesex marriage year ago is a backlash brewing franklin board modifies some district policy after discussion astronomical society to hold public night saturday editorial minnesota shooting shatter trust faith bridge builder announces first recipient of technical career investment grant year ago june state issue warning on fake inheritance scam column pursue smarter choice on the northern border scatec asa subscription for the employee share purchase programme exclusive shell in early talk to acquire rival bp wsj palantir stock hit alltime high whats going on vimergy brings mouth of america campaign to washington dc to expose a system that profit while american get sicker cpsc urge firework safety ahead of july th holiday metas insane technology give user something no screen today can deliver say mark zuckerberg in the future ill just beam in is charles river laboratory stock underperforming the sp is charles river laboratory stock underperforming the sp national survey find american favor a federal budget completely different from the one congress is developing bumble to cut of workforce a online dating apps aim to improve user experience wsj why aerovironment stock is soaring today why aerovironment stock is soaring today nvidia stock soar near record high whats driving the rally forget crossfit this million fitness event is taking over how teacher are using chatgptand getting their time back how seattle won over fifas club world cup skeptic bitcoin rise nyse battle for trump etf and crypto may be coming to mortgage next ai for impact day explores the potential for ai to improve decisionmaking and increase efficiency across critical national security operation should you buy slide insurance stock after the slde ipo should you buy slide insurance stock after the slde ipo carnival booking surge ha wall street talking already solstad renews partnership with marlink for it next stage of digital transformation forester financial welcome new leadership to it board of director trump megabill and economic agenda would spur growth and reduce national debt according to white house report here how much invested in oracle year ago would be worth today amazon is selling a espresso machine for and shopper say it make great coffee just like starbucks another huge retail chain liquidating after chapter bankruptcy duck return to a long island farm that lost it entire flock to the bird flu duck return to a long island farm that lost it entire flock to the bird flu duck return to a long island farm that lost it entire flock to the bird flu duck return to a long island farm that lost it entire flock to the bird flu siili solution plc share repurchase duck return to a long island farm that lost it entire flock to the bird flu aigenerated scam claim more victim yearoveryear despite declining consumer concern new sift report reveals duck return to a long island farm that lost it entire flock to the bird flu duck return to a long island farm that lost it entire flock to the bird flu duck return to a long island farm that lost it entire flock to the bird flu duck return to a long island farm that lost it entire flock to the bird flu russia to boost export of china favorite russian crude in july duck return to a long island farm that lost it entire flock to the bird flu how data analytics power and governs nextgen digital twin duck return to a long island farm that lost it entire flock to the bird flu shiba inu to be left in pepe dollar tokenomics attract institutional investor over shiba inus massive dilution risk intrinsic therapeutic announces the first implantation of the barricaid annular closure device via endoscopic approach happy city holding limited announces closing of initial public offering duck return to a long island farm that lost it entire flock to the bird flu duck return to a long island farm that lost it entire flock to the bird flu duck return to a long island farm that lost it entire flock to the bird flu duck return to a long island farm that lost it entire flock to the bird flu fed chair powell the crypto industry is maturing becoming more mainstream duck return to a long island farm that lost it entire flock to the bird flu invent inventor develops temporary replacement for windshield wiper mho duck return to a long island farm that lost it entire flock to the bird flu duck return to a long island farm that lost it entire flock to the bird flu duck return to a long island farm that lost it entire flock to the bird flu nostalgic pepsi brand from the s roll out new flavor week after rival coke launch it version pictory introduces one of the world first ai video mcp server pictory introduces one of the world first ai video mcp server rosen a trusted and leading law firm encourages rocket pharmaceutical inc investor to secure counsel before important deadline in security class action rckt have the wheel fallen off the corn market have the wheel fallen off the corn market senate minority leader schumer treated for dehydration at area hospital his office say study find trump most favored nation drug proposal could still raise outofpocket cost without pbm reform study find trump most favored nation drug proposal could still raise outofpocket cost without pbm reform valuesinaction foundation honor leadership from across the u valuesinaction foundation honor leadership from across the u new home sale plummet more than expected a high mortgage rate sink demand bi claim stablecoins fail a money call for strict limit on their role tidy up your patio in second get off the aerobroom in cordless leaf blower broom is skin cancer linked to climate change hims hers health ceo say compounding novo weightloss drug will continue report himsnyse seeking alpha ahold delhaize usa tap food lion executive a cfo paychex stock take a hit a margin squeeze overshadows outlook spotify stock hit record high get pricetarget hike american became millionaire in way your neigbors are getting rich and how to keep up pacific life introduces new variable universal life insurance product now available through state farm ulta beauty cfo paula oyibo quits pick insider for interim role u state to roll out huge bottle change in new july law and the ban target all of your shower supply you are cordially invited to critique jeff bezos and lauren sanchez wedding invitation robinhood ceo highlight retail investor interest in nvidia tesla despite middle east tension barely a blip hot weather safety trick for your pet hot weather safety advice for your pet mark walter and lakers say sale of the team is expected to close later this year clever carnivore announces scalable costcompetitive and delicious cultivated pork clever carnivore announces scalable costcompetitive and delicious cultivated pork medium advisory federal government to make housing announcement in cape breton stock see support a reduced middle east tension spark riskon stock see support a reduced middle east tension spark riskon piston raise m for cardless fuel payment solution piston raise m for cardless fuel payment solution tsa say these common childrens toy may not be allowed on plane why share of tesla are sinking today navigating the complexity of crossborder freight invent inventor develops new shoe cleaning device mho overture map launch gers a global standard for interoperable geospatial id to drive data interoperability big gain start small best new meme coin to join this month before they moon kandal m venture limited announces pricing of initial public offering and listing on nasdaq woodside close stake sale in louisiana lng project kandal m venture limited announces pricing of initial public offering and listing on nasdaq ap business summarybrief at am edt wary of washington europe fret it will be left behind on an ai battlefield senate prepares for vote on big beautiful bill trump say u will meet with iran next week trump megabill and economic agenda would spur growth and reduce national debt according to white house report fox news racist smear against zohran mamdani fail in new york mayoral race un official say agency cant locate iran uranium after u strike yakima start work on water and wastewater connection in several neighborhood trump israel say u airstrike destroyed crucial nuclear facility and set iran back year denver judge to decide fate of ice subpoena a state employee sue gov polis to halt compliance reader opinion preparing the landscape trump label nycs mamdani a communist lunatic senate gop leader make opening offer on hospital fund california found in violation of title ix in clash with trump official over transgender athlete man indicted on hate crime charge in attack on boulder demonstration for israeli hostage house republican inch closer to answer a former biden advisor lose executive privilege shield you are cordially invited to critique jeff bezos and lauren sanchez wedding invitation man get stuck in chimney while trying to rescue dog trapped in building san francisco mayor daniel lurie unveils family zoning plan to boost homebuilding trump denies iranian moved nuclear material before u strike trump denies iranian moved nuclear material before u strike donald trump should be ashamed of betraying our afghan ally opinion trump denies iranian moved nuclear material before u strike kennedy new vaccine adviser meet for first time kennedy new vaccine adviser meet for first time kennedy new vaccine adviser meet for first time kennedy new vaccine adviser meet for first time kennedy new vaccine adviser meet for first time kennedy new vaccine adviser meet for first time cayuga county budget reality raise tax or cut deeper trump denies iranian moved nuclear material before u strike trump denies iranian moved nuclear material before u strike trump denies iranian moved nuclear material before u strike trump hegseth seethe at fake news medium for doubting u strike obliterated iranian nuclear site scum maverick select cooper flagg no overall in nba draft early u intelligence report suggests u strike only set back iran nuclear program by month trump attack on iran pushed diplomacy with kim jong un further out of reach tracking every firstround pick in the nba draft trump affirms his commitment to nato article pledge for mutual defense he like me trump on nato chief mark rutte calling him daddy unanimous wisconsin supreme court curtails governor partial veto power unanimous wisconsin supreme court curtails governor partial veto power dead congressman social medium account resurrected to boost former chief of staff congressional bid schumer hospitalized for dehydration a dc nears degree the myth of iran invincibility ha been broken and the fallout could be farreaching pope leo xiv urge all side in iranisrael war to reject bullying and arrogance and talk peace new york man arrested in maine on drug trafficking charge longlasting insulin take another step forward with latest clinical trial result tony abbott tell advance supporter bequeathing money to rightwing group will protect australian value excessive social medium found to harm teenager mental health but expert say moderation may be key cruel joke tax concession drive donation to australia richest private school and must stop critic argue trump lay into spain over nato defense spending trump lay into spain over nato defense spending trump lay into spain over nato defense spending we may not agree on climate but we all feel the heat past public policy make today crisis more costly past public policy make today crisis more costly past public policy make today crisis more costly hood our lawmaker arent deadlocked on regulation toyota tlmoda and the salvation army team up to distribute backpack and school supply to student nationwide can i partner with a different attorney on my appeal appeal lawyer wichita wa donald trump decision to strike iran legal trump lay into spain over nato defense spending trump lay into spain over nato defense spending trump lay into spain over nato defense spending shasti conrad leader of the wa democratic party win dnc vice chair race durbin tee off on bove a judiciary hearing kick off trump say assessment of iran nuclear facility damage wa not a complete report zohran mamdani ha nycs business community terrified lawless act of defiance doj say biden judge is refusing to follow supreme court order how chatgpt and other ai tool are changing the teaching profession microsoft sued by author over use of book in ai training democrat primary voter reward first prosecutor to indict trump senator air concern about doj budget proposal billionaire ackman and musk rebuke zohran mamdanis win in nyc mayoral primary senate bill a sensible cure for ada abuse senate bill a sensible cure for ada abuse senate bill a sensible cure for ada abuse senate bill a sensible cure for ada abuse former democrat staffer arrested for abducting assaulting woman on the loose after posting bond baumgartner northwest republican ask rfk jr to reopen niosh worker safety office in spokane thing to know about senate bill navigating new noncompete restriction for healthcare practitioner in texas trump say u will meet with iran next week israel and iran both claim win a trumpbrokered truce hold carlisle vote to sell fire engine address upcoming project gop leader back florida ag uthmeier at u supreme court on immigration trump state visit to the uk to take place this year say buckingham palace u stock hang near their record a wall street take a breath following two big day hamas is preparing attack on american contractor helping distribute aid in gaza bezos arrives in venice a protester say his starstudded wedding highlight growing inequality new dogsized dinosaur specie discovered tax collection tumble again in latest washington budget forecast trump white house clear way for biden aide to tell all i am sweating badly new yorkers and visitor cope with extreme heat no social security tax cut in trump new bill what retiree need to know jerald mcnair while school are out our youth need to continue to read jeff bezos italian wedding by the number the senate majority run through moderate america eric dane and jensen ackles in countdown youre not dreaming score dozen of early th of july deal on mattress vulnerable long island dem warns mamdani too extreme for nyc after primary upset not just alligator alcatraz desantis float building another immigration detention center federal judge order u labor department to keep job corp running during lawsuit federal judge order u labor department to keep job corp running during lawsuit federal judge order u labor department to keep job corp running during lawsuit federal judge order u labor department to keep job corp running during lawsuit federal judge order u labor department to keep job corp running during lawsuit eric adam ha a real chance to stop mamdani but andrew cuomo need to announce he dropping out trump admin sue every federal judge in maryland over immigration order faith leader and family sue to block texas new ten commandment in school law faith leader and family sue to block texas new ten commandment in school law faith leader and family sue to block texas new ten commandment in school law faith leader and family sue to block texas new ten commandment in school law faith leader and family sue to block texas new ten commandment in school law faith leader and family sue to block texas new ten commandment in school law</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>jeff bezos blue origin engaged trump administration government contract amid elon musk rift president report best smart glass camera buy iran confirms nuclear site damaged trump promise meeting next sitime corporation announces pricing followon public offering analysisinvestors shore defence another august market rout kroger parent company ralphs plan close dozen grocery store investor shore defence another august market rout reuters council committee minimum wage hospitality worker winning innovation race new analysis matter avermedia unveils new hdmi capture device creator level winning innovation race new analysis matter trump world believe iran nuclear program obliterated japan alaska pioneered global market lng alaska town center trump billion lng push ai reasoning problem thinking model smarter bik data analysis indicates bnpl transaction data credit history help almost thinfile customer improve creditworthiness north korea opening tourist site east coast next thats tourism eu rule production aid blow battery cleantech industry hong kong price little changed electricity commercial computing surpass space cooling ventilation tim draper fate bitcoin dollar billionaire highlight apps built btc matter california raise bar starred restaurant joining selection storage project planned laurel oak ranch veteran analyst drop bold new call nvidia stock yahoo finance buyer emerge northvolt carlsbad newly opened lilo restaurant crowned michelin star fujitsus uvance wayfinders consulting empowers customer evolve business foundation leveraging data ai strongest naruto character ranked oxford cambridge fall global college ranking expert red flag uk innovation trump familybacked world liberty financial plan launch new app easy lay investor crypto least trump reject nobel peace prize china fintech giant ant double health care new ai app global meme coin buy real narrative epic roadmaps beijing ramp stimulus uschina trade tension threaten recovery kratos defense security solution price public offering common stock asia fx firm dollar hit yr low trump call rate cut amid powell feud political fashion item ever south korea central bank adjusts open market operation boost money supply mark zuckerbergs meta beat lawsuit ai training book judge find meaningful evidence market dilution analysis trump claim press demeaning military questioning power patriotic colorado native nique clifford selected overall pick nba draft wall street panic socialist set take new york reit tumble idiocy enthusiast gaming announces annual general meeting desktop deal alienware lenovo hp enthusiast gaming announces annual general meeting colorado proposal seek double income tax rate taxpayer earn least million bitcoin level institution pile ethereum dogecoin rangebound analyst buying btc buying blacklisted backed beijing chinese ai startup caught openais attention vietnam remove death penalty embezzlement sparing tycoon life trump strike iran north korea determined ever nuke acen upc renewables break ground mw new renewable energy project india firm outline audit iedc operation past rove pest control join force greenix pest control optiva announces annual meeting mar acquisition pringles maker trigger eu alarm dw isisinspired drone war plan leaked national security council china take forceful step boost consumption premier li fema replacement insurance coverage risk expert cnbc open funny sp teasing new high amid uncertainty poco phone r nordic announces annual general meeting voting judge reject author claim meta ai training violated copyright variety trump organization scrap usa tag gold smartphone asian stock hesitant dollar slide trump attack powell australia job vacancy bounce quarter ab data hm share jump flag summer shopping pickup islamic bomb israel planned failed stop pakistan nuclear asos shopper banned making sembrando vida mexinol establish publicprivate partnership sinaloa build local capacity tesla begin rolling self driving service texas flexiview lending close million fixandflip loan montpelier vermont daddy trump ruttes bromance stole nato spotlight htc partner ntt com forge new model immersive entertainment japan murata push capacitor design world fvdc mlcc inch size automotive application bay miner launch aipowered cloud mining supporting bitcoin ethereum sol xrp litecoin dogecoin jefferson announces pricing initial public offering jefferson announces pricing initial public offering responsibility working autonomyrestricting algorithm facilitates unethical behavior displacement responsibility new covidwave scarecampaign massive flop secret meme coin buy taking crypto influencer portfolio best malayalam cop thriller ott cant miss craft telemedicine launch redefine specialty care humancentered bos lead understanding institutionalization ethic impact supervisor leadership style michael novogratzs galaxy invesco file launch solana qsol trump judicial nominee bove denies advising justice department lawyer ignore order treasury yield fall concern grow trump criticism powell inplay oil corp announces annual meeting voting election director trump admin move borrower crypto mortgage application alaska commissioner revenue adam crum prospr aligned announce launch frontier economic fund nyse akaf getchell gold corp announces total debenture conversion walmart selling easy assemble gaming chair shopper quality excellent cathie wood double shopify buy dip dump million worth robinhood stock peak tariff cost boost demand efficiency reverse logistics technology pm technology pm chatgpt ai tool changing teaching profession modernday monopoly gop senator sound alarm mega corporation hijacking beef supply hims investor alert robbins geller rudman dowd llp announces hims health investor substantial loss opportunity lead hims class action lawsuit denis villeneuve direct next james bond film international paper release secondquarter earnings trump latest rejection intelligence assessment reflects distrust spy agency editorial stay date status water recreation option trump give classified briefing congress iran strike iran confirms nuclear site damaged trump promise meeting next republican congresswoman office evacuated proabortion activist send chilling threat cal thomas america clean john hood nc lawmaker arent deadlocked regulation bull take yearold noa essengue central division lone firstround pick eu meet discus tougher russia sanction tariff middle east conflict trump give classified briefing congress iran strike trump give classified briefing congress iran strike trump latest rejection intelligence assessment reflects distrust spy agency trump latest rejection intelligence assessment reflects distrust spy agency senior fastestgrowing age bay area nationwide dear neighbor value turn running caregiver im scared future larry efird uncommon spirit trump world believe iran nuclear program obliterated california psychology student exposed dark therapy education turn usa bombed iran electrical grid network crosshairs editor watt support editorial baltimore sun trump entry iran war left congress mia editor public work steven borne absentee ballot access help people vote keith kuenning new hampshire budget betrays child trump announces iran nuclear following strike severely damaged iranian nuclear program little league serra mesa tierrasanta septum set vote budget proposal thursday real doomsday scenario jonah goldberg bomb iran without nuclear specter ted talley tinkering trump creates problem none exist kratos defense security solution price public offering common stock political fashion item ever analysis trump claim press demeaning military questioning power patriotic vietnam remove death penalty embezzlement sparing tycoon life mamdani listening making affordable part campaign trump considering several candidate next federal reserve chair florida rep kat cammack office evacuated due death threat florida rep kat cammack office evacuated due death threat trump strike iran north korea determined ever nuke miranda devine trumpderangement syndrome drive deep leaker cnn treasonous length deny prez victory update hegseth new conference respond intelligence report iran strike nato survives another sf resident hike trash fee sembrando vida mexinol establish publicprivate partnership sinaloa build local capacity minnesota solar energy advocate mourn loss champion rep melissa hortman author boosting industry htc partner ntt com forge new model immersive entertainment japan citrix release emergency patch actively exploited cve netscaler adc cooper flagg new face maine cooper flagg new face maine donation local organization matching boost mexican vacation refund weve waiting month run gang recaptured florida alligator alcatraz minnesota face federal lawsuit offering illegal immigrant college tuition benefit denied american gloversvilles antonucci surprised self mayoral primary honduras discus immigration security tense start relation trump administration feeling gutted msnbcs nicolle wallace sad tren de aragua gang deported cecot exclusive leading house conservative call senate bluff trump bill la immigration detention facility ticking bomb immigration lawyer expert warns senate tax cut plan add far deficit expected trump administration sue maryland federal judge order blocking removal immigrant trump administration suing minnesota break higher education immigrant student young cuban girl asks trump lift travel ban stopping joining mom fed keeping rate steady rental impact fee discussed obstacle college station affordable housing breaking whistleblower claim trump judicial pick denver judge subpoena doesnt comply doesnt prohibit polis responding bombproof bunker mountain analysis battered iran face uncertain future grinding war israel sabrina carpenter release alternate album cover online backlash approved god federal judge block trump admin ending collective bargaining federal worker independence drone spark council debate lt cmdr nathan ouellette retires service veteran deerfield named nyu truman scholar yearold billing boy remembered stepfather sentenced murder armed immigration officer arent telling local police raid leak problem congress feud trump limit sharing intel duke phenom cooper flagg dallas maverick overall pick nba draft cia evidence iran nuclear program severely damaged assessment strike impact continue little league north park cholla lake mar pending acquisition kellanova ftc antitrust review oklahoma supreme begin oral argument trump spy chief new intel iran nuclear facility destroyed meta artificial intelligence copyright blow author republican suddenly realize voter hate health care cut editorial class youve earned place trump drop usa label new phone debate ensues define trump drop usa label new phone debate ensues define trump drop usa label new phone debate ensues define trump drop usa label new phone debate ensues define trump lifelong democrat autoworker bill vehicle loan tax benefit oregon house pas bipartisan bill combat chronic absenteeism school republican candidate ran maxine water admits misusing campaign donation scoop protrump unleashes tv ad massie trump administration investigate university california hiring practice ltte noise uv pilot site</t>
+          <t>ignitex sponsor taiwan blockchain hackathon empowering next generation web innovator rule unattainable typical household spend income afford medianpriced b rfg advisory launch suite active free settlement money att qualifies file claim cnet house senate republican cant agree trump tax bill pony ai next trillion robotaxi play fcps look next decade school construction enrollment growth tri pointe announces quarter earnings release conference call date growth stock turned investment ago million everglades foundation name shannon estenoz chief policy officer santech announces unaudited financial half fiscal b bleakley add advisor coach ray sclafani board director air canada completes million substantial issuer bid acting commitment balanced longterm allocation zapp ev report financial six month ended march provides operational update ufe doesnt remove fibroidsheres woman arent quincy data precision exchange service recognized best stamping measurement system tradingtech insight award santech announces unaudited financial half fiscal regulation fade nonprofit push voluntary rule unattainable typical household spend income afford medianpriced improvement playground accessible underway east texas bbb warns major data breach chainlink whale diversifying bitcoin solaris inevitable price explosion quantum provides notice quarter everglades foundation name shannon estenoz chief policy officer patient enrolled aclarions groundbreaking clarity trial pure property named best workplace hidden cost homeownership exceed kalmar cagliari roro terminal continue collaboration order terminal tractor expected oil price crash quantum provides notice quarter sweden riksbank probability rate cut amid murky outlook buy pay later plan soon impact credit scorewhat fargo hike microsoft price target ai business reach billion revenue cd rate take teenage sprint sensation gout gout break australian record race abroad china india cut import lowerquality coal indonesia fueling ai data center behind meter solution cherry bekaert appoints dan wheadon cfo advisory apa stock underperforming dow bitget head milan sponsor ethmilan watch fed chair jerome powell testify senate banking panel berkshire hathaway stock double without warren buffett berkshire hathaway stock double without warren buffett trimble tdks advanced navigation solution enhance automotive positioning drone maker aerovironment pop earnings beat american line pocket k data breach settlement exact date note sp future muted focus powell testimony finding mentor success expert tip finding place qdoba restaurant expands location florida skelton budget linger crime medical delta tunnel circuit clinical colleague join force form health care startup coreweave stock social security privatization change role ira portfolio wayfair selling lounge chair shopper turn patio little oasis tariff impact car price brand exclusive uber palantir alum raise disrupt corporate recruitment ai fortune amazon selling stunning citizen ecodrive watch buyer call eyecatcher amazon prime start date early deal shopping tip wr berkley corporation nysewrb purchased kentucky retirement system insurance trust fund kentucky retirement system insurance trust fund investment eversource energy nysees alaska department revenue buy hyatt hotel corporation nyseh york closer electing democratic socialist mayor business mixed feeling blackberry trading higher around stock moving premarket kentucky retirement system insurance trust fund invests citizen financial nysecfg williamssonoma nysewsm bought janney montgomery scott kentucky retirement system insurance trust fund stock tyson nysetsn jfs wealth advisor purchase johnson control international plc nysejci omnicom nyseomc stake reduced continuum advisory xml financial eaton corporation plc nyseetn exchange traded concept raise stock allegion plc nysealle exchange traded concept stock air product chemical nyseapd gm nysegms alaska department revenue williamssonoma nysewsm acquired janney montgomery scott trump advisor stephen miller reportedly stake worth million contractor palantir easilyhave direct predictable impact micron face earnings test price doubled since april nba owner unanimously approve b sale wolf wnbas lynx taylor lorerodriguez female reporter kpnx phoenix diane kalas dy bitcoin price rise crypto boosted factor verizon team nokia hightech g boost busy british port verizon team nokia hightech g boost busy british port usdinr inch market weighs middle east ceasefire amid fed rbi action jadwa investment buy majority stake saudi retailer makhazen alenaya people calling mcdonalds boycott alexandria real estate equity nyseare purchased flagship harbor advisor kentucky retirement system insurance trust fund acquires synchrony financial nysesyf kentucky retirement system insurance trust fund cut darden restaurant nysedri flagship harbor advisor purchase dexcom nasdaqdxcm private rebuilding america palantir stock outperforming dow palantir stock outperforming dow retirement system alabama million stock firstenergy corporation nysefe retirement system alabama sell cm energy corporation nysecms retirement system alabama reduces kellanova nysek pfg investment decrease stake ishares msci emerging market nysearcaeem quordle hint answer detroit station open coffee shop connecting community trump medium stock edge higher premarket nyse file list truth social bitcoin ethereum flagship harbor advisor stake edward lifesciences corporation nyseew retirement system alabama lower devon energy corporation nysedvn wealth enhancement advisory service increase public service enterprise incorporated nysepeg promise remove worst worst arrested known immigrant murderer success lose touch identity beef price record high trump attack iran pushed diplomacy kim jong un reach idaho airman deployed middle east safe impactful bill passed idaho legislative session childrens hospital los angeles threw trans kid overboard teenage sprint sensation gout gout break australian record race abroad longest battle world war occurred around french federalist society isnt anywhere federalist society isnt anywhere trump united surveillance america data deployed glen alpine alderman step cite board behavior highschoollike squabble resignation orangeburg county council reject homeowner request close road sioux resident express concern staff sen joni ernst federal budget cut york closer electing democratic socialist mayor business mixed feeling reader view dont doubt protesting powerful reader view bill cut service editorial cartoon rubio hegseth slam medium iran strike leak professional stabber undermining victory upper township renews liquor license deauville inn condition bamberg county sheriff office detention center honor employee behind curtain ai urgency call modern marshall plan gop accused pressuring lobbyist drop gaming client ugly pa budget fight whirlwind hour trump israeliran ceasefire agreement came together lose bidwells legacy lose bidwells legacy tremendous victory everybody trump iran strike cable vision pro luxshare replacing foxconn apple ecosystem trump hoping comprehensive peace agreement iran witkoff order trump administration another wrongly deported man overdoses iredell county proactive approach helping eliminating fluoridation carry health risk eliminating fluoridation carry health risk whirlwind hour trump israeliran ceasefire agreement came together whirlwind hour trump israeliran ceasefire agreement came together kennedyappointed cdc vaccine panel scrutinize childhood vaccine schedule trust president pray country trust president pray country everyday ethic everyday ethic columbia trustee view higher education crossroad choose builder destroyer im veteran democratic congressman gop ought hard iran bill include sale public land opinion bill include sale public land opinion rare earth startup without subsidy support cant shake china control asra nomani iran ideological foot soldier wage proxy war america death heart attack whats killing instead trump lawyer doj enforcer face confirmation hearing federal judgeship opinion berkshire carousel horse ride carry downtown destination sustainability normalization american indecency iran strategic blunder paved humiliating defeat expert happier healthier kid play decade obergefell lgbtq threat exclusive thune urge light touch ai regulation everything trump pick appeal judge seen illsuited lifetime appointment skinnytok rebranded eating disorder dangerously fast scoop trump admin cut contract scientific publishing giant contact cayuga county federal county elected iranian royalty fed local rumor mill ago bomb peace dont work together bomb peace dont work together marine sentenced sexual assault japan feeling represented district congressman feeling represented district congressman nato summit yield defense spending trump alliance trump isnt ready ceasefire massie zambian president burial halted begin promise remove worst worst arrested known immigrant murderer super coral supplement inside lab save great barrier reef hygiene rating handed doncaster establishment trump israeli intelligence significant damage iran nuclear facility halfcentury legal logjam killer coast banker wife face execution patriotic season searching america public forum bill threatens mental health care aging entrepreneur face policy hurdle help highyielding dividend stock buy haul trump triumph nato bow pressure defense pledge rep mike quigley trump put ego pocket rep mike quigley intel suggesting limited damage iran nuclear program criminal justice expert implication karen verdict morning brief nato commits defense spike nyc pick socialist expert push transing kid trump pick appeal judge draw controversy zohran mamdani set defeat cuomo nyc mayoral primary upset history korean war begin australian outback transformed water rubio dont believe report modest damage iran pell grant cut blow maine economic future opinion pell grant cut blow maine economic future opinion supreme blessed samesex marriage ago backlash brewing franklin board modifies district policy discussion astronomical society public night saturday editorial minnesota shooting shatter trust faith bridge builder announces recipient technical career investment grant ago issue warning fake inheritance scam column pursue smarter choice northern border scatec asa subscription employee purchase programme exclusive shell early acquire rival bp wsj palantir stock hit alltime high whats vimergy brings mouth america campaign washington dc expose system profit american sicker cpsc urge firework safety ahead holiday metas insane technology give user something screen deliver mark zuckerberg future ill beam charles river laboratory stock underperforming sp charles river laboratory stock underperforming sp national survey find american favor federal budget completely different congress developing bumble cut workforce online dating apps aim improve user experience wsj aerovironment stock soaring aerovironment stock soaring nvidia stock soar near record high whats driving rally forget crossfit million fitness event taking teacher chatgptand getting seattle fifas club world cup skeptic bitcoin rise nyse battle trump crypto coming mortgage next ai impact explores potential ai improve decisionmaking increase efficiency across critical national security operation buy slide insurance stock slde ipo buy slide insurance stock slde ipo carnival booking surge wall street talking solstad renews partnership marlink next stage digital transformation forester financial welcome leadership board director trump megabill economic agenda spur growth reduce national debt according white house report invested oracle ago worth amazon selling espresso machine shopper great coffee starbucks another retail chain liquidating chapter bankruptcy island flu island flu island flu island flu siili solution plc repurchase island flu aigenerated scam claim victim yearoveryear declining consumer concern sift report reveals island flu island flu island flu island flu russia boost export china favorite russian crude island flu data analytics power governs nextgen digital twin island flu shiba inu left pepe dollar tokenomics attract institutional investor shiba inus massive dilution risk intrinsic therapeutic announces implantation barricaid annular closure device via endoscopic approach happy limited announces closing initial public offering island flu island flu island flu island flu fed chair powell crypto industry maturing becoming mainstream island flu invent inventor develops temporary replacement windshield wiper mho island flu island flu island flu nostalgic pepsi brand roll flavor rival coke launch version pictory introduces world ai video mcp server pictory introduces world ai video mcp server rosen trusted leading firm encourages rocket pharmaceutical investor secure counsel important deadline security class action rckt wheel fallen corn market wheel fallen corn market senate minority schumer treated dehydration area hospital office study find trump favored nation drug proposal raise outofpocket cost without pbm reform study find trump favored nation drug proposal raise outofpocket cost without pbm reform valuesinaction foundation honor leadership across valuesinaction foundation honor leadership across sale plummet expected high mortgage rate sink demand bi claim stablecoins fail money call strict limit role tidy patio aerobroom cordless leaf blower broom skin cancer linked climate change hims health ceo compounding novo weightloss drug continue report himsnyse seeking alpha ahold delhaize usa tap lion executive cfo paychex stock take hit margin squeeze overshadows outlook spotify stock hit record high pricetarget hike american became millionaire neigbors getting rich pacific life introduces variable universal life insurance product available ulta beauty cfo paula oyibo quits pick insider interim role roll bottle change ban target shower supply cordially invited critique jeff bezos lauren sanchez wedding invitation robinhood ceo highlight retail investor interest nvidia tesla middle east tension barely blip hot weather safety trick pet hot weather safety advice pet mark walter lakers sale team expected close later clever carnivore announces scalable costcompetitive delicious cultivated pork clever carnivore announces scalable costcompetitive delicious cultivated pork medium advisory federal government housing announcement cape breton stock support reduced middle east tension spark riskon stock support reduced middle east tension spark riskon piston raise cardless fuel payment solution piston raise cardless fuel payment solution tsa common childrens toy allowed plane tesla sinking navigating complexity crossborder freight invent inventor develops shoe cleaning device mho overture map launch gers global interoperable geospatial id drive data interoperability gain start small best meme coin join month moon kandal venture limited announces pricing initial public offering listing nasdaq woodside close stake sale louisiana lng project kandal venture limited announces pricing initial public offering listing nasdaq business wary washington europe fret left behind ai battlefield senate prepares vote bill trump meet iran next trump megabill economic agenda spur growth reduce national debt according white house report fox racist smear zohran mamdani fail york mayoral race un agency cant locate iran uranium strike yakima start work water wastewater connection several neighborhood trump israel airstrike destroyed crucial nuclear facility set iran denver judge decide fate subpoena employee sue gov polis halt compliance reader opinion preparing landscape trump label nycs mamdani communist lunatic senate gop opening offer hospital fund california found violation title ix clash trump transgender athlete man indicted hate crime charge attack boulder demonstration israeli hostage house republican inch closer answer biden advisor lose executive privilege shield cordially invited critique jeff bezos lauren sanchez wedding invitation man stuck chimney rescue dog trapped building san francisco mayor daniel lurie unveils family zoning plan boost homebuilding trump denies iranian moved nuclear material strike trump denies iranian moved nuclear material strike donald trump ashamed betraying afghan ally opinion trump denies iranian moved nuclear material strike kennedy vaccine adviser meet kennedy vaccine adviser meet kennedy vaccine adviser meet kennedy vaccine adviser meet kennedy vaccine adviser meet kennedy vaccine adviser meet cayuga county budget reality raise tax cut deeper trump denies iranian moved nuclear material strike trump denies iranian moved nuclear material strike trump denies iranian moved nuclear material strike trump hegseth seethe fake medium doubting strike obliterated iranian nuclear site scum maverick select cooper flagg overall nba draft early intelligence report suggests strike set iran nuclear program month trump attack iran pushed diplomacy kim jong un reach tracking firstround pick nba draft trump affirms commitment nato article pledge mutual defense trump nato chief mark rutte calling daddy unanimous wisconsin supreme curtails governor partial veto power unanimous wisconsin supreme curtails governor partial veto power dead congressman social medium account resurrected boost chief staff congressional bid schumer hospitalized dehydration dc nears degree myth iran invincibility broken fallout farreaching pope leo xiv urge iranisrael war reject bullying arrogance peace york man arrested maine drug trafficking charge longlasting insulin take another step forward latest clinical trial tony abbott advance supporter bequeathing money rightwing protect australian value excessive social medium found harm teenager mental health expert moderation cruel joke tax concession drive donation australia richest private school must stop critic argue trump lay spain nato defense spending trump lay spain nato defense spending trump lay spain nato defense spending agree climate feel heat past public policy crisis costly past public policy crisis costly past public policy crisis costly hood lawmaker arent deadlocked regulation toyota tlmoda salvation army team distribute backpack school supply student nationwide partner different attorney appeal appeal lawyer wichita donald trump decision strike iran legal trump lay spain nato defense spending trump lay spain nato defense spending trump lay spain nato defense spending shasti conrad democratic party dnc vice chair race durbin tee bove judiciary hearing kick trump assessment iran nuclear facility damage complete report zohran mamdani nycs business community terrified lawless act defiance doj biden judge refusing follow supreme order chatgpt ai tool changing teaching profession microsoft sued author book ai training democrat primary voter reward prosecutor indict trump senator air concern doj budget proposal billionaire ackman musk rebuke zohran mamdanis nyc mayoral primary senate bill sensible cure ada abuse senate bill sensible cure ada abuse senate bill sensible cure ada abuse senate bill sensible cure ada abuse democrat staffer arrested abducting assaulting woman loose posting bond baumgartner northwest republican rfk jr reopen niosh worker safety office spokane senate bill navigating noncompete restriction healthcare practitioner texas trump meet iran next israel iran claim trumpbrokered truce carlisle vote sell fire engine address upcoming project gop florida ag uthmeier supreme immigration trump visit uk take place buckingham palace stock hang near record wall street take breath following hamas preparing attack american contractor helping distribute aid gaza bezos arrives venice protester starstudded wedding highlight growing inequality dogsized dinosaur specie discovered tax collection tumble latest washington budget forecast trump white house biden aide sweating badly yorkers visitor cope extreme heat social security tax cut trump bill retiree jerald mcnair school youth continue jeff bezos italian wedding senate majority run moderate america eric dane jensen ackles countdown youre dreaming score dozen early deal mattress vulnerable island dem warns mamdani extreme nyc primary upset alligator alcatraz desantis float building another immigration detention center federal judge order labor department job corp running lawsuit federal judge order labor department job corp running lawsuit federal judge order labor department job corp running lawsuit federal judge order labor department job corp running lawsuit federal judge order labor department job corp running lawsuit eric adam real chance stop mamdani andrew cuomo announce dropping trump admin sue federal judge maryland immigration order faith family sue block texas ten commandment school faith family sue block texas ten commandment school faith family sue block texas ten commandment school faith family sue block texas ten commandment school faith family sue block texas ten commandment school faith family sue block texas ten commandment school</t>
         </is>
       </c>
     </row>
@@ -586,12 +582,12 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>why you should get your boot to beyonces cowboy carter tour a sermon for the weary while you can chinese battery giant and tesla supplier catl is expanding globally here why it matter how to stay on top of google search faraday x preparation are in the final stage for the private preview and cocreation launch event on june th for the groundbreaking fx super one mpv biocon biologics receives health canada approval for yesafilitm aflibercept first global launch scheduled for july china factory activity expected to shrink for third month amid trade tension reuters poll nike vomero quietly became a million franchise in day a ceo say it time to turn the page investor gary black cheer afterhours rally ap technology summarybrief at am edt ap technology summarybrief at am edt ap technology summarybrief at am edt ap technology summarybrief at am edt amazon google not far behind but dan ives say microsoft clearly leading in these segment price target is probably conservative why your to feel more like report say analysisin dovish tilt boj zoom in on obscure underlying inflation trend find the best crypto to join for emerging project reshaping the digital economy tesla shakeup who is omead afshar senior executive reportedly fired by elon musk amid slumping sale i time of india ap business summarybrief at am edt ap business summarybrief at am edt asian share are mostly higher after u stock rise to the brink of a record trump tariff have unsettled thailand pet food exporter germany tell apple google to block deepseek a the chinese ai app face rising pressure in europe hugging face cofounder challenge ai optimist model cant ask original scientific question you might not have bezoslevel buck but you still might consider a prenup vertex founder boger donates m to boston art academy trump big beautiful bill might be unloved and a mess but it will still probably pas here how the luxury real estate market is splitting up how company profit from your data without consent full circle boy leap forward with debut ep jete and official music video this go out to you out now increase of share capital in connection with realization of the employee option programm and subscription result more than an ev charger it peace of mind wherever the road take you cutting u energy credit doesnt save money it steal it from ratepayer local government ansi officially approves two new seia standard on consumer protection and operation and maintenance kymera therapeutic announces pricing of million public offering kymera therapeutic announces pricing of million public offering solaredge expands u manufacturing in salt lake city utah why denver homeowner are investing more in renovation project leap power national grid virtual power plant initiative in massachusetts hawaiian airline report cybersecurity event no flight disruption kitv boeing dreamliner black box recovered data under scrutiny to provide insight into fatal air india crash cso receives grant from mt charitable foundation achieve life science announces pricing of million underwritten public offering the mobility house and schneider electric unveil solar charging depot for turlock unifieds electric school bus fleet trump crypto advisor david sack say july will be a big month say president support legislation on market structure and stablecoins amazon grocery chief blame ridiculous red tape for holding back initiative at whole food were wasting time year old driver from tripura treated with eastern india firstever bachmanns bundle pacing vdh in the end everyone hated the iranian theocracy oklahoma governor kevin stitt and u secretary of health and human service robert f kennedy jr visit mom meal to highlight food a medicine leadership japan executes twitter killer who murdered and dismembered nine people saratoga county celebrates m airport revitalization ap business summarybrief at pm edt ap business summarybrief at pm edt ap business summarybrief at pm edt ap business summarybrief at pm edt ap technology summarybrief at pm edt driver crash nearly plummet over san mateo county cliff north korea just opened a beach resort for people but who will visit jeep gladiator rank first in midsize pickup segment in jd power u initial quality study chrysler jeep and dodge brand improve iq score over thailand will hold trade talk with u next week finance minister say meta say it winning the talent war with openai the verge china u agree on detail of london trade framework beijing say saratogians remember mark straus a pioneer sp cut colombia debt rating to bb over declining fiscal result why lumen technology stock wa winning this week annovis bio to present key finding at alzheimers association international conference iraq war veteran hegseths news conference wa conduct unbecoming chinese influence in climate change lawsuit threatens to derail u energy industry asia fx muted dollar struggle at yr low with pce data on tap demolition start at former kera hq clearing way for new uptown tower european stock extend gain after white house hint at tariff extension baseball player wander franco found guilty in sexual abuse case imposed twoyear suspended sentence china skirt u sanction a top buyer of iranian oil here how and why thats unlikely to change soon china may industrial profit slip back into sharp decline reuters gold head for weekly loss a middle east truce sap demand uk auto production for may slump to lowest level since a trump tariff hit hard mgi announces partnership with negedia enhance genomic sequencing technology at the service of scientific research and precision medicine in italy mgi announces partnership with negedia enhance genomic sequencing technology at the service of scientific research and precision medicine in italy informal mining boom is biggest fear for peru copper investor best cryptos to buy now one already up and climbing bill gate say he know for a fact that more child will die due to u health aid cut and he taking the proof to congress cancer patient recover by taking repurposed antiparasitic drug india economy to hold top spot for growth but underlying weakness remain reuters poll cnbc daily open wall street is tuning out the noise and catching ray turkish farmer pioneer xag agricultural drone for watersmart practice treasury yield inch higher a investor await the fed preferred inflation print bitcoin ethereum rangebound dogecoin dip amid potential july tariff deadline extension analyst predicts btcs next big move once it break out of this range softbank ceo say he all in on openai reveals he long wanted microsofts spot a main backer mexico investigating contamination from spacex explosion debris sandia national laboratory to cut up to workforce by early fall canada approves law to fasttrack resource project face indigenous opposition lithium industry bemoans paradox of low price rising demand china industrial profit slip back into sharp decline in may two north texas school board increase teacher pay in final budget confusion a trump say deal with china signed yet both side violate term of ceasefire share rally but dollar weakens with fed independence seen under threat courtney b vance on book ban protest in los angeles and narrating the audiobook of the biography of web du bois atlantic strategic mineral start commercial production at virginia operation u food and drug administration approves streamlined patient monitoring requirement and removal of rem program within bristol myers squibbs cell therapy label u food and drug administration approves streamlined patient monitoring requirement and removal of rem program within bristol myers squibbs cell therapy label u food and drug administration approves streamlined patient monitoring requirement and removal of rem program within bristol myers squibbs cell therapy label u food and drug administration approves streamlined patient monitoring requirement and removal of rem program within bristol myers squibbs cell therapy label why you should get your boot to beyonces cowboy carter tour a sermon for the weary while you can clarence page did you miss a holiday mr president arthur cyr bombing iran mideast stability and the role of the u former minnesota house speaker melissa hortman to lie in state a suspect face court date former minnesota house speaker melissa hortman to lie in state a suspect face court date democrat are trying to figure out what to do about john fetterman one of them is stepping up democrat are trying to figure out what to do about john fetterman one of them is stepping up democrat are trying to figure out what to do about john fetterman one of them is stepping up supreme court meet friday to decide remaining case including birthright citizenship supreme court meet friday to decide remaining case including birthright citizenship supreme court meet friday to decide remaining case including birthright citizenship supreme court meet friday to decide remaining case including birthright citizenship you might not have bezoslevel buck but you still might consider a prenup summer league basketball islander rattler trump big beautiful bill might be unloved and a mess but it will still probably pas edward d shanshala ii billion in waste fraud and abuse maybe but look in the right place editorial go slow on waymo several caution before selfdriving car arrive rev allison palm rev jonathan hopkins gov ayotte reneged on promise to meet with faith leader senator diverge sharply on damage done by iran strike after classified briefing japan executes twitter killer who murdered and dismembered nine people oregon senate vote to override governor veto a first since dallas place future of the franchise in cooper flagg a southwest division get better north korea just opened a beach resort for people but who will visit panton named johnstown knox elementary school principal former top aide to jill biden subpoenaed in house gop biden age probe iraq war veteran hegseths news conference wa conduct unbecoming selling public land isnt the answer to affordable housing title lx protection matter more than ever trump appointing a shadow chair at the fed ha put dollar under pressure meanwhile china is dumping the greenback and hoarding gold baseball player wander franco found guilty in sexual abuse case imposed twoyear suspended sentence abbott trump approval rating poll show economy thc reduce favorability among texan family file for release in lawsuit considered first involving child challenging arrest at court family file for release in lawsuit considered first involving child challenging arrest at court family sue over u detention in what may be first challenge to courthouse arrest involving kid gov ferguson warns medicaid cut could devastate washington health care system review gloversvilles stump city brewing is modern version of oldtime public house pintsized louisiana is latest state to redefine natural gas a planetwarming fossil fuel a green energy change coming for wilco voter courtney b vance on book ban protest in los angeles and narrating the audiobook of the biography of web du bois critical rce flaw in cisco ise and isepic allow unauthenticated attacker to gain root access pete hegseth air medium coverage grievance towards cnn and others the latest pretrial development in the idaho student killing case green leader larissa water on holding the labor government to account australian politics podcast labor must protect environment while rewriting law written to facilitate development larissa water say wife of minnesota suspect say she wa blindsided by shooting of state politician cnn this is your brain on chatgpt white house confirms u china have reached additional trade agreement trump threatens cnn and new york time with lawsuit over iran report senate parliamentarian ok gop cut to federal food assistance former trail blazer ben mclemore say sex wa consensual while taking the stand during rape trial woman accused of stealing from jewelry store in washington oregon former defense secy iranian nuclear facility damage assessment will take week community rally in massive show of support for caesar palace time square u tariff may sideline youth sport for many family making it harder for kid to stay active rep josh gottheimer american dont like trump big policy bill court issue opinion on centennial at tejon ranch cnn medium analyst responds to false attack on iranian nuclear site report let go through it zohran mamdani tell erin burnett how he plan to pay for his policy fireball fly across the sky and cause sonic boom america controversial iran airstrike letter to the editor june china on alert a nato boost defense spending mamdani vow to stand up to trump border czar and ice canadian official press u government for detail on canadian citizen who died in ice custody at a florida detention center former montana u rep pat williams who won a liberal conservative showdown dy at portland city council pass resolution to strengthen portland street response a look at legal threat facing samesex marriage year after obergefell decision it judgement time for john thune on the big beautiful bill guest commentary rtc targeting senior with displacement former pantagraph building get positive recommendation for landmark status eu leader on wto we need to come up with something else senate democrat question obliteration of iran nuclear site after classified briefing on strike officer placed on leave after shooting in bangor at least orgs urge senator to support iran war power resolution lawsuit filed on behalf of nex benedict estate against owasso public school trump spotlight parent who have lost kid due to open border during big beautiful bill event former trump lawyer kenneth chesebro disbarred in new york over election interference case donald trump say uschina trade truce ha been signed hegseth defends success of u strike on iran nuclear site amid doubt over impact standing up to bullying unscientific transgender activist mob canadian man held by immigration official dy in south florida federal facility official say canadian man held by immigration official dy in south florida federal facility official say canadian man held by immigration official dy in south florida federal facility official say canadian man held by immigration official dy in south florida federal facility official say canadian man held by immigration official dy in south florida federal facility official say canadian man held by immigration official dy in south florida federal facility official say illinois gov jb pritzker announces bid for historic third term amidst presidential buzz interior secretary doug burgum answer question about the big beautiful bill and public land trump doj is targeting daily ko agent mental health passport led to push for secured bond famous preston night rodeo gearing up for it th annual community experience</t>
+          <t>jeff bezos and blue origin engaged with trump administration for government contract amid elon musk rift with the president report best smart glass with camera to buy in iran confirms nuclear site damaged a trump promise a meeting next week sitime corporation announces pricing of followon public offering analysisinvestors shore up defence against another august market rout kroger parent company of ralphs plan to close dozen of grocery store investor shore up defence against another august market rout reuters city council committee back minimum wage for hospitality worker who winning the innovation race new year analysis point to what matter most avermedia unveils two new hdmi capture device for creator at every level who winning the innovation race new year analysis point to what matter most why trump need the world to believe iran nuclear program is obliterated how japan and alaska pioneered the global market for lng the alaska town at the center of trump billion lng push ai reasoning problem why thinking model may not actually be smarter bik data analysis indicates including bnpl transaction data in credit history could help almost every second thinfile customer improve their creditworthiness north korea opening a tourist site on it east coast next week thats key to it tourism hope eu rule out production aid in blow to battery cleantech industry hong kong home price little changed in may electricity use for commercial computing could surpass space cooling ventilation tim draper say this will be the fate of bitcoin and the dollar in year billionaire highlight apps built on btc that matter california raise the bar with two three starred restaurant joining selection storage project planned for laurel oak ranch veteran analyst drop bold new call on nvidia stock yahoo finance buyer emerge for northvolt carlsbad newly opened lilo restaurant crowned with a michelin star fujitsus uvance wayfinders consulting empowers customer to evolve business foundation leveraging data and ai strongest naruto character ranked oxford cambridge fall in global college ranking expert say it a red flag for uk innovation trump familybacked world liberty financial plan to launch a new app that will make it easy for lay investor to use crypto at least reason why trump should reject a nobel peace prize china fintech giant ant double down on health care with new ai app and it want it to go global top meme coin to buy for with real narrative and epic roadmaps beijing ramp up stimulus a uschina trade tension threaten recovery kratos defense security solution inc price public offering of common stock asia fx firm dollar hit yr low a trump call for rate cut amid powell feud is this the most political fashion item ever south korea central bank adjusts open market operation to boost money supply mark zuckerbergs meta beat lawsuit over ai training on book judge find no meaningful evidence on market dilution analysis trump claim the press is demeaning the military but questioning power is patriotic colorado native nique clifford selected with no overall pick in nba draft wall street panic a socialist set to take over new york reit tumble at the idiocy of it all enthusiast gaming announces annual general meeting top desktop deal for june alienware lenovo hp and more enthusiast gaming announces annual general meeting colorado proposal seek to double income tax rate for taxpayer who earn at least million bitcoin top this key level a institution pile on ethereum dogecoin rangebound analyst say buying btc now is like buying it for in blacklisted by the u and backed by beijing this chinese ai startup ha caught openais attention vietnam to remove death penalty for embezzlement sparing tycoon life why trump strike on iran will leave north korea more determined than ever to keep it nuke acen and upc renewables break ground on over mw of new renewable energy project in india firm outline audit into iedc operation over past year rove pest control join force with greenix pest control optiva inc announces result of annual meeting mar acquisition of pringles maker trigger eu alarm dw isisinspired drone war plan leaked from u national security council china will take forceful step to boost consumption premier li say fema is not a replacement for insurance coverage risk management expert say here why cnbc daily open funny how the sp is teasing a new high amid uncertainty top poco phone under r first nordic announces annual general meeting voting result judge reject author claim that meta ai training violated copyright variety trump organization scrap made in the usa tag for it gold t smartphone asian stock hesitant dollar slide on trump attack on powell australia job vacancy bounce in may quarter ab data show hm share jump a it flag summer shopping pickup why not an islamic bomb how israel planned failed to stop pakistan going nuclear asos shopper say they were banned for making too many return sembrando vida and mexinol establish the first publicprivate partnership in sinaloa to build local capacity tesla begin rolling out self driving service in texas flexiview lending close million fixandflip loan in montpelier vermont how daddy talk and trump and ruttes bromance stole the nato spotlight htc partner with ntt com to forge a new model for immersive entertainment in japan murata push capacitor design with world first fvdc mlcc in inch size for automotive application bay miner launch aipowered cloud mining supporting bitcoin ethereum sol xrp litecoin and dogecoin jefferson capital announces pricing of initial public offering jefferson capital announces pricing of initial public offering it not my responsibility working with autonomyrestricting algorithm facilitates unethical behavior and displacement of responsibility new covidwave scarecampaign a massive flop the secret out top meme coin to buy that are taking over crypto influencer portfolio best malayalam cop thriller on ott you cant miss craft telemedicine launch to redefine specialty care with humancentered my bos lead the right way understanding how and when the institutionalization of ethic impact supervisor leadership style michael novogratzs galaxy and invesco file to launch solana etf what you should know about qsol trump judicial nominee bove denies advising justice department lawyer to ignore court order treasury yield fall a concern grow over trump criticism of powell inplay oil corp announces annual meeting voting result for election of director trump admin move to let borrower use crypto in mortgage application alaska commissioner of revenue adam crum and prospr aligned announce launch of the frontier economic fund nyse akaf getchell gold corp announces total debenture conversion walmart is selling an easy to assemble gaming chair for and shopper say it quality is excellent cathie wood double down on shopify buy the dip dump million worth of robinhood stock at peak tariff cost boost demand for efficiency in reverse logistics ap technology summarybrief at pm edt ap technology summarybrief at pm edt how chatgpt and other ai tool are changing the teaching profession modernday monopoly gop senator sound alarm on mega corporation hijacking u beef supply hims investor alert robbins geller rudman dowd llp announces that hims hers health inc investor with substantial loss have opportunity to lead the hims hers class action lawsuit denis villeneuve to direct next james bond film international paper to release secondquarter earnings on july trump latest rejection of intelligence assessment reflects a long distrust of spy agency editorial stay up to date on status of water recreation option trump official to give first classified briefing to congress on iran strike iran confirms nuclear site damaged a trump promise a meeting next week republican congresswoman office evacuated after proabortion activist send chilling threat cal thomas make america clean again john hood nc lawmaker arent deadlocked on regulation bull take yearold noa essengue at no for central division lone firstround pick eu leader meet to discus tougher russia sanction u tariff and middle east conflict trump official to give first classified briefing to congress on iran strike trump official to give first classified briefing to congress on iran strike trump latest rejection of intelligence assessment reflects a long distrust of spy agency trump latest rejection of intelligence assessment reflects a long distrust of spy agency senior are the fastestgrowing age group in the bay area and nationwide dear neighbor it because of my value my turn were running out of caregiver im scared for the future larry efird an uncommon spirit why trump need the world to believe iran nuclear program is obliterated how a california psychology student exposed the dark side of therapy education my turn usa bombed iran now the electrical grid and your network are in the crosshairs letter to the editor watt need your support editorial baltimore sun trump entry into iran war left congress mia letter to the editor thanks to city public work steven borne absentee ballot and access help people vote keith kuenning new hampshire budget betrays it child trump announces iran nuclear talk following u strike that severely damaged iranian nuclear program little league serra mesa tierrasanta septum set to vote on budget proposal thursday this is a real doomsday scenario jonah goldberg u right to bomb iran with or without nuclear specter ted talley tinkering trump creates problem where none exist kratos defense security solution inc price public offering of common stock is this the most political fashion item ever analysis trump claim the press is demeaning the military but questioning power is patriotic vietnam to remove death penalty for embezzlement sparing tycoon life mamdani say listening making city affordable key part of campaign trump considering several candidate for next federal reserve chair florida rep kat cammack say her office wa evacuated due to death threat florida rep kat cammack say her office wa evacuated due to death threat why trump strike on iran will leave north korea more determined than ever to keep it nuke miranda devine trumpderangement syndrome drive deep state leaker cnn to treasonous length to deny prez a victory live update hegseth will hold new conference to respond to intelligence report on iran strike nato survives another day sf resident to see a hike in trash fee sembrando vida and mexinol establish the first publicprivate partnership in sinaloa to build local capacity minnesota solar energy advocate mourn the loss of champion rep melissa hortman author of law boosting industry htc partner with ntt com to forge a new model for immersive entertainment in japan citrix release emergency patch for actively exploited cve in netscaler adc cooper flagg is the new face of maine cooper flagg is the new face of maine donation to local organization get matching boost this week where is our mexican vacation refund weve been waiting for month after more than a year on the run gang leader recaptured florida alligator alcatraz what to know minnesota face federal lawsuit for offering illegal immigrant college tuition benefit denied to american gloversvilles antonucci surprised self with mayoral primary win honduras u discus immigration security after tense start to relation under trump administration feeling gutted msnbcs nicolle wallace is sad tren de aragua gang member were deported to cecot exclusive leading house conservative call senate bluff on trump beautiful bill la immigration detention facility a ticking time bomb immigration lawyer say expert warns senate tax cut plan could add far more to the deficit than expected trump administration sue all maryland federal judge over order blocking removal of immigrant the trump administration is suing minnesota over break in higher education for immigrant student young cuban girl asks trump to lift travel ban stopping her from joining mom in u why the fed is keeping rate steady for now rental impact fee discussed a obstacle to college station affordable housing breaking down whistleblower claim against trump judicial pick denver judge say ice subpoena doesnt comply with state law but doesnt prohibit polis from responding the u also ha a bombproof bunker in a mountain analysis a battered iran face an uncertain future after it grinding war with israel sabrina carpenter release alternate album cover after online backlash approved by god federal judge block trump admin from ending collective bargaining for some federal worker independence day drone show spark council debate lt cmdr nathan ouellette retires after year of service veteran from deerfield named nyu truman scholar yearold billing boy remembered a stepfather is sentenced for his murder armed immigration officer arent even telling local police at time about their raid leak are a problem congress feud over trump limit on sharing intel duke phenom cooper flagg go to dallas maverick with no overall pick in nba draft cia say it ha evidence iran nuclear program wa severely damaged a assessment of u strike impact continue little league north park cholla lake mar pending acquisition of kellanova clear ftc antitrust review oklahoma supreme court begin oral argument on state question trump spy chief say new intel show iran nuclear facility were destroyed meta win artificial intelligence copyright case in blow to author republican suddenly realize voter hate their health care cut editorial class of youve earned your place this is your time trump drop made in the usa label for new phone and a debate ensues how to define made trump drop made in the usa label for new phone and a debate ensues how to define made trump drop made in the usa label for new phone and a debate ensues how to define made trump drop made in the usa label for new phone and a debate ensues how to define made trump win over lifelong democrat autoworker with big beautiful bill vehicle loan tax benefit oregon house pass bipartisan bill to combat chronic absenteeism in school republican candidate who ran against maxine water admits to misusing campaign donation scoop protrump group unleashes first tv ad against massie trump administration to investigate university of california hiring practice ltte noise at the uv pilot site</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>boot beyonces cowboy carter tour sermon weary chinese battery giant tesla supplier catl expanding globally matter stay google search faraday x preparation final stage private preview cocreation launch event groundbreaking fx super mpv biocon biologics receives health canada approval yesafilitm aflibercept global launch scheduled china factory activity expected shrink third month amid trade tension reuters poll nike vomero quietly became million franchise ceo turn page investor gary black cheer afterhours rally technology technology technology technology amazon google far behind dan ives microsoft clearly leading segment price target probably conservative feel report analysisin dovish tilt boj zoom obscure underlying inflation trend find best crypto join emerging project reshaping digital economy tesla shakeup omead afshar senior executive reportedly fired elon musk amid slumping sale india business business asian share mostly higher stock rise brink record trump tariff unsettled thailand pet exporter germany apple google block deepseek chinese ai app face rising pressure europe hugging face cofounder challenge ai optimist model cant original scientific bezoslevel buck consider prenup vertex founder boger donates boston art academy trump bill unloved mess probably pa luxury real estate market splitting company profit data without consent full circle boy leap forward debut ep jete music video increase share connection realization employee option programm subscription ev charger peace mind wherever road take cutting energy credit doesnt save money steal ratepayer local government ansi officially approves new seia consumer protection operation maintenance kymera therapeutic announces pricing million public offering kymera therapeutic announces pricing million public offering solaredge expands manufacturing salt lake utah denver homeowner investing renovation project leap power national grid virtual power plant initiative massachusetts hawaiian airline report cybersecurity event flight disruption kitv boeing dreamliner black box recovered data scrutiny provide insight fatal air india crash cso receives grant mt charitable foundation achieve life science announces pricing million underwritten public offering mobility house schneider electric unveil solar charging depot turlock unifieds electric school bus fleet trump crypto advisor david sack month president support legislation market structure stablecoins amazon grocery chief blame ridiculous red tape initiative wasting old driver tripura treated eastern india firstever bachmanns bundle pacing vdh end everyone hated iranian theocracy oklahoma governor kevin stitt secretary health human service robert f kennedy jr visit mom meal highlight medicine leadership japan executes twitter killer murdered dismembered nine people saratoga county celebrates airport revitalization business pm business pm business pm business pm technology pm driver crash nearly plummet san mateo county cliff north korea opened beach resort people visit jeep gladiator rank midsize pickup segment jd power initial quality study chrysler jeep dodge brand improve iq score thailand trade next finance minister meta winning talent war openai verge china agree detail london trade framework beijing saratogians remember mark straus pioneer sp cut colombia debt rating bb declining fiscal lumen technology stock winning annovis bio present finding alzheimers association international conference iraq war veteran hegseths conference conduct unbecoming chinese influence climate change lawsuit threatens derail energy industry asia fx muted dollar struggle yr low pce data tap demolition start kera hq clearing new uptown tower european stock extend gain white house hint tariff extension baseball player wander franco found guilty sexual abuse imposed twoyear suspended sentence china skirt sanction buyer iranian oil thats unlikely change soon china industrial profit slip sharp decline reuters gold head weekly loss middle east truce sap demand uk auto production slump lowest level since trump tariff hit hard mgi announces partnership negedia enhance genomic sequencing technology service scientific research precision medicine italy mgi announces partnership negedia enhance genomic sequencing technology service scientific research precision medicine italy informal mining boom biggest fear peru copper investor best cryptos buy climbing bill gate fact child die due health aid cut taking proof congress cancer patient recover taking repurposed antiparasitic drug india economy spot growth underlying weakness reuters poll cnbc open wall street tuning noise catching ray turkish farmer pioneer xag agricultural drone watersmart practice treasury yield inch higher investor await fed preferred inflation print bitcoin ethereum rangebound dogecoin dip amid potential tariff deadline extension analyst predicts btcs next move break range softbank ceo openai reveals wanted microsofts spot main backer mexico investigating contamination spacex explosion debris sandia national laboratory cut workforce early fall canada approves fasttrack resource project face indigenous opposition lithium industry bemoans paradox low price rising demand china industrial profit slip sharp decline north texas school board increase teacher pay final budget confusion trump deal china signed yet violate term ceasefire share rally dollar weakens fed independence seen threat courtney b vance book ban protest los angeles narrating audiobook biography web du bois atlantic strategic mineral start commercial production virginia operation drug administration approves streamlined patient monitoring requirement removal rem program bristol myers squibbs cell therapy label drug administration approves streamlined patient monitoring requirement removal rem program bristol myers squibbs cell therapy label drug administration approves streamlined patient monitoring requirement removal rem program bristol myers squibbs cell therapy label drug administration approves streamlined patient monitoring requirement removal rem program bristol myers squibbs cell therapy label boot beyonces cowboy carter tour sermon weary clarence page miss holiday mr president arthur cyr bombing iran mideast stability role minnesota house speaker melissa hortman lie suspect face date minnesota house speaker melissa hortman lie suspect face date democrat figure john fetterman stepping democrat figure john fetterman stepping democrat figure john fetterman stepping supreme meet friday decide remaining birthright citizenship supreme meet friday decide remaining birthright citizenship supreme meet friday decide remaining birthright citizenship supreme meet friday decide remaining birthright citizenship bezoslevel buck consider prenup summer league basketball islander rattler trump bill unloved mess probably pa edward shanshala ii billion waste fraud abuse maybe look place editorial slow waymo several caution selfdriving car arrive rev allison palm rev jonathan hopkins gov ayotte reneged promise meet faith senator diverge sharply damage iran strike classified briefing japan executes twitter killer murdered dismembered nine people oregon senate vote override governor veto since dallas place future franchise cooper flagg southwest division better north korea opened beach resort people visit panton named johnstown knox elementary school principal aide jill biden subpoenaed house gop biden age probe iraq war veteran hegseths conference conduct unbecoming selling public land isnt answer affordable housing title lx protection matter ever trump appointing shadow chair fed put dollar pressure meanwhile china dumping greenback hoarding gold baseball player wander franco found guilty sexual abuse imposed twoyear suspended sentence abbott trump approval rating poll economy thc reduce favorability among texan family file release lawsuit considered involving child challenging arrest family file release lawsuit considered involving child challenging arrest family sue detention challenge courthouse arrest involving kid gov ferguson warns medicaid cut devastate washington health care system review gloversvilles stump brewing modern version oldtime public house pintsized louisiana latest redefine natural gas planetwarming fossil fuel green energy change coming wilco voter courtney b vance book ban protest los angeles narrating audiobook biography web du bois critical rce flaw cisco ise isepic allow unauthenticated attacker gain root access pete hegseth air medium coverage grievance towards cnn others latest pretrial development idaho student killing green larissa water labor government account australian politics podcast labor must protect environment rewriting written facilitate development larissa water wife minnesota suspect blindsided shooting politician cnn brain chatgpt white house confirms china reached additional trade agreement trump threatens cnn new york lawsuit iran report senate parliamentarian ok gop cut federal assistance trail blazer ben mclemore sex consensual taking stand rape trial woman accused stealing jewelry store washington oregon defense secy iranian nuclear facility damage assessment take community rally massive support caesar palace square tariff sideline youth sport family making harder kid stay active rep josh gottheimer american dont trump policy bill issue opinion centennial tejon ranch cnn medium analyst responds false attack iranian nuclear site report zohran mamdani erin burnett plan pay policy fireball fly across sky cause sonic boom america controversial iran airstrike editor china alert nato boost defense spending mamdani vow stand trump border czar canadian press government detail canadian citizen died custody florida detention center montana rep pat williams liberal conservative showdown dy portland council pas resolution strengthen portland street response look legal threat facing samesex marriage obergefell decision judgement john thune bill guest commentary rtc targeting senior displacement pantagraph building positive recommendation landmark status eu wto come something else senate democrat obliteration iran nuclear site classified briefing strike officer placed shooting bangor least orgs urge senator support iran war power resolution lawsuit filed behalf nex benedict estate owasso public school trump spotlight parent kid due open border bill event trump lawyer kenneth chesebro disbarred new york election interference donald trump uschina trade truce signed hegseth defends success strike iran nuclear site amid doubt impact standing bullying unscientific transgender activist mob canadian man immigration dy south florida federal facility canadian man immigration dy south florida federal facility canadian man immigration dy south florida federal facility canadian man immigration dy south florida federal facility canadian man immigration dy south florida federal facility canadian man immigration dy south florida federal facility illinois gov jb pritzker announces bid historic third term amidst presidential buzz interior secretary doug burgum answer bill public land trump doj targeting ko agent mental health passport led push secured bond famous preston night rodeo gearing annual community experience</t>
+          <t>jeff bezos blue origin engaged trump administration government contract amid elon musk rift president report best smart glass camera buy iran confirms nuclear site damaged trump promise meeting next sitime corporation announces pricing followon public offering analysisinvestors shore defence another august market rout kroger parent company ralphs plan close dozen grocery store investor shore defence another august market rout reuters council committee minimum wage hospitality worker winning innovation race analysis matter avermedia unveils hdmi capture device creator level winning innovation race analysis matter trump world believe iran nuclear program obliterated japan alaska pioneered global market lng alaska town center trump billion lng push ai reasoning problem thinking model smarter bik data analysis indicates bnpl transaction data credit history help almost thinfile customer improve creditworthiness north korea opening tourist site east coast next thats tourism eu rule production aid blow battery cleantech industry hong kong price little changed electricity commercial computing surpass space cooling ventilation tim draper fate bitcoin dollar billionaire highlight apps built btc matter california raise bar starred restaurant joining selection storage project planned laurel oak ranch veteran analyst drop bold call nvidia stock yahoo finance buyer emerge northvolt carlsbad newly opened lilo restaurant crowned michelin star fujitsus uvance wayfinders consulting empowers customer evolve business foundation leveraging data ai strongest naruto character ranked oxford cambridge fall global college ranking expert red flag uk innovation trump familybacked world liberty financial plan launch app easy lay investor crypto least trump reject nobel peace prize china fintech giant ant double health care ai app global meme coin buy real narrative epic roadmaps beijing ramp stimulus uschina trade tension threaten recovery kratos defense security solution price public offering common stock asia fx firm dollar hit yr low trump call rate cut amid powell feud political fashion item ever south korea central bank adjusts open market operation boost money supply mark zuckerbergs meta beat lawsuit ai training book judge find meaningful evidence market dilution analysis trump claim press demeaning military questioning power patriotic colorado native nique clifford selected overall pick nba draft wall street panic socialist set take york reit tumble idiocy enthusiast gaming announces annual general meeting desktop deal alienware lenovo hp enthusiast gaming announces annual general meeting colorado proposal seek double income tax rate taxpayer earn least million bitcoin level institution pile ethereum dogecoin rangebound analyst buying btc buying blacklisted backed beijing chinese ai startup caught openais attention vietnam remove death penalty embezzlement sparing tycoon life trump strike iran north korea determined ever nuke acen upc renewables break ground mw renewable energy project india firm outline audit iedc operation past rove pest control join force greenix pest control optiva announces annual meeting mar acquisition pringles maker trigger eu alarm dw isisinspired drone war plan leaked national security council china take forceful step boost consumption premier li fema replacement insurance coverage risk expert cnbc open funny sp teasing high amid uncertainty poco phone r nordic announces annual general meeting voting judge reject author claim meta ai training violated copyright variety trump organization scrap usa tag gold smartphone asian stock hesitant dollar slide trump attack powell australia job vacancy bounce quarter ab data hm jump flag summer shopping pickup islamic bomb israel planned failed stop pakistan nuclear asos shopper banned making sembrando vida mexinol establish publicprivate partnership sinaloa build local capacity tesla begin rolling self driving service texas flexiview lending close million fixandflip loan montpelier vermont daddy trump ruttes bromance stole nato spotlight htc partner ntt com forge model immersive entertainment japan murata push capacitor design world fvdc mlcc inch size automotive application bay miner launch aipowered cloud mining supporting bitcoin ethereum sol xrp litecoin dogecoin jefferson announces pricing initial public offering jefferson announces pricing initial public offering responsibility working autonomyrestricting algorithm facilitates unethical behavior displacement responsibility covidwave scarecampaign massive flop secret meme coin buy taking crypto influencer portfolio best malayalam cop thriller ott cant miss craft telemedicine launch redefine specialty care humancentered bos lead understanding institutionalization ethic impact supervisor leadership style michael novogratzs galaxy invesco file launch solana qsol trump judicial nominee bove denies advising justice department lawyer ignore order treasury yield fall concern grow trump criticism powell inplay oil corp announces annual meeting voting election director trump admin move borrower crypto mortgage application alaska commissioner revenue adam crum prospr aligned announce launch frontier economic fund nyse akaf getchell gold corp announces total debenture conversion walmart selling easy assemble gaming chair shopper quality excellent cathie wood double shopify buy dip dump million worth robinhood stock peak tariff cost boost demand efficiency reverse logistics technology pm technology pm chatgpt ai tool changing teaching profession modernday monopoly gop senator sound alarm mega corporation hijacking beef supply hims investor alert robbins geller rudman dowd llp announces hims health investor substantial loss opportunity lead hims class action lawsuit denis villeneuve direct next james bond film international paper release secondquarter earnings trump latest rejection intelligence assessment reflects distrust spy agency editorial stay date status water recreation option trump give classified briefing congress iran strike iran confirms nuclear site damaged trump promise meeting next republican congresswoman office evacuated proabortion activist send chilling threat cal thomas america clean john hood nc lawmaker arent deadlocked regulation bull take yearold noa essengue central division lone firstround pick eu meet discus tougher russia sanction tariff middle east conflict trump give classified briefing congress iran strike trump give classified briefing congress iran strike trump latest rejection intelligence assessment reflects distrust spy agency trump latest rejection intelligence assessment reflects distrust spy agency senior fastestgrowing age bay area nationwide dear neighbor value turn running caregiver im scared future larry efird uncommon spirit trump world believe iran nuclear program obliterated california psychology student exposed dark therapy education turn usa bombed iran electrical grid network crosshairs editor watt support editorial baltimore sun trump entry iran war left congress mia editor public work steven borne absentee ballot access help people vote keith kuenning hampshire budget betrays child trump announces iran nuclear following strike severely damaged iranian nuclear program little league serra mesa tierrasanta septum set vote budget proposal thursday real doomsday scenario jonah goldberg bomb iran without nuclear specter ted talley tinkering trump creates problem none exist kratos defense security solution price public offering common stock political fashion item ever analysis trump claim press demeaning military questioning power patriotic vietnam remove death penalty embezzlement sparing tycoon life mamdani listening making affordable part campaign trump considering several candidate next federal reserve chair florida rep kat cammack office evacuated due death threat florida rep kat cammack office evacuated due death threat trump strike iran north korea determined ever nuke miranda devine trumpderangement syndrome drive deep leaker cnn treasonous length deny prez victory update hegseth conference respond intelligence report iran strike nato survives another sf resident hike trash fee sembrando vida mexinol establish publicprivate partnership sinaloa build local capacity minnesota solar energy advocate mourn loss champion rep melissa hortman author boosting industry htc partner ntt com forge model immersive entertainment japan citrix release emergency patch actively exploited cve netscaler adc cooper flagg face maine cooper flagg face maine donation local organization matching boost mexican vacation refund weve waiting month run gang recaptured florida alligator alcatraz minnesota face federal lawsuit offering illegal immigrant college tuition benefit denied american gloversvilles antonucci surprised self mayoral primary honduras discus immigration security tense start relation trump administration feeling gutted msnbcs nicolle wallace sad tren de aragua gang deported cecot exclusive leading house conservative call senate bluff trump bill la immigration detention facility ticking bomb immigration lawyer expert warns senate tax cut plan add far deficit expected trump administration sue maryland federal judge order blocking removal immigrant trump administration suing minnesota break higher education immigrant student young cuban girl asks trump lift travel ban stopping joining mom fed keeping rate steady rental impact fee discussed obstacle college station affordable housing breaking whistleblower claim trump judicial pick denver judge subpoena doesnt comply doesnt prohibit polis responding bombproof bunker mountain analysis battered iran face uncertain future grinding war israel sabrina carpenter release alternate album cover online backlash approved god federal judge block trump admin ending collective bargaining federal worker independence drone spark council debate lt cmdr nathan ouellette retires service veteran deerfield named nyu truman scholar yearold billing boy remembered stepfather sentenced murder armed immigration officer arent telling local police raid leak problem congress feud trump limit sharing intel duke phenom cooper flagg dallas maverick overall pick nba draft cia evidence iran nuclear program severely damaged assessment strike impact continue little league north park cholla lake mar pending acquisition kellanova ftc antitrust review oklahoma supreme begin oral argument trump spy chief intel iran nuclear facility destroyed meta artificial intelligence copyright blow author republican suddenly realize voter hate health care cut editorial class youve earned place trump drop usa label phone debate ensues define trump drop usa label phone debate ensues define trump drop usa label phone debate ensues define trump drop usa label phone debate ensues define trump lifelong democrat autoworker bill vehicle loan tax benefit oregon house pas bipartisan bill combat chronic absenteeism school republican candidate ran maxine water admits misusing campaign donation scoop protrump unleashes tv ad massie trump administration investigate university california hiring practice ltte noise uv pilot site</t>
         </is>
       </c>
     </row>
@@ -622,12 +618,12 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t xml:space="preserve">plan unveiled for story link at boca at west yamato road in boca raton fact check trump make big false claim about his big domestic policy bill biogen genentech may stay mum on damage at trial inside the trading desk that surfed day of oil market mayhem bloomberg trader bet on interest rate cut from jay powell successor at the fed financial time etf are booming mutual fund want in on the action analyst amd stock will close the gap with nvidia by should you buy amd stock here leadership style arent staticheres why that myth is costing you good manager microservices in healthcare market size to hit usd million by driven by cloud adoption and healthcare digitization sn insider meme coin like pepe and wif lose steamozak ai gain investor attention brilliant stock that could soar by to according to wall street balfour beatty community foundation award over in scholarship hims hers stock investor need to know this before buying or selling this growth stock whats going on with adobe stock nyt wordle hint and answer for june puzzle lpro investor have the opportunity to lead the open lending security fraud lawsuit with faruqi faruqi llp ftre investor deadline fortrea holding inc investor with loss may have been affected by fraud contact bfa law by august court deadline nasdaqftre ogn investor deadline organon co investor with loss may have been affected by fraud contact bfa law by july court deadline nyseogn breaking hims news a security fraud class action ha been filed on behalf of hims hers health inc nysehims investor contact bfa law if you lost money aapl investor deadline apple inc investor with loss may have been affected by fraud contact bfa law by august court deadline nasdaqaapl civi investor deadline civitas resource inc investor with loss may have been affected by fraud contact bfa law by july court deadline nysecivi rddt investor deadline reddit inc investor with loss may have been affected by fraud contact bfa law by august court deadline nyserddt breaking codi news compass diversified holding nysecodi announces nonreliance on financial statement for contact bfa law by july iova investor deadline iovance biotherapeutics investor with loss may have been affected by fraud contact bfa law by july court deadline nasdaqiova womens sober housing along the mississippi ha a bright future following troubled past this stock is up since it ipo here reason it could still be a smart buy oppenheimer co inc raise stock position in marsh mclennan company inc nysemmc kremlin reacts to nato defense spending hike no significant effect house republican don bacon of nebraska will not seek reelection stock market pullback coming etf to buy meta platform inc nasdaqmeta share bought by pinnacle bancorp inc golden state wealth management llc boost stock position in lam research corporation nasdaqlrcx hims hers stock financial analysis following huge stock price crash incredible news for quantumscape stock investor this blackrock etf could soar according to billionaire michael saylor new owner to keep childrens exchange open for rochester family how to start learning math for data science a simple guide at bezos venetian wedding buzz bling and backlash the new york time spire wealth management purchase share of doordash inc nasdaqdash bessemer group inc sell share of ameriprise financial inc nyseamp cambridge investment research advisor inc cut position in huntington bancshares incorporated nasdaqhban beloved grocery chain better than costco to open new store a part of expansion after buying closed winndixie site amd v arista network which artificial intelligence ai stock is a better buy right now tariff drive up firework price ahead of fourth of july tip to save for your celebration tariff drive up firework price ahead of fourth of july tip to save for your celebration tariff drive up firework price ahead of fourth of july tip to save for your celebration agg is a great choice for most but i like this vanguard etf better can disney stock keep rising after hitting a new week high memory of muscatine a post card of the golden state tampa outsource call center firm name new ceo whats going on with micron stock america newest space ipo wa a smashing success reigning ballon dor winner aitana bonmati hospitalized with meningitis less than a week before euro i make a year and want to retire at should i invest more in stock or focus on real estate jeff bezos lauren sanchez join list of richest married couple here how prenups for wealthiest people take place hindustan time hindustan time farm labor land cost dominate discussion at inaugural lake county agricultural summit here what the new condo law requires is it too much to handle here what the new condo law requires is it too much to handle developer file preapplication for mixeduse project at nw th st miami florida debt is a growing force influencing jobseekers choice career expert say here how im year old and the father of functional medicine here my daily routine for a healthy life target face serious challenge a ceo cornell retirement nears walmart slash price on popular summer essential to just and it even cheaper than target version the end of bank branch how europe digital euro and stablecoins are reshaping finance luvmes independence day wig sale limitedtime countdown deal old navy is selling americana flip flop for just theyre identical to havaianas but and nearly cheaper new la trader joes open across the street from another trader joes amid messiness at the social security administration more people are taking benefit early asking the right question can reframe how you respond to challenge grandfather k seized by chase in sudden account closure it destroyed his credit forced him to delay retirement macro trend likely to send bitcoin and xrp skyrocketing in how to budget weekly pay when freight is inconsistent why ai resume are overwhelming recruiter and manager after lahaina burned an experiment in housing the most vulnerable golden state wealth management llc purchase share of diageo plc nysedeo rob biederman join the stage at all stage family and business are concerned about the effect of tariff on youth sport share in meta platform inc nasdaqmeta acquired by mokan wealth management inc meta platform inc nasdaqmeta share sold by moran wealth management llc bessemer group inc reduces stake in tmobile u inc nasdaqtmus bessemer group inc lower stock holding in stryker corporation nysesyk aurora private wealth inc purchase share of meta platform inc nasdaqmeta first pacific financial trim position in meta platform inc nasdaqmeta meta platform inc nasdaqmeta stake lifted by symmetry partner llc gamma investing llc ha million stock holding in meta platform inc nasdaqmeta share in carnival corporation nyseccl bought by oppenheimer asset management inc which stock will dominate the weight management market through thing every tesla investor need to watch right now asset management one co ltd sell share of expeditors international of washington inc nasdaqexpd sch financial advisor inc ha million position in alphabet inc nasdaqgoogl walkner condon financial advisor llc acquires share of alphabet inc nasdaqgoogl fidelity national financial inc nysefnf stake increased by oppenheimer co inc nobrainer stock to buy for under right now house republican don bacon of nebraska will not seek reelection wealth enhancement advisory service llc ha million stock holding in darden restaurant inc nysedri llm project every ai enthusiast should build for a stronger resume how europe can mitigate it mighty defence cost challenge ing which cryptocurrency is more likely to be a millionaire maker xrp v shiba inu mortgage rate hit lowest level since early may why you should drop this phrase from your business email colorado health official brace for layoff amid loss of federal funding from trump administration broadcast bias network shield nyc socialist mamdani from extreme label they apply to conservative fact check trump make big false claim about his big domestic policy bill why donald trump is trying to make an example out of this one house republican colorado play about israelgaza debate explores difficult conversation a crisis deepens editorial cartoon for saturday june letter dial back the false rhetoric that inspires violence memory of firework lyon fall and a childhood fueled by curiosity and imagination albemarle look to add more school zone speed camera after initial success column limit of free speech shouldnt be condoned why it time to make america think again deportation nation trump is gunning for new record in immigration prosecution person rescued friday from the penobscot river supreme court limit judge power to block trump order take a stand against the fascist takeover of america policy change could have big consequence for veteran va care drop the charade when it come to social security medicare tesla say it made it first driverless delivery of a new car to a customer this stock is up since it ipo here reason it could still be a smart buy developer lay out their latest vision for the former pleasant hill golf course opinion what doe it mean to be a patriot reader view protect minnesota resource from data center reader view u hypocritical when sending troop senate to hold initial vote today on trump big beautiful bill senate to hold initial vote today on trump big beautiful bill fall river school employee out after arrest on serious charge how psychiatry and activism created the dangerous concept of transgender child reigning ballon dor winner aitana bonmati hospitalized with meningitis less than a week before euro fbi attack on fentanyl is working to reduce overdose death opinion democrat are trying to figure out what to do about john fetterman conor lamb is stepping up letter to the editor truth aint what it used to be why wouldnt there be a regime change what if a hurricane hit alligator alcatraz florida drawing up evacuation plan opinion john tayer that uncomfortable situation where economic and social interest converge opinion max boykoff what will we say in community editorial board considering the sale of public land who is mitchell berger the fort lauderdale democrat chairing david jolly governor campaign canadian man who died in miami detention lived in daytona beach kenosha festivity to change parking traffic downtown old bogeyman reunite maga after explosive iran divide colorado supreme court accepts case on parole revocation debt collection congressional candidate allard see little need for campaign spending limit a look back colorado republican jeff crank get up close look at fire station air base and a convenience store bridging the lgbtq wealth gap the left political philosophy persuasion with a government club roger koopman thing you need to know about new idf chief canceled screening stalled grant federal cut hit iowa group fighting cancer new ut tyler poll reflects texas voter view on current issue political matchup keep our public land public letter hitching a flight tell your story hitching a flight tell your story letter to the editor flag day deserves to be a federal holiday more than other holiday lost in translation off the record lost in translation off the record i dont shy away from a fight pritzkers run for atypical third term fit unprecedented time what happens if wisconsin budget isnt passed on time i dont shy away from a fight pritzkers run for atypical third term fit unprecedented time i dont shy away from a fight pritzkers run for atypical third term fit unprecedented time abbott paxton can withhold uvalde jan related record texas supreme court rule uw nurse bid to reclaim union status rejected by wisconsin supreme court unanimously dont take me out to the ballgame editorial cartoon for saturday june walter five year on the pandemic still plague california employee safety net legislator review kurth disappointed by republican education funding plan legislator review kurth disappointed by republican education funding plan editorial veto speed cam tax credit bill measure to protect hawaii fishing industry one of five food and farm bill signed friday mayor name nominee to future ocean safety commission gop leader boost rural hospital fund rewrite medicaid provision to save trump megabill gop leader boost rural hospital fund rewrite medicaid provision to save trump megabill gop leader boost rural hospital fund rewrite medicaid provision to save trump megabill republican race toward crucial vote on trump megabill despite uncertainty republican race toward crucial vote on trump megabill despite uncertainty republican race toward crucial vote on trump megabill despite uncertainty gop leader boost rural hospital fund rewrite medicaid provision to save trump megabill gop leader boost rural hospital fund rewrite medicaid provision to save trump megabill gop leader boost rural hospital fund rewrite medicaid provision to save trump megabill republican race toward crucial vote on trump megabill despite uncertainty republican race toward crucial vote on trump megabill despite uncertainty republican race toward crucial vote on trump megabill despite uncertainty the tribune quote of the week quiz for june letter route series neglect to capture the beauty along the road in new mexico final day of scotus decision brings wave of historymaking ruling trump nato turnaround from threatening to pull u out to daddy of the alliance msgr charles j dubois is travis decker alive a fruitless week manhunt ha produced no certain evidence republican plan to overhaul medicaid are already shaking up the midterm trump immigration arrest are seeing a wave of resistance wanda ammons regina gina marie williams baccigalopi letter trump like staging spectacle more than he like helping people heat dome pass but climatefueled wave arent going anywhere word of the week eudaimonia what is the meaning of the pursuit of happiness tom sawyer fence painting closed to girl the jackpod taking a break cnn report from the huge crowd attending state funeral in tehran oreo is bringing back a fanfavorite flavor after year stop yelling at u biden join thousand paying final respect to slain minnesota lawmaker and husband ge appliance moving production from china to republican state matthew schaefer honor late mother after getting selected first overall by new york islander in nhl draft letter city could do better to help north tulsa grow thing every rivian investor need to watch right now shiba inu and cardano price prediction leave investor nervous many are joining the remittix train after gain walmart is selling an excellent soundbar for and shopper say it quite impressive bigfoot stomp in from east county mountain it your business bigfoot stomp in from east county mountain it your business unpacking the content strategy definition a modern marketer guide delta operation recovering through weekend more delay and cancellation sunday alivecom la vega strip casino cant escape troubling trend in their shoe what is life like a an olympic longdistance runner the type of load board when and how to use each bart improves in safety cleanliness and satisfaction yet ridership recovery remains slow uptown aventura planned for biscayne blvd miami fl house gop leadership discussing new way to limit classified information on capitol hill from hallucination to hardware lesson from a realworld computer vision project gone sideways this psychedelic drug flopped on trial result should you buy the dip ai stock up to in that should continue moving higher this ridiculously cheap warren buffett stock could make you richer iranian hacker could become more active after military strike here how to protect your business im not putting on a fing hijab uk singer refuse to virtue signal for palestine pull out of festival three sneaky way sam club trick you into buying a tv worth plus easy tip to maximize your home viewing marktomarket middle east conflict whipsaw energy price cheer to year abc fine wine spirit renews support for pediatric cancer research marktomarket middle east conflict whipsaw energy price xrp price prediction payment token surge incoming xrp rtx xlm expected to outperform in july trump tax bill conflict with trump trade goal editorial supreme court ruling restores right to parent walmart is selling a burner expert grill for just and it cheaper than the lowes version borderland mexico winner in global tariff war could be mexico report say global sport medicine leader smithnephew to sponsor select player competing at wimbledon highlighting advanced solution for joint repair an energy star inside u home is under attack from trump with the cost to homeowner uncertain costco branded insane and archaic a shopper beg chain to speed up roll out of popular checkout method used by rival autodesk inc nasdaqadsk share acquired by spire wealth management spire wealth management raise stock holding in autodesk inc nasdaqadsk alphabet inc nasdaqgoogl is apeiron capital ltds th largest position promising robotics stock to consider june th ameriprise financial inc nyseamp share bought by spire wealth management sequoia financial advisor llc buy share of yum brand inc nyseyum elevance health inc nyseelv share bought by sequoia financial advisor llc robeco institutional asset management bv ha million stock position in paychex inc nasdaqpayx top streaming stock worth watching june th steele capital management inc ha million holding in nvidia corporation nasdaqnvda amphenol corporation nyseaph share purchased by cambridge investment research advisor inc robeco institutional asset management bv purchase share of the charles schwab corporation nyseschw sequoia financial advisor llc buy share of public storage nysepsa nvidia corporation nasdaqnvda share purchased by ipswich investment management co inc spire wealth management boost stock position in ameriprise financial inc nyseamp nvidia corporation nasdaqnvda share bought by bigsur wealth management llc can this burnsville land go from garbage dump to golf destination litecoin remittix and algorand to rally hardest in july while pi coin face further struggle in spy could turn into million french minister call for extension of euus trade talk sen thom tillis say he wont seek reelection after opposing trump megabill the chanzuckerbergs stopped funding social cause kid lost their school shohei ohtani throw fastest pitch of mlb career in third mound start for los angeles dodger watch somebody feed phil at the food wine classic in aspen walmarts sam club make bold move to steal costco customer down should you buy the dip on ionq dogecoin remittix and solana price ready to surge technical setup signal upcoming breakout top ai job recruiter you should know in the u artificial intelligence ai company to buy now and hold forever sol capital management co sell share of meta platform inc nasdaqmeta golden state wealth management llc increase stock position in analog device inc nasdaqadi bessemer group inc ha million holding in celsius holding inc nasdaqcelh the nhl is changing it most bizarre rule is it a big win or a terrible loss the law qa snack packaging a cause for confusion un nuclear watchdog chief say iran could again begin enriching uranium in matter of month nvidia insider dump more than billion in stock according to report it your business i corn crib of newman reopens bar expert forecast new high for bnb rtx hbar in july but which is tipped for gain i have million will my plan to invest for monthly work robeco institutional asset management bv purchase share of toast inc nysetost autodesk inc nasdaqadsk share acquired by cambridge investment research advisor inc portland general electric company nysepor share sold by envestnet portfolio solution inc oped it time for u to treat rare earth metal a instrument of geopolitical power china already doe dividend snowball building predictable cash flow sequoia financial advisor llc increase stock holding in cv health corporation nysecvs equinix inc nasdaqeqix share acquired by perigon wealth management llc robeco institutional asset management bv grows position in cv health corporation nysecvs sequoia financial advisor llc ha million position in dte energy company nysedte kratos defense security solution inc nasdaqktos share purchased by sequoia financial advisor llc robeco institutional asset management bv acquires share of te connectivity ltd nysetel nike inc nysenke share purchased by gamma investing llc head to head review nvidia nasdaqnvda and amtech system nasdaqasys sequoia financial advisor llc acquires share of revvity inc nyservty sequoia financial advisor llc sell share of motorola solution inc nysemsi president trump government cutback could be a serious problem for next year social security cola governor seek clean slate to appoint new hawaii tourism authority board rubrik inc nyserbrk director sell in stock pinterest inc nysepins director sell in stock trump canada trade flip oil market shock and nvidias rise to the top this week in economy ivanka trump hubby jared kushners eightword demand at bezos lavish venice wedding revealed shed like to hindustan time ivanka trump hubby jared kushners eightword demand at bezos lavish venice wedding revealed shed like to hindustan time hindustan time day turn to night in the bar minneapolis rebuilt gay living room a father grief when a light to the world is put out prophecy not politics may also shape america clash with iran tip to quickly start and grow a business is archer aviation stock a buy now amazon member just got early access to hundred of prime day dealsshop the best one up to off travel leisure tariff turmoil uncertainty higher price the new norm across colorado outdoor industry data analytics internship you can apply for this weekend focus group whats your response to u bombing iran axios explains inside ice superpower national hurricane center issue tropical storm warning for tropical depression two what to know reader view antiwar president guess not the high and low of our weather page editor note the high and low of our weather page editor note in silicon valley backyard pescadero struggle with unclean water rising rate oh the horror cyberspace help ruin plot for scaredy cat new in town oh the horror cyberspace help ruin plot for scaredy cat new in town opinion clarence page did you miss a holiday mr president im a christian pastor who wa born in egypt here are fact i learned about iran nuclear obsession opinion alex schwartz what if universal rental assistance were implemented to deal with the housing crisis editorial losing international student will be a blow to cu and boulder house gop leadership discussing new way to limit classified information on capitol hill opinion jim martin boeberts bill to delist gray wolf not surprising given her little hat comment letter to the editor council should set up a citizen advisory panel decision to fire teacher is shameful callous commentary america history of foreign intervention isnt encouraging why trump budget bill could mean america electric vehicle surrender brian howey when masked men are not hero here who made the acadiana advocate allmetro boy track and field team boy scout retiring u flag berry tramel thunder belongs to the entire state which is relishing in nba championship sunday letter gop goal comfort the rich afflict the poor will israeli strike strain iran alliance with russia nebraska prisoner have killed their cellmates while being double bunked lawmaker have yet to limit the practice gen z and millennials push into politics editorial pritzker to run again before he make really big run voicesdebra karplus old dog learning new trick llewellyn king doge kid crude cut to research undermine american strength shohei ohtani throw fastest pitch of mlb career in third mound start for los angeles dodger watch somebody feed phil at the food wine classic in aspen letter to the editor other state are taking advantage of pa for solar wind power ronald brownstein the gop is still trying to repeal obamacare un nuclear watchdog chief say iran could again begin enriching uranium in matter of month another voice diocese followed an oblique unfair process in determining payment the california story we keep erasing democrat howling over iran forced to defend own party history democrat howling over iran forced to defend own party history the year rule of social security a retirement rule democrat howling over iran forced to defend own party history democrat howling over iran forced to defend own party history democrat howling over iran forced to defend own party history democrat howling over iran forced to defend own party history will caron tea for two editorial why chicago ha a restaurant crisis edward keegan nascar ha embraced the chicago backdrop but will it return clarence page new york mayoral race could be a testing ground for a democratic comeback asra nomani how socialist muslim pulled off a year takeover of the democratic party faith leader we cannot be silent about what is happening in america a father grief when a light to the world is put out prophecy not politics may also shape america clash with iran policy that could be affected by supreme court decision on nationwide injunction letter climate job training show what we can accomplish at the state level don wooten iran is a problem of our own making chris mccabe dont let politics abandon our park in tulsa my view tattered letter from the fifty tell a surprising love story thing to catch viewpoint when school is out our child need to keep reading the biomedical research enterprise is under attack trans right distracted driving and paid leave new iowa law take effect july former chief of staff to late rep gerry connolly win democratic nomination for his seat leaving trump side didnt make elon musk much more popular letter option is best choice for bidwell park greensboro unveils fiveyear plan to reduce violent crime raihala meet the minnesotan who coined the term gay pride and tossed a pie in anita bryants face letter congress must approve war resolution act letter congress must approve war resolution act the column nothing to hide yet something to fear are you owed money thanks to the ssfa you might need to do something to get it big trump win boomerang appeal define supreme court term to fight trump funding freeze state try a new gambit withholding federal payment letter mullins leadership key but more is needed beyonce pause performance in houston after prop car tilt midair over crowd convicted boston city councilor tania fernandes anderson prays to avoid time in jail reader speak subpoena ct pura phone before it too late man arrested in deadly stabbing of mother boyfriend in middleborough da say reader view medical research brain drain concerning protester line highway in florida everglades to oppose alligator alcatraz trump approval rating tariff deadline schumers criticism and defense budget shift this week in politics against the odds gen z is breaking into the housing market the spanish town where local soak each other with wine from sport to birth certificate supreme court to confront more antitransgender policy she helped texas close a loophole preventing sexual assault survivor from getting justice why cant more state do it what are voluntary layoff rfk jr move on vaccine cause problem for louisiana bill cassidy lisa kelly medicaid cut will worsen the caregiver crisis weve already seen the warning sign evan brown strengthening america defense start in oklahoma join the item challenge feed the hungry in louisiana by donating this specific list welcome to the louisiana town where highspeed internet line end here how resident make do year into home insurance crisis when will louisiana resident get relief renovating northgate mall will take lot of work jacoby landry say he is up for the challenge this louisiana lawyer is suing big oil for billion but dont call him a tree hugger upstate sc senator enters governor race with endorsement from two lawmaker there a blue drawbridge near myrtle beach why it remains after year of non use lsu interim president matt lee want to keep winning thats what the big dog do you are my sunshine and exlouisiana gov jimmie davis are eternally bound author writes letter some oklahoma lawmaker are putting their party before their country piston malik beasley under federal investigation for nba gambling allegation letter a closer look at face claim letter a closer look at face claim londonbased startup laverock therapeutic raise over million for it gene control tech robinhood expands it global push minute from crypto chief old cramped apartment in cannes medium advisory justice is a common cause day commemoration of the downing of flight p and first memorial unveiled webuy global ltd integrates coinbase to accept stablecoin payment leading the way in travel technology and digital payment in market rally back to record best sp tech trade hasnt been mag or tech sector itself inspirational quote albert einstein virginia woolf and others u dollar suffers worst start to year since financial time canada talk show tariff have created a new world for investor axios doc alleged bribe came before antioch homebuilder played all legal card moderna report phase flu data teeing up new submission with federal support uncertain state and nonprofit scramble to safeguard access to vaccine houstonbased developer proposes story highrise for nw th st miami fl brookfield business partner to host second quarter result conference call expert tip for securing debt financing in a challenging market option flow alert bull making their move in googl stock modernas flu vaccine show positive latestage trial result paving way for combination covid shot ardagh metal packaging sa q result and investor call notification shatterproof name public affair and health leader pam jenkins a new ceo killam apartment reit announces normal course issuer bid largest crossmod neighborhood provides blueprint for scaling new attainable home inventory across the country should you buy xrp ripple while it under first merchant corporation to report second quarter financial result host conference call and webcast st louisarea business opening and closing in june lantronix enters into cooperation agreement with investor group led by chain of lake investment fund llc amazon miss out on switch sale after nintendo pulled product from u site bloomberg signify share repurchase period update avadel pharmaceutical announces unanimous appeal court decision upholding fda approval of lumryz in narcolepsy in administrative procedure act litigation work advice my bos want me to install a work app on my personal phone brookfield infrastructure to host second quarter result conference call king street close oversubscribed european real estate special situation fund ii oncolytics biotech appoints former ambrx executive a chief business officer to drive business development strategy how flower by edie parker landed million social impression with a single campaign jinkosolar and ib vogt partner to deliver highefficiency tiger neo module for spain mwp segovia solar cluster wesco publishes sustainability report modine launch dsu destratification fan bringing bestinclass airflow solution to commercial and industrial space cielo announces agm result and extension of unit offering intershunt enrolls first patient in new heart failure study canadian premium sand inc provides operational update core natural resource provides update on ongoing effort to resume longwall operation at leer south iterum name christine coyne a chief commercial officer to lead orlynvahtm launch and commercial growth way chief marketing officer are harnessing ai right now tonix pharmaceutical announces inclusion in the russell and russell index regenx amends debenture term and announces nonbrokered financing for gross proceeds of king street close oversubscribed european real estate special situation fund ii first legal step taken this time by wsta to untangle the legal knot of the clean truck partnership regenx amends debenture term and announces nonbrokered financing for gross proceeds of cdr foundation announces grant to five nonprofit organization in new york city digital worker have arrived in banking wsj miss a accelerates national growth aiming for store by q iterum name christine coyne a chief commercial officer to lead orlynvahtm launch and commercial growth mty food group inc announces renewal of normal course issuer bid brookfield infrastructure to host second quarter result conference call largest crossmod neighborhood provides blueprint for scaling new attainable home inventory across the country oncolytics biotech appoints former ambrx executive a chief </t>
+          <t>why you should get your boot to beyonces cowboy carter tour a sermon for the weary while you can chinese battery giant and tesla supplier catl is expanding globally here why it matter how to stay on top of google search faraday x preparation are in the final stage for the private preview and cocreation launch event on june th for the groundbreaking fx super one mpv biocon biologics receives health canada approval for yesafilitm aflibercept first global launch scheduled for july china factory activity expected to shrink for third month amid trade tension reuters poll nike vomero quietly became a million franchise in day a ceo say it time to turn the page investor gary black cheer afterhours rally ap technology summarybrief at am edt ap technology summarybrief at am edt ap technology summarybrief at am edt ap technology summarybrief at am edt amazon google not far behind but dan ives say microsoft clearly leading in these segment price target is probably conservative why your to feel more like report say analysisin dovish tilt boj zoom in on obscure underlying inflation trend find the best crypto to join for emerging project reshaping the digital economy tesla shakeup who is omead afshar senior executive reportedly fired by elon musk amid slumping sale i time of india ap business summarybrief at am edt ap business summarybrief at am edt asian share are mostly higher after u stock rise to the brink of a record trump tariff have unsettled thailand pet food exporter germany tell apple google to block deepseek a the chinese ai app face rising pressure in europe hugging face cofounder challenge ai optimist model cant ask original scientific question you might not have bezoslevel buck but you still might consider a prenup vertex founder boger donates m to boston art academy trump big beautiful bill might be unloved and a mess but it will still probably pas here how the luxury real estate market is splitting up how company profit from your data without consent full circle boy leap forward with debut ep jete and official music video this go out to you out now increase of share capital in connection with realization of the employee option programm and subscription result more than an ev charger it peace of mind wherever the road take you cutting u energy credit doesnt save money it steal it from ratepayer local government ansi officially approves two new seia standard on consumer protection and operation and maintenance kymera therapeutic announces pricing of million public offering kymera therapeutic announces pricing of million public offering solaredge expands u manufacturing in salt lake city utah why denver homeowner are investing more in renovation project leap power national grid virtual power plant initiative in massachusetts hawaiian airline report cybersecurity event no flight disruption kitv boeing dreamliner black box recovered data under scrutiny to provide insight into fatal air india crash cso receives grant from mt charitable foundation achieve life science announces pricing of million underwritten public offering the mobility house and schneider electric unveil solar charging depot for turlock unifieds electric school bus fleet trump crypto advisor david sack say july will be a big month say president support legislation on market structure and stablecoins amazon grocery chief blame ridiculous red tape for holding back initiative at whole food were wasting time year old driver from tripura treated with eastern india firstever bachmanns bundle pacing vdh in the end everyone hated the iranian theocracy oklahoma governor kevin stitt and u secretary of health and human service robert f kennedy jr visit mom meal to highlight food a medicine leadership japan executes twitter killer who murdered and dismembered nine people saratoga county celebrates m airport revitalization ap business summarybrief at pm edt ap business summarybrief at pm edt ap business summarybrief at pm edt ap business summarybrief at pm edt ap technology summarybrief at pm edt driver crash nearly plummet over san mateo county cliff north korea just opened a beach resort for people but who will visit jeep gladiator rank first in midsize pickup segment in jd power u initial quality study chrysler jeep and dodge brand improve iq score over thailand will hold trade talk with u next week finance minister say meta say it winning the talent war with openai the verge china u agree on detail of london trade framework beijing say saratogians remember mark straus a pioneer sp cut colombia debt rating to bb over declining fiscal result why lumen technology stock wa winning this week annovis bio to present key finding at alzheimers association international conference iraq war veteran hegseths news conference wa conduct unbecoming chinese influence in climate change lawsuit threatens to derail u energy industry asia fx muted dollar struggle at yr low with pce data on tap demolition start at former kera hq clearing way for new uptown tower european stock extend gain after white house hint at tariff extension baseball player wander franco found guilty in sexual abuse case imposed twoyear suspended sentence china skirt u sanction a top buyer of iranian oil here how and why thats unlikely to change soon china may industrial profit slip back into sharp decline reuters gold head for weekly loss a middle east truce sap demand uk auto production for may slump to lowest level since a trump tariff hit hard mgi announces partnership with negedia enhance genomic sequencing technology at the service of scientific research and precision medicine in italy mgi announces partnership with negedia enhance genomic sequencing technology at the service of scientific research and precision medicine in italy informal mining boom is biggest fear for peru copper investor best cryptos to buy now one already up and climbing bill gate say he know for a fact that more child will die due to u health aid cut and he taking the proof to congress cancer patient recover by taking repurposed antiparasitic drug india economy to hold top spot for growth but underlying weakness remain reuters poll cnbc daily open wall street is tuning out the noise and catching ray turkish farmer pioneer xag agricultural drone for watersmart practice treasury yield inch higher a investor await the fed preferred inflation print bitcoin ethereum rangebound dogecoin dip amid potential july tariff deadline extension analyst predicts btcs next big move once it break out of this range softbank ceo say he all in on openai reveals he long wanted microsofts spot a main backer mexico investigating contamination from spacex explosion debris sandia national laboratory to cut up to workforce by early fall canada approves law to fasttrack resource project face indigenous opposition lithium industry bemoans paradox of low price rising demand china industrial profit slip back into sharp decline in may two north texas school board increase teacher pay in final budget confusion a trump say deal with china signed yet both side violate term of ceasefire share rally but dollar weakens with fed independence seen under threat courtney b vance on book ban protest in los angeles and narrating the audiobook of the biography of web du bois atlantic strategic mineral start commercial production at virginia operation u food and drug administration approves streamlined patient monitoring requirement and removal of rem program within bristol myers squibbs cell therapy label u food and drug administration approves streamlined patient monitoring requirement and removal of rem program within bristol myers squibbs cell therapy label u food and drug administration approves streamlined patient monitoring requirement and removal of rem program within bristol myers squibbs cell therapy label u food and drug administration approves streamlined patient monitoring requirement and removal of rem program within bristol myers squibbs cell therapy label why you should get your boot to beyonces cowboy carter tour a sermon for the weary while you can clarence page did you miss a holiday mr president arthur cyr bombing iran mideast stability and the role of the u former minnesota house speaker melissa hortman to lie in state a suspect face court date former minnesota house speaker melissa hortman to lie in state a suspect face court date democrat are trying to figure out what to do about john fetterman one of them is stepping up democrat are trying to figure out what to do about john fetterman one of them is stepping up democrat are trying to figure out what to do about john fetterman one of them is stepping up supreme court meet friday to decide remaining case including birthright citizenship supreme court meet friday to decide remaining case including birthright citizenship supreme court meet friday to decide remaining case including birthright citizenship supreme court meet friday to decide remaining case including birthright citizenship you might not have bezoslevel buck but you still might consider a prenup summer league basketball islander rattler trump big beautiful bill might be unloved and a mess but it will still probably pas edward d shanshala ii billion in waste fraud and abuse maybe but look in the right place editorial go slow on waymo several caution before selfdriving car arrive rev allison palm rev jonathan hopkins gov ayotte reneged on promise to meet with faith leader senator diverge sharply on damage done by iran strike after classified briefing japan executes twitter killer who murdered and dismembered nine people oregon senate vote to override governor veto a first since dallas place future of the franchise in cooper flagg a southwest division get better north korea just opened a beach resort for people but who will visit panton named johnstown knox elementary school principal former top aide to jill biden subpoenaed in house gop biden age probe iraq war veteran hegseths news conference wa conduct unbecoming selling public land isnt the answer to affordable housing title lx protection matter more than ever trump appointing a shadow chair at the fed ha put dollar under pressure meanwhile china is dumping the greenback and hoarding gold baseball player wander franco found guilty in sexual abuse case imposed twoyear suspended sentence abbott trump approval rating poll show economy thc reduce favorability among texan family file for release in lawsuit considered first involving child challenging arrest at court family file for release in lawsuit considered first involving child challenging arrest at court family sue over u detention in what may be first challenge to courthouse arrest involving kid gov ferguson warns medicaid cut could devastate washington health care system review gloversvilles stump city brewing is modern version of oldtime public house pintsized louisiana is latest state to redefine natural gas a planetwarming fossil fuel a green energy change coming for wilco voter courtney b vance on book ban protest in los angeles and narrating the audiobook of the biography of web du bois critical rce flaw in cisco ise and isepic allow unauthenticated attacker to gain root access pete hegseth air medium coverage grievance towards cnn and others the latest pretrial development in the idaho student killing case green leader larissa water on holding the labor government to account australian politics podcast labor must protect environment while rewriting law written to facilitate development larissa water say wife of minnesota suspect say she wa blindsided by shooting of state politician cnn this is your brain on chatgpt white house confirms u china have reached additional trade agreement trump threatens cnn and new york time with lawsuit over iran report senate parliamentarian ok gop cut to federal food assistance former trail blazer ben mclemore say sex wa consensual while taking the stand during rape trial woman accused of stealing from jewelry store in washington oregon former defense secy iranian nuclear facility damage assessment will take week community rally in massive show of support for caesar palace time square u tariff may sideline youth sport for many family making it harder for kid to stay active rep josh gottheimer american dont like trump big policy bill court issue opinion on centennial at tejon ranch cnn medium analyst responds to false attack on iranian nuclear site report let go through it zohran mamdani tell erin burnett how he plan to pay for his policy fireball fly across the sky and cause sonic boom america controversial iran airstrike letter to the editor june china on alert a nato boost defense spending mamdani vow to stand up to trump border czar and ice canadian official press u government for detail on canadian citizen who died in ice custody at a florida detention center former montana u rep pat williams who won a liberal conservative showdown dy at portland city council pass resolution to strengthen portland street response a look at legal threat facing samesex marriage year after obergefell decision it judgement time for john thune on the big beautiful bill guest commentary rtc targeting senior with displacement former pantagraph building get positive recommendation for landmark status eu leader on wto we need to come up with something else senate democrat question obliteration of iran nuclear site after classified briefing on strike officer placed on leave after shooting in bangor at least orgs urge senator to support iran war power resolution lawsuit filed on behalf of nex benedict estate against owasso public school trump spotlight parent who have lost kid due to open border during big beautiful bill event former trump lawyer kenneth chesebro disbarred in new york over election interference case donald trump say uschina trade truce ha been signed hegseth defends success of u strike on iran nuclear site amid doubt over impact standing up to bullying unscientific transgender activist mob canadian man held by immigration official dy in south florida federal facility official say canadian man held by immigration official dy in south florida federal facility official say canadian man held by immigration official dy in south florida federal facility official say canadian man held by immigration official dy in south florida federal facility official say canadian man held by immigration official dy in south florida federal facility official say canadian man held by immigration official dy in south florida federal facility official say illinois gov jb pritzker announces bid for historic third term amidst presidential buzz interior secretary doug burgum answer question about the big beautiful bill and public land trump doj is targeting daily ko agent mental health passport led to push for secured bond famous preston night rodeo gearing up for it th annual community experience plan unveiled for story link at boca at west yamato road in boca raton fact check trump make big false claim about his big domestic policy bill biogen genentech may stay mum on damage at trial inside the trading desk that surfed day of oil market mayhem bloomberg trader bet on interest rate cut from jay powell successor at the fed financial time etf are booming mutual fund want in on the action analyst amd stock will close the gap with nvidia by should you buy amd stock here leadership style arent staticheres why that myth is costing you good manager microservices in healthcare market size to hit usd million by driven by cloud adoption and healthcare digitization sn insider meme coin like pepe and wif lose steamozak ai gain investor attention brilliant stock that could soar by to according to wall street balfour beatty community foundation award over in scholarship hims hers stock investor need to know this before buying or selling this growth stock whats going on with adobe stock nyt wordle hint and answer for june puzzle lpro investor have the opportunity to lead the open lending security fraud lawsuit with faruqi faruqi llp ftre investor deadline fortrea holding inc investor with loss may have been affected by fraud contact bfa law by august court deadline nasdaqftre ogn investor deadline organon co investor with loss may have been affected by fraud contact bfa law by july court deadline nyseogn breaking hims news a security fraud class action ha been filed on behalf of hims hers health inc nysehims investor contact bfa law if you lost money aapl investor deadline apple inc investor with loss may have been affected by fraud contact bfa law by august court deadline nasdaqaapl civi investor deadline civitas resource inc investor with loss may have been affected by fraud contact bfa law by july court deadline nysecivi rddt investor deadline reddit inc investor with loss may have been affected by fraud contact bfa law by august court deadline nyserddt breaking codi news compass diversified holding nysecodi announces nonreliance on financial statement for contact bfa law by july iova investor deadline iovance biotherapeutics investor with loss may have been affected by fraud contact bfa law by july court deadline nasdaqiova womens sober housing along the mississippi ha a bright future following troubled past this stock is up since it ipo here reason it could still be a smart buy oppenheimer co inc raise stock position in marsh mclennan company inc nysemmc kremlin reacts to nato defense spending hike no significant effect house republican don bacon of nebraska will not seek reelection stock market pullback coming etf to buy meta platform inc nasdaqmeta share bought by pinnacle bancorp inc golden state wealth management llc boost stock position in lam research corporation nasdaqlrcx hims hers stock financial analysis following huge stock price crash incredible news for quantumscape stock investor this blackrock etf could soar according to billionaire michael saylor new owner to keep childrens exchange open for rochester family how to start learning math for data science a simple guide at bezos venetian wedding buzz bling and backlash the new york time spire wealth management purchase share of doordash inc nasdaqdash bessemer group inc sell share of ameriprise financial inc nyseamp cambridge investment research advisor inc cut position in huntington bancshares incorporated nasdaqhban beloved grocery chain better than costco to open new store a part of expansion after buying closed winndixie site amd v arista network which artificial intelligence ai stock is a better buy right now tariff drive up firework price ahead of fourth of july tip to save for your celebration tariff drive up firework price ahead of fourth of july tip to save for your celebration tariff drive up firework price ahead of fourth of july tip to save for your celebration agg is a great choice for most but i like this vanguard etf better can disney stock keep rising after hitting a new week high memory of muscatine a post card of the golden state tampa outsource call center firm name new ceo whats going on with micron stock america newest space ipo wa a smashing success reigning ballon dor winner aitana bonmati hospitalized with meningitis less than a week before euro i make a year and want to retire at should i invest more in stock or focus on real estate jeff bezos lauren sanchez join list of richest married couple here how prenups for wealthiest people take place hindustan time hindustan time farm labor land cost dominate discussion at inaugural lake county agricultural summit here what the new condo law requires is it too much to handle here what the new condo law requires is it too much to handle developer file preapplication for mixeduse project at nw th st miami florida debt is a growing force influencing jobseekers choice career expert say here how im year old and the father of functional medicine here my daily routine for a healthy life target face serious challenge a ceo cornell retirement nears walmart slash price on popular summer essential to just and it even cheaper than target version the end of bank branch how europe digital euro and stablecoins are reshaping finance luvmes independence day wig sale limitedtime countdown deal old navy is selling americana flip flop for just theyre identical to havaianas but and nearly cheaper new la trader joes open across the street from another trader joes amid messiness at the social security administration more people are taking benefit early asking the right question can reframe how you respond to challenge grandfather k seized by chase in sudden account closure it destroyed his credit forced him to delay retirement macro trend likely to send bitcoin and xrp skyrocketing in how to budget weekly pay when freight is inconsistent why ai resume are overwhelming recruiter and manager after lahaina burned an experiment in housing the most vulnerable golden state wealth management llc purchase share of diageo plc nysedeo rob biederman join the stage at all stage family and business are concerned about the effect of tariff on youth sport share in meta platform inc nasdaqmeta acquired by mokan wealth management inc meta platform inc nasdaqmeta share sold by moran wealth management llc bessemer group inc reduces stake in tmobile u inc nasdaqtmus bessemer group inc lower stock holding in stryker corporation nysesyk aurora private wealth inc purchase share of meta platform inc nasdaqmeta first pacific financial trim position in meta platform inc nasdaqmeta meta platform inc nasdaqmeta stake lifted by symmetry partner llc gamma investing llc ha million stock holding in meta platform inc nasdaqmeta share in carnival corporation nyseccl bought by oppenheimer asset management inc which stock will dominate the weight management market through thing every tesla investor need to watch right now asset management one co ltd sell share of expeditors international of washington inc nasdaqexpd sch financial advisor inc ha million position in alphabet inc nasdaqgoogl walkner condon financial advisor llc acquires share of alphabet inc nasdaqgoogl fidelity national financial inc nysefnf stake increased by oppenheimer co inc nobrainer stock to buy for under right now house republican don bacon of nebraska will not seek reelection wealth enhancement advisory service llc ha million stock holding in darden restaurant inc nysedri llm project every ai enthusiast should build for a stronger resume how europe can mitigate it mighty defence cost challenge ing which cryptocurrency is more likely to be a millionaire maker xrp v shiba inu mortgage rate hit lowest level since early may why you should drop this phrase from your business email colorado health official brace for layoff amid loss of federal funding from trump administration broadcast bias network shield nyc socialist mamdani from extreme label they apply to conservative fact check trump make big false claim about his big domestic policy bill why donald trump is trying to make an example out of this one house republican colorado play about israelgaza debate explores difficult conversation a crisis deepens editorial cartoon for saturday june letter dial back the false rhetoric that inspires violence memory of firework lyon fall and a childhood fueled by curiosity and imagination albemarle look to add more school zone speed camera after initial success column limit of free speech shouldnt be condoned why it time to make america think again deportation nation trump is gunning for new record in immigration prosecution person rescued friday from the penobscot river supreme court limit judge power to block trump order take a stand against the fascist takeover of america policy change could have big consequence for veteran va care drop the charade when it come to social security medicare tesla say it made it first driverless delivery of a new car to a customer this stock is up since it ipo here reason it could still be a smart buy developer lay out their latest vision for the former pleasant hill golf course opinion what doe it mean to be a patriot reader view protect minnesota resource from data center reader view u hypocritical when sending troop senate to hold initial vote today on trump big beautiful bill senate to hold initial vote today on trump big beautiful bill fall river school employee out after arrest on serious charge how psychiatry and activism created the dangerous concept of transgender child reigning ballon dor winner aitana bonmati hospitalized with meningitis less than a week before euro fbi attack on fentanyl is working to reduce overdose death opinion democrat are trying to figure out what to do about john fetterman conor lamb is stepping up letter to the editor truth aint what it used to be why wouldnt there be a regime change what if a hurricane hit alligator alcatraz florida drawing up evacuation plan opinion john tayer that uncomfortable situation where economic and social interest converge opinion max boykoff what will we say in community editorial board considering the sale of public land who is mitchell berger the fort lauderdale democrat chairing david jolly governor campaign canadian man who died in miami detention lived in daytona beach kenosha festivity to change parking traffic downtown old bogeyman reunite maga after explosive iran divide colorado supreme court accepts case on parole revocation debt collection congressional candidate allard see little need for campaign spending limit a look back colorado republican jeff crank get up close look at fire station air base and a convenience store bridging the lgbtq wealth gap the left political philosophy persuasion with a government club roger koopman thing you need to know about new idf chief canceled screening stalled grant federal cut hit iowa group fighting cancer new ut tyler poll reflects texas voter view on current issue political matchup keep our public land public letter hitching a flight tell your story hitching a flight tell your story letter to the editor flag day deserves to be a federal holiday more than other holiday lost in translation off the record lost in translation off the record i dont shy away from a fight pritzkers run for atypical third term fit unprecedented time what happens if wisconsin budget isnt passed on time i dont shy away from a fight pritzkers run for atypical third term fit unprecedented time i dont shy away from a fight pritzkers run for atypical third term fit unprecedented time abbott paxton can withhold uvalde jan related record texas supreme court rule uw nurse bid to reclaim union status rejected by wisconsin supreme court unanimously dont take me out to the ballgame editorial cartoon for saturday june walter five year on the pandemic still plague california employee safety net legislator review kurth disappointed by republican education funding plan legislator review kurth disappointed by republican education funding plan editorial veto speed cam tax credit bill measure to protect hawaii fishing industry one of five food and farm bill signed friday mayor name nominee to future ocean safety commission gop leader boost rural hospital fund rewrite medicaid provision to save trump megabill gop leader boost rural hospital fund rewrite medicaid provision to save trump megabill gop leader boost rural hospital fund rewrite medicaid provision to save trump megabill republican race toward crucial vote on trump megabill despite uncertainty republican race toward crucial vote on trump megabill despite uncertainty republican race toward crucial vote on trump megabill despite uncertainty gop leader boost rural hospital fund rewrite medicaid provision to save trump megabill gop leader boost rural hospital fund rewrite medicaid provision to save trump megabill gop leader boost rural hospital fund rewrite medicaid provision to save trump megabill republican race toward crucial vote on trump megabill despite uncertainty republican race toward crucial vote on trump megabill despite uncertainty republican race toward crucial vote on trump megabill despite uncertainty the tribune quote of the week quiz for june letter route series neglect to capture the beauty along the road in new mexico final day of scotus decision brings wave of historymaking ruling trump nato turnaround from threatening to pull u out to daddy of the alliance msgr charles j dubois is travis decker alive a fruitless week manhunt ha produced no certain evidence republican plan to overhaul medicaid are already shaking up the midterm trump immigration arrest are seeing a wave of resistance wanda ammons regina gina marie williams baccigalopi letter trump like staging spectacle more than he like helping people heat dome pass but climatefueled wave arent going anywhere word of the week eudaimonia what is the meaning of the pursuit of happiness tom sawyer fence painting closed to girl the jackpod taking a break cnn report from the huge crowd attending state funeral in tehran oreo is bringing back a fanfavorite flavor after year stop yelling at u biden join thousand paying final respect to slain minnesota lawmaker and husband ge appliance moving production from china to republican state matthew schaefer honor late mother after getting selected first overall by new york islander in nhl draft letter city could do better to help north tulsa grow thing every rivian investor need to watch right now shiba inu and cardano price prediction leave investor nervous many are joining the remittix train after gain walmart is selling an excellent soundbar for and shopper say it quite impressive bigfoot stomp in from east county mountain it your business bigfoot stomp in from east county mountain it your business unpacking the content strategy definition a modern marketer guide delta operation recovering through weekend more delay and cancellation sunday alivecom la vega strip casino cant escape troubling trend in their shoe what is life like a an olympic longdistance runner the type of load board when and how to use each bart improves in safety cleanliness and satisfaction yet ridership recovery remains slow uptown aventura planned for biscayne blvd miami fl house gop leadership discussing new way to limit classified information on capitol hill from hallucination to hardware lesson from a realworld computer vision project gone sideways this psychedelic drug flopped on trial result should you buy the dip ai stock up to in that should continue moving higher this ridiculously cheap warren buffett stock could make you richer iranian hacker could become more active after military strike here how to protect your business im not putting on a fing hijab uk singer refuse to virtue signal for palestine pull out of festival three sneaky way sam club trick you into buying a tv worth plus easy tip to maximize your home viewing marktomarket middle east conflict whipsaw energy price cheer to year abc fine wine spirit renews support for pediatric cancer research marktomarket middle east conflict whipsaw energy price xrp price prediction payment token surge incoming xrp rtx xlm expected to outperform in july trump tax bill conflict with trump trade goal editorial supreme court ruling restores right to parent walmart is selling a burner expert grill for just and it cheaper than the lowes version borderland mexico winner in global tariff war could be mexico report say global sport medicine leader smithnephew to sponsor select player competing at wimbledon highlighting advanced solution for joint repair an energy star inside u home is under attack from trump with the cost to homeowner uncertain costco branded insane and archaic a shopper beg chain to speed up roll out of popular checkout method used by rival autodesk inc nasdaqadsk share acquired by spire wealth management spire wealth management raise stock holding in autodesk inc nasdaqadsk alphabet inc nasdaqgoogl is apeiron capital ltds th largest position promising robotics stock to consider june th ameriprise financial inc nyseamp share bought by spire wealth management sequoia financial advisor llc buy share of yum brand inc nyseyum elevance health inc nyseelv share bought by sequoia financial advisor llc robeco institutional asset management bv ha million stock position in paychex inc nasdaqpayx top streaming stock worth watching june th steele capital management inc ha million holding in nvidia corporation nasdaqnvda amphenol corporation nyseaph share purchased by cambridge investment research advisor inc robeco institutional asset management bv purchase share of the charles schwab corporation nyseschw sequoia financial advisor llc buy share of public storage nysepsa nvidia corporation nasdaqnvda share purchased by ipswich investment management co inc spire wealth management boost stock position in ameriprise financial inc nyseamp nvidia cor</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>plan unveiled story link boca west yamato road boca raton fact trump false claim domestic policy bill biogen genentech stay mum damage trial inside trading desk surfed oil market mayhem bloomberg trader bet interest rate cut jay powell successor fed financial booming mutual fund action analyst amd stock close gap nvidia buy amd stock leadership style arent staticheres myth costing good manager microservices healthcare market size hit usd million driven cloud adoption healthcare digitization sn insider meme coin pepe wif lose steamozak ai gain investor attention brilliant stock soar according wall street balfour beatty community foundation award scholarship hims stock investor buying selling growth stock whats adobe stock nyt wordle hint answer puzzle lpro investor opportunity lead open lending security fraud lawsuit faruqi faruqi llp ftre investor deadline fortrea investor loss affected fraud contact bfa august deadline nasdaqftre ogn investor deadline organon co investor loss affected fraud contact bfa deadline nyseogn breaking hims security fraud class action filed behalf hims health nysehims investor contact bfa money aapl investor deadline apple investor loss affected fraud contact bfa august deadline nasdaqaapl civi investor deadline civitas resource investor loss affected fraud contact bfa deadline nysecivi rddt investor deadline reddit investor loss affected fraud contact bfa august deadline nyserddt breaking codi compass diversified nysecodi announces nonreliance financial statement contact bfa iova investor deadline iovance biotherapeutics investor loss affected fraud contact bfa deadline nasdaqiova womens sober housing along mississippi bright future following troubled past stock since ipo smart buy oppenheimer co raise stock marsh mclennan company nysemmc kremlin reacts nato defense spending hike significant effect house republican bacon nebraska seek reelection stock market pullback coming buy meta platform nasdaqmeta share bought pinnacle bancorp golden wealth boost stock lam research corporation nasdaqlrcx hims stock financial analysis following stock price crash incredible quantumscape stock investor blackrock soar according billionaire michael saylor new owner childrens exchange open rochester family start learning math data science simple guide bezos venetian wedding buzz bling backlash new york spire wealth purchase share doordash nasdaqdash bessemer sell share ameriprise financial nyseamp cambridge investment research advisor cut huntington bancshares incorporated nasdaqhban beloved grocery chain better costco open new store part expansion buying closed winndixie site amd v arista network artificial intelligence ai stock better buy tariff drive firework price ahead fourth tip save celebration tariff drive firework price ahead fourth tip save celebration tariff drive firework price ahead fourth tip save celebration agg great choice vanguard better disney stock rising hitting new high memory muscatine post card golden tampa outsource call center firm name new ceo whats micron stock america newest space ipo smashing success reigning ballon dor winner aitana bonmati hospitalized meningitis less euro retire invest stock focus real estate jeff bezos lauren sanchez join list richest married couple prenups wealthiest people take place hindustan hindustan labor land cost dominate discussion inaugural lake county agricultural summit new condo requires handle new condo requires handle developer file preapplication mixeduse project nw st miami florida debt growing force influencing jobseekers choice career expert im old father functional medicine routine healthy life target face serious challenge ceo cornell retirement nears walmart slash price popular summer essential cheaper target version end bank branch europe digital euro stablecoins reshaping finance luvmes independence wig sale limitedtime countdown deal old navy selling americana flip flop theyre identical havaianas nearly cheaper new la trader joes open across street another trader joes amid messiness social security administration people taking benefit early asking reframe respond challenge grandfather k seized chase sudden account closure destroyed credit forced delay retirement macro trend likely send bitcoin xrp skyrocketing budget weekly pay freight inconsistent ai resume overwhelming recruiter manager lahaina burned experiment housing vulnerable golden wealth purchase share diageo plc nysedeo rob biederman join stage stage family business concerned effect tariff youth sport share meta platform nasdaqmeta acquired mokan wealth meta platform nasdaqmeta share moran wealth bessemer reduces stake tmobile nasdaqtmus bessemer lower stock stryker corporation nysesyk aurora private wealth purchase share meta platform nasdaqmeta pacific financial trim meta platform nasdaqmeta meta platform nasdaqmeta stake lifted symmetry partner gamma investing million stock meta platform nasdaqmeta share carnival corporation nyseccl bought oppenheimer asset stock dominate weight market tesla investor watch asset co ltd sell share expeditors international washington nasdaqexpd sch financial advisor million alphabet nasdaqgoogl walkner condon financial advisor acquires share alphabet nasdaqgoogl fidelity national financial nysefnf stake increased oppenheimer co nobrainer stock buy house republican bacon nebraska seek reelection wealth enhancement advisory service million stock darden restaurant nysedri llm project ai enthusiast build stronger resume europe mitigate mighty defence cost challenge ing cryptocurrency likely millionaire maker xrp v shiba inu mortgage rate hit lowest level since early drop phrase business email colorado health brace layoff amid loss federal funding trump administration broadcast bias network shield nyc socialist mamdani extreme label apply conservative fact trump false claim domestic policy bill donald trump example house republican colorado play israelgaza debate explores difficult conversation crisis deepens editorial cartoon saturday dial false rhetoric inspires violence memory firework lyon fall childhood fueled curiosity imagination albemarle look add school zone speed camera initial success column limit free speech shouldnt condoned america deportation nation trump gunning new record immigration prosecution rescued friday penobscot river supreme limit judge power block trump order take stand fascist takeover america policy change consequence veteran va care drop charade come social security medicare tesla driverless delivery new car customer stock since ipo smart buy developer lay latest vision pleasant hill golf course opinion doe patriot reader view protect minnesota resource data center reader view hypocritical sending troop senate initial vote trump bill senate initial vote trump bill fall river school employee arrest serious charge psychiatry activism created dangerous concept transgender child reigning ballon dor winner aitana bonmati hospitalized meningitis less euro fbi attack fentanyl working reduce overdose death opinion democrat figure john fetterman conor lamb stepping editor truth aint used wouldnt regime change hurricane hit alligator alcatraz florida drawing evacuation plan opinion john tayer uncomfortable situation economic social interest converge opinion max boykoff community editorial board considering sale public land mitchell berger fort lauderdale democrat chairing david jolly governor campaign canadian man died miami detention lived daytona beach kenosha festivity change parking traffic downtown old bogeyman reunite maga explosive iran divide colorado supreme accepts parole revocation debt collection congressional candidate allard little campaign spending limit look colorado republican jeff crank close look fire station air base convenience store bridging lgbtq wealth gap left political philosophy persuasion government club roger koopman new idf chief canceled screening stalled grant federal cut hit iowa fighting cancer new ut tyler poll reflects texas voter view issue political matchup public land public hitching flight story hitching flight story editor flag deserves federal holiday holiday translation record translation record dont shy away fight pritzkers run atypical third term fit unprecedented happens wisconsin budget isnt passed dont shy away fight pritzkers run atypical third term fit unprecedented dont shy away fight pritzkers run atypical third term fit unprecedented abbott paxton withhold uvalde jan related record texas supreme rule uw nurse bid reclaim union status rejected wisconsin supreme unanimously dont take ballgame editorial cartoon saturday walter five pandemic plague california employee safety net legislator review kurth disappointed republican education funding plan legislator review kurth disappointed republican education funding plan editorial veto speed cam tax credit bill measure protect hawaii fishing industry five bill signed friday mayor name nominee future ocean safety commission gop boost rural hospital fund rewrite medicaid provision save trump megabill gop boost rural hospital fund rewrite medicaid provision save trump megabill gop boost rural hospital fund rewrite medicaid provision save trump megabill republican race crucial vote trump megabill uncertainty republican race crucial vote trump megabill uncertainty republican race crucial vote trump megabill uncertainty gop boost rural hospital fund rewrite medicaid provision save trump megabill gop boost rural hospital fund rewrite medicaid provision save trump megabill gop boost rural hospital fund rewrite medicaid provision save trump megabill republican race crucial vote trump megabill uncertainty republican race crucial vote trump megabill uncertainty republican race crucial vote trump megabill uncertainty tribune quiz route series neglect capture beauty along road new mexico final scotus decision brings wave historymaking ruling trump nato turnaround threatening pull daddy alliance msgr charles j dubois travis decker alive fruitless manhunt produced certain evidence republican plan overhaul medicaid shaking midterm trump immigration arrest seeing wave resistance wanda ammons regina gina marie williams baccigalopi trump staging spectacle helping people heat dome pas climatefueled wave arent anywhere word eudaimonia meaning pursuit happiness tom sawyer fence painting closed girl jackpod taking break cnn report crowd attending funeral tehran oreo bringing fanfavorite flavor stop yelling biden join thousand paying final respect slain minnesota lawmaker husband ge appliance moving production china republican matthew schaefer honor late mother getting selected overall new york islander nhl draft better help north tulsa grow rivian investor watch shiba inu cardano price prediction investor nervous joining remittix train gain walmart selling excellent soundbar shopper impressive bigfoot stomp east county mountain business bigfoot stomp east county mountain business unpacking content strategy definition modern marketer guide delta operation recovering weekend delay cancellation sunday alivecom la vega strip casino cant escape troubling trend shoe life olympic longdistance runner type load board bart improves safety cleanliness satisfaction yet ridership recovery remains slow uptown aventura planned biscayne blvd miami fl house gop leadership discussing new limit classified information capitol hill hallucination hardware lesson realworld computer vision project sideways psychedelic drug flopped trial buy dip ai stock continue moving higher ridiculously cheap warren buffett stock richer iranian hacker become active military strike protect business im putting fing hijab uk singer refuse virtue signal palestine pull festival sneaky sam club trick buying tv worth plus easy tip maximize viewing marktomarket middle east conflict whipsaw energy price cheer abc fine wine spirit renews support pediatric cancer research marktomarket middle east conflict whipsaw energy price xrp price prediction payment token surge incoming xrp rtx xlm expected outperform trump tax bill conflict trump trade goal editorial supreme ruling restores parent walmart selling burner expert grill cheaper lowes version borderland mexico winner global tariff war mexico report global sport medicine smithnephew sponsor select player competing wimbledon highlighting advanced solution joint repair energy star inside attack trump cost homeowner uncertain costco branded insane archaic shopper beg chain speed roll popular checkout method used rival autodesk nasdaqadsk share acquired spire wealth spire wealth raise stock autodesk nasdaqadsk alphabet nasdaqgoogl apeiron ltds largest promising robotics stock consider ameriprise financial nyseamp share bought spire wealth sequoia financial advisor buy share yum brand nyseyum elevance health nyseelv share bought sequoia financial advisor robeco institutional asset bv million stock paychex nasdaqpayx streaming stock worth watching steele million nvidia corporation nasdaqnvda amphenol corporation nyseaph share purchased cambridge investment research advisor robeco institutional asset bv purchase share charles schwab corporation nyseschw sequoia financial advisor buy share public storage nysepsa nvidia corporation nasdaqnvda share purchased ipswich investment co spire wealth boost stock ameriprise financial nyseamp nvidia corporation nasdaqnvda share bought bigsur wealth burnsville land garbage dump golf destination litecoin remittix algorand rally hardest pi coin face struggle spy turn million french minister call extension euus trade sen thom tillis wont seek reelection opposing trump megabill chanzuckerbergs stopped funding social cause kid school shohei ohtani throw fastest pitch mlb career third mound start los angeles dodger watch somebody feed phil wine classic aspen walmarts sam club bold move steal costco customer buy dip ionq dogecoin remittix solana price ready surge technical setup signal upcoming breakout ai job recruiter artificial intelligence ai company buy forever sol co sell share meta platform nasdaqmeta golden wealth increase stock analog device nasdaqadi bessemer million celsius nasdaqcelh nhl changing bizarre rule terrible loss qa snack packaging cause confusion un nuclear watchdog chief iran begin enriching uranium matter month nvidia insider dump billion stock according report business corn crib newman reopens bar expert forecast new high bnb rtx hbar tipped gain million plan invest monthly work robeco institutional asset bv purchase share toast nysetost autodesk nasdaqadsk share acquired cambridge investment research advisor portland general electric company nysepor share envestnet portfolio solution oped treat rare earth metal instrument geopolitical power china doe dividend snowball building predictable cash flow sequoia financial advisor increase stock cv health corporation nysecvs equinix nasdaqeqix share acquired perigon wealth robeco institutional asset bv grows cv health corporation nysecvs sequoia financial advisor million dte energy company nysedte kratos defense security solution nasdaqktos share purchased sequoia financial advisor robeco institutional asset bv acquires share te connectivity ltd nysetel nike nysenke share purchased gamma investing head head review nvidia nasdaqnvda amtech system nasdaqasys sequoia financial advisor acquires share revvity nyservty sequoia financial advisor sell share motorola solution nysemsi president trump government cutback serious problem next social security cola governor seek clean slate appoint new hawaii tourism authority board rubrik nyserbrk director sell stock pinterest nysepins director sell stock trump canada trade flip oil market shock nvidias rise economy ivanka trump hubby jared kushners eightword demand bezos lavish venice wedding revealed shed hindustan ivanka trump hubby jared kushners eightword demand bezos lavish venice wedding revealed shed hindustan hindustan turn night bar minneapolis rebuilt gay living room father grief light world put prophecy politics shape america clash iran tip quickly start grow business archer aviation stock buy amazon got early access hundred prime dealsshop best travel leisure tariff turmoil uncertainty higher price new norm across colorado outdoor industry data analytics internship apply weekend focus whats response bombing iran axios explains inside superpower national hurricane center issue tropical storm warning tropical depression reader view antiwar president guess high low weather page editor note high low weather page editor note silicon valley backyard pescadero struggle unclean water rising rate oh horror cyberspace help ruin plot scaredy cat new town oh horror cyberspace help ruin plot scaredy cat new town opinion clarence page miss holiday mr president im christian pastor born egypt fact learned iran nuclear obsession opinion alex schwartz universal rental assistance implemented deal housing crisis editorial losing international student blow cu boulder house gop leadership discussing new limit classified information capitol hill opinion jim martin boeberts bill delist gray wolf surprising little hat editor council set citizen advisory panel decision fire teacher shameful callous commentary america history foreign intervention isnt encouraging trump budget bill america electric vehicle surrender brian howey masked men hero acadiana advocate allmetro boy track field team boy scout retiring flag berry tramel thunder belongs relishing nba championship sunday gop goal comfort rich afflict poor israeli strike strain iran alliance russia nebraska prisoner killed cellmates double bunked lawmaker yet limit practice gen z millennials push politics editorial pritzker run run voicesdebra karplus old dog learning new trick llewellyn king doge kid crude cut research undermine american strength shohei ohtani throw fastest pitch mlb career third mound start los angeles dodger watch somebody feed phil wine classic aspen editor taking advantage pa solar wind power ronald brownstein gop repeal obamacare un nuclear watchdog chief iran begin enriching uranium matter month another voice diocese followed oblique unfair process determining payment california story erasing democrat howling iran forced defend party history democrat howling iran forced defend party history rule social security retirement rule democrat howling iran forced defend party history democrat howling iran forced defend party history democrat howling iran forced defend party history democrat howling iran forced defend party history caron tea editorial chicago restaurant crisis edward keegan nascar embraced chicago backdrop clarence page new york mayoral race testing ground democratic comeback asra nomani socialist muslim pulled takeover democratic party faith silent happening america father grief light world put prophecy politics shape america clash iran policy affected supreme decision nationwide injunction climate job training accomplish level wooten iran problem making chris mccabe dont politics abandon park tulsa view tattered fifty surprising love story catch viewpoint school child reading biomedical research enterprise attack trans distracted driving paid new iowa take effect chief staff late rep gerry connolly democratic nomination seat leaving trump didnt elon musk popular option best choice bidwell park greensboro unveils fiveyear plan reduce violent crime raihala meet minnesotan coined term gay pride tossed pie anita bryants face congress must approve war resolution act congress must approve war resolution act column nothing hide yet something fear owed money ssfa something trump boomerang appeal define supreme term fight trump funding freeze try new gambit withholding federal payment mullins leadership needed beyonce pause performance houston prop car tilt midair crowd convicted boston councilor tania fernandes anderson prays avoid jail reader speak subpoena ct pura phone late man arrested deadly stabbing mother boyfriend middleborough da reader view medical research brain drain concerning protester line highway florida everglades oppose alligator alcatraz trump approval rating tariff deadline schumers criticism defense budget shift politics odds gen z breaking housing market spanish town local soak wine sport birth certificate supreme confront antitransgender policy helped texas close loophole preventing sexual assault survivor getting justice cant voluntary layoff rfk jr move vaccine cause problem louisiana bill cassidy lisa kelly medicaid cut worsen caregiver crisis weve seen warning sign evan brown strengthening america defense start oklahoma join item challenge feed hungry louisiana donating specific list welcome louisiana town highspeed internet line end resident insurance crisis louisiana resident relief renovating northgate mall take lot work jacoby landry challenge louisiana lawyer suing oil billion dont call tree hugger upstate sc senator enters governor race endorsement lawmaker blue drawbridge near myrtle beach remains non lsu interim president matt lee winning thats dog sunshine exlouisiana gov jimmie davis eternally bound author writes oklahoma lawmaker putting party country piston malik beasley federal investigation nba gambling allegation closer look face claim closer look face claim londonbased startup laverock therapeutic raise million gene control tech robinhood expands global push crypto chief old cramped apartment cannes medium advisory justice common cause commemoration downing flight p memorial unveiled webuy global ltd integrates coinbase accept stablecoin payment leading travel technology digital payment market rally record best sp tech trade hasnt mag tech sector inspirational albert einstein virginia woolf others dollar suffers worst start since financial canada tariff created new world investor axios doc alleged bribe came antioch homebuilder played legal card moderna report phase flu data teeing new submission federal support uncertain nonprofit scramble safeguard access vaccine houstonbased developer proposes story highrise nw st miami fl brookfield business partner host quarter conference call expert tip securing debt financing challenging market option flow alert bull making move googl stock modernas flu vaccine positive latestage trial paving combination covid shot ardagh metal packaging sa q investor call notification shatterproof name public affair health pam jenkins new ceo killam apartment reit announces normal course issuer bid largest crossmod neighborhood provides blueprint scaling new attainable inventory across country buy xrp ripple merchant corporation report quarter financial host conference call webcast st louisarea business opening closing lantronix enters cooperation agreement investor led chain lake investment fund amazon miss switch sale nintendo pulled product site bloomberg signify share repurchase period update avadel pharmaceutical announces unanimous appeal decision upholding fda approval lumryz narcolepsy administrative procedure act litigation work advice bos install work app personal phone brookfield infrastructure host quarter conference call king street close oversubscribed european real estate special situation fund ii oncolytics biotech appoints ambrx executive chief business officer drive business development strategy flower edie parker landed million social impression single campaign jinkosolar ib vogt partner deliver highefficiency tiger neo module spain mwp segovia solar cluster wesco publishes sustainability report modine launch dsu destratification fan bringing bestinclass airflow solution commercial industrial space cielo announces agm extension unit offering intershunt enrolls patient new heart failure study canadian premium sand provides operational update core natural resource provides update ongoing effort resume longwall operation leer south iterum name christine coyne chief commercial officer lead orlynvahtm launch commercial growth chief marketing officer harnessing ai tonix pharmaceutical announces inclusion russell russell index regenx amends debenture term announces nonbrokered financing gross proceeds king street close oversubscribed european real estate special situation fund ii legal step taken wsta untangle legal knot clean truck partnership regenx amends debenture term announces nonbrokered financing gross proceeds cdr foundation announces grant five nonprofit organization new york digital worker arrived banking wsj miss accelerates national growth aiming store q iterum name christine coyne chief commercial officer lead orlynvahtm launch commercial growth mty announces renewal normal course issuer bid brookfield infrastructure host quarter conference call largest crossmod neighborhood provides blueprint scaling new attainable inventory across country oncolytics biotech appoints ambrx executive chief</t>
+          <t>boot beyonces cowboy carter tour sermon weary chinese battery giant tesla supplier catl expanding globally matter stay google search faraday x preparation final stage private preview cocreation launch event groundbreaking fx super mpv biocon biologics receives health canada approval yesafilitm aflibercept global launch scheduled china factory activity expected shrink third month amid trade tension reuters poll nike vomero quietly became million franchise ceo turn page investor gary black cheer afterhours rally technology technology technology technology amazon google far behind dan ives microsoft clearly leading segment price target probably conservative feel report analysisin dovish tilt boj zoom obscure underlying inflation trend find best crypto join emerging project reshaping digital economy tesla shakeup omead afshar senior executive reportedly fired elon musk amid slumping sale india business business asian mostly higher stock rise brink record trump tariff unsettled thailand pet exporter germany apple google block deepseek chinese ai app face rising pressure europe hugging face cofounder challenge ai optimist model cant original scientific bezoslevel buck consider prenup vertex founder boger donates boston art academy trump bill unloved mess probably pa luxury real estate market splitting company profit data without consent full circle boy leap forward debut ep jete music video increase connection realization employee option programm subscription ev charger peace mind wherever road take cutting energy credit doesnt save money steal ratepayer local government ansi officially approves seia consumer protection operation maintenance kymera therapeutic announces pricing million public offering kymera therapeutic announces pricing million public offering solaredge expands manufacturing salt lake utah denver homeowner investing renovation project leap power national grid virtual power plant initiative massachusetts hawaiian airline report cybersecurity event flight disruption kitv boeing dreamliner black box recovered data scrutiny provide insight fatal air india crash cso receives grant mt charitable foundation achieve life science announces pricing million underwritten public offering mobility house schneider electric unveil solar charging depot turlock unifieds electric school bus fleet trump crypto advisor david sack month president support legislation market structure stablecoins amazon grocery chief blame ridiculous red tape initiative wasting old driver tripura treated eastern india firstever bachmanns bundle pacing vdh end everyone hated iranian theocracy oklahoma governor kevin stitt secretary health human service robert f kennedy jr visit mom meal highlight medicine leadership japan executes twitter killer murdered dismembered nine people saratoga county celebrates airport revitalization business pm business pm business pm business pm technology pm driver crash nearly plummet san mateo county cliff north korea opened beach resort people visit jeep gladiator rank midsize pickup segment jd power initial quality study chrysler jeep dodge brand improve iq score thailand trade next finance minister meta winning talent war openai verge china agree detail london trade framework beijing saratogians remember mark straus pioneer sp cut colombia debt rating bb declining fiscal lumen technology stock winning annovis bio present finding alzheimers association international conference iraq war veteran hegseths conference conduct unbecoming chinese influence climate change lawsuit threatens derail energy industry asia fx muted dollar struggle yr low pce data tap demolition start kera hq clearing uptown tower european stock extend gain white house hint tariff extension baseball player wander franco found guilty sexual abuse imposed twoyear suspended sentence china skirt sanction buyer iranian oil thats unlikely change soon china industrial profit slip sharp decline reuters gold head weekly loss middle east truce sap demand uk auto production slump lowest level since trump tariff hit hard mgi announces partnership negedia enhance genomic sequencing technology service scientific research precision medicine italy mgi announces partnership negedia enhance genomic sequencing technology service scientific research precision medicine italy informal mining boom biggest fear peru copper investor best cryptos buy climbing bill gate fact child die due health aid cut taking proof congress cancer patient recover taking repurposed antiparasitic drug india economy spot growth underlying weakness reuters poll cnbc open wall street tuning noise catching ray turkish farmer pioneer xag agricultural drone watersmart practice treasury yield inch higher investor await fed preferred inflation print bitcoin ethereum rangebound dogecoin dip amid potential tariff deadline extension analyst predicts btcs next move break range softbank ceo openai reveals wanted microsofts spot main backer mexico investigating contamination spacex explosion debris sandia national laboratory cut workforce early fall canada approves fasttrack resource project face indigenous opposition lithium industry bemoans paradox low price rising demand china industrial profit slip sharp decline north texas school board increase teacher pay final budget confusion trump deal china signed yet violate term ceasefire rally dollar weakens fed independence seen threat courtney b vance book ban protest los angeles narrating audiobook biography web du bois atlantic strategic mineral start commercial production virginia operation drug administration approves streamlined patient monitoring requirement removal rem program bristol myers squibbs cell therapy label drug administration approves streamlined patient monitoring requirement removal rem program bristol myers squibbs cell therapy label drug administration approves streamlined patient monitoring requirement removal rem program bristol myers squibbs cell therapy label drug administration approves streamlined patient monitoring requirement removal rem program bristol myers squibbs cell therapy label boot beyonces cowboy carter tour sermon weary clarence page miss holiday mr president arthur cyr bombing iran mideast stability role minnesota house speaker melissa hortman lie suspect face date minnesota house speaker melissa hortman lie suspect face date democrat figure john fetterman stepping democrat figure john fetterman stepping democrat figure john fetterman stepping supreme meet friday decide remaining birthright citizenship supreme meet friday decide remaining birthright citizenship supreme meet friday decide remaining birthright citizenship supreme meet friday decide remaining birthright citizenship bezoslevel buck consider prenup summer league basketball islander rattler trump bill unloved mess probably pa edward shanshala ii billion waste fraud abuse maybe look place editorial slow waymo several caution selfdriving car arrive rev allison palm rev jonathan hopkins gov ayotte reneged promise meet faith senator diverge sharply damage iran strike classified briefing japan executes twitter killer murdered dismembered nine people oregon senate vote override governor veto since dallas place future franchise cooper flagg southwest division better north korea opened beach resort people visit panton named johnstown knox elementary school principal aide jill biden subpoenaed house gop biden age probe iraq war veteran hegseths conference conduct unbecoming selling public land isnt answer affordable housing title lx protection matter ever trump appointing shadow chair fed put dollar pressure meanwhile china dumping greenback hoarding gold baseball player wander franco found guilty sexual abuse imposed twoyear suspended sentence abbott trump approval rating poll economy thc reduce favorability among texan family file release lawsuit considered involving child challenging arrest family file release lawsuit considered involving child challenging arrest family sue detention challenge courthouse arrest involving kid gov ferguson warns medicaid cut devastate washington health care system review gloversvilles stump brewing modern version oldtime public house pintsized louisiana latest redefine natural gas planetwarming fossil fuel green energy change coming wilco voter courtney b vance book ban protest los angeles narrating audiobook biography web du bois critical rce flaw cisco ise isepic allow unauthenticated attacker gain root access pete hegseth air medium coverage grievance towards cnn others latest pretrial development idaho student killing green larissa water labor government account australian politics podcast labor must protect environment rewriting written facilitate development larissa water wife minnesota suspect blindsided shooting politician cnn brain chatgpt white house confirms china reached additional trade agreement trump threatens cnn york lawsuit iran report senate parliamentarian ok gop cut federal assistance trail blazer ben mclemore sex consensual taking stand rape trial woman accused stealing jewelry store washington oregon defense secy iranian nuclear facility damage assessment take community rally massive support caesar palace square tariff sideline youth sport family making harder kid stay active rep josh gottheimer american dont trump policy bill issue opinion centennial tejon ranch cnn medium analyst responds false attack iranian nuclear site report zohran mamdani erin burnett plan pay policy fireball fly across sky cause sonic boom america controversial iran airstrike editor china alert nato boost defense spending mamdani vow stand trump border czar canadian press government detail canadian citizen died custody florida detention center montana rep pat williams liberal conservative showdown dy portland council pas resolution strengthen portland street response look legal threat facing samesex marriage obergefell decision judgement john thune bill guest commentary rtc targeting senior displacement pantagraph building positive recommendation landmark status eu wto come something else senate democrat obliteration iran nuclear site classified briefing strike officer placed shooting bangor least orgs urge senator support iran war power resolution lawsuit filed behalf nex benedict estate owasso public school trump spotlight parent kid due open border bill event trump lawyer kenneth chesebro disbarred york election interference donald trump uschina trade truce signed hegseth defends success strike iran nuclear site amid doubt impact standing bullying unscientific transgender activist mob canadian man immigration dy south florida federal facility canadian man immigration dy south florida federal facility canadian man immigration dy south florida federal facility canadian man immigration dy south florida federal facility canadian man immigration dy south florida federal facility canadian man immigration dy south florida federal facility illinois gov jb pritzker announces bid historic third term amidst presidential buzz interior secretary doug burgum answer bill public land trump doj targeting ko agent mental health passport led push secured bond famous preston night rodeo gearing annual community experience plan unveiled story link boca west yamato road boca raton fact trump false claim domestic policy bill biogen genentech stay mum damage trial inside trading desk surfed oil market mayhem bloomberg trader bet interest rate cut jay powell successor fed financial booming mutual fund action analyst amd stock close gap nvidia buy amd stock leadership style arent staticheres myth costing good manager microservices healthcare market size hit usd million driven cloud adoption healthcare digitization sn insider meme coin pepe wif lose steamozak ai gain investor attention brilliant stock soar according wall street balfour beatty community foundation award scholarship hims stock investor buying selling growth stock whats adobe stock nyt wordle hint answer puzzle lpro investor opportunity lead open lending security fraud lawsuit faruqi faruqi llp ftre investor deadline fortrea investor loss affected fraud contact bfa august deadline nasdaqftre ogn investor deadline organon co investor loss affected fraud contact bfa deadline nyseogn breaking hims security fraud class action filed behalf hims health nysehims investor contact bfa money aapl investor deadline apple investor loss affected fraud contact bfa august deadline nasdaqaapl civi investor deadline civitas resource investor loss affected fraud contact bfa deadline nysecivi rddt investor deadline reddit investor loss affected fraud contact bfa august deadline nyserddt breaking codi compass diversified nysecodi announces nonreliance financial statement contact bfa iova investor deadline iovance biotherapeutics investor loss affected fraud contact bfa deadline nasdaqiova womens sober housing along mississippi bright future following troubled past stock since ipo smart buy oppenheimer co raise stock marsh mclennan company nysemmc kremlin reacts nato defense spending hike significant effect house republican bacon nebraska seek reelection stock market pullback coming buy meta platform nasdaqmeta bought pinnacle bancorp golden wealth boost stock lam research corporation nasdaqlrcx hims stock financial analysis following stock price crash incredible quantumscape stock investor blackrock soar according billionaire michael saylor owner childrens exchange open rochester family start learning math data science simple guide bezos venetian wedding buzz bling backlash york spire wealth purchase doordash nasdaqdash bessemer sell ameriprise financial nyseamp cambridge investment research advisor cut huntington bancshares incorporated nasdaqhban beloved grocery chain better costco open store part expansion buying closed winndixie site amd v arista network artificial intelligence ai stock better buy tariff drive firework price ahead fourth tip save celebration tariff drive firework price ahead fourth tip save celebration tariff drive firework price ahead fourth tip save celebration agg great choice vanguard better disney stock rising hitting high memory muscatine post card golden tampa outsource call center firm name ceo whats micron stock america newest space ipo smashing success reigning ballon dor winner aitana bonmati hospitalized meningitis less euro retire invest stock focus real estate jeff bezos lauren sanchez join list richest married couple prenups wealthiest people take place hindustan hindustan labor land cost dominate discussion inaugural lake county agricultural summit condo requires handle condo requires handle developer file preapplication mixeduse project nw st miami florida debt growing force influencing jobseekers choice career expert im old father functional medicine routine healthy life target face serious challenge ceo cornell retirement nears walmart slash price popular summer essential cheaper target version end bank branch europe digital euro stablecoins reshaping finance luvmes independence wig sale limitedtime countdown deal old navy selling americana flip flop theyre identical havaianas nearly cheaper la trader joes open across street another trader joes amid messiness social security administration people taking benefit early asking reframe respond challenge grandfather k seized chase sudden account closure destroyed credit forced delay retirement macro trend likely send bitcoin xrp skyrocketing budget weekly pay freight inconsistent ai resume overwhelming recruiter manager lahaina burned experiment housing vulnerable golden wealth purchase diageo plc nysedeo rob biederman join stage stage family business concerned effect tariff youth sport meta platform nasdaqmeta acquired mokan wealth meta platform nasdaqmeta moran wealth bessemer reduces stake tmobile nasdaqtmus bessemer lower stock stryker corporation nysesyk aurora private wealth purchase meta platform nasdaqmeta pacific financial trim meta platform nasdaqmeta meta platform nasdaqmeta stake lifted symmetry partner gamma investing million stock meta platform nasdaqmeta carnival corporation nyseccl bought oppenheimer asset stock dominate weight market tesla investor watch asset co ltd sell expeditors international washington nasdaqexpd sch financial advisor million alphabet nasdaqgoogl walkner condon financial advisor acquires alphabet nasdaqgoogl fidelity national financial nysefnf stake increased oppenheimer co nobrainer stock buy house republican bacon nebraska seek reelection wealth enhancement advisory service million stock darden restaurant nysedri llm project ai enthusiast build stronger resume europe mitigate mighty defence cost challenge ing cryptocurrency likely millionaire maker xrp v shiba inu mortgage rate hit lowest level since early drop phrase business email colorado health brace layoff amid loss federal funding trump administration broadcast bias network shield nyc socialist mamdani extreme label apply conservative fact trump false claim domestic policy bill donald trump example house republican colorado play israelgaza debate explores difficult conversation crisis deepens editorial cartoon saturday dial false rhetoric inspires violence memory firework lyon fall childhood fueled curiosity imagination albemarle look add school zone speed camera initial success column limit free speech shouldnt condoned america deportation nation trump gunning record immigration prosecution rescued friday penobscot river supreme limit judge power block trump order take stand fascist takeover america policy change consequence veteran va care drop charade come social security medicare tesla driverless delivery car customer stock since ipo smart buy developer lay latest vision pleasant hill golf course opinion doe patriot reader view protect minnesota resource data center reader view hypocritical sending troop senate initial vote trump bill senate initial vote trump bill fall river school employee arrest serious charge psychiatry activism created dangerous concept transgender child reigning ballon dor winner aitana bonmati hospitalized meningitis less euro fbi attack fentanyl working reduce overdose death opinion democrat figure john fetterman conor lamb stepping editor truth aint used wouldnt regime change hurricane hit alligator alcatraz florida drawing evacuation plan opinion john tayer uncomfortable situation economic social interest converge opinion max boykoff community editorial board considering sale public land mitchell berger fort lauderdale democrat chairing david jolly governor campaign canadian man died miami detention lived daytona beach kenosha festivity change parking traffic downtown old bogeyman reunite maga explosive iran divide colorado supreme accepts parole revocation debt collection congressional candidate allard little campaign spending limit look colorado republican jeff crank close look fire station air base convenience store bridging lgbtq wealth gap left political philosophy persuasion government club roger koopman idf chief canceled screening stalled grant federal cut hit iowa fighting cancer ut tyler poll reflects texas voter view issue political matchup public land public hitching flight story hitching flight story editor flag deserves federal holiday holiday translation record translation record dont shy away fight pritzkers run atypical third term fit unprecedented happens wisconsin budget isnt passed dont shy away fight pritzkers run atypical third term fit unprecedented dont shy away fight pritzkers run atypical third term fit unprecedented abbott paxton withhold uvalde jan related record texas supreme rule uw nurse bid reclaim union status rejected wisconsin supreme unanimously dont take ballgame editorial cartoon saturday walter five pandemic plague california employee safety net legislator review kurth disappointed republican education funding plan legislator review kurth disappointed republican education funding plan editorial veto speed cam tax credit bill measure protect hawaii fishing industry five bill signed friday mayor name nominee future ocean safety commission gop boost rural hospital fund rewrite medicaid provision save trump megabill gop boost rural hospital fund rewrite medicaid provision save trump megabill gop boost rural hospital fund rewrite medicaid provision save trump megabill republican race crucial vote trump megabill uncertainty republican race crucial vote trump megabill uncertainty republican race crucial vote trump megabill uncertainty gop boost rural hospital fund rewrite medicaid provision save trump megabill gop boost rural hospital fund rewrite medicaid provision save trump megabill gop boost rural hospital fund rewrite medicaid provision save trump megabill republican race crucial vote trump megabill uncertainty republican race crucial vote trump megabill uncertainty republican race crucial vote trump megabill uncertainty tribune quiz route series neglect capture beauty along road mexico final scotus decision brings wave historymaking ruling trump nato turnaround threatening pull daddy alliance msgr charles j dubois travis decker alive fruitless manhunt produced certain evidence republican plan overhaul medicaid shaking midterm trump immigration arrest seeing wave resistance wanda ammons regina gina marie williams baccigalopi trump staging spectacle helping people heat dome pas climatefueled wave arent anywhere word eudaimonia meaning pursuit happiness tom sawyer fence painting closed girl jackpod taking break cnn report crowd attending funeral tehran oreo bringing fanfavorite flavor stop yelling biden join thousand paying final respect slain minnesota lawmaker husband ge appliance moving production china republican matthew schaefer honor late mother getting selected overall york islander nhl draft better help north tulsa grow rivian investor watch shiba inu cardano price prediction investor nervous joining remittix train gain walmart selling excellent soundbar shopper impressive bigfoot stomp east county mountain business bigfoot stomp east county mountain business unpacking content strategy definition modern marketer guide delta operation recovering weekend delay cancellation sunday alivecom la vega strip casino cant escape troubling trend shoe life olympic longdistance runner type load board bart improves safety cleanliness satisfaction yet ridership recovery remains slow uptown aventura planned biscayne blvd miami fl house gop leadership discussing limit classified information capitol hill hallucination hardware lesson realworld computer vision project sideways psychedelic drug flopped trial buy dip ai stock continue moving higher ridiculously cheap warren buffett stock richer iranian hacker become active military strike protect business im putting fing hijab uk singer refuse virtue signal palestine pull festival sneaky sam club trick buying tv worth plus easy tip maximize viewing marktomarket middle east conflict whipsaw energy price cheer abc fine wine spirit renews support pediatric cancer research marktomarket middle east conflict whipsaw energy price xrp price prediction payment token surge incoming xrp rtx xlm expected outperform trump tax bill conflict trump trade goal editorial supreme ruling restores parent walmart selling burner expert grill cheaper lowes version borderland mexico winner global tariff war mexico report global sport medicine smithnephew sponsor select player competing wimbledon highlighting advanced solution joint repair energy star inside attack trump cost homeowner uncertain costco branded insane archaic shopper beg chain speed roll popular checkout method used rival autodesk nasdaqadsk acquired spire wealth spire wealth raise stock autodesk nasdaqadsk alphabet nasdaqgoogl apeiron ltds largest promising robotics stock consider ameriprise financial nyseamp bought spire wealth sequoia financial advisor buy yum brand nyseyum elevance health nyseelv bought sequoia financial advisor robeco institutional asset bv million stock paychex nasdaqpayx streaming stock worth watching steele million nvidia corporation nasdaqnvda amphenol corporation nyseaph purchased cambridge investment research advisor robeco institutional asset bv purchase charles schwab corporation nyseschw sequoia financial advisor buy public storage nysepsa nvidia corporation nasdaqnvda purchased ipswich investment co spire wealth boost stock ameriprise financial nyseamp nvidia cor</t>
         </is>
       </c>
     </row>
@@ -658,12 +654,12 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>esperion appoints craig thompson to board of director mercadolibre applied material and a healthcare stock on cnbcs final trade ap business summarybrief at am edt ap business summarybrief at am edt how to plan in an uncertain economy senate churn through overnight session a republican seek support for trump big bill senate churn through overnight session a republican seek support for trump big bill bbg launch data center specialty practice appoints industry veteran chris fudacz to lead new specialty practice mara report june bitcoin production and mining operation update issue midyear outlook the bond canary in the big beautiful coal mine nasdaq welcome ipo in the first half of ameresco receives frost sullivan global company of the year award for excellence in energy service nasdaq welcome ipo in the first half of outlook therapeutic appoints biopharmaceutical industry and commercial leader bob jahr a chief executive officer outlook therapeutic appoints biopharmaceutical industry and commercial leader bob jahr a chief executive officer beyond the number analyst discus taysha gene therapy stock deep dive into new fortress energy stock analyst perspective rating trevi therapeutic to attend leerink partner therapeutic forum ii and metabolism beyond the number analyst discus lineage stock stock market today dow jones fall ahead of powell talk tesla dive on trumpmusk feud live coverage analyst assess ionis pharmaceutical what you need to know where robinhood market stand with analyst deep dive into weyerhaeuser stock analyst perspective rating should you expect demand growth in range resource rrc alphyns zabalafin hydrogel for atopic dermatitis highlighted in leading peerreviewed journal oppo reno pro price availability spec more qapel medical appoints stewart strong a president and chief executive officer highspring and vaco by highspring earn top honor from staffing industry analyst what make pinnacle financial partner pnfp a longterm bet ap technology summarybrief at am edt july is flush smart month who need a refresher on potty training basic historic hip hop def jam memorabilia auction to benefit rush philanthropic art foundation bidding close july july is flush smart month who need a refresher on potty training basic bounce empire debut world largest indoor circular transparent led screen surpasses visitor in two year rohrer aesthetic unveils new clinical study highlighting pixe a the future of regenerative aesthetic can community health launch susan terry foundation to empower individual living with hiv blackrock esg capital allocation term trust ecat certified result of annual meeting announced td synnex acquires apptium to accelerate innovation breadth of cloud and everythingasaservice offering masco corporation announces date for earnings release and conference call for second quarter fifth third wealth advisor surpasses billion in net new asset under management expands platform capability thredd expands global footprint with new office in the u intrabio inc completes recruitment for ib at pivotal clinical trial dakota announces formation of advisory board to accelerate strategic growth and product evolution uber eats expands partnership with beloved local grocer marea therapeutic appoints shishir gadam phd a chief technical officer lynq set july th launch date for realtime interestbearing settlement network retail investor use ethransaction btc xrp usdc and other mainstream currency for cloud mining earning a stable income of per day cordia pittsburgh win system of the year award at idea senate strike ai provision from gop bill after uproar from the state senate strike ai provision from gop bill after uproar from the state senate strike ai provision from gop bill after uproar from the state senate strike ai provision from gop bill after uproar from the state thermo fisher scientific to hold earnings conference call on wednesday july amentum to host third quarter fiscal year earnings conference call on august momentus and orbit fab partner to advance space servicing with podracer and rafti demonstration flight this stock is still the very best place you can put your money tailor expands series a to m with privatepublic support operation hope and georgia state university launch groundbreaking ai literacy program for underserved youth levelblue to acquire trustwave becoming largest pureplay managed security service provider this stock is still the very best place you can put your money nline energy and penn state health milton s hershey medical center win joseph m brillhart innovation award at idea pepper launch the first open and extensible endless aisle platform in the foodservice industry fresenius expands biosimilars portfolio with the launch of denosumab biosimilars in the u sofi schedule conference call to discus q result valley national bancorp announces new general counsel unnatural product tap argenxs help for ringed molecule expands internal work into obesity brightspring health lead company in line for tripledigit profit growth brightspring health lead company in line for tripledigit profit growth i tried amazon bestselling beckham hotel collection pillow to see if theyre actually any good transcript velina peneva swiss re chief investment officer elon musk and donald trump are fighting again miami beach city commission grant final approval to terras redevelopment of the historic deauville hotel site canadian cuisine food that reflect the country size and diversity is nvidia stock a buy at new record high jewelry sale outperform a u spending for most luxury good falter citi report find cnbc oportun responds to comment by findell capital actelis network announces private placement priced atthemarket under nasdaq rule deepki accelerates u operation to help commercial real estate tackle sustainability challenge manage risk and drive financial performance duo technology added to russell microcap index dih appoints rehazentrum valens a a dih center of excellence lendmark financial service announces expiration and result of it tender offer for it senior note due cole engineering awarded m u army production contract for nextgeneration stinger training system zohran mamdanis primary win is a warning to every legacy brand travtus partner with engrain to bring spatial intelligence to it everyday ai platform jd martin expands partnership with nvent eriflex to florida north carolina and south carolina radius recycling report third quarter fiscal financial result stryker to announce financial result for it second quarter of fiscal year richtech robotics announces inclusion in u smallcap russell and russell index oncternal therapeutic announces the sale of select development program and the winddown of it operation arevon secures million credit facility to accelerate renewable energy growth in the united state dih appoints rehazentrum valens a a dih center of excellence kavalan blitz iwc taking trio of whisky distillery and master distiller of the year prize inriver research reveals widespread ai deployment in pim of company have moved beyond pilot randamu and chengdu university of information technology collaborate to advance cryptographic research and web coordination infrastructure kestra medical technology ltd to report fourth quarter and fiscal year result on july genmab announces change to it executive committee document available regarding ramacos brook mine rare earth and critical mineral project condo price dropped in maythe second largest decline on record independent preliminary economic assessment report from fluor corporation confirms commercial and technical feasibility of ramacos brook mine rare earth deposit realme series set to shake up india midrange smartphone market aocs childhood nickname revealed amid bronx girl claim second democrat announces campaign to unseat gop congressman in competitive michigan district these new colorado law take effect tuesday regulating gun shop sexual assault case youth detention and more these new colorado law take effect tuesday regulating gun shop sexual assault case youth detention and more the multiverse scandal how academia is redefining science to avoid god senate strike ai provision from gop bill after uproar from the state senate strike ai provision from gop bill after uproar from the state i tried amazon bestselling beckham hotel collection pillow to see if theyre actually any good elon musk and donald trump are fighting again dan gainor the good the bad and the absurd june wildest political moment and celebrity meltdown canadian cuisine food that reflect the country size and diversity la new budget kick in today here what your tax dollar are paying for montana leader need to protect our export economy mark noland letter bad outcome if medicare is cut editorial cartoon for tuesday july cant wait for saturday today texas state to the pac then what james walkinshaw win democratic contest to likely replace u rep connolly in northern virginia mystery surround the jeffrey epstein file after bondi claim ten of thousand of video amendment targeting medicaid expansion wont get a senate vote trump say doge might have to go back and eat elon musk after his criticism of the gop bill president lee jaemyung hope for a better interkorean relationship hickory public housing authority officially abolished after final meeting monday well break your leg un accused of mafiatype response to usled gaza relief effort usaid cut could cause staggering number of avoidable death study say how iran lost the short war with israel and america republican struggle to pas trump massive tax bill after hour of drama opinion senate bill undermines decade of progress in disability service thousand of cancer patient fear disruption in care due to insurance contract dispute supreme court medina ruling free state to defund planned parenthood muscatine contingent visit china trump blame att after conference call with faith leader disrupted takeaway from aps report on attorney general bondis comment about evidence in epstein case takeaway from aps report on attorney general bondis comment about evidence in epstein case texas democrat who lost to ted cruz month ago jump into senate race watching area near florida for possible tropical development saudi arabia alhilal had to climb mount everest without oxygen in shock club world cup win over manchester city trump score major victory a vance help push big beautiful bill through senate maybe he ha a knife yulia putintseva asks for crazy wimbledon spectator to be ejected over safety fear senate hold votearama on trump big beautiful bill senate votearama on gop megabill go all night most american feel democracy is theatened poll show and mamdani speaks with npr new jersey phil murphy take heat from all side in final budget a governor south korea energy policy under lee jaemyung american opinion deportation alone cant fix u immigration problem can south korea achieve peace in a chaotic world trump big beautiful bill awaits final senate vote opinion spense havlick scam are everywhere these day dont be fooled the future of air combat how long will the u military still need pilot california new consumer protection law go into effect july amc theater will start placing even more ad in cinema nationwide starting today letter to the editor power must be maintained at all cost extend freedom beyond our own specie we need a shared morality major insurance change are coming to glp drug for weight loss here how that could affect patient editorial american deserve clearer explanation of what happened in iran maglite pedestrian safety institute and additional partner to promote traffic and pedestrian safety during national roadside traffic safety awareness month egg harbor township approves year affordable housing plan remembering the men and woman who serve our country do the saint have their qb of the future in the building this season should decide that trump relief for farmer look like control by fear guest commentary florida resident get a new roof now and receive free exterior painting just in time for hurricane season letter democrat seem incapable of praising trump for anything whats the point of being a u senator if you dont have gut bob brown the most undervalued asset for a leader it these hour the bully pulpit ron waterman what sdas latest win signal for military space republican still pushing to pas trump big beautiful bill he hasnt played in mlb for more than two decade one team is paying him million a year until senate republican closing in on final vote on gop spending bill more republican than dems vote to raise tax on billionaire in latenight senate vote house democrat announces he wont seek reelection in trump doge is the monster that might have to go back and eat elon will state assembly save energy independence california focus will state assembly save energy independence california focus watch out for weirdo facebook scammer promising the world scam of the week letter obama policy necessitated u strike on nuclear site opinion state bill pausing new building code risk climate change progress public health expert trump big beautiful bill will cause misery and death my turn we need to be a twohospital town my turn thanks extremist for making me reexamine who i want to be and what our nation should be my turn state democrat play dirty trick with legislation my turn another four year of the idiot council doofus thing to know for july trump megabill israelgaza alligator alcatraz idaho shooting hurricane data debate over trump big bill continues tuesday morning in u senate hundred of national guard force deployed to la by trump could be returned to calif wildfire duty editorial cartoon for july reader view congress must reject any cut to medicaid who to say anybodys vote is safe trump doj target north carolina voter roll here how president trump mega tax bill would impact illinois council lower real estate tax rate yet restores funding for service program concern in north dakota grow about increased aca cost medical debt flood drown out lancaster county roadway in aftermath of monday storm hundred of child told to test for disease in australia after childcare worker charged with child sex abuse here are offensive player who can contribute for southern football in wisconsin governor gop reach budget deal to cut tax fund university maha report call for fighting chronic disease but trump and kennedy have yanked funding local expert detail potential effect of federal funding cut lagniappe next up the steve miller band jay take isolation a doubleedged sword letter catholic must stand in unity and sacrifice a jesus did letter america most beautiful wild land are in grave danger burke catawba mcdowell iredell city county close for july see garbage impact</t>
+          <t>londonbased startup laverock therapeutic raise over million for it gene control tech robinhood expands it global push minute from crypto chief old cramped apartment in cannes medium advisory justice is a common cause day commemoration of the downing of flight p and first memorial unveiled webuy global ltd integrates coinbase to accept stablecoin payment leading the way in travel technology and digital payment in market rally back to record best sp tech trade hasnt been mag or tech sector itself inspirational quote albert einstein virginia woolf and others u dollar suffers worst start to year since financial time canada talk show tariff have created a new world for investor axios doc alleged bribe came before antioch homebuilder played all legal card moderna report phase flu data teeing up new submission with federal support uncertain state and nonprofit scramble to safeguard access to vaccine houstonbased developer proposes story highrise for nw th st miami fl brookfield business partner to host second quarter result conference call expert tip for securing debt financing in a challenging market option flow alert bull making their move in googl stock modernas flu vaccine show positive latestage trial result paving way for combination covid shot ardagh metal packaging sa q result and investor call notification shatterproof name public affair and health leader pam jenkins a new ceo killam apartment reit announces normal course issuer bid largest crossmod neighborhood provides blueprint for scaling new attainable home inventory across the country should you buy xrp ripple while it under first merchant corporation to report second quarter financial result host conference call and webcast st louisarea business opening and closing in june lantronix enters into cooperation agreement with investor group led by chain of lake investment fund llc amazon miss out on switch sale after nintendo pulled product from u site bloomberg signify share repurchase period update avadel pharmaceutical announces unanimous appeal court decision upholding fda approval of lumryz in narcolepsy in administrative procedure act litigation work advice my bos want me to install a work app on my personal phone brookfield infrastructure to host second quarter result conference call king street close oversubscribed european real estate special situation fund ii oncolytics biotech appoints former ambrx executive a chief business officer to drive business development strategy how flower by edie parker landed million social impression with a single campaign jinkosolar and ib vogt partner to deliver highefficiency tiger neo module for spain mwp segovia solar cluster wesco publishes sustainability report modine launch dsu destratification fan bringing bestinclass airflow solution to commercial and industrial space cielo announces agm result and extension of unit offering intershunt enrolls first patient in new heart failure study canadian premium sand inc provides operational update core natural resource provides update on ongoing effort to resume longwall operation at leer south iterum name christine coyne a chief commercial officer to lead orlynvahtm launch and commercial growth way chief marketing officer are harnessing ai right now tonix pharmaceutical announces inclusion in the russell and russell index regenx amends debenture term and announces nonbrokered financing for gross proceeds of king street close oversubscribed european real estate special situation fund ii first legal step taken this time by wsta to untangle the legal knot of the clean truck partnership regenx amends debenture term and announces nonbrokered financing for gross proceeds of cdr foundation announces grant to five nonprofit organization in new york city digital worker have arrived in banking wsj miss a accelerates national growth aiming for store by q iterum name christine coyne a chief commercial officer to lead orlynvahtm launch and commercial growth mty food group inc announces renewal of normal course issuer bid brookfield infrastructure to host second quarter result conference call largest crossmod neighborhood provides blueprint for scaling new attainable home inventory across the country oncolytics biotech appoints former ambrx executive a chief business officer to drive business development strategy poet technology provides result of annual general and special meeting brookfield business partner to host second quarter result conference call northstar announces receipt of letter of interest on potential funding for up to four united state asphalt shingle reprocessing facility carobway launch foodforward prebiotic fiber innovation at ift selling downtown minneapolis skyscraper a tall order these day core natural resource provides update on ongoing effort to resume longwall operation at leer south nls pharmaceutic and kadimastem announce pricing and closing of million equity financing cassava present promising preclinical simufilam data at tsc alliance meeting editorial embrace the real solution to our health care crisis huachen ai parking management technology holding co ltd and hangzhou qianhui electric technology co ltd establish cooperative relationship to enhance twowheeled echarging infrastructure indivior announces inclusion in the u russell and index credicorp ltd credicorp take legal action to defend rule of law in tax dispute with sunat signify share repurchase period update best cryptos to buy on th june nls pharmaceutic and kadimastem announce pricing and closing of million equity financing what you need to know ahead of blackrocks earnings release zscaler announces proposed offering of billion of convertible senior note due down is jetblue stock a buy zscaler announces proposed offering of billion of convertible senior note due plug power stock is rising why hydrogen just got a boost from the senate bill barrons ap business summarybrief at am edt klarna boost banking effort a it prepares to go public judge rule against human right group claim that the uk is illegally arming israel judge rule against human right group claim that the uk is illegally arming israel what you need to know ahead of steel dynamic earnings release verny capital sign agreement to sell rg gold verny capital sign agreement to sell rg gold ahold delhaize usa cyberattack exposed million people data petroperu seek partner for amazon oil block reactivation zohran mamdani admits he hate capitalism allied with socialist operative linked to marxist terror group white house expects more country will drop digital service tax after canada back down friend reunited why it wasnt just lionel messi who faced paris saintgermain at the fifa club world cup share in jpmorgan chase co nysejpm acquired by ffg partner llc cambridge investment research advisor inc ha million position in otis worldwide corporation nyseotis hbk sorce advisory llc ha million stock position in jpmorgan chase co nysejpm ferguson shapiro llc trim stake in jpmorgan chase co nysejpm jpmorgan chase co nysejpm is pinnacle bancorp inc th largest position cambridge investment research advisor inc ha million stake in otis worldwide corporation nyseotis cambridge investment research advisor inc boost stock holding in paccar inc nasdaqpcar carux to buy pioneer for bn perigon wealth management llc acquires share of the bank of new york mellon corporation nysebk robeco institutional asset management bv lower stock position in the allstate corporation nyseall amphenol corporation nyseaph share sold by bartlett co wealth management llc social security july payment schedule here when beneficiary get their check russia deploys new shadow fleet lng carrier to load gas at sanctioned arctic project india aprilmay fiscal deficit at of fullyear target with federal support uncertain state and nonprofit scramble to safeguard access to vaccine canada talk show tariff create new world for investor letter to the editor we must keep trying to understand one another better keep attendance up at rec center class i lost my yearold son to suicide from addictive ai algorithm we cant let big tech destroy our child zohran mamdanis primary victory spark debate over israel antisemitism and nycs future editorial supreme court once more give trump wide power on deportation further statement re u budget reconciliation bill cnn ha no one to blame but itself zefiro subsidiary plant goodwin awarded additional governmentfunded remediation work in ohio capitol agenda thune head into a perilous votearama tuesday aldermanic election pit mayor spencer v president green reader view stauber still ha time to save legacy a hardright lawmaker is sworn in a greece migration minister nasrallahs status at risk a hezbollah face israeli blitz zoren here a look at main philly july activity some of which will be on tv bill and jan friend reunited why it wasnt just lionel messi who faced paris saintgermain at the fifa club world cup average age of a firsttime homebuyer is just under year old fed clear plan for more medicaid aid for nebraska hospital statesvilles sinkhole at tradd and front street to be repaired by midjuly fed clear plan for more medicaid aid for nebraska hospital italy meloni break bread with trump at the hague warren buffett donates record billion berkshire share the rise of ai in ceo communicationsand the credibility threat it pose answer to pressing social security question senate republican are in a sprint on trump big bill after a weekend of setback senator consider proposed amendment to trump big bill of tax break and spending cut senate republican are in a sprint on trump big bill after a weekend of setback senate republican are in a sprint on trump big bill after a weekend of setback editorial cartoon for june thing to know for june idaho shooting trump bill uscanada iran escaped inmate in china crackdown on gay erotica woman bear the brunt iga swiatek slam intense calendar a player feel the grind to protect ranking plan submitted to convert burnley terrace into shared housing the flip of a coin today will determine who sits on the pasadena city council letter parking and other policy reveal city dysfunction social security cola estimate are out how do they compare to past year bob asmussen the thing i love and enjoy is helping people move forward letter williamsville need to rethink priority canadaus trade talk resuming after canada kill plan to tax u tech firm carney say trump had railed against it senate gop look to pas marathon final test on trump big beautiful bill senate gop look to pas marathon final test on trump big beautiful bill after picking up million player option with the los angeles lakers what doe the future hold for lebron james senate gop look to pas marathon final test on trump big beautiful bill senate gop look to pas marathon final test on trump big beautiful bill senate gop look to pas marathon final test on trump big beautiful bill senate gop look to pas marathon final test on trump big beautiful bill janet march ruled dead focus turn to husband notorious nashville jason chaffetz ten sneaky way the deep state steal your data and how trump can help you stop it editorial is brandon johnson pitching wall streeters on moving to chicago postmamdani we thought not editorial driver sport bettor vapers and airbnb user wont be toasting this fiscal new year in illinois zohran mamdani want to build government supermarket america already ha them iranisrael conflict after the war enter the diplomat gov jb pritzker is running for reelection who will he pick a his no trump th week set to focus on big beautiful bill passage ahead of independence day deadline letter the victory of a progressive mayoral candidate in new york is not a signal to democrat john t shaw wesleyan university president stand up for higher education a it under assault new law taking effect july impact seat belt waterworks and more unexpected roadblock for woman entrepreneursand how to overcome them rochester police department daily incident report june july fan follow hagen thru hole of match boston police sergeant charged with aggravated rape of a minor what is meant by a fait accompli nasa plan to stream rocket launch on netflix starting this summer lucas obama and the democrat paved the way for iran nuclear program ace bailey say he blessed to be with the utah jazz after he fell to them in the nba draft total ambush idaho firefighter gunned down suspect found dead in apparent trap most peaceful country fight over transit skill game and overall spending mean the pa budget will again be late canada pm say trade talk with u resuming in auburn regional gop leader urge battle tested lawler to run for ny governor allegheny county finance not yet dire but unsustainable say oconnor pa lawmaker consider new state board to fasttrack electricity project new doc get schooled in old disease a vaccine rate fall q a with the president of connecticut association of board of education over accuser filed sex abuse claim in race to beat cap on child victim act why is ice masked up china favorite coffee chain arrives in u reader speak ct is fortunate lamont is our governor trump tell fox news he ha group of wealthy people to buy tiktok morning brief trump big beautiful bill nears finish line scotus rein in judicial overreach the gaudy tie that bind trump and bezos trump new american doctrine mean peace through strength ha returned loss of clean energy tax credit would be a step backward for maine opinion loss of clean energy tax credit would be a step backward for maine opinion loss of clean energy tax credit would be a step backward for maine opinion this could be the summer of economic hell hhs cut cdc staff who made sure birth control is safe for woman at risk loeffler trump one big beautiful bill could cement economic legacy for decade door and dream are no match for feline frolic left lefter and leftist democrat could be defined by radical big city mayor million of u kid attend school in urban heat zone trumpstarmer trade deal kick in uk luxury car get tariff rollsroyce engine fly dutyfree into u republican leader struggle to find balance on reconciliation bill sen ron johnson on why he decided to support president trump spending agenda traditional business planning doesnt cut it anymore here what leader should embrace instead senate move ahead on massive tax and spending bill the trump administration is building a national citizenship system coverage of no king had the wrong focus letter is maine enthusiasm for firework fizzling out</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>esperion appoints craig thompson board director mercadolibre applied material healthcare stock cnbcs final trade business business plan uncertain economy senate churn overnight session republican seek support trump bill senate churn overnight session republican seek support trump bill bbg launch data center specialty practice appoints industry veteran chris fudacz lead new specialty practice mara report bitcoin production mining operation update issue midyear outlook bond canary coal mine nasdaq welcome ipo half ameresco receives frost sullivan global company award excellence energy service nasdaq welcome ipo half outlook therapeutic appoints biopharmaceutical industry commercial bob jahr chief executive officer outlook therapeutic appoints biopharmaceutical industry commercial bob jahr chief executive officer beyond analyst discus taysha gene therapy stock deep dive new fortress energy stock analyst perspective rating trevi therapeutic attend leerink partner therapeutic forum ii metabolism beyond analyst discus lineage stock stock market dow jones fall ahead powell tesla dive trumpmusk feud coverage analyst assess ionis pharmaceutical robinhood market stand analyst deep dive weyerhaeuser stock analyst perspective rating expect demand growth range resource rrc alphyns zabalafin hydrogel atopic dermatitis highlighted leading peerreviewed journal oppo reno pro price availability spec qapel medical appoints stewart strong president chief executive officer highspring vaco highspring earn honor staffing industry analyst pinnacle financial partner pnfp longterm bet technology flush smart month refresher potty training basic historic hip hop def jam memorabilia auction benefit rush philanthropic art foundation bidding close flush smart month refresher potty training basic bounce empire debut world largest indoor circular transparent led screen surpasses visitor rohrer aesthetic unveils new clinical study highlighting pixe future regenerative aesthetic community health launch susan terry foundation empower individual living hiv blackrock esg allocation term trust ecat certified annual meeting announced td synnex acquires apptium accelerate innovation breadth cloud everythingasaservice offering masco corporation announces date earnings release conference call quarter fifth third wealth advisor surpasses billion net new asset expands platform capability thredd expands global footprint new office intrabio completes recruitment ib pivotal clinical trial dakota announces formation advisory board accelerate strategic growth product evolution uber eats expands partnership beloved local grocer marea therapeutic appoints shishir gadam phd chief technical officer lynq set launch date realtime interestbearing settlement network retail investor ethransaction btc xrp usdc mainstream currency cloud mining earning stable income per cordia pittsburgh system award idea senate strike ai provision gop bill uproar senate strike ai provision gop bill uproar senate strike ai provision gop bill uproar senate strike ai provision gop bill uproar thermo fisher scientific earnings conference call wednesday amentum host third quarter fiscal earnings conference call august momentus orbit fab partner advance space servicing podracer rafti demonstration flight stock best place put money tailor expands series privatepublic support operation georgia university launch groundbreaking ai literacy program underserved youth levelblue acquire trustwave becoming largest pureplay managed security service provider stock best place put money nline energy penn health milton hershey medical center joseph brillhart innovation award idea pepper launch open extensible endless aisle platform foodservice industry fresenius expands biosimilars portfolio launch denosumab biosimilars sofi schedule conference call discus q valley national bancorp announces new general counsel unnatural product tap argenxs help ringed molecule expands internal work obesity brightspring health lead company line tripledigit profit growth brightspring health lead company line tripledigit profit growth tried amazon bestselling beckham hotel collection pillow theyre good transcript velina peneva swiss chief investment officer elon musk donald trump fighting miami beach commission grant final approval terras redevelopment historic deauville hotel site canadian cuisine reflect country size diversity nvidia stock buy new record high jewelry sale outperform spending luxury good falter citi report find cnbc oportun responds findell actelis network announces private placement priced atthemarket nasdaq rule deepki accelerates operation help commercial real estate tackle sustainability challenge manage risk drive financial performance duo technology added russell microcap index dih appoints rehazentrum valens dih center excellence lendmark financial service announces expiration tender offer senior note due cole engineering awarded army production contract nextgeneration stinger training system zohran mamdanis primary warning legacy brand travtus partner engrain spatial intelligence everyday ai platform jd martin expands partnership nvent eriflex florida north carolina south carolina radius recycling report third quarter fiscal financial stryker announce financial quarter fiscal richtech robotics announces inclusion smallcap russell russell index oncternal therapeutic announces sale select development program winddown operation arevon secures million credit facility accelerate renewable energy growth united dih appoints rehazentrum valens dih center excellence kavalan blitz iwc taking trio whisky distillery master distiller prize inriver research reveals widespread ai deployment pim company moved beyond pilot randamu chengdu university information technology collaborate advance cryptographic research web coordination infrastructure kestra medical technology ltd report fourth quarter fiscal genmab announces change executive committee document available regarding ramacos brook mine rare earth critical mineral project condo price dropped maythe largest decline record independent preliminary economic assessment report fluor corporation confirms commercial technical feasibility ramacos brook mine rare earth deposit realme series set shake india midrange smartphone market aocs childhood nickname revealed amid bronx girl claim democrat announces campaign unseat gop congressman competitive michigan district new colorado take effect tuesday regulating gun shop sexual assault youth detention new colorado take effect tuesday regulating gun shop sexual assault youth detention multiverse scandal academia redefining science avoid god senate strike ai provision gop bill uproar senate strike ai provision gop bill uproar tried amazon bestselling beckham hotel collection pillow theyre good elon musk donald trump fighting dan gainor good bad absurd wildest political moment celebrity meltdown canadian cuisine reflect country size diversity la new budget kick tax dollar paying montana protect export economy mark noland bad outcome medicare cut editorial cartoon tuesday cant wait saturday texas pac james walkinshaw democratic contest likely replace rep connolly northern virginia mystery surround jeffrey epstein file bondi claim ten thousand video amendment targeting medicaid expansion wont senate vote trump doge eat elon musk criticism gop bill president lee jaemyung better interkorean relationship hickory public housing authority officially abolished final meeting monday break leg un accused mafiatype response usled gaza relief effort usaid cut cause staggering avoidable death study iran short war israel america republican struggle pa trump massive tax bill hour drama opinion senate bill undermines decade progress disability service thousand cancer patient fear disruption care due insurance contract dispute supreme medina ruling free defund planned parenthood muscatine contingent visit china trump blame att conference call faith disrupted takeaway aps report attorney general bondis evidence epstein takeaway aps report attorney general bondis evidence epstein texas democrat ted cruz month ago jump senate race watching area near florida possible tropical development saudi arabia alhilal climb mount everest without oxygen shock club world cup manchester trump score major victory vance help push bill senate maybe knife yulia putintseva asks crazy wimbledon spectator ejected safety fear senate votearama trump bill senate votearama gop megabill night american feel democracy theatened poll mamdani speaks npr new jersey phil murphy take heat final budget governor south korea energy policy lee jaemyung american opinion deportation alone cant fix immigration problem south korea achieve peace chaotic world trump bill awaits final senate vote opinion spense havlick scam everywhere dont fooled future air combat military pilot california new consumer protection effect amc theater start placing ad cinema nationwide starting editor power must maintained cost extend freedom beyond specie shared morality major insurance change coming glp drug weight loss affect patient editorial american deserve clearer explanation happened iran maglite pedestrian safety institute additional partner promote traffic pedestrian safety national roadside traffic safety awareness month egg harbor township approves affordable housing plan remembering men woman country saint qb future building season decide trump relief farmer look control fear guest commentary florida resident new roof receive free exterior painting hurricane season democrat seem incapable praising trump anything whats senator dont gut bob brown undervalued asset hour bully pulpit ron waterman sdas latest signal military space republican pushing pa trump bill hasnt played mlb decade team paying million senate republican closing final vote gop spending bill republican dems vote raise tax billionaire latenight senate vote house democrat announces wont seek reelection trump doge monster eat elon assembly save energy independence california focus assembly save energy independence california focus watch weirdo facebook scammer promising world scam obama policy necessitated strike nuclear site opinion bill pausing new building code risk climate change progress public health expert trump bill cause misery death turn twohospital town turn extremist making reexamine nation turn democrat play dirty trick legislation turn another idiot council doofus trump megabill israelgaza alligator alcatraz idaho shooting hurricane data debate trump bill continues tuesday morning senate hundred national guard force deployed la trump returned calif wildfire duty editorial cartoon reader view congress must reject cut medicaid anybodys vote safe trump doj target north carolina voter roll president trump mega tax bill impact illinois council lower real estate tax rate yet restores funding service program concern north dakota grow increased aca cost medical debt flood drown lancaster county roadway aftermath monday storm hundred child test disease australia childcare worker charged child sex abuse offensive player contribute southern football wisconsin governor gop reach budget deal cut tax fund university maha report call fighting chronic disease trump kennedy yanked funding local expert detail potential effect federal funding cut lagniappe next steve miller band jay take isolation doubleedged sword catholic must stand unity sacrifice jesus america wild land grave danger burke catawba mcdowell iredell county close garbage impact</t>
+          <t>londonbased startup laverock therapeutic raise million gene control tech robinhood expands global push crypto chief old cramped apartment cannes medium advisory justice common cause commemoration downing flight p memorial unveiled webuy global ltd integrates coinbase accept stablecoin payment leading travel technology digital payment market rally record best sp tech trade hasnt mag tech sector inspirational albert einstein virginia woolf others dollar suffers worst start since financial canada tariff created world investor axios doc alleged bribe came antioch homebuilder played legal card moderna report phase flu data teeing submission federal support uncertain nonprofit scramble safeguard access vaccine houstonbased developer proposes story highrise nw st miami fl brookfield business partner host quarter conference call expert tip securing debt financing challenging market option flow alert bull making move googl stock modernas flu vaccine positive latestage trial paving combination covid shot ardagh metal packaging sa q investor call notification shatterproof name public affair health pam jenkins ceo killam apartment reit announces normal course issuer bid largest crossmod neighborhood provides blueprint scaling attainable inventory across country buy xrp ripple merchant corporation report quarter financial host conference call webcast st louisarea business opening closing lantronix enters cooperation agreement investor led chain lake investment fund amazon miss switch sale nintendo pulled product site bloomberg signify repurchase period update avadel pharmaceutical announces unanimous appeal decision upholding fda approval lumryz narcolepsy administrative procedure act litigation work advice bos install work app personal phone brookfield infrastructure host quarter conference call king street close oversubscribed european real estate special situation fund ii oncolytics biotech appoints ambrx executive chief business officer drive business development strategy flower edie parker landed million social impression single campaign jinkosolar ib vogt partner deliver highefficiency tiger neo module spain mwp segovia solar cluster wesco publishes sustainability report modine launch dsu destratification fan bringing bestinclass airflow solution commercial industrial space cielo announces agm extension unit offering intershunt enrolls patient heart failure study canadian premium sand provides operational update core natural resource provides update ongoing effort resume longwall operation leer south iterum name christine coyne chief commercial officer lead orlynvahtm launch commercial growth chief marketing officer harnessing ai tonix pharmaceutical announces inclusion russell russell index regenx amends debenture term announces nonbrokered financing gross proceeds king street close oversubscribed european real estate special situation fund ii legal step taken wsta untangle legal knot clean truck partnership regenx amends debenture term announces nonbrokered financing gross proceeds cdr foundation announces grant five nonprofit organization york digital worker arrived banking wsj miss accelerates national growth aiming store q iterum name christine coyne chief commercial officer lead orlynvahtm launch commercial growth mty announces renewal normal course issuer bid brookfield infrastructure host quarter conference call largest crossmod neighborhood provides blueprint scaling attainable inventory across country oncolytics biotech appoints ambrx executive chief business officer drive business development strategy poet technology provides annual general special meeting brookfield business partner host quarter conference call northstar announces receipt interest potential funding united asphalt shingle reprocessing facility carobway launch foodforward prebiotic fiber innovation ift selling downtown minneapolis skyscraper tall order core natural resource provides update ongoing effort resume longwall operation leer south nls pharmaceutic kadimastem announce pricing closing million equity financing cassava present promising preclinical simufilam data tsc alliance meeting editorial embrace real solution health care crisis huachen ai parking technology co ltd hangzhou qianhui electric technology co ltd establish cooperative relationship enhance twowheeled echarging infrastructure indivior announces inclusion russell index credicorp ltd credicorp take legal action defend rule tax dispute sunat signify repurchase period update best cryptos buy nls pharmaceutic kadimastem announce pricing closing million equity financing ahead blackrocks earnings release zscaler announces proposed offering billion convertible senior note due jetblue stock buy zscaler announces proposed offering billion convertible senior note due plug power stock rising hydrogen got boost senate bill barrons business klarna boost banking effort prepares public judge rule human claim uk illegally arming israel judge rule human claim uk illegally arming israel ahead steel dynamic earnings release verny sign agreement sell rg gold verny sign agreement sell rg gold ahold delhaize usa cyberattack exposed million people data petroperu seek partner amazon oil block reactivation zohran mamdani admits hate capitalism allied socialist operative linked marxist terror white house expects country drop digital service tax canada friend reunited wasnt lionel messi faced paris saintgermain fifa club world cup jpmorgan chase co nysejpm acquired ffg partner cambridge investment research advisor million otis worldwide corporation nyseotis hbk sorce advisory million stock jpmorgan chase co nysejpm ferguson shapiro trim stake jpmorgan chase co nysejpm jpmorgan chase co nysejpm pinnacle bancorp largest cambridge investment research advisor million stake otis worldwide corporation nyseotis cambridge investment research advisor boost stock paccar nasdaqpcar carux buy pioneer bn perigon wealth acquires bank york mellon corporation nysebk robeco institutional asset bv lower stock allstate corporation nyseall amphenol corporation nyseaph bartlett co wealth social security payment schedule beneficiary russia deploys shadow fleet lng carrier load gas sanctioned arctic project india aprilmay fiscal deficit fullyear target federal support uncertain nonprofit scramble safeguard access vaccine canada tariff create world investor editor must understand another better attendance rec center class yearold son suicide addictive ai algorithm cant tech destroy child zohran mamdanis primary victory spark debate israel antisemitism nycs future editorial supreme give trump wide power deportation statement budget reconciliation bill cnn blame zefiro subsidiary plant goodwin awarded additional governmentfunded remediation work ohio capitol agenda thune head perilous votearama tuesday aldermanic election pit mayor spencer v president green reader view stauber save legacy hardright lawmaker sworn greece migration minister nasrallahs status risk hezbollah face israeli blitz zoren look main philly activity tv bill jan friend reunited wasnt lionel messi faced paris saintgermain fifa club world cup average age firsttime homebuyer old fed plan medicaid aid nebraska hospital statesvilles sinkhole tradd front street repaired midjuly fed plan medicaid aid nebraska hospital italy meloni break bread trump hague warren buffett donates record billion berkshire rise ai ceo communicationsand credibility threat pose answer pressing social security senate republican sprint trump bill weekend setback senator consider proposed amendment trump bill tax break spending cut senate republican sprint trump bill weekend setback senate republican sprint trump bill weekend setback editorial cartoon idaho shooting trump bill uscanada iran escaped inmate china crackdown gay erotica woman bear brunt iga swiatek slam intense calendar player feel grind protect ranking plan submitted convert burnley terrace shared housing flip coin determine sits pasadena council parking policy reveal dysfunction social security cola estimate compare past bob asmussen love enjoy helping people move forward williamsville rethink priority canadaus trade resuming canada kill plan tax tech firm carney trump railed senate gop look pa marathon final test trump bill senate gop look pa marathon final test trump bill picking million player option los angeles lakers doe future lebron james senate gop look pa marathon final test trump bill senate gop look pa marathon final test trump bill senate gop look pa marathon final test trump bill senate gop look pa marathon final test trump bill janet march ruled dead focus turn husband notorious nashville jason chaffetz ten sneaky deep steal data trump help stop editorial brandon johnson pitching wall streeters moving chicago postmamdani thought editorial driver sport bettor vapers airbnb user wont toasting fiscal illinois zohran mamdani build government supermarket america iranisrael conflict war enter diplomat gov jb pritzker running reelection pick trump set focus bill passage ahead independence deadline victory progressive mayoral candidate york signal democrat john shaw wesleyan university president stand higher education assault taking effect impact seat belt waterworks unexpected roadblock woman entrepreneursand overcome rochester police department incident report fan follow hagen thru hole match boston police sergeant charged aggravated rape minor meant fait accompli nasa plan stream rocket launch netflix starting summer lucas obama democrat paved iran nuclear program ace bailey blessed utah jazz fell nba draft total ambush idaho firefighter gunned suspect found dead apparent trap peaceful country fight transit skill game overall spending pa budget late canada pm trade resuming auburn regional gop urge battle tested lawler run ny governor allegheny county finance yet dire unsustainable oconnor pa lawmaker consider board fasttrack electricity project doc schooled old disease vaccine rate fall q president connecticut association board education accuser filed sex abuse claim race beat cap child victim act masked china favorite coffee chain arrives reader speak ct fortunate lamont governor trump fox wealthy people buy tiktok morning brief trump bill nears finish line scotus rein judicial overreach gaudy tie bind trump bezos trump american doctrine peace strength returned loss clean energy tax credit step backward maine opinion loss clean energy tax credit step backward maine opinion loss clean energy tax credit step backward maine opinion summer economic hell hhs cut cdc staff sure birth control safe woman risk loeffler trump bill cement economic legacy decade door dream match feline frolic left lefter leftist democrat defined radical mayor million kid attend school urban heat zone trumpstarmer trade deal kick uk luxury car tariff rollsroyce engine fly dutyfree republican struggle find balance reconciliation bill sen ron johnson decided support president trump spending agenda traditional business planning doesnt cut anymore embrace instead senate move ahead massive tax spending bill trump administration building national citizenship system coverage king focus maine enthusiasm firework fizzling</t>
         </is>
       </c>
     </row>
@@ -694,12 +690,12 @@
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>halftime show icon take big fall get injured during wnba commissioner cup championship after paying u tariff on it product busy baby look to europe and australia a future market dan ives urge apple to make a move saying that perplexity acquisition is a nobrainer it a matter of when and not if centene stock plummet what sparked the brutal selloff centene stock plummet what sparked the brutal selloff barrons iran president approves law suspending cooperation with un nuclear watchdog invivyd and leading researcher form spear spike protein elimination and recovery study group first horizon corporation announces redemption of series b preferred stock and corresponding series b depositary share new study reveals brutal hit that u employer face from trump tariff huffpost fortnite how to get the battle bus suv try this trick wildfire kill people in spain a part of europe bake in heat wave think you missed the ai rally these gridbacked play are just getting warmed up tech billionaire launch erebor bank to fill svbs gap invivyd and leading researcher form spear spike protein elimination and recovery study group to assess the effect of monoclonal antibody therapy for long covid and covid postvaccination syndrome diversified energy promotes michael garrett to chief accounting officer diversified energy promotes michael garrett to chief accounting officer uk investor see not one but two pathway to rail merger developer acquire land for westgate village at north congress avenue west palm beach florida argon ai raise m to build the ai workspace powering the future of life science nationsbenefits integrates with dollar general to enable greater access to healthy food and wellness essential for million of healthcare consumer nationwide nationsbenefits integrates with dollar general to enable greater access to healthy food and wellness essential for million of healthcare consumer nationwide trump to cut protection for home health aide migrant farmworkers is atlantic hurricane season behind schedule here whats really going on a striking trend after texas banned abortion more woman nearly bled to death during miscarriage america tariffdriven buying spree leaf household saddled with debt and financially vulnerable elon musk want to create a new political party building rocket may be easier ge aerospace bear put spread could return in the next few month the humn etf let you invest in humanoid robotics stock should you buy in now the humn etf let you invest in humanoid robotics stock should you buy in now ge aerospace bear put spread could return in the next few month mortgage refinance demand surge a interest rate drop further cnbc u of m health care consulting fee adding up at rate of to per hour mortgage refinance demand surge a interest rate drop further certik hackd fortress building product accelerates fencing and steel framing growth strategy divests railing and lighting business to primesource brand inventus sign milling agreement with mcewen mining alta equipment group announces preferred stock dividend erdene commences trading on the otcqb riley permian announces closing of new mexico acquisition tonix pharmaceutical announces peerreviewed publication in cancer cell journal highlighting positive preclinical data of mtnx in gastric cancer animal model have an allamerican fourth of july with beef on the grill greystone logistics share information on stock buyback this is the key to building a personal brand that resonates with others olipops latest marketing stunt drew a person waitlistand sold out immediately alta equipment group announces preferred stock dividend pasinex announces annual and q financial result green thumb industry to hold second quarter earnings conference call on august whitestone reit announces second quarter earnings webcast and conference call the bestperforming sp stock of the last year have key commonality other than being ai stock can you guess it whitestone reit announces second quarter earnings webcast and conference call cipher mining surpasses hashrate growth forecast at black pearl and announces june operational update inventus sign milling agreement with mcewen mining riley permian announces closing of new mexico acquisition amc network announces early result and upsizing of tender offer for it senior note due amc network announces early result and upsizing of tender offer for it senior note due cardano price prediction ada price struggle to surpass a newcomer remittix gain ground with ico surge the bestperforming sp stock of the last year have key commonality other than being ai stock can you guess it token crypto presale go live price prediction x potential and what early buyer need to know now is bitcoin getting ready for a big price move in july water way technology enters strategic partnership for exclusive tomato hybrid development for vertical farming editorial stop the bleeding for colorado medicaid paramount resource ltd announces renewal of normal course issuer bid and july dividend pyrogenesis sign contract targeting plastic waste management problem in europe mda space completes acquisition of satixfy communication cipher mining surpasses hashrate growth forecast at black pearl and announces june operational update valore report result from successful hole trado auger drilling campaign at pedra branca including m at gt pgeau from surface dr phone fix expands partnership with assurant to accelerate certified preowned phone sale across canada what are the best vanguard etf for a wellrounded portfolio first horizon corporation announces redemption of series b preferred stock and corresponding series b depositary share what are the best vanguard etf for a wellrounded portfolio wallbridge exploration drilling continues to intercept highgrade gold mineralization at martiniere consumertech brand nothing tap cevas realspace software to bring immersive spatial audio to headphone and earbuds primesource brand acquires fortress railing product shattuck lab announces participation in upcoming leerink partner therapeutic forum ii and metabolism pyrogenesis sign contract targeting plastic waste management problem in europe dayforce empowers canadian small and midsized business with powerpay by dayforce identiv partner with narravero to accelerate digital product passport adoption and compliance blue sky uranium acquires key subsurface data for corcovo uranium project mendoza province argentina verkkokauppacom to publish januaryjune halfyear report on july crypto loss surpass billion in h certik report reveals alarming rise in phishing attack blue sky uranium acquires key subsurface data for corcovo uranium project mendoza province argentina main street announces followon portfolio investment paramount global and donald trump settle for million inside america department store tarifftriggered price hike are picking up robeco institutional asset management bv ha million position in dollar general corporation nysedg after trump warns elon musk to close up shop china rally behind world richest man there no need to keep putting up with it year old grocery store staple file for bankruptcy northisle announces near surface intercept and highergrade intercept at depth at west goodspeed on it north island project stock market news dow set to open higher after senate pass spending bill barrons meeka metal begin gold production at murchison project australia seeking stable passive income in crypto quid miner offer a sustainable new cloud mining solution democrat the last holdout bear could be the key to a new stockmarket rally marketwatch smart gas meter market worth billion by marketsandmarketstm yieldmax etf announces distribution on smcy ulty msty wntr lfgy and others yieldmax etf announces distribution on smcy ulty msty wntr lfgy and others aldi is selling a comfort sandal for just it a perfect oofos dupe but cheaper kkr bet on sustainable protein demand with proten investment in australia kitron receive eur million contract for defense airborne radar application northern trust q earnings what to expect northern trust q earnings what to expect murkowski got to yes on t megabill thanks to spending for alaska how the megabill will limit health care access and plan to ease gun regulation iran president approves law suspending cooperation with un nuclear watchdog new study reveals brutal hit that u employer face from trump tariff another one bite the dust cbs settle with trump over infamous kamala minute segment letter to the editor a plea to boulder earbud hiker no excuse for not repaying student loan guthrie song is a relevant a ever guest opinion stuart c lord education wa my way out this bill slam that door shut house republican race toward a final vote on trump tax bill daring critic to oppose guest opinion christopher schweitzer the siren song of unreason is a dangerous plunge into darkness hollywood lost the plot now rebel are making movie great again what the rd budget proposal say about the future of war is atlantic hurricane season behind schedule here whats really going on trump immigration crackdown ripple through economy a striking trend after texas banned abortion more woman nearly bled to death during miscarriage america tariffdriven buying spree leaf household saddled with debt and financially vulnerable elon musk want to create a new political party building rocket may be easier politician push jobkilling minimum wage hike while ignoring the devastating economic reality editorial attacking zohran mamdanis u citizenship is contemptible and dangerous republican rep jim jordan discusses trumpbacked megabill after senate passage rash kid have been abducted from ukraine these midwest senator want to find them a welcome shift in federal financial reporting wednesday letter sen budd where is your courage where is your honesty grow keep an eye out for brown patch disease in coolseason grass american opinion instead of ice raid on farmworkers overhaul this visa program cytosorbents provides u fda and health canada regulatory update for drugsorbatr best of the babylon bee defeated cuomo left groping for answer berry tramel rising valuation of nba franchise will prompt thunder ownership to sell opinion minneapolis police chief brian ohara is getting a bum rap over lake street raid year old grocery store staple file for bankruptcy democratic gov janet mill discusses how the gop megabill will impact maine maine cant afford to lose federal funding governor say modestly bipartisan budget could go to full wisconsin legislature wednesday gop megabill head back to the house for final approval u wont send some weapon pledged to ukraine following a pentagon review of military aid what the mar elia church bombing mean for syria future artificial intelligence saving you money and helping massdot build faster republican holdout head to the white house to discus trump bill letter patriot not saying much on ice treatment of veteran opinion a july approach supreme court sign away american democracy trump put senate in play in wall street journal new jersey gubernatorial candidate to speak at made in nj manufacturing day trump put senate in play in wall street journal nelly denies he maga say kamala harris locked up black ha white husband trump put senate in play in wall street journal trump put senate in play in wall street journal trump put senate in play in wall street journal trump put senate in play in wall street journal trump put senate in play in wall street journal trump put senate in play in wall street journal lawrence odonnells unfiltered reaction to bonkers trump presser moment say it all how ai can help ease the strain on health care service man charged in deadly brockton stabbing pleads not guilty house republican race toward a final vote on trump tax bill sen ron johnson a yes on trump budget bill sen tammy baldwin disgusted by it holy cow history happy july whatever green bay prison would close by under republican budget proposal gen z is the worst at work right wrong thing to know for july usaid ukraine munition trump megabill climate change paramount settlement former insurance commissioner say lara should go california focus former insurance commissioner say lara should go california focus letter spending choice make republican leader priority clear incredible growth stock poised for longterm gain win an ar old state saloon present conspiracy theory trivia and salooncast with ian carroll a twonight blast of truth tech and patriotism analysis show trump tariff would cost u employer billion if elon stick to rocket i will stick to finance bessent shrug off musk debt drama lancashire need to set investment priority to get biggest bang for buck can south korea deescalate north korea without u support how to be editor for a day notorious husband and wife professional tenant indicted on criminal charge we will not let hate win provincetown town manager say following second incident protect your pet on the fourth of july editor for a day letter constitutional system seems abandoned the u military cant quit the middle east another voice financial restitution is necessary but not sufficient for abuse survivor letter war against diversity education in unjust and disrespect history sean diddy comb found guilty on count acquitted of most serious charge firework warehouse explodes in california dalai lama say he intends to reincarnate after death ukraine look to jointly produce weapon with ally while u halt some shipment honolulu board of water supply sue navy for b over red hill fuel leak governor state budget veto trim public school maintenance new hawaii firework law take effect today hooser walking through my thought and value federal climate website go dark a trump administration promise policy reset house gop leader scrambling to rally holdout behind trump megabill house gop leader scrambling to rally holdout behind trump megabill house gop leader scrambling to rally holdout behind trump megabill house gop leader scrambling to rally holdout behind trump megabill house gop leader scrambling to rally holdout behind trump megabill house gop leader scrambling to rally holdout behind trump megabill leore james kowarsch liz shulman will big tech transform school into an ai video game jerald mcnair doe student use of ai spell the end for homework trump lit a fire under nato but more need to be done to contain the russiachina axis north korea to send a many a troop to bolster russia force ukrainian official say trump pick to run federal watchdog a yearold who once shared a conspiracy video and ha tie to a holocaust denier letter keep an eye on what matter not just what seems exciting editorial financial hit keep on coming and city hall only response is excuse steve chapman congress and the supreme court approve donald trump drive for absolute power letter why centrism doesnt have enough bite to make an impact</t>
+          <t>esperion appoints craig thompson to board of director mercadolibre applied material and a healthcare stock on cnbcs final trade ap business summarybrief at am edt ap business summarybrief at am edt how to plan in an uncertain economy senate churn through overnight session a republican seek support for trump big bill senate churn through overnight session a republican seek support for trump big bill bbg launch data center specialty practice appoints industry veteran chris fudacz to lead new specialty practice mara report june bitcoin production and mining operation update issue midyear outlook the bond canary in the big beautiful coal mine nasdaq welcome ipo in the first half of ameresco receives frost sullivan global company of the year award for excellence in energy service nasdaq welcome ipo in the first half of outlook therapeutic appoints biopharmaceutical industry and commercial leader bob jahr a chief executive officer outlook therapeutic appoints biopharmaceutical industry and commercial leader bob jahr a chief executive officer beyond the number analyst discus taysha gene therapy stock deep dive into new fortress energy stock analyst perspective rating trevi therapeutic to attend leerink partner therapeutic forum ii and metabolism beyond the number analyst discus lineage stock stock market today dow jones fall ahead of powell talk tesla dive on trumpmusk feud live coverage analyst assess ionis pharmaceutical what you need to know where robinhood market stand with analyst deep dive into weyerhaeuser stock analyst perspective rating should you expect demand growth in range resource rrc alphyns zabalafin hydrogel for atopic dermatitis highlighted in leading peerreviewed journal oppo reno pro price availability spec more qapel medical appoints stewart strong a president and chief executive officer highspring and vaco by highspring earn top honor from staffing industry analyst what make pinnacle financial partner pnfp a longterm bet ap technology summarybrief at am edt july is flush smart month who need a refresher on potty training basic historic hip hop def jam memorabilia auction to benefit rush philanthropic art foundation bidding close july july is flush smart month who need a refresher on potty training basic bounce empire debut world largest indoor circular transparent led screen surpasses visitor in two year rohrer aesthetic unveils new clinical study highlighting pixe a the future of regenerative aesthetic can community health launch susan terry foundation to empower individual living with hiv blackrock esg capital allocation term trust ecat certified result of annual meeting announced td synnex acquires apptium to accelerate innovation breadth of cloud and everythingasaservice offering masco corporation announces date for earnings release and conference call for second quarter fifth third wealth advisor surpasses billion in net new asset under management expands platform capability thredd expands global footprint with new office in the u intrabio inc completes recruitment for ib at pivotal clinical trial dakota announces formation of advisory board to accelerate strategic growth and product evolution uber eats expands partnership with beloved local grocer marea therapeutic appoints shishir gadam phd a chief technical officer lynq set july th launch date for realtime interestbearing settlement network retail investor use ethransaction btc xrp usdc and other mainstream currency for cloud mining earning a stable income of per day cordia pittsburgh win system of the year award at idea senate strike ai provision from gop bill after uproar from the state senate strike ai provision from gop bill after uproar from the state senate strike ai provision from gop bill after uproar from the state senate strike ai provision from gop bill after uproar from the state thermo fisher scientific to hold earnings conference call on wednesday july amentum to host third quarter fiscal year earnings conference call on august momentus and orbit fab partner to advance space servicing with podracer and rafti demonstration flight this stock is still the very best place you can put your money tailor expands series a to m with privatepublic support operation hope and georgia state university launch groundbreaking ai literacy program for underserved youth levelblue to acquire trustwave becoming largest pureplay managed security service provider this stock is still the very best place you can put your money nline energy and penn state health milton s hershey medical center win joseph m brillhart innovation award at idea pepper launch the first open and extensible endless aisle platform in the foodservice industry fresenius expands biosimilars portfolio with the launch of denosumab biosimilars in the u sofi schedule conference call to discus q result valley national bancorp announces new general counsel unnatural product tap argenxs help for ringed molecule expands internal work into obesity brightspring health lead company in line for tripledigit profit growth brightspring health lead company in line for tripledigit profit growth i tried amazon bestselling beckham hotel collection pillow to see if theyre actually any good transcript velina peneva swiss re chief investment officer elon musk and donald trump are fighting again miami beach city commission grant final approval to terras redevelopment of the historic deauville hotel site canadian cuisine food that reflect the country size and diversity is nvidia stock a buy at new record high jewelry sale outperform a u spending for most luxury good falter citi report find cnbc oportun responds to comment by findell capital actelis network announces private placement priced atthemarket under nasdaq rule deepki accelerates u operation to help commercial real estate tackle sustainability challenge manage risk and drive financial performance duo technology added to russell microcap index dih appoints rehazentrum valens a a dih center of excellence lendmark financial service announces expiration and result of it tender offer for it senior note due cole engineering awarded m u army production contract for nextgeneration stinger training system zohran mamdanis primary win is a warning to every legacy brand travtus partner with engrain to bring spatial intelligence to it everyday ai platform jd martin expands partnership with nvent eriflex to florida north carolina and south carolina radius recycling report third quarter fiscal financial result stryker to announce financial result for it second quarter of fiscal year richtech robotics announces inclusion in u smallcap russell and russell index oncternal therapeutic announces the sale of select development program and the winddown of it operation arevon secures million credit facility to accelerate renewable energy growth in the united state dih appoints rehazentrum valens a a dih center of excellence kavalan blitz iwc taking trio of whisky distillery and master distiller of the year prize inriver research reveals widespread ai deployment in pim of company have moved beyond pilot randamu and chengdu university of information technology collaborate to advance cryptographic research and web coordination infrastructure kestra medical technology ltd to report fourth quarter and fiscal year result on july genmab announces change to it executive committee document available regarding ramacos brook mine rare earth and critical mineral project condo price dropped in maythe second largest decline on record independent preliminary economic assessment report from fluor corporation confirms commercial and technical feasibility of ramacos brook mine rare earth deposit realme series set to shake up india midrange smartphone market aocs childhood nickname revealed amid bronx girl claim second democrat announces campaign to unseat gop congressman in competitive michigan district these new colorado law take effect tuesday regulating gun shop sexual assault case youth detention and more these new colorado law take effect tuesday regulating gun shop sexual assault case youth detention and more the multiverse scandal how academia is redefining science to avoid god senate strike ai provision from gop bill after uproar from the state senate strike ai provision from gop bill after uproar from the state i tried amazon bestselling beckham hotel collection pillow to see if theyre actually any good elon musk and donald trump are fighting again dan gainor the good the bad and the absurd june wildest political moment and celebrity meltdown canadian cuisine food that reflect the country size and diversity la new budget kick in today here what your tax dollar are paying for montana leader need to protect our export economy mark noland letter bad outcome if medicare is cut editorial cartoon for tuesday july cant wait for saturday today texas state to the pac then what james walkinshaw win democratic contest to likely replace u rep connolly in northern virginia mystery surround the jeffrey epstein file after bondi claim ten of thousand of video amendment targeting medicaid expansion wont get a senate vote trump say doge might have to go back and eat elon musk after his criticism of the gop bill president lee jaemyung hope for a better interkorean relationship hickory public housing authority officially abolished after final meeting monday well break your leg un accused of mafiatype response to usled gaza relief effort usaid cut could cause staggering number of avoidable death study say how iran lost the short war with israel and america republican struggle to pas trump massive tax bill after hour of drama opinion senate bill undermines decade of progress in disability service thousand of cancer patient fear disruption in care due to insurance contract dispute supreme court medina ruling free state to defund planned parenthood muscatine contingent visit china trump blame att after conference call with faith leader disrupted takeaway from aps report on attorney general bondis comment about evidence in epstein case takeaway from aps report on attorney general bondis comment about evidence in epstein case texas democrat who lost to ted cruz month ago jump into senate race watching area near florida for possible tropical development saudi arabia alhilal had to climb mount everest without oxygen in shock club world cup win over manchester city trump score major victory a vance help push big beautiful bill through senate maybe he ha a knife yulia putintseva asks for crazy wimbledon spectator to be ejected over safety fear senate hold votearama on trump big beautiful bill senate votearama on gop megabill go all night most american feel democracy is theatened poll show and mamdani speaks with npr new jersey phil murphy take heat from all side in final budget a governor south korea energy policy under lee jaemyung american opinion deportation alone cant fix u immigration problem can south korea achieve peace in a chaotic world trump big beautiful bill awaits final senate vote opinion spense havlick scam are everywhere these day dont be fooled the future of air combat how long will the u military still need pilot california new consumer protection law go into effect july amc theater will start placing even more ad in cinema nationwide starting today letter to the editor power must be maintained at all cost extend freedom beyond our own specie we need a shared morality major insurance change are coming to glp drug for weight loss here how that could affect patient editorial american deserve clearer explanation of what happened in iran maglite pedestrian safety institute and additional partner to promote traffic and pedestrian safety during national roadside traffic safety awareness month egg harbor township approves year affordable housing plan remembering the men and woman who serve our country do the saint have their qb of the future in the building this season should decide that trump relief for farmer look like control by fear guest commentary florida resident get a new roof now and receive free exterior painting just in time for hurricane season letter democrat seem incapable of praising trump for anything whats the point of being a u senator if you dont have gut bob brown the most undervalued asset for a leader it these hour the bully pulpit ron waterman what sdas latest win signal for military space republican still pushing to pas trump big beautiful bill he hasnt played in mlb for more than two decade one team is paying him million a year until senate republican closing in on final vote on gop spending bill more republican than dems vote to raise tax on billionaire in latenight senate vote house democrat announces he wont seek reelection in trump doge is the monster that might have to go back and eat elon will state assembly save energy independence california focus will state assembly save energy independence california focus watch out for weirdo facebook scammer promising the world scam of the week letter obama policy necessitated u strike on nuclear site opinion state bill pausing new building code risk climate change progress public health expert trump big beautiful bill will cause misery and death my turn we need to be a twohospital town my turn thanks extremist for making me reexamine who i want to be and what our nation should be my turn state democrat play dirty trick with legislation my turn another four year of the idiot council doofus thing to know for july trump megabill israelgaza alligator alcatraz idaho shooting hurricane data debate over trump big bill continues tuesday morning in u senate hundred of national guard force deployed to la by trump could be returned to calif wildfire duty editorial cartoon for july reader view congress must reject any cut to medicaid who to say anybodys vote is safe trump doj target north carolina voter roll here how president trump mega tax bill would impact illinois council lower real estate tax rate yet restores funding for service program concern in north dakota grow about increased aca cost medical debt flood drown out lancaster county roadway in aftermath of monday storm hundred of child told to test for disease in australia after childcare worker charged with child sex abuse here are offensive player who can contribute for southern football in wisconsin governor gop reach budget deal to cut tax fund university maha report call for fighting chronic disease but trump and kennedy have yanked funding local expert detail potential effect of federal funding cut lagniappe next up the steve miller band jay take isolation a doubleedged sword letter catholic must stand in unity and sacrifice a jesus did letter america most beautiful wild land are in grave danger burke catawba mcdowell iredell city county close for july see garbage impact</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>halftime icon take fall injured wnba commissioner cup championship paying tariff product busy baby look europe australia future market dan ives urge apple move saying perplexity acquisition nobrainer matter centene stock plummet sparked brutal selloff centene stock plummet sparked brutal selloff barrons iran president approves suspending cooperation un nuclear watchdog invivyd leading researcher form spear spike protein elimination recovery study horizon corporation announces redemption series b preferred stock corresponding series b depositary share new study reveals brutal hit employer face trump tariff huffpost fortnite battle bus suv try trick wildfire kill people spain part europe bake heat wave missed ai rally gridbacked play getting warmed tech billionaire launch erebor bank fill svbs gap invivyd leading researcher form spear spike protein elimination recovery study assess effect monoclonal antibody therapy covid covid postvaccination syndrome diversified energy promotes michael garrett chief accounting officer diversified energy promotes michael garrett chief accounting officer uk investor pathway rail merger developer acquire land westgate village north congress avenue west palm beach florida argon ai raise build ai workspace powering future life science nationsbenefits integrates dollar general enable greater access healthy wellness essential million healthcare consumer nationwide nationsbenefits integrates dollar general enable greater access healthy wellness essential million healthcare consumer nationwide trump cut protection health aide migrant farmworkers atlantic hurricane season behind schedule whats striking trend texas banned abortion woman nearly bled death miscarriage america tariffdriven buying spree leaf household saddled debt financially vulnerable elon musk create new political party building rocket easier ge aerospace bear put spread next month humn invest humanoid robotics stock buy humn invest humanoid robotics stock buy ge aerospace bear put spread next month mortgage refinance demand surge interest rate drop cnbc health care consulting fee adding rate per hour mortgage refinance demand surge interest rate drop certik hackd fortress building product accelerates fencing steel framing growth strategy divests railing lighting business primesource brand inventus sign milling agreement mcewen mining alta equipment announces preferred stock dividend erdene commences trading otcqb riley permian announces closing new mexico acquisition tonix pharmaceutical announces peerreviewed publication cancer cell journal highlighting positive preclinical data mtnx gastric cancer animal model allamerican fourth beef grill greystone logistics share information stock buyback building personal brand resonates others olipops latest marketing stunt drew waitlistand immediately alta equipment announces preferred stock dividend pasinex announces annual q financial green thumb industry quarter earnings conference call august whitestone reit announces quarter earnings webcast conference call bestperforming sp stock commonality ai stock guess whitestone reit announces quarter earnings webcast conference call cipher mining surpasses hashrate growth forecast black pearl announces operational update inventus sign milling agreement mcewen mining riley permian announces closing new mexico acquisition amc network announces early upsizing tender offer senior note due amc network announces early upsizing tender offer senior note due cardano price prediction ada price struggle surpass newcomer remittix gain ground ico surge bestperforming sp stock commonality ai stock guess token crypto presale price prediction x potential early buyer bitcoin getting ready price move water technology enters strategic partnership exclusive tomato hybrid development vertical farming editorial stop bleeding colorado medicaid paramount resource ltd announces renewal normal course issuer bid dividend pyrogenesis sign contract targeting plastic waste problem europe mda space completes acquisition satixfy communication cipher mining surpasses hashrate growth forecast black pearl announces operational update valore report successful hole trado auger drilling campaign pedra branca gt pgeau surface dr phone fix expands partnership assurant accelerate certified preowned phone sale across canada best vanguard wellrounded portfolio horizon corporation announces redemption series b preferred stock corresponding series b depositary share best vanguard wellrounded portfolio wallbridge exploration drilling continues intercept highgrade gold mineralization martiniere consumertech brand nothing tap cevas realspace software immersive spatial audio headphone earbuds primesource brand acquires fortress railing product shattuck lab announces participation upcoming leerink partner therapeutic forum ii metabolism pyrogenesis sign contract targeting plastic waste problem europe dayforce empowers canadian small midsized business powerpay dayforce identiv partner narravero accelerate digital product passport adoption compliance blue sky uranium acquires subsurface data corcovo uranium project mendoza province argentina verkkokauppacom publish januaryjune halfyear report crypto loss surpass billion h certik report reveals alarming rise phishing attack blue sky uranium acquires subsurface data corcovo uranium project mendoza province argentina main street announces followon portfolio investment paramount global donald trump settle million inside america department store tarifftriggered price hike picking robeco institutional asset bv million dollar general corporation nysedg trump warns elon musk close shop china rally behind world richest man putting old grocery store staple file bankruptcy northisle announces near surface intercept highergrade intercept depth west goodspeed north island project stock market dow set open higher senate pas spending bill barrons meeka metal begin gold production murchison project australia seeking stable passive income crypto quid miner offer sustainable new cloud mining solution democrat holdout bear new stockmarket rally marketwatch smart gas meter market worth billion marketsandmarketstm yieldmax announces distribution smcy ulty msty wntr lfgy others yieldmax announces distribution smcy ulty msty wntr lfgy others aldi selling comfort sandal perfect oofos dupe cheaper kkr bet sustainable protein demand proten investment australia kitron receive eur million contract defense airborne radar application northern trust q earnings expect northern trust q earnings expect murkowski got yes megabill spending alaska megabill limit health care access plan ease gun regulation iran president approves suspending cooperation un nuclear watchdog new study reveals brutal hit employer face trump tariff another bite dust cbs settle trump infamous kamala segment editor plea boulder earbud hiker excuse repaying student loan guthrie song relevant ever guest opinion stuart c lord education bill slam door shut house republican race final vote trump tax bill daring critic oppose guest opinion christopher schweitzer siren song unreason dangerous plunge darkness hollywood plot rebel making movie great rd budget proposal future war atlantic hurricane season behind schedule whats trump immigration crackdown ripple economy striking trend texas banned abortion woman nearly bled death miscarriage america tariffdriven buying spree leaf household saddled debt financially vulnerable elon musk create new political party building rocket easier politician push jobkilling minimum wage hike ignoring devastating economic reality editorial attacking zohran mamdanis citizenship contemptible dangerous republican rep jim jordan discusses trumpbacked megabill senate passage rash kid abducted ukraine midwest senator find welcome shift federal financial reporting wednesday sen budd courage honesty grow eye brown patch disease coolseason grass american opinion instead raid farmworkers overhaul visa program cytosorbents provides fda health canada regulatory update drugsorbatr best babylon bee defeated cuomo left groping answer berry tramel rising valuation nba franchise prompt thunder ownership sell opinion minneapolis police chief brian ohara getting bum rap lake street raid old grocery store staple file bankruptcy democratic gov janet mill discusses gop megabill impact maine maine cant afford lose federal funding governor modestly bipartisan budget full wisconsin legislature wednesday gop megabill head house final approval wont send weapon pledged ukraine following pentagon review military aid mar elia church bombing syria future artificial intelligence saving money helping massdot build faster republican holdout head white house discus trump bill patriot saying treatment veteran opinion approach supreme sign away american democracy trump put senate play wall street journal new jersey gubernatorial candidate speak nj manufacturing trump put senate play wall street journal nelly denies maga kamala harris locked black white husband trump put senate play wall street journal trump put senate play wall street journal trump put senate play wall street journal trump put senate play wall street journal trump put senate play wall street journal trump put senate play wall street journal lawrence odonnells unfiltered reaction bonkers trump presser moment ai help ease strain health care service man charged deadly brockton stabbing pleads guilty house republican race final vote trump tax bill sen ron johnson yes trump budget bill sen tammy baldwin disgusted holy cow history happy whatever green bay prison close republican budget proposal gen z worst work usaid ukraine munition trump megabill climate change paramount settlement insurance commissioner lara california focus insurance commissioner lara california focus spending choice republican priority incredible growth stock poised longterm gain ar old saloon present conspiracy theory trivia salooncast ian carroll twonight blast truth tech patriotism analysis trump tariff cost employer billion elon stick rocket stick finance bessent shrug musk debt drama lancashire set investment priority biggest bang buck south korea deescalate north korea without support editor notorious husband wife professional tenant indicted criminal charge hate provincetown town manager following incident protect pet fourth editor constitutional system seems abandoned military cant quit middle east another voice financial restitution necessary sufficient abuse survivor war diversity education unjust disrespect history sean diddy comb found guilty count acquitted serious charge firework warehouse explodes california dalai lama intends reincarnate death ukraine look jointly produce weapon ally halt shipment honolulu board water supply sue navy b red hill fuel leak governor budget veto trim public school maintenance new hawaii firework take effect hooser walking thought value federal climate website dark trump administration promise policy reset house gop scrambling rally holdout behind trump megabill house gop scrambling rally holdout behind trump megabill house gop scrambling rally holdout behind trump megabill house gop scrambling rally holdout behind trump megabill house gop scrambling rally holdout behind trump megabill house gop scrambling rally holdout behind trump megabill leore james kowarsch liz shulman tech transform school ai video game jerald mcnair doe student ai spell end homework trump lit fire nato contain russiachina axis north korea send troop bolster russia force ukrainian trump pick run federal watchdog yearold shared conspiracy video tie holocaust denier eye matter seems exciting editorial financial hit coming hall response excuse steve chapman congress supreme approve donald trump drive absolute power centrism doesnt enough bite impact</t>
+          <t>esperion appoints craig thompson board director mercadolibre applied material healthcare stock cnbcs final trade business business plan uncertain economy senate churn overnight session republican seek support trump bill senate churn overnight session republican seek support trump bill bbg launch data center specialty practice appoints industry veteran chris fudacz lead specialty practice mara report bitcoin production mining operation update issue midyear outlook bond canary coal mine nasdaq welcome ipo half ameresco receives frost sullivan global company award excellence energy service nasdaq welcome ipo half outlook therapeutic appoints biopharmaceutical industry commercial bob jahr chief executive officer outlook therapeutic appoints biopharmaceutical industry commercial bob jahr chief executive officer beyond analyst discus taysha gene therapy stock deep dive fortress energy stock analyst perspective rating trevi therapeutic attend leerink partner therapeutic forum ii metabolism beyond analyst discus lineage stock stock market dow jones fall ahead powell tesla dive trumpmusk feud coverage analyst assess ionis pharmaceutical robinhood market stand analyst deep dive weyerhaeuser stock analyst perspective rating expect demand growth range resource rrc alphyns zabalafin hydrogel atopic dermatitis highlighted leading peerreviewed journal oppo reno pro price availability spec qapel medical appoints stewart strong president chief executive officer highspring vaco highspring earn honor staffing industry analyst pinnacle financial partner pnfp longterm bet technology flush smart month refresher potty training basic historic hip hop def jam memorabilia auction benefit rush philanthropic art foundation bidding close flush smart month refresher potty training basic bounce empire debut world largest indoor circular transparent led screen surpasses visitor rohrer aesthetic unveils clinical study highlighting pixe future regenerative aesthetic community health launch susan terry foundation empower individual living hiv blackrock esg allocation term trust ecat certified annual meeting announced td synnex acquires apptium accelerate innovation breadth cloud everythingasaservice offering masco corporation announces date earnings release conference call quarter fifth third wealth advisor surpasses billion net asset expands platform capability thredd expands global footprint office intrabio completes recruitment ib pivotal clinical trial dakota announces formation advisory board accelerate strategic growth product evolution uber eats expands partnership beloved local grocer marea therapeutic appoints shishir gadam phd chief technical officer lynq set launch date realtime interestbearing settlement network retail investor ethransaction btc xrp usdc mainstream currency cloud mining earning stable income per cordia pittsburgh system award idea senate strike ai provision gop bill uproar senate strike ai provision gop bill uproar senate strike ai provision gop bill uproar senate strike ai provision gop bill uproar thermo fisher scientific earnings conference call wednesday amentum host third quarter fiscal earnings conference call august momentus orbit fab partner advance space servicing podracer rafti demonstration flight stock best place put money tailor expands series privatepublic support operation georgia university launch groundbreaking ai literacy program underserved youth levelblue acquire trustwave becoming largest pureplay managed security service provider stock best place put money nline energy penn health milton hershey medical center joseph brillhart innovation award idea pepper launch open extensible endless aisle platform foodservice industry fresenius expands biosimilars portfolio launch denosumab biosimilars sofi schedule conference call discus q valley national bancorp announces general counsel unnatural product tap argenxs help ringed molecule expands internal work obesity brightspring health lead company line tripledigit profit growth brightspring health lead company line tripledigit profit growth tried amazon bestselling beckham hotel collection pillow theyre good transcript velina peneva swiss chief investment officer elon musk donald trump fighting miami beach commission grant final approval terras redevelopment historic deauville hotel site canadian cuisine reflect country size diversity nvidia stock buy record high jewelry sale outperform spending luxury good falter citi report find cnbc oportun responds findell actelis network announces private placement priced atthemarket nasdaq rule deepki accelerates operation help commercial real estate tackle sustainability challenge manage risk drive financial performance duo technology added russell microcap index dih appoints rehazentrum valens dih center excellence lendmark financial service announces expiration tender offer senior note due cole engineering awarded army production contract nextgeneration stinger training system zohran mamdanis primary warning legacy brand travtus partner engrain spatial intelligence everyday ai platform jd martin expands partnership nvent eriflex florida north carolina south carolina radius recycling report third quarter fiscal financial stryker announce financial quarter fiscal richtech robotics announces inclusion smallcap russell russell index oncternal therapeutic announces sale select development program winddown operation arevon secures million credit facility accelerate renewable energy growth united dih appoints rehazentrum valens dih center excellence kavalan blitz iwc taking trio whisky distillery master distiller prize inriver research reveals widespread ai deployment pim company moved beyond pilot randamu chengdu university information technology collaborate advance cryptographic research web coordination infrastructure kestra medical technology ltd report fourth quarter fiscal genmab announces change executive committee document available regarding ramacos brook mine rare earth critical mineral project condo price dropped maythe largest decline record independent preliminary economic assessment report fluor corporation confirms commercial technical feasibility ramacos brook mine rare earth deposit realme series set shake india midrange smartphone market aocs childhood nickname revealed amid bronx girl claim democrat announces campaign unseat gop congressman competitive michigan district colorado take effect tuesday regulating gun shop sexual assault youth detention colorado take effect tuesday regulating gun shop sexual assault youth detention multiverse scandal academia redefining science avoid god senate strike ai provision gop bill uproar senate strike ai provision gop bill uproar tried amazon bestselling beckham hotel collection pillow theyre good elon musk donald trump fighting dan gainor good bad absurd wildest political moment celebrity meltdown canadian cuisine reflect country size diversity la budget kick tax dollar paying montana protect export economy mark noland bad outcome medicare cut editorial cartoon tuesday cant wait saturday texas pac james walkinshaw democratic contest likely replace rep connolly northern virginia mystery surround jeffrey epstein file bondi claim ten thousand video amendment targeting medicaid expansion wont senate vote trump doge eat elon musk criticism gop bill president lee jaemyung better interkorean relationship hickory public housing authority officially abolished final meeting monday break leg un accused mafiatype response usled gaza relief effort usaid cut cause staggering avoidable death study iran short war israel america republican struggle pa trump massive tax bill hour drama opinion senate bill undermines decade progress disability service thousand cancer patient fear disruption care due insurance contract dispute supreme medina ruling free defund planned parenthood muscatine contingent visit china trump blame att conference call faith disrupted takeaway aps report attorney general bondis evidence epstein takeaway aps report attorney general bondis evidence epstein texas democrat ted cruz month ago jump senate race watching area near florida possible tropical development saudi arabia alhilal climb mount everest without oxygen shock club world cup manchester trump score major victory vance help push bill senate maybe knife yulia putintseva asks crazy wimbledon spectator ejected safety fear senate votearama trump bill senate votearama gop megabill night american feel democracy theatened poll mamdani speaks npr jersey phil murphy take heat final budget governor south korea energy policy lee jaemyung american opinion deportation alone cant fix immigration problem south korea achieve peace chaotic world trump bill awaits final senate vote opinion spense havlick scam everywhere dont fooled future air combat military pilot california consumer protection effect amc theater start placing ad cinema nationwide starting editor power must maintained cost extend freedom beyond specie shared morality major insurance change coming glp drug weight loss affect patient editorial american deserve clearer explanation happened iran maglite pedestrian safety institute additional partner promote traffic pedestrian safety national roadside traffic safety awareness month egg harbor township approves affordable housing plan remembering men woman country saint qb future building season decide trump relief farmer look control fear guest commentary florida resident roof receive free exterior painting hurricane season democrat seem incapable praising trump anything whats senator dont gut bob brown undervalued asset hour bully pulpit ron waterman sdas latest signal military space republican pushing pa trump bill hasnt played mlb decade team paying million senate republican closing final vote gop spending bill republican dems vote raise tax billionaire latenight senate vote house democrat announces wont seek reelection trump doge monster eat elon assembly save energy independence california focus assembly save energy independence california focus watch weirdo facebook scammer promising world scam obama policy necessitated strike nuclear site opinion bill pausing building code risk climate change progress public health expert trump bill cause misery death turn twohospital town turn extremist making reexamine nation turn democrat play dirty trick legislation turn another idiot council doofus trump megabill israelgaza alligator alcatraz idaho shooting hurricane data debate trump bill continues tuesday morning senate hundred national guard force deployed la trump returned calif wildfire duty editorial cartoon reader view congress must reject cut medicaid anybodys vote safe trump doj target north carolina voter roll president trump mega tax bill impact illinois council lower real estate tax rate yet restores funding service program concern north dakota grow increased aca cost medical debt flood drown lancaster county roadway aftermath monday storm hundred child test disease australia childcare worker charged child sex abuse offensive player contribute southern football wisconsin governor gop reach budget deal cut tax fund university maha report call fighting chronic disease trump kennedy yanked funding local expert detail potential effect federal funding cut lagniappe next steve miller band jay take isolation doubleedged sword catholic must stand unity sacrifice jesus america wild land grave danger burke catawba mcdowell iredell county close garbage impact</t>
         </is>
       </c>
     </row>
@@ -730,12 +726,12 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>u employer added a surprising job last month despite uncertainty over economic policy canada trade deficit in may narrow export to u drop millionaire renter surge in nyc a high earner opt for luxury lease report trader pare bet on fed rate cut after job report here lindsell train global equity fund comment on nintendo co ltd ntdoy stock market today dow sp and nasdaq future advance after strong payroll data trump tax and spending bill face vote marketwatch new online casino canada reddit user share the leading real money online casino for tcl csot exclusively supply display for xiaomi mix flip and xiaomi yu powering xiaomis new beginning blowout june payroll k job added smashing expectation unemployment rate drop to avdx alert monsey firm of wohl fruchter investigating fairness of the sale of avidxchange holding to tpg global and corpay dune awakening drop massive july update fix exploit and rebalances pvp zone clearmind medicine announces irb approval for phase a clinical trial for alcohol use disorder at tel aviv sourasky medical center u stock and bond market are open on eve of july but they close early trump want the world to squeeze out china he starting with vietnam u application for jobless aid fell to last week a layoff remain low u application for jobless aid fell to last week a layoff remain low u application for jobless aid fell to last week a layoff remain low u application for jobless aid fell to last week a layoff remain low u application for jobless aid fell to last week a layoff remain low u application for jobless aid fell to last week a layoff remain low u application for jobless aid fell to last week a layoff remain low trader pare bet on fed rate cut after job report yahoo finance u application for jobless aid fell to last week a layoff remain low u application for jobless aid fell to last week a layoff remain low u application for jobless aid fell to last week a layoff remain low u application for jobless aid fell to last week a layoff remain low parazero receives a recurring bulk order of safeair system from an australian distributor nyt strand july serf a sweet scoop with icecream a spangram half yearly report on lvmhs liquidity contract with oddo bhf sca half yearly report on lvmhs liquidity contract with oddo bhf sca these fossil fuel stock rallied a senate passed trump tax spending plan deep tristate layoff leave continuing jobless claim stuck at highest since canada trade deficit narrow in may a export rise these fossil fuel stock rallied a senate passed trump tax spending plan investor business daily ford jpmorgan amazon executive predict deep job cut a ai advance u weekly firsttime unemployment claim fewest since may ap business summarybrief at am edt u application for jobless aid fell to last week a layoff remain low u application for jobless aid fell to last week a layoff remain low review liquid death on fire plus one of the most unique thc drink yet hog look to close thing out ahead of holiday break cotton mixed in early thursday trade corn pushing gain into thursday morning trade cattle look to round out short week wheat sneaking out gain ahead of threeday weekend soybean strength continuing on thursday am top financial stock you may want to dump this quarter house beat and hidden venue a new sound is emerging in abu dhabi u employer added a surprising job last month despite uncertainty over economic policy u employer added a surprising job last month despite uncertainty over economic policy starbucks offer million stock bonus to exec but should you buy it share here what technical analysis show fed rate cut appears less likely after strongerthanforecast june payroll data green science alliance established an electric vehicle ev company utilizing next generation inwheel motor technology developed by a japanese engineer who pioneered supercar ev named eliica over year ago u economy add new job unemployment rate dip to percent in june stock market today dow sp nasdaq future hit pause after a solid job report liveone synervoz partner for nextgen voice experience u employer added job in june strategy stock rise after key trading signal jobless claim fall to lowest level since midmay sp build on record high future rising after strong job report barrons my parent gifted me what should i do with it u economy add job in june more than expected popular restaurant chain close all location no bankruptcy u application for jobless aid fell to last week a layoff remain low u application for jobless aid fell to last week a layoff remain low u application for jobless aid fell to last week a layoff remain low trade deficit widens surpassing both forecast and previous figure u job growth beat expectation in june celebrate independence wilmatm set aba practice free from manual workflow with powerful patient relationship management nike is back in the race billionaire bill ackman urge tired subdued andrew cuomo to drop out of nyc mayoral race begrudgingly endorses eric adam u payroll increased by in june more than expected navitas semiconductor to participate in upcoming cjs security conference u add k job in june beating expectation u initial jobless claim dip below expectation bolstering usd u employer added job in june a labor market show resilience despite uncertainty over trump economic policy u employer added job in june a labor market show resilience despite uncertainty over trump economic policy labor market stay afloat a hiring top forecastsagain u employer added job in june a labor market show resilience despite uncertainty over trump economic policy airline face investor after strong but cheaper july holiday cnbc lamplight luxury rv park invite traveler to discover their perfect texas getaway at holiday road rv park dsh hotel advisor close jacksonville fl candlewood suite sale a hospitality market heat up lamplight luxury rv park invite traveler to discover their perfect texas getaway at holiday road rv park navitas semiconductor to participate in upcoming cjs security conference dsh hotel advisor close jacksonville fl candlewood suite sale a hospitality market heat up nonfarm payroll beat expectation indicating robust u job market coinex research june report bitcoin in the crossfire u payroll increased by in june more than expected cnbc etoro appoints former sec commissioner laura unger and wix cfo lior shemesh a board member beauty and the bear michael burry estee lauder snub china smci stock get price target bump but it still below current share price agf announces passing of kevin mccreadie ceo and cio coreweave is the first cloud provider to deploy nvidias latest ai chip why kelly slater moved headquarters of his sustainable clothing brand from la to san diego why kelly slater moved headquarters of his sustainable clothing brand from la to san diego why kelly slater moved headquarters of his sustainable clothing brand from la to san diego why kelly slater moved headquarters of his sustainable clothing brand from la to san diego why kelly slater moved headquarters of his sustainable clothing brand from la to san diego why kelly slater moved headquarters of his sustainable clothing brand from la to san diego why kelly slater moved headquarters of his sustainable clothing brand from la to san diego can california democrat require ice agent to unmask and show id trump show america wont tolerate nuclear threat james fitzpatrick trump show america wont tolerate nuclear threat james fitzpatrick texas internet porn law is constitutional common sense prevails dallas morning news texas internet porn law is constitutional common sense prevails dallas morning news texas internet porn law is constitutional common sense prevails dallas morning news trump show america wont tolerate nuclear threat james fitzpatrick trump show america wont tolerate nuclear threat james fitzpatrick texas internet porn law is constitutional common sense prevails dallas morning news trump show america wont tolerate nuclear threat james fitzpatrick texas internet porn law is constitutional common sense prevails dallas morning news texas internet porn law is constitutional common sense prevails dallas morning news trump show america wont tolerate nuclear threat james fitzpatrick texas internet porn law is constitutional common sense prevails dallas morning news texas internet porn law is constitutional common sense prevails dallas morning news texas internet porn law is constitutional common sense prevails dallas morning news trump show america wont tolerate nuclear threat james fitzpatrick trump show america wont tolerate nuclear threat james fitzpatrick trump show america wont tolerate nuclear threat james fitzpatrick texas internet porn law is constitutional common sense prevails dallas morning news congressional intern killed in dc shooting scrum alliance ranked on comparablys list of best leadership team among small company judge strike down trump policy that deleted transgender page from govt website house beat and hidden venue a new sound is emerging in abu dhabi federal judge rule noncalifornia resident can apply for concealedcarry gun permit the latest house leader rush toward a final vote a democrat hold the floor what maga mean to american u application for jobless aid fell to last week a layoff remain low u application for jobless aid fell to last week a layoff remain low aclu sue to block ice raid in southern california alleging constitutional violation u employer added job in june a labor market show resilience despite uncertainty over trump economic policy u employer added job in june a labor market show resilience despite uncertainty over trump economic policy california boost film and tv tax credit to million to preserve job attorney general tap politically connected billing lawyer for judicial discipline panel dnrcs drought outlook for montana is grim going into hot dry summer attorney general tap politically connected billing lawyer for judicial discipline panel attorney general tap politically connected billing lawyer for judicial discipline panel double standard no no standard did the pentagon spread false ufo story were skeptical trump t megabill set house record for longest vote in history number of megarounds drop in first half a biotech struggle against worsening slump california school official say video show immigration agent urinating in public view homeland security investigating iran suspends cooperation with un nuclear monitoring agency a slider a milestone and a heartfelt thank you kershaws th strikeout federal funding for contraceptive access return to missouri nonprofit after threemonth freeze dan walter california lawmaker finally achieve holy grail reform of state key environmental law jeffries us magic minute to delay vote on trump megabill after settling with trump cbs news staffer fear what come next some education grant in limbo were used for leftwing agenda trump administration say some education grant in limbo were used for leftwing agenda trump administration say some education grant in limbo were used for leftwing agenda trump administration say some education grant in limbo were used for leftwing agenda trump administration say some education grant in limbo were used for leftwing agenda trump administration say some education grant in limbo were used for leftwing agenda trump administration say some education grant in limbo were used for leftwing agenda trump administration say some education grant in limbo were used for leftwing agenda trump administration say some education grant in limbo were used for leftwing agenda trump administration say some education grant in limbo were used for leftwing agenda trump administration say some education grant in limbo were used for leftwing agenda trump administration say family of slain police officer krystal rivera shot by a fellow officer want an independent investigation vance boelter man charged in minnesota lawmaker shooting due back in federal court how george washington america reluctant leader contrast with today frederic j fransen choosing war over diplomacy increase danger for u elizabeth shackelford choosing war over diplomacy increase danger for u elizabeth shackelford choosing war over diplomacy increase danger for u elizabeth shackelford how george washington america reluctant leader contrast with today frederic j fransen choosing war over diplomacy increase danger for u elizabeth shackelford how george washington america reluctant leader contrast with today frederic j fransen choosing war over diplomacy increase danger for u elizabeth shackelford choosing war over diplomacy increase danger for u elizabeth shackelford how george washington america reluctant leader contrast with today frederic j fransen how george washington america reluctant leader contrast with today frederic j fransen how george washington america reluctant leader contrast with today frederic j fransen choosing war over diplomacy increase danger for u elizabeth shackelford choosing war over diplomacy increase danger for u elizabeth shackelford how george washington america reluctant leader contrast with today frederic j fransen choosing war over diplomacy increase danger for u elizabeth shackelford choosing war over diplomacy increase danger for u elizabeth shackelford choosing war over diplomacy increase danger for u elizabeth shackelford how george washington america reluctant leader contrast with today frederic j fransen how george washington america reluctant leader contrast with today frederic j fransen how george washington america reluctant leader contrast with today frederic j fransen how can azerbaijan be ally with iran and israel nova ukraine earns platinum seal of transparency from candid ukraine kill one of the highestranking russian officer of the conflict federal budget megabill would shift billion in cost to missouri taxpayer ups violates teamster national contract with plan for buyout chile cut up to of red tape promise streamlined mining approval colorado education leader urge trump to release million in k school funding capitol walkway backed by gov polis is a bridge to nowhere key lawmaker say a project face criticism colorado education leader urge trump to release million in k school funding capitol walkway backed by gov polis is a bridge to nowhere key lawmaker say a project face criticism colorado education leader urge trump to release million in k school funding colorado education leader urge trump to release million in k school funding opinion pb is a national treasure worthy of government support the best american express credit card for picked by a frequent traveler trump cut are squeezing america most popular national park in peak season here what mental health study should look like at a christian college steven eng a christian crisis across our nation and in our backyard the united state just cut off key defense aid to ukraine</t>
+          <t>halftime show icon take big fall get injured during wnba commissioner cup championship after paying u tariff on it product busy baby look to europe and australia a future market dan ives urge apple to make a move saying that perplexity acquisition is a nobrainer it a matter of when and not if centene stock plummet what sparked the brutal selloff centene stock plummet what sparked the brutal selloff barrons iran president approves law suspending cooperation with un nuclear watchdog invivyd and leading researcher form spear spike protein elimination and recovery study group first horizon corporation announces redemption of series b preferred stock and corresponding series b depositary share new study reveals brutal hit that u employer face from trump tariff huffpost fortnite how to get the battle bus suv try this trick wildfire kill people in spain a part of europe bake in heat wave think you missed the ai rally these gridbacked play are just getting warmed up tech billionaire launch erebor bank to fill svbs gap invivyd and leading researcher form spear spike protein elimination and recovery study group to assess the effect of monoclonal antibody therapy for long covid and covid postvaccination syndrome diversified energy promotes michael garrett to chief accounting officer diversified energy promotes michael garrett to chief accounting officer uk investor see not one but two pathway to rail merger developer acquire land for westgate village at north congress avenue west palm beach florida argon ai raise m to build the ai workspace powering the future of life science nationsbenefits integrates with dollar general to enable greater access to healthy food and wellness essential for million of healthcare consumer nationwide nationsbenefits integrates with dollar general to enable greater access to healthy food and wellness essential for million of healthcare consumer nationwide trump to cut protection for home health aide migrant farmworkers is atlantic hurricane season behind schedule here whats really going on a striking trend after texas banned abortion more woman nearly bled to death during miscarriage america tariffdriven buying spree leaf household saddled with debt and financially vulnerable elon musk want to create a new political party building rocket may be easier ge aerospace bear put spread could return in the next few month the humn etf let you invest in humanoid robotics stock should you buy in now the humn etf let you invest in humanoid robotics stock should you buy in now ge aerospace bear put spread could return in the next few month mortgage refinance demand surge a interest rate drop further cnbc u of m health care consulting fee adding up at rate of to per hour mortgage refinance demand surge a interest rate drop further certik hackd fortress building product accelerates fencing and steel framing growth strategy divests railing and lighting business to primesource brand inventus sign milling agreement with mcewen mining alta equipment group announces preferred stock dividend erdene commences trading on the otcqb riley permian announces closing of new mexico acquisition tonix pharmaceutical announces peerreviewed publication in cancer cell journal highlighting positive preclinical data of mtnx in gastric cancer animal model have an allamerican fourth of july with beef on the grill greystone logistics share information on stock buyback this is the key to building a personal brand that resonates with others olipops latest marketing stunt drew a person waitlistand sold out immediately alta equipment group announces preferred stock dividend pasinex announces annual and q financial result green thumb industry to hold second quarter earnings conference call on august whitestone reit announces second quarter earnings webcast and conference call the bestperforming sp stock of the last year have key commonality other than being ai stock can you guess it whitestone reit announces second quarter earnings webcast and conference call cipher mining surpasses hashrate growth forecast at black pearl and announces june operational update inventus sign milling agreement with mcewen mining riley permian announces closing of new mexico acquisition amc network announces early result and upsizing of tender offer for it senior note due amc network announces early result and upsizing of tender offer for it senior note due cardano price prediction ada price struggle to surpass a newcomer remittix gain ground with ico surge the bestperforming sp stock of the last year have key commonality other than being ai stock can you guess it token crypto presale go live price prediction x potential and what early buyer need to know now is bitcoin getting ready for a big price move in july water way technology enters strategic partnership for exclusive tomato hybrid development for vertical farming editorial stop the bleeding for colorado medicaid paramount resource ltd announces renewal of normal course issuer bid and july dividend pyrogenesis sign contract targeting plastic waste management problem in europe mda space completes acquisition of satixfy communication cipher mining surpasses hashrate growth forecast at black pearl and announces june operational update valore report result from successful hole trado auger drilling campaign at pedra branca including m at gt pgeau from surface dr phone fix expands partnership with assurant to accelerate certified preowned phone sale across canada what are the best vanguard etf for a wellrounded portfolio first horizon corporation announces redemption of series b preferred stock and corresponding series b depositary share what are the best vanguard etf for a wellrounded portfolio wallbridge exploration drilling continues to intercept highgrade gold mineralization at martiniere consumertech brand nothing tap cevas realspace software to bring immersive spatial audio to headphone and earbuds primesource brand acquires fortress railing product shattuck lab announces participation in upcoming leerink partner therapeutic forum ii and metabolism pyrogenesis sign contract targeting plastic waste management problem in europe dayforce empowers canadian small and midsized business with powerpay by dayforce identiv partner with narravero to accelerate digital product passport adoption and compliance blue sky uranium acquires key subsurface data for corcovo uranium project mendoza province argentina verkkokauppacom to publish januaryjune halfyear report on july crypto loss surpass billion in h certik report reveals alarming rise in phishing attack blue sky uranium acquires key subsurface data for corcovo uranium project mendoza province argentina main street announces followon portfolio investment paramount global and donald trump settle for million inside america department store tarifftriggered price hike are picking up robeco institutional asset management bv ha million position in dollar general corporation nysedg after trump warns elon musk to close up shop china rally behind world richest man there no need to keep putting up with it year old grocery store staple file for bankruptcy northisle announces near surface intercept and highergrade intercept at depth at west goodspeed on it north island project stock market news dow set to open higher after senate pass spending bill barrons meeka metal begin gold production at murchison project australia seeking stable passive income in crypto quid miner offer a sustainable new cloud mining solution democrat the last holdout bear could be the key to a new stockmarket rally marketwatch smart gas meter market worth billion by marketsandmarketstm yieldmax etf announces distribution on smcy ulty msty wntr lfgy and others yieldmax etf announces distribution on smcy ulty msty wntr lfgy and others aldi is selling a comfort sandal for just it a perfect oofos dupe but cheaper kkr bet on sustainable protein demand with proten investment in australia kitron receive eur million contract for defense airborne radar application northern trust q earnings what to expect northern trust q earnings what to expect murkowski got to yes on t megabill thanks to spending for alaska how the megabill will limit health care access and plan to ease gun regulation iran president approves law suspending cooperation with un nuclear watchdog new study reveals brutal hit that u employer face from trump tariff another one bite the dust cbs settle with trump over infamous kamala minute segment letter to the editor a plea to boulder earbud hiker no excuse for not repaying student loan guthrie song is a relevant a ever guest opinion stuart c lord education wa my way out this bill slam that door shut house republican race toward a final vote on trump tax bill daring critic to oppose guest opinion christopher schweitzer the siren song of unreason is a dangerous plunge into darkness hollywood lost the plot now rebel are making movie great again what the rd budget proposal say about the future of war is atlantic hurricane season behind schedule here whats really going on trump immigration crackdown ripple through economy a striking trend after texas banned abortion more woman nearly bled to death during miscarriage america tariffdriven buying spree leaf household saddled with debt and financially vulnerable elon musk want to create a new political party building rocket may be easier politician push jobkilling minimum wage hike while ignoring the devastating economic reality editorial attacking zohran mamdanis u citizenship is contemptible and dangerous republican rep jim jordan discusses trumpbacked megabill after senate passage rash kid have been abducted from ukraine these midwest senator want to find them a welcome shift in federal financial reporting wednesday letter sen budd where is your courage where is your honesty grow keep an eye out for brown patch disease in coolseason grass american opinion instead of ice raid on farmworkers overhaul this visa program cytosorbents provides u fda and health canada regulatory update for drugsorbatr best of the babylon bee defeated cuomo left groping for answer berry tramel rising valuation of nba franchise will prompt thunder ownership to sell opinion minneapolis police chief brian ohara is getting a bum rap over lake street raid year old grocery store staple file for bankruptcy democratic gov janet mill discusses how the gop megabill will impact maine maine cant afford to lose federal funding governor say modestly bipartisan budget could go to full wisconsin legislature wednesday gop megabill head back to the house for final approval u wont send some weapon pledged to ukraine following a pentagon review of military aid what the mar elia church bombing mean for syria future artificial intelligence saving you money and helping massdot build faster republican holdout head to the white house to discus trump bill letter patriot not saying much on ice treatment of veteran opinion a july approach supreme court sign away american democracy trump put senate in play in wall street journal new jersey gubernatorial candidate to speak at made in nj manufacturing day trump put senate in play in wall street journal nelly denies he maga say kamala harris locked up black ha white husband trump put senate in play in wall street journal trump put senate in play in wall street journal trump put senate in play in wall street journal trump put senate in play in wall street journal trump put senate in play in wall street journal trump put senate in play in wall street journal lawrence odonnells unfiltered reaction to bonkers trump presser moment say it all how ai can help ease the strain on health care service man charged in deadly brockton stabbing pleads not guilty house republican race toward a final vote on trump tax bill sen ron johnson a yes on trump budget bill sen tammy baldwin disgusted by it holy cow history happy july whatever green bay prison would close by under republican budget proposal gen z is the worst at work right wrong thing to know for july usaid ukraine munition trump megabill climate change paramount settlement former insurance commissioner say lara should go california focus former insurance commissioner say lara should go california focus letter spending choice make republican leader priority clear incredible growth stock poised for longterm gain win an ar old state saloon present conspiracy theory trivia and salooncast with ian carroll a twonight blast of truth tech and patriotism analysis show trump tariff would cost u employer billion if elon stick to rocket i will stick to finance bessent shrug off musk debt drama lancashire need to set investment priority to get biggest bang for buck can south korea deescalate north korea without u support how to be editor for a day notorious husband and wife professional tenant indicted on criminal charge we will not let hate win provincetown town manager say following second incident protect your pet on the fourth of july editor for a day letter constitutional system seems abandoned the u military cant quit the middle east another voice financial restitution is necessary but not sufficient for abuse survivor letter war against diversity education in unjust and disrespect history sean diddy comb found guilty on count acquitted of most serious charge firework warehouse explodes in california dalai lama say he intends to reincarnate after death ukraine look to jointly produce weapon with ally while u halt some shipment honolulu board of water supply sue navy for b over red hill fuel leak governor state budget veto trim public school maintenance new hawaii firework law take effect today hooser walking through my thought and value federal climate website go dark a trump administration promise policy reset house gop leader scrambling to rally holdout behind trump megabill house gop leader scrambling to rally holdout behind trump megabill house gop leader scrambling to rally holdout behind trump megabill house gop leader scrambling to rally holdout behind trump megabill house gop leader scrambling to rally holdout behind trump megabill house gop leader scrambling to rally holdout behind trump megabill leore james kowarsch liz shulman will big tech transform school into an ai video game jerald mcnair doe student use of ai spell the end for homework trump lit a fire under nato but more need to be done to contain the russiachina axis north korea to send a many a troop to bolster russia force ukrainian official say trump pick to run federal watchdog a yearold who once shared a conspiracy video and ha tie to a holocaust denier letter keep an eye on what matter not just what seems exciting editorial financial hit keep on coming and city hall only response is excuse steve chapman congress and the supreme court approve donald trump drive for absolute power letter why centrism doesnt have enough bite to make an impact</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>employer added surprising job month uncertainty economic policy canada trade deficit narrow export drop millionaire renter surge nyc high earner opt luxury lease report trader pare bet fed rate cut job report lindsell train global equity fund nintendo co ltd ntdoy stock market dow sp nasdaq future advance strong payroll data trump tax spending bill face vote marketwatch new online casino canada reddit user share leading real money online casino tcl csot exclusively supply display xiaomi mix flip xiaomi yu powering xiaomis new beginning blowout payroll k job added smashing expectation unemployment rate drop avdx alert monsey firm wohl fruchter investigating fairness sale avidxchange tpg global corpay dune awakening drop massive update fix exploit rebalances pvp zone clearmind medicine announces irb approval phase clinical trial alcohol disorder tel aviv sourasky medical center stock bond market open eve close early trump world squeeze china starting vietnam application jobless aid fell layoff low application jobless aid fell layoff low application jobless aid fell layoff low application jobless aid fell layoff low application jobless aid fell layoff low application jobless aid fell layoff low application jobless aid fell layoff low trader pare bet fed rate cut job report yahoo finance application jobless aid fell layoff low application jobless aid fell layoff low application jobless aid fell layoff low application jobless aid fell layoff low parazero receives recurring bulk order safeair system australian distributor nyt strand serf sweet scoop icecream spangram half yearly report lvmhs liquidity contract oddo bhf sca half yearly report lvmhs liquidity contract oddo bhf sca fossil fuel stock rallied senate passed trump tax spending plan deep tristate layoff continuing jobless claim stuck highest since canada trade deficit narrow export rise fossil fuel stock rallied senate passed trump tax spending plan investor business ford jpmorgan amazon executive predict deep job cut ai advance weekly firsttime unemployment claim fewest since business application jobless aid fell layoff low application jobless aid fell layoff low review liquid death fire plus unique thc drink yet hog look close ahead holiday break cotton mixed early thursday trade corn pushing gain thursday morning trade cattle look round short wheat sneaking gain ahead threeday weekend soybean strength continuing thursday financial stock dump quarter house beat hidden venue new sound emerging abu dhabi employer added surprising job month uncertainty economic policy employer added surprising job month uncertainty economic policy starbucks offer million stock bonus exec buy share technical analysis fed rate cut less likely strongerthanforecast payroll data green science alliance established electric vehicle ev company utilizing next generation inwheel technology developed japanese engineer pioneered supercar ev named eliica ago economy add new job unemployment rate dip percent stock market dow sp nasdaq future hit pause solid job report liveone synervoz partner nextgen voice experience employer added job strategy stock rise trading signal jobless claim fall lowest level since midmay sp build record high future rising strong job report barrons parent gifted economy add job expected popular restaurant chain close location bankruptcy application jobless aid fell layoff low application jobless aid fell layoff low application jobless aid fell layoff low trade deficit widens surpassing forecast previous figure job growth beat expectation celebrate independence wilmatm set aba practice free manual powerful patient relationship nike race billionaire bill ackman urge tired subdued andrew cuomo drop nyc mayoral race begrudgingly endorses eric adam payroll increased expected navitas semiconductor participate upcoming cjs security conference add k job beating expectation initial jobless claim dip expectation bolstering usd employer added job labor market resilience uncertainty trump economic policy employer added job labor market resilience uncertainty trump economic policy labor market stay afloat hiring forecastsagain employer added job labor market resilience uncertainty trump economic policy airline face investor strong cheaper holiday cnbc lamplight luxury rv park invite traveler discover perfect texas getaway holiday road rv park dsh hotel advisor close jacksonville fl candlewood suite sale hospitality market heat lamplight luxury rv park invite traveler discover perfect texas getaway holiday road rv park navitas semiconductor participate upcoming cjs security conference dsh hotel advisor close jacksonville fl candlewood suite sale hospitality market heat nonfarm payroll beat expectation indicating robust job market coinex research report bitcoin crossfire payroll increased expected cnbc etoro appoints sec commissioner laura unger wix cfo lior shemesh board beauty bear michael burry estee snub china smci stock price target bump share price agf announces passing kevin mccreadie ceo cio coreweave cloud provider deploy nvidias latest ai chip kelly slater moved sustainable clothing brand la san diego kelly slater moved sustainable clothing brand la san diego kelly slater moved sustainable clothing brand la san diego kelly slater moved sustainable clothing brand la san diego kelly slater moved sustainable clothing brand la san diego kelly slater moved sustainable clothing brand la san diego kelly slater moved sustainable clothing brand la san diego california democrat require agent unmask id trump america wont tolerate nuclear threat james fitzpatrick trump america wont tolerate nuclear threat james fitzpatrick texas internet porn constitutional common sense prevails dallas morning texas internet porn constitutional common sense prevails dallas morning texas internet porn constitutional common sense prevails dallas morning trump america wont tolerate nuclear threat james fitzpatrick trump america wont tolerate nuclear threat james fitzpatrick texas internet porn constitutional common sense prevails dallas morning trump america wont tolerate nuclear threat james fitzpatrick texas internet porn constitutional common sense prevails dallas morning texas internet porn constitutional common sense prevails dallas morning trump america wont tolerate nuclear threat james fitzpatrick texas internet porn constitutional common sense prevails dallas morning texas internet porn constitutional common sense prevails dallas morning texas internet porn constitutional common sense prevails dallas morning trump america wont tolerate nuclear threat james fitzpatrick trump america wont tolerate nuclear threat james fitzpatrick trump america wont tolerate nuclear threat james fitzpatrick texas internet porn constitutional common sense prevails dallas morning congressional intern killed dc shooting scrum alliance ranked comparablys list best leadership team among small company judge strike trump policy deleted transgender page govt website house beat hidden venue new sound emerging abu dhabi federal judge rule noncalifornia resident apply concealedcarry gun permit latest house rush final vote democrat floor maga american application jobless aid fell layoff low application jobless aid fell layoff low aclu sue block raid southern california alleging constitutional violation employer added job labor market resilience uncertainty trump economic policy employer added job labor market resilience uncertainty trump economic policy california boost film tv tax credit million preserve job attorney general tap politically connected billing lawyer judicial discipline panel dnrcs drought outlook montana grim hot dry summer attorney general tap politically connected billing lawyer judicial discipline panel attorney general tap politically connected billing lawyer judicial discipline panel double pentagon spread false ufo story skeptical trump megabill set house record longest vote history megarounds drop half biotech struggle worsening slump california school video immigration agent urinating public view homeland security investigating iran suspends cooperation un nuclear monitoring agency slider milestone heartfelt kershaws strikeout federal funding contraceptive access missouri nonprofit threemonth freeze dan walter california lawmaker finally achieve holy grail reform environmental jeffries u magic delay vote trump megabill settling trump cbs staffer fear come next education grant limbo used leftwing agenda trump administration education grant limbo used leftwing agenda trump administration education grant limbo used leftwing agenda trump administration education grant limbo used leftwing agenda trump administration education grant limbo used leftwing agenda trump administration education grant limbo used leftwing agenda trump administration education grant limbo used leftwing agenda trump administration education grant limbo used leftwing agenda trump administration education grant limbo used leftwing agenda trump administration education grant limbo used leftwing agenda trump administration education grant limbo used leftwing agenda trump administration family slain police officer krystal rivera shot fellow officer independent investigation vance boelter man charged minnesota lawmaker shooting due federal george washington america reluctant contrast frederic j fransen choosing war diplomacy increase danger elizabeth shackelford choosing war diplomacy increase danger elizabeth shackelford choosing war diplomacy increase danger elizabeth shackelford george washington america reluctant contrast frederic j fransen choosing war diplomacy increase danger elizabeth shackelford george washington america reluctant contrast frederic j fransen choosing war diplomacy increase danger elizabeth shackelford choosing war diplomacy increase danger elizabeth shackelford george washington america reluctant contrast frederic j fransen george washington america reluctant contrast frederic j fransen george washington america reluctant contrast frederic j fransen choosing war diplomacy increase danger elizabeth shackelford choosing war diplomacy increase danger elizabeth shackelford george washington america reluctant contrast frederic j fransen choosing war diplomacy increase danger elizabeth shackelford choosing war diplomacy increase danger elizabeth shackelford choosing war diplomacy increase danger elizabeth shackelford george washington america reluctant contrast frederic j fransen george washington america reluctant contrast frederic j fransen george washington america reluctant contrast frederic j fransen azerbaijan ally iran israel nova ukraine earns platinum seal transparency candid ukraine kill highestranking russian officer conflict federal budget megabill shift billion cost missouri taxpayer ups violates teamster national contract plan buyout chile cut red tape promise streamlined mining approval colorado education urge trump release million k school funding capitol walkway backed gov polis bridge nowhere lawmaker project face criticism colorado education urge trump release million k school funding capitol walkway backed gov polis bridge nowhere lawmaker project face criticism colorado education urge trump release million k school funding colorado education urge trump release million k school funding opinion pb national treasure worthy government support best american express credit card picked frequent traveler trump cut squeezing america popular national park peak season mental health study look christian college steven eng christian crisis across nation backyard united cut defense aid ukraine</t>
+          <t>halftime icon take fall injured wnba commissioner cup championship paying tariff product busy baby look europe australia future market dan ives urge apple move saying perplexity acquisition nobrainer matter centene stock plummet sparked brutal selloff centene stock plummet sparked brutal selloff barrons iran president approves suspending cooperation un nuclear watchdog invivyd leading researcher form spear spike protein elimination recovery study horizon corporation announces redemption series b preferred stock corresponding series b depositary study reveals brutal hit employer face trump tariff huffpost fortnite battle bus suv try trick wildfire kill people spain part europe bake heat wave missed ai rally gridbacked play getting warmed tech billionaire launch erebor bank fill svbs gap invivyd leading researcher form spear spike protein elimination recovery study assess effect monoclonal antibody therapy covid covid postvaccination syndrome diversified energy promotes michael garrett chief accounting officer diversified energy promotes michael garrett chief accounting officer uk investor pathway rail merger developer acquire land westgate village north congress avenue west palm beach florida argon ai raise build ai workspace powering future life science nationsbenefits integrates dollar general enable greater access healthy wellness essential million healthcare consumer nationwide nationsbenefits integrates dollar general enable greater access healthy wellness essential million healthcare consumer nationwide trump cut protection health aide migrant farmworkers atlantic hurricane season behind schedule whats striking trend texas banned abortion woman nearly bled death miscarriage america tariffdriven buying spree leaf household saddled debt financially vulnerable elon musk create political party building rocket easier ge aerospace bear put spread next month humn invest humanoid robotics stock buy humn invest humanoid robotics stock buy ge aerospace bear put spread next month mortgage refinance demand surge interest rate drop cnbc health care consulting fee adding rate per hour mortgage refinance demand surge interest rate drop certik hackd fortress building product accelerates fencing steel framing growth strategy divests railing lighting business primesource brand inventus sign milling agreement mcewen mining alta equipment announces preferred stock dividend erdene commences trading otcqb riley permian announces closing mexico acquisition tonix pharmaceutical announces peerreviewed publication cancer cell journal highlighting positive preclinical data mtnx gastric cancer animal model allamerican fourth beef grill greystone logistics information stock buyback building personal brand resonates others olipops latest marketing stunt drew waitlistand immediately alta equipment announces preferred stock dividend pasinex announces annual q financial green thumb industry quarter earnings conference call august whitestone reit announces quarter earnings webcast conference call bestperforming sp stock commonality ai stock guess whitestone reit announces quarter earnings webcast conference call cipher mining surpasses hashrate growth forecast black pearl announces operational update inventus sign milling agreement mcewen mining riley permian announces closing mexico acquisition amc network announces early upsizing tender offer senior note due amc network announces early upsizing tender offer senior note due cardano price prediction ada price struggle surpass newcomer remittix gain ground ico surge bestperforming sp stock commonality ai stock guess token crypto presale price prediction x potential early buyer bitcoin getting ready price move water technology enters strategic partnership exclusive tomato hybrid development vertical farming editorial stop bleeding colorado medicaid paramount resource ltd announces renewal normal course issuer bid dividend pyrogenesis sign contract targeting plastic waste problem europe mda space completes acquisition satixfy communication cipher mining surpasses hashrate growth forecast black pearl announces operational update valore report successful hole trado auger drilling campaign pedra branca gt pgeau surface dr phone fix expands partnership assurant accelerate certified preowned phone sale across canada best vanguard wellrounded portfolio horizon corporation announces redemption series b preferred stock corresponding series b depositary best vanguard wellrounded portfolio wallbridge exploration drilling continues intercept highgrade gold mineralization martiniere consumertech brand nothing tap cevas realspace software immersive spatial audio headphone earbuds primesource brand acquires fortress railing product shattuck lab announces participation upcoming leerink partner therapeutic forum ii metabolism pyrogenesis sign contract targeting plastic waste problem europe dayforce empowers canadian small midsized business powerpay dayforce identiv partner narravero accelerate digital product passport adoption compliance blue sky uranium acquires subsurface data corcovo uranium project mendoza province argentina verkkokauppacom publish januaryjune halfyear report crypto loss surpass billion h certik report reveals alarming rise phishing attack blue sky uranium acquires subsurface data corcovo uranium project mendoza province argentina main street announces followon portfolio investment paramount global donald trump settle million inside america department store tarifftriggered price hike picking robeco institutional asset bv million dollar general corporation nysedg trump warns elon musk close shop china rally behind world richest man putting old grocery store staple file bankruptcy northisle announces near surface intercept highergrade intercept depth west goodspeed north island project stock market dow set open higher senate pas spending bill barrons meeka metal begin gold production murchison project australia seeking stable passive income crypto quid miner offer sustainable cloud mining solution democrat holdout bear stockmarket rally marketwatch smart gas meter market worth billion marketsandmarketstm yieldmax announces distribution smcy ulty msty wntr lfgy others yieldmax announces distribution smcy ulty msty wntr lfgy others aldi selling comfort sandal perfect oofos dupe cheaper kkr bet sustainable protein demand proten investment australia kitron receive eur million contract defense airborne radar application northern trust q earnings expect northern trust q earnings expect murkowski got yes megabill spending alaska megabill limit health care access plan ease gun regulation iran president approves suspending cooperation un nuclear watchdog study reveals brutal hit employer face trump tariff another bite dust cbs settle trump infamous kamala segment editor plea boulder earbud hiker excuse repaying student loan guthrie song relevant ever guest opinion stuart c lord education bill slam door shut house republican race final vote trump tax bill daring critic oppose guest opinion christopher schweitzer siren song unreason dangerous plunge darkness hollywood plot rebel making movie great rd budget proposal future war atlantic hurricane season behind schedule whats trump immigration crackdown ripple economy striking trend texas banned abortion woman nearly bled death miscarriage america tariffdriven buying spree leaf household saddled debt financially vulnerable elon musk create political party building rocket easier politician push jobkilling minimum wage hike ignoring devastating economic reality editorial attacking zohran mamdanis citizenship contemptible dangerous republican rep jim jordan discusses trumpbacked megabill senate passage rash kid abducted ukraine midwest senator find welcome shift federal financial reporting wednesday sen budd courage honesty grow eye brown patch disease coolseason grass american opinion instead raid farmworkers overhaul visa program cytosorbents provides fda health canada regulatory update drugsorbatr best babylon bee defeated cuomo left groping answer berry tramel rising valuation nba franchise prompt thunder ownership sell opinion minneapolis police chief brian ohara getting bum rap lake street raid old grocery store staple file bankruptcy democratic gov janet mill discusses gop megabill impact maine maine cant afford lose federal funding governor modestly bipartisan budget full wisconsin legislature wednesday gop megabill head house final approval wont send weapon pledged ukraine following pentagon review military aid mar elia church bombing syria future artificial intelligence saving money helping massdot build faster republican holdout head white house discus trump bill patriot saying treatment veteran opinion approach supreme sign away american democracy trump put senate play wall street journal jersey gubernatorial candidate speak nj manufacturing trump put senate play wall street journal nelly denies maga kamala harris locked black white husband trump put senate play wall street journal trump put senate play wall street journal trump put senate play wall street journal trump put senate play wall street journal trump put senate play wall street journal trump put senate play wall street journal lawrence odonnells unfiltered reaction bonkers trump presser moment ai help ease strain health care service man charged deadly brockton stabbing pleads guilty house republican race final vote trump tax bill sen ron johnson yes trump budget bill sen tammy baldwin disgusted holy cow history happy whatever green bay prison close republican budget proposal gen z worst work usaid ukraine munition trump megabill climate change paramount settlement insurance commissioner lara california focus insurance commissioner lara california focus spending choice republican priority incredible growth stock poised longterm gain ar old saloon present conspiracy theory trivia salooncast ian carroll twonight blast truth tech patriotism analysis trump tariff cost employer billion elon stick rocket stick finance bessent shrug musk debt drama lancashire set investment priority biggest bang buck south korea deescalate north korea without support editor notorious husband wife professional tenant indicted criminal charge hate provincetown town manager following incident protect pet fourth editor constitutional system seems abandoned military cant quit middle east another voice financial restitution necessary sufficient abuse survivor war diversity education unjust disrespect history sean diddy comb found guilty count acquitted serious charge firework warehouse explodes california dalai lama intends reincarnate death ukraine look jointly produce weapon ally halt shipment honolulu board water supply sue navy b red hill fuel leak governor budget veto trim public school maintenance hawaii firework take effect hooser walking thought value federal climate website dark trump administration promise policy reset house gop scrambling rally holdout behind trump megabill house gop scrambling rally holdout behind trump megabill house gop scrambling rally holdout behind trump megabill house gop scrambling rally holdout behind trump megabill house gop scrambling rally holdout behind trump megabill house gop scrambling rally holdout behind trump megabill leore james kowarsch liz shulman tech transform school ai video game jerald mcnair doe student ai spell end homework trump lit fire nato contain russiachina axis north korea send troop bolster russia force ukrainian trump pick run federal watchdog yearold shared conspiracy video tie holocaust denier eye matter seems exciting editorial financial hit coming hall response excuse steve chapman congress supreme approve donald trump drive absolute power centrism doesnt enough bite impact</t>
         </is>
       </c>
     </row>
@@ -766,12 +762,12 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>stock to buy with less than nordstrom rack is selling a gorgeous kendra scott necklace for and shopper get so many compliment openai ceo sam altman say he politically homeless in july post bashing democrat what to expect from boston scientifics next quarterly earnings report buttonwood financial advisor inc ha million holding in meta platform inc nasdaqmeta crown wealth group llc buy share of meta platform inc nasdaqmeta bankplus wealth management llc grows position in meta platform inc nasdaqmeta shilanski associate inc raise holding in meta platform inc nasdaqmeta amalgamated bank acquires share of meta platform inc nasdaqmeta monument capital management buy share of meta platform inc nasdaqmeta best car insurance company of july risk remains of uschina trade truce breakdown capital economics say ups make drastic change it never done before in year history a part of major overhaul the secret to great grilled kabob it all in the cut prediction this magnificent artificial intelligence ai stock will skyrocket to new high in july bitcoin price on the brink a congress introduces a new groundbreaking crypto bill forbes veraltos quarterly earnings preview what you need to know oppo pad se india launch check variant spec price breakdown sofi stock skyrocket in a year how high can it go in consolidated lithium metal announces exposure of a new libearing pegmatite at it preissac project and close financing bmo announces special cash distribution for etf series unit of bmo money market fund consolidated lithium metal announces exposure of a new libearing pegmatite at it preissac project and close financing niurstour i utboi rikisbrefa riks is trader joes open on the th of july best podcast headphone of auction result of treasury bond riks rtx corporation q earnings what to expect how to fix lenovo fingerprint scanner issue fast quick easy guide what to expect from dover q earnings report what you need to know ahead of erie indemnity earnings release petrovictory energy corp and azevedo travassos energia sa sign binding memorandum of understanding petrovictory energy corp and azevedo travassos energia sa sign binding memorandum of understanding sakana ai treequest deploy multimodel team that outperform individual llm by sony break exclusivity helldivers land on xbox this august tesla ha a problem and it not just the elon musk backlash bloombergcom eu stick with timeline for ai rule reuters lot of speculation is swirling around the sumy front wildfire cripple alberta oil production this is why tesla robotaxi launch needed human babysitter what to expect from raymond james financials q earnings report which store are open and closed on independence day kusacom btc hit k why pro trader arent fully confident yet the fiscal treadmill is speeding up and washington keep jogging after year of grinding i have million but am burned out what are my option these catalyst could lift micron stock higher in and beyond costco stock analysis buy sell or hold every breath you take affect how you move here how to fix both my smartest dividend stock to buy today earnings preview what to expect from globe life report here what to expect from ameriprise financials next earnings report key headwind facing usdc cme group quarterly earnings preview what you need to know is subway open on the fourth of july west fargo new herbz and spicez store offer customer allnatural alternative be resilient by accepting adversity and learning from it why black unemployment just rose to it highest level since january littleknown item in trump big agenda bill riley gaines ha been one of lia thomas most vocal critic she just scored two major win in her antitrans effort who the coolest person at your july barbecue they got six thing goin on according to a new study construction start on beacon at princeton hill at s dixie hwy homestead fl i visited universal studio and people were on their phone everywhereeven rollercoasters that habit is really hard to break expert say company in the new york city metro area that are great place to work the strategy that will make your sale call more successful editorial today we celebrate the real no king holiday how glen powell condiment brand made more than million in it first month azi announces receipt of minimum bid price notice from nasdaq fourth of july weekend lotterycom and sportscom driver revved up for midohio challenge stoneform launch a tokenized real estate platform to open up investment opportunity northwest copper announces closing of oversubscribed private placement bybit tradfi x crypto report regulatory tailwind drive coinbase outperformance despite premium valuation stoneform launch a tokenized real estate platform to open up investment opportunity esg hitgen release it inaugural sustainability report is chickfila closed on july northwest copper announces closing of oversubscribed private placement china using tiktok a a pawn to squeeze trump in trade talk source net zero now clear key milestone on acre energy campus accelerating alberta lowcarbon data center infrastructure build out whats open whats closed on july th what grocery store are open walmart costco target more alcom u future slide after trump say hell start sending tariff letter today setting levy up to musk back sen paul criticism of trump megabill in first comment since it passed cf cfrp market worth billion in exclusive report by marketsandmarketstm cf cfrp market worth billion in exclusive report by marketsandmarketstm trump vietnam pact take aim at china but it raise more question than answer cnbc new york state teacher retirement system sell share of avery dennison corporation nyseavy ameritas advisory service llc buy share of ulta beauty inc nasdaqulta these were the bestperforming stock in the dow jones industrial average in june hot dog eating contest host share prediction for this year winner partner value investment lp announces tenforone unit split xrp and ozak ai price prediction which token ha the clearer path to massive gain american flight diverts after nosy passenger cause bomb scare one mile at a time trump bill secures billion for u arctic surge six new icebreaker to counter russian and chinese dominance ethereum is powering wall street future the crypto scene at cannes show how far it come apex group appoints wang a chief ai and data science officer kinterra score small win in new world copper takeover fight new york state teacher retirement system reduces position in oge energy corporation nyseoge u patriotism among democrat crash a marxist demand grow louder birdie for charity in the final stretch to reach m milestone what oracle meta platform and nvidia stock investor should know about recent ai update amber international raise m to enhance m crypto ecosystem reserve best horror game that test your morality marsden launch workplace saving with charity pledge for first business in today gop there is no choice at all multiple suspect charged in separate drug dealing case in billing the secret to great grilled kabob it all in the cut is central asia the next target of russian aggression opinion congress making big mistake with energy tax credit what the justice department push to bring denaturalization case mean what the justice department push to bring denaturalization case mean what the justice department push to bring denaturalization case mean what the justice department push to bring denaturalization case mean what the justice department push to bring denaturalization case mean what the justice department push to bring denaturalization case mean what the justice department push to bring denaturalization case mean what the justice department push to bring denaturalization case mean the house just did our patriotic duty to deliver tax relief and uphold our value what the justice department push to bring denaturalization case mean what the justice department push to bring denaturalization case mean controversy a staggering amount of usmexico border is now militarized what is trump new realism in foreign policy to celebrate july fully consider the context of the declaration of independence selfevident truth every breath you take affect how you move here how to fix both my smartest dividend stock to buy today army experiment with integrating attack drone into artillery formation trump admin to adjust national park fee to prioritize american family over foreign tourist flooding in texas cause multiple fatality a guadalupe river surge to record level jocko willink in a sea of imperfect voice i heard the anthem and the spirit of a nation this july th a family wait american hostage father pleads for son freedom from hamas terrorist opinion bill lueders reason to celebrate july th why black unemployment just rose to it highest level since january littleknown item in trump big agenda bill riley gaines ha been one of lia thomas most vocal critic she just scored two major win in her antitrans effort guest opinion bj and brecken jones u supreme court got it right on parental right and education who the coolest person at your july barbecue they got six thing goin on according to a new study trump ha big plan for america next birthday historian have question trump to sign big beautiful bill in july fourth ceremony at white house editorial after year righteousness and truth must prevail letter to the editor county should be compensated for iris field honoring superintendent extraordinary service trump crowning moment is ammo for dems in america nonstop birthday party watt happening tonis weekly energy highlight hot dog eating contest host share prediction for this year winner opinion supreme court unitary executive theory threatens our balance of power trump concedes he made no progress on achieving top campaign promise democratic rep katherine clark discusses gop megabill heading for trump signature president trump take victory lap after congress pass tax cut and policy bill elote churrasco and churros alligator alcatraz worker fed by miami food truck scientist issue warning after detecting concerning surge in infection in domestic cat should be closely monitored chef who feed penn state student make summer shift helping family with meal are the worst of the storm behind u hateful trump trashed over fking disgusting line about half the country for th of july the allamerican director you dont know by name katy perry and orlando bloom confirm split what we know about the death of liverpool soccer star diogo jota and his brother la activist indicted after handing out face shield to antiice protester president trump to honor iran strike flight team at the white house glenn eden who is chicago greatest ambassador you editorial on july of all day a naturalized citizen is not less than a u citizen editorial america is soon to turn remember the warmth of the bicentennial heidi stevens on long list of thing being cut art may seem inconsequential it not zohran mamdani ha big housing plan here what stand in the way letter what july fourth mean to me a an ahmadi muslim american rep bob morgan what patriotism mean to me three year after the highland park mass shooting this artist hope to be chosen to make a sculpture for trump garden of american hero how ice raid turned part of los angeles into ghost town maggie mulqueen what doe summer mean for my family and me the beach and book a declaration of independence for these time trump pardon cost at least billion in restitution tax hike in december is helping local library raise worker wage and restore lost position ny official react to passage of big beautiful bill through congress impending signature into law who broke george washington walking stick at the sc statehouse yankee rebel an exgovernor hegseth halted weapon for ukraine despite military analysis that the aid wouldnt jeopardize u readiness legislature should act on the pernicious effect of cellphone in school trump success rate in the court so far letter budget cut harmful for health nutrition letter budget cut harmful for health nutrition think youre smarter than a slate associate writer find out with this week news quiz editorial cartoon for july world share are mostly down a trump tariff deadline loom while u stock set record trump pitch plan allowing farmer to vouch for illegal immigrant worker facing deportation blaze engulfs four home in la amid active firework a strike by air traffic controller is disrupting travel to from and over france trump ag secretary ha irony meter exploding left right and center with beyond parody spin trump decision to end taxfree loophole for lowvalue good from china lead to a sharp decline in air cargo shipment cyber school facing wrongful death suit say it unreasonable for teacher to see student weekly opinion blockbuster made me do it questionable advice from big summer movie pa republican gamble on rural health care a megabill push through cumberland county official optimistic that new memo will improve coordination with library system galasso look forward to tomorrow expectantly beyond current circumstance joey chestnut return to coney island expected to dominate hot dog eating contest trump proposes ufc fight at white house to celebrate year of independence will new england sky stay clear for friday night big firework show u colombia announce recall of envoy amid diplomatic rift lucas trump should demand the unconditional surrender of the democrat party food hygiene rating handed to four doncaster establishment one need major improvement elephant kill two female tourist from the uk and new zealand in zambian national park many missouri law restricting abortion blocked again by state judge iredell county name rodney harris a the new deputy county manager iran try keeping new military commander a secret mossad offer guessing game confirms winner atlanta clogged road bring out the rage in motorist opinion challenge opportunity and bright future in ct for dairy farming trump tear into marxist lunatic mamdani honor american hero in bold rebuke play these p plus free game in july xrp hold market confidence while lightchain ai latejuly launch prepares to broaden investor option rosen nationally regarded investor counsel encourages reckitt benckiser group plc investor to secure counsel before important deadline in security class action rbgly robinhood want to redo wall street on the blockchain gizmodo why tempus ai stock soared in june japan brace for more quake authority dismiss doomsday hype opec plus agrees to pump more oil in august the new york time trump reportedly told iran it wa ok to strike back after u attack i said go ahead i understand poland blast trumpputin dialogue after drone strike escalation walmart is selling calvin klein eternity perfume for only and shopper say it an unbeatable deal ap business summarybrief at pm edt ap business summarybrief at pm edt ap business summarybrief at pm edt ap business summarybrief at pm edt the newest stock in the sp ha soared since it ipo and it a buy right now according to wall street the newest stock in the sp ha soared since it ipo and it a buy right now according to wall street were watching a brain drain in real time openai hit hard a top researcher defect to rival tech giant meta rude baguette the best amazon prime day deal under save on gear from blink anker samsung and others engadget nextgen ai and social startup backed by thrive capital and y combinator shaping were on the brink of another big consumer wave click like sugar gambling in a world of quick pleasure an addiction expert say it might be time for a dopamine fast a amazon double down on robotaxis is amzn stock a buy charlize theron is choosing to be single she told call her daddy that can be a sign of strength say relationship expert the future of ai selfdriving car mechanical weeding health care assistant and more patriotic parade at the park the market hidden current delivering fast gain top romantic drama on ott to watch this weekend daily habit that separate high achiever from everyone else best altcoins for next bull run blockdags m summer raffle roi feature alongside inj rndr tia a forgotten megatrend that could be key to the ai economy quality nonus stock to buy in simply staggering cnn correspondent describes floodwater impact in texas good stock still worth buying in this market matt mower after nato summit europe free ride is on the line archer aviation the bet that could take off sooner than you think oneofakind brewery taproom closing no bankruptcy oneofakind brewery taproom closing no bankruptcy trump hit with backlash over use of antisemitic slur at iowa rally stage almost over arctic pablos price hike imminent a myro and housecoin push forward shopper race to get off all item in major closing down sale after iconic activewear brand shuts store investor deadline robbins geller rudman dowd llp announces that sarepta therapeutic inc srpt investor with substantial loss have opportunity to lead class action lawsuit one big beautiful budget deficit opec to increase output by barrel a day in august what it mean for oil market btc miner cloud mining platform strives to offer stability security a bitcoin recently crossed k amazon prime day the best deal live right now plus everything else you need to know engadget an iowa law rolling back trans civil right protection in the state ha taken effect here what to know thinkcarebelieve week of america victory walmart is selling a sleek digital camera for and shopper say it look professional subaru launch killer legacy lease offer for july top short anime to watch this weekend odd taxi death parade more safeway strike end a albertsons and local union reach agreement colorado public radio headed for sentencing sean diddy comb lawyer aim to show he no longer a bad boy for life the average american family is a millionaire how you can join them your kid is getting a trump account should you put your money in it unstoppable growth stock to hold for the next year big solar battery news from egypt south africa will lower mortgage rate save california housing market will lower mortgage rate save california housing market rep mark green resigns from congress leaving speaker johnson with an even narrower republican majority in the house council to vote on new fire chief monday direct payday loan lender in the u for globenewswire fbi sheriff office arrest motorcycle gang member in operation mongolian beef oasis return after year hiatus to a uk crowd ecstatic for the band s hit dave ramsey say real estate can outperform stock but warned that higer return dont come free best cryptos to buy in for longterm growth bdag hbar fil algo pipeline disruption slash ecuador output by bpd life saver lawrence general paramedic can now bring blood right at accident scene why smart founder build company that run without them an excia advisor presentation suggests u could enter postdebt era without raising taxesthanks to overlooked federal asset how to make an atsfriendly resume for free using ai tip and trick chipotle customer uncovers receipt from here how much price have changed in a decade new york post ap business summarybrief at am edt ap business summarybrief at am edt china first legoland open to visitor in shanghai opec surprise with oversized output hike jim cramer say he not going to fight joby aviation jim cramer on titan international i cant go for it jim cramer say i like domino here jim cramer say danaher can make a comeback jim cramer on centene very painful story jim cramer say he very happy with well fargo jim cramer considers morgan stanley a tremendous investment bank jim cramer call jpmorgan the big dog in the banking sector jim cramer call goldman sachs cramer fave jim cramer on citigroup the best in the group yet it ha the cheapest stock jim cramer call bank of america the weakest in the group jim cramer on capital one were going to see great thing out of them jim cramer on etsy the franchise is worth more than the stock jim cramer on palantir cant avoid buying another data center jim cramer on procter gamble theyll be able to beat the number jim cramer say whirlpool in the driver seat jim cramer on kontoor brand i like that story jim cramer say levi had a decent story jim cramer say williamssonomas ceo moved a ton of manufacturing to vietnam shipping climate reckoning the imo billion pivot uk foreign secretary visit syria after easing sanction pepsi shockingly discontinuous two big name soda an electric solar sailpowered catamaran the modx columbia to pay million to settle lawsuit over u news college ranking data xrp mining introduces allnew cloud mining app seamless profitable green crypto earning for all shiba inu price prediction why shib could surge soon japan brace for more quake authority dismiss doomsday hype in sinaloas capital news of a boxing scion arrest and allegation of cartel tie cause unease click like sugar gambling in a world of quick pleasure an addiction expert say it might be time for a dopamine fast if the u president threatens to take away freedom are we no longer free the civil war that never ended a trip through the america destroyed by inevitable progress these popular sovietera fighter used to give nato nightmare american veteran injured in grenade attack while distributing aid in gaza kamala harris skewered on social medium over somber july post with photo that crop out joe biden iran supreme leader resurfaces in public simply staggering cnn correspondent describes floodwater impact in texas which kpop idol is the ultimate fashion trendsetter vote now at least people killed in central texas flood apple rescue cupertinos transit project u deports men from asia and latin america with criminal record to south sudan after legal saga an iowa law rolling back trans civil right protection in the state ha taken effect here what to know thinkcarebelieve week of america victory letter a question of decency letter title x and planned parenthood headed for sentencing sean diddy comb lawyer aim to show he no longer a bad boy for life musk say steve bannon will go to prison for a long time after deportation jab he ha lifetime of crime to pay for will u continue to fall in world university ranking bloated ice spending show the worst of trump letter u deports men from asia and latin america to south sudan after legal saga oasis return after year hiatus to a uk crowd ecstatic for the band s hit where will crypto mining go next pfmcrypto launch new mobile cloud mining app for earning harris and newsom diverge a polling show democrat race is wide open harris and newsom diverge a polling show democrat race is wide open harris and newsom diverge a polling show democrat race is wide open harris and newsom diverge a polling show democrat race is wide open you voted for budget cut why are you cry now alaska steve mann lodi native swimming with shark bernie sander say the middle class is shrinking he wrong hood america freedom clock need winding the northrop f is getting a new lease on lifein iran simon davidson at inka grill peruvian flavor and charlottesville are a dream come true ukraine zelensky say latest call with trump wa most productive yet trump say he very satisfied with the official narrative on butler assassination exposed jdwp interface lead to crypto mining hpingbot target ssh for ddos improperly thrown away firework lead to garage fire in fond du lac home susan shelley scotus restores needed balance to our government susan shelley scotus restores needed balance to our government susan shelley scotus restores needed balance to our government susan shelley scotus restores needed balance to our government injured in july shooting on north elm street in greensboro letter remembering gloucester july victory reader view stauber duplicitous regarding public radio tv measles case surge to record high since disease wa declared eliminated in the u this is too rich msnbc panel loses it over republican budget vote defense letter retreat from constitution an affront ronda rich the summer leaf and heartache photo suv crash into pool on cape cod letter to the editor parental law a good idea letter to the editor fight back against trump letter to the editor sleep should not come easy letter to the editor new law add protection letter to the editor u failing to meet goal letter to the editor abortion is not equitable letter to the editor where is compassion letter to the editor unhappy about parade change california trial lawyer racket and how to end it california trial lawyer racket and how to end it california trial lawyer racket and how to end it california trial lawyer racket and how to end it amid the terror of smashandgrab mob is retail theft actually up i will never regret coming amid israel devastating strike on iran a woman traveling solo had to find her way out larry wilson what the mamdani win mean for the democratic party larry wilson what the mamdani win mean for the democratic party larry wilson what the mamdani win mean for the democratic party larry wilson what the mamdani win mean for the democratic party july protester in midtown sound the alarm against trump big beautiful bill now the law of the land xi jinpings surprise noshow at brics summit fuel speculation about china global standing how sensationalized headline about brain plastic are undermining trust in safe sustainable material the next megabill congress need to worry about housing funding cut in illinois budget a homelessness increase laura mccall a new weather station honor a charlottesville weather connoisseur the marine are getting rid of their fa hornet jetsfor new f housing funding cut in illinois budget a homelessness increase matt fleming the lunacy of socialism in new york city matt fleming the lunacy of socialism in new york city matt fleming the lunacy of socialism in new york city matt fleming the lunacy of socialism in new york city burcum im haunted by the minnesota shooter uncanny police impersonation letter having class and caring are example for u koerth what go on behind the scene to make a good fishing hole in the city opinion supreme court decision on citizenship and injunction divide american unity reader opinion a terrible thing north carolina governor veto republicanled anti dei and trans legislation battle over public land loom even after selloff proposal fails battle over public land loom even after selloff proposal fails battle over public land loom even after selloff proposal fails battle over public land loom even after selloff proposal fails battle over public land loom even after selloff proposal fails battle over public land loom even after selloff proposal fails turkey arrest more opposition mayor how to protect yourself from tick yearround bitcoin return to the mark and cloud mining platform quid miner attracts much covering the hit dont wait for amazon prime day our expert found deal worth shopping early how trump big beautiful bill will make china great again iova day deadline alert iovances iova promising cell therapy falter triggering ubs downgrade and investor lawsuit hagens berman from day to chevron cloud migration roi in real number walmart is selling a pair of travel bag for only and shopper call them wonderful costcos ev charging ha been developed by spacex engineer it low price could usher in a new wave of car buyer get paid to share your opinion the benefit of paid survey bitcoins bull springboard why diversifying into altcoins make sense shiba inu price prediction can shib rally to or will little pepe lilpepe overtake it and hit billion market cap by codi day deadline alert hagens berman alert compass diversified codi investor to security class action over accounting irregularity encourages investor with loss to contact the firm edge of eternity bonus sheet leak are disappointing dud mtg rock ozzy osbourne reunites with original black sabbath band member during farewell performance content marketing idea for august zelenskys latest call with trump wa most productive he ever had couple unable to pay bill after having social security check slashed from k to a recipient face july cut hims investor alert kessler topaz meltzer check llp urge hims investor with loss to contact the firm on gps what defines a good society man spends day searching for wallet hiding in plain sight thanks to this optical illusion trending hindustan time hindustan time on gps tom friedman on making sense of the middle east serafina to open trattoria at latest anagram apartment tower on gps why cant we build nice thing dot miner trusted crypto cloud mining platform launch new mobile app on gps three expert on trump transformation of the world order a beer pioneer south africa first black female brewery owner train a new generation on gps a debate on regime change in iran ap business summarybrief at pm edt ap business summarybrief at pm edt ap business summarybrief at pm edt amazon prime day we found the best deal to shop before the sale officially kick off yahoo the rise of bitcoin stock and bond lyn alden investment strategy business people new brighton mayor kari niedfeldtthomas to lead regional bbb treasury secretary say some country will see tariff boomerang to april rate by aug california urban housing development exempted from ceqa a game changer steve milloy president trump terminate the green new scam now tariff dealine fed minute and other key thing to watch this week summer buzz build a blockdag launch m summer raffle while doge and bnb lose momentum new u sanction on iran increase pressure on iraq meet one of the men searching for body after tragic texas flood watauga county road closed mount airy firm doing highway work there tchir the risk for stock is that the administration decides it wa correct all along on tariff final week for m lottery jackpot winner to claim prize before it expires a player check floor for winning slip asiapacific market set for mixed open after trump shift goalpost on tariff again harder than it look cnn panel reacts to musk saying he launching a new political party ton surge on uae golden visa news crypto community reacts with excitement and doubt gov beshear trump domestic policy law an attack on rural america full interview bessent tariff will boomerang to liberation day level if country dont make deal full interview shiba inu price prediction shib wont reach even if it hit xrps ath market cap here the best meme coin to buy instead propane council of texas offer key safety reminder after recent flooding absolutely devastating texas congressman on deadly flood bessent say tariff will boomerang to liberation day level if country fail to negotiate deal u close to several trade deal bessent say bitcoin worth billion moved for the first time since bought for just k techspot u tariff on european good threaten to shake up the world largest trade relationship u tariff on european good threaten to shake up the world largest trade relationship u tariff on european good threaten to shake up the world largest trade relationship u tariff on european good threaten to shake up the world largest trade relationship anthony scaramucci want to discus new party with musk mark cuban offer ballot access aid tuesday investor deadline compass diversified holding investor with substantial loss have opportunity to lead class action lawsuit codi tropical storm chantal make landfall all eye on possible nyc path how soundhound ai is quietly building a global ai empire the motley fool dan ives predicts a strong second half for tech top ai stock to buy now how soundhound ai is quietly building a global ai empire u tariff on european good threaten to shake up the world largest trade relationship yearold texas restaurant chain close all location chron robert kiyosaki this is the easiest money ever how will tesla stock react a elon musk form america party ev giant loses tax credit mining stock to buy on an ai boom the sp is soaring nobrainer vanguard etf to buy right now solaxys surge grab attention but blockdags m presale tool remain the key focus for trader salmar q trading update the sp is soaring nobrainer vanguard etf to buy right now davenport co llc cut stock holding in intel corporation nasdaqintc urban automotive open u hq in phoenix to serve luxury tuning market explosive device likely damaged greek tanker off libya last week bessent tariff will boomerang back to april level by aug for country without deal the mindmachine merge how braincomputer interface could transform everything musk form new political party after split with trump over president signature tax cut law tesla robotaxi hit parked car in first recorded accident pcmag social security no tax message on trump bill raise eyebrow russia report ammonia leak at leningrad ustluga seaport expert revea</t>
+          <t xml:space="preserve">u employer added a surprising job last month despite uncertainty over economic policy canada trade deficit in may narrow export to u drop millionaire renter surge in nyc a high earner opt for luxury lease report trader pare bet on fed rate cut after job report here lindsell train global equity fund comment on nintendo co ltd ntdoy stock market today dow sp and nasdaq future advance after strong payroll data trump tax and spending bill face vote marketwatch new online casino canada reddit user share the leading real money online casino for tcl csot exclusively supply display for xiaomi mix flip and xiaomi yu powering xiaomis new beginning blowout june payroll k job added smashing expectation unemployment rate drop to avdx alert monsey firm of wohl fruchter investigating fairness of the sale of avidxchange holding to tpg global and corpay dune awakening drop massive july update fix exploit and rebalances pvp zone clearmind medicine announces irb approval for phase a clinical trial for alcohol use disorder at tel aviv sourasky medical center u stock and bond market are open on eve of july but they close early trump want the world to squeeze out china he starting with vietnam u application for jobless aid fell to last week a layoff remain low u application for jobless aid fell to last week a layoff remain low u application for jobless aid fell to last week a layoff remain low u application for jobless aid fell to last week a layoff remain low u application for jobless aid fell to last week a layoff remain low u application for jobless aid fell to last week a layoff remain low u application for jobless aid fell to last week a layoff remain low trader pare bet on fed rate cut after job report yahoo finance u application for jobless aid fell to last week a layoff remain low u application for jobless aid fell to last week a layoff remain low u application for jobless aid fell to last week a layoff remain low u application for jobless aid fell to last week a layoff remain low parazero receives a recurring bulk order of safeair system from an australian distributor nyt strand july serf a sweet scoop with icecream a spangram half yearly report on lvmhs liquidity contract with oddo bhf sca half yearly report on lvmhs liquidity contract with oddo bhf sca these fossil fuel stock rallied a senate passed trump tax spending plan deep tristate layoff leave continuing jobless claim stuck at highest since canada trade deficit narrow in may a export rise these fossil fuel stock rallied a senate passed trump tax spending plan investor business daily ford jpmorgan amazon executive predict deep job cut a ai advance u weekly firsttime unemployment claim fewest since may ap business summarybrief at am edt u application for jobless aid fell to last week a layoff remain low u application for jobless aid fell to last week a layoff remain low review liquid death on fire plus one of the most unique thc drink yet hog look to close thing out ahead of holiday break cotton mixed in early thursday trade corn pushing gain into thursday morning trade cattle look to round out short week wheat sneaking out gain ahead of threeday weekend soybean strength continuing on thursday am top financial stock you may want to dump this quarter house beat and hidden venue a new sound is emerging in abu dhabi u employer added a surprising job last month despite uncertainty over economic policy u employer added a surprising job last month despite uncertainty over economic policy starbucks offer million stock bonus to exec but should you buy it share here what technical analysis show fed rate cut appears less likely after strongerthanforecast june payroll data green science alliance established an electric vehicle ev company utilizing next generation inwheel motor technology developed by a japanese engineer who pioneered supercar ev named eliica over year ago u economy add new job unemployment rate dip to percent in june stock market today dow sp nasdaq future hit pause after a solid job report liveone synervoz partner for nextgen voice experience u employer added job in june strategy stock rise after key trading signal jobless claim fall to lowest level since midmay sp build on record high future rising after strong job report barrons my parent gifted me what should i do with it u economy add job in june more than expected popular restaurant chain close all location no bankruptcy u application for jobless aid fell to last week a layoff remain low u application for jobless aid fell to last week a layoff remain low u application for jobless aid fell to last week a layoff remain low trade deficit widens surpassing both forecast and previous figure u job growth beat expectation in june celebrate independence wilmatm set aba practice free from manual workflow with powerful patient relationship management nike is back in the race billionaire bill ackman urge tired subdued andrew cuomo to drop out of nyc mayoral race begrudgingly endorses eric adam u payroll increased by in june more than expected navitas semiconductor to participate in upcoming cjs security conference u add k job in june beating expectation u initial jobless claim dip below expectation bolstering usd u employer added job in june a labor market show resilience despite uncertainty over trump economic policy u employer added job in june a labor market show resilience despite uncertainty over trump economic policy labor market stay afloat a hiring top forecastsagain u employer added job in june a labor market show resilience despite uncertainty over trump economic policy airline face investor after strong but cheaper july holiday cnbc lamplight luxury rv park invite traveler to discover their perfect texas getaway at holiday road rv park dsh hotel advisor close jacksonville fl candlewood suite sale a hospitality market heat up lamplight luxury rv park invite traveler to discover their perfect texas getaway at holiday road rv park navitas semiconductor to participate in upcoming cjs security conference dsh hotel advisor close jacksonville fl candlewood suite sale a hospitality market heat up nonfarm payroll beat expectation indicating robust u job market coinex research june report bitcoin in the crossfire u payroll increased by in june more than expected cnbc etoro appoints former sec commissioner laura unger and wix cfo lior shemesh a board member beauty and the bear michael burry estee lauder snub china smci stock get price target bump but it still below current share price agf announces passing of kevin mccreadie ceo and cio coreweave is the first cloud provider to deploy nvidias latest ai chip why kelly slater moved headquarters of his sustainable clothing brand from la to san diego why kelly slater moved headquarters of his sustainable clothing brand from la to san diego why kelly slater moved headquarters of his sustainable clothing brand from la to san diego why kelly slater moved headquarters of his sustainable clothing brand from la to san diego why kelly slater moved headquarters of his sustainable clothing brand from la to san diego why kelly slater moved headquarters of his sustainable clothing brand from la to san diego why kelly slater moved headquarters of his sustainable clothing brand from la to san diego can california democrat require ice agent to unmask and show id trump show america wont tolerate nuclear threat james fitzpatrick trump show america wont tolerate nuclear threat james fitzpatrick texas internet porn law is constitutional common sense prevails dallas morning news texas internet porn law is constitutional common sense prevails dallas morning news texas internet porn law is constitutional common sense prevails dallas morning news trump show america wont tolerate nuclear threat james fitzpatrick trump show america wont tolerate nuclear threat james fitzpatrick texas internet porn law is constitutional common sense prevails dallas morning news trump show america wont tolerate nuclear threat james fitzpatrick texas internet porn law is constitutional common sense prevails dallas morning news texas internet porn law is constitutional common sense prevails dallas morning news trump show america wont tolerate nuclear threat james fitzpatrick texas internet porn law is constitutional common sense prevails dallas morning news texas internet porn law is constitutional common sense prevails dallas morning news texas internet porn law is constitutional common sense prevails dallas morning news trump show america wont tolerate nuclear threat james fitzpatrick trump show america wont tolerate nuclear threat james fitzpatrick trump show america wont tolerate nuclear threat james fitzpatrick texas internet porn law is constitutional common sense prevails dallas morning news congressional intern killed in dc shooting scrum alliance ranked on comparablys list of best leadership team among small company judge strike down trump policy that deleted transgender page from govt website house beat and hidden venue a new sound is emerging in abu dhabi federal judge rule noncalifornia resident can apply for concealedcarry gun permit the latest house leader rush toward a final vote a democrat hold the floor what maga mean to american u application for jobless aid fell to last week a layoff remain low u application for jobless aid fell to last week a layoff remain low aclu sue to block ice raid in southern california alleging constitutional violation u employer added job in june a labor market show resilience despite uncertainty over trump economic policy u employer added job in june a labor market show resilience despite uncertainty over trump economic policy california boost film and tv tax credit to million to preserve job attorney general tap politically connected billing lawyer for judicial discipline panel dnrcs drought outlook for montana is grim going into hot dry summer attorney general tap politically connected billing lawyer for judicial discipline panel attorney general tap politically connected billing lawyer for judicial discipline panel double standard no no standard did the pentagon spread false ufo story were skeptical trump t megabill set house record for longest vote in history number of megarounds drop in first half a biotech struggle against worsening slump california school official say video show immigration agent urinating in public view homeland security investigating iran suspends cooperation with un nuclear monitoring agency a slider a milestone and a heartfelt thank you kershaws th strikeout federal funding for contraceptive access return to missouri nonprofit after threemonth freeze dan walter california lawmaker finally achieve holy grail reform of state key environmental law jeffries us magic minute to delay vote on trump megabill after settling with trump cbs news staffer fear what come next some education grant in limbo were used for leftwing agenda trump administration say some education grant in limbo were used for leftwing agenda trump administration say some education grant in limbo were used for leftwing agenda trump administration say some education grant in limbo were used for leftwing agenda trump administration say some education grant in limbo were used for leftwing agenda trump administration say some education grant in limbo were used for leftwing agenda trump administration say some education grant in limbo were used for leftwing agenda trump administration say some education grant in limbo were used for leftwing agenda trump administration say some education grant in limbo were used for leftwing agenda trump administration say some education grant in limbo were used for leftwing agenda trump administration say some education grant in limbo were used for leftwing agenda trump administration say family of slain police officer krystal rivera shot by a fellow officer want an independent investigation vance boelter man charged in minnesota lawmaker shooting due back in federal court how george washington america reluctant leader contrast with today frederic j fransen choosing war over diplomacy increase danger for u elizabeth shackelford choosing war over diplomacy increase danger for u elizabeth shackelford choosing war over diplomacy increase danger for u elizabeth shackelford how george washington america reluctant leader contrast with today frederic j fransen choosing war over diplomacy increase danger for u elizabeth shackelford how george washington america reluctant leader contrast with today frederic j fransen choosing war over diplomacy increase danger for u elizabeth shackelford choosing war over diplomacy increase danger for u elizabeth shackelford how george washington america reluctant leader contrast with today frederic j fransen how george washington america reluctant leader contrast with today frederic j fransen how george washington america reluctant leader contrast with today frederic j fransen choosing war over diplomacy increase danger for u elizabeth shackelford choosing war over diplomacy increase danger for u elizabeth shackelford how george washington america reluctant leader contrast with today frederic j fransen choosing war over diplomacy increase danger for u elizabeth shackelford choosing war over diplomacy increase danger for u elizabeth shackelford choosing war over diplomacy increase danger for u elizabeth shackelford how george washington america reluctant leader contrast with today frederic j fransen how george washington america reluctant leader contrast with today frederic j fransen how george washington america reluctant leader contrast with today frederic j fransen how can azerbaijan be ally with iran and israel nova ukraine earns platinum seal of transparency from candid ukraine kill one of the highestranking russian officer of the conflict federal budget megabill would shift billion in cost to missouri taxpayer ups violates teamster national contract with plan for buyout chile cut up to of red tape promise streamlined mining approval colorado education leader urge trump to release million in k school funding capitol walkway backed by gov polis is a bridge to nowhere key lawmaker say a project face criticism colorado education leader urge trump to release million in k school funding capitol walkway backed by gov polis is a bridge to nowhere key lawmaker say a project face criticism colorado education leader urge trump to release million in k school funding colorado education leader urge trump to release million in k school funding opinion pb is a national treasure worthy of government support the best american express credit card for picked by a frequent traveler trump cut are squeezing america most popular national park in peak season here what mental health study should look like at a christian college steven eng a christian crisis across our nation and in our backyard the united state just cut off key defense aid to ukraine stock to buy with less than nordstrom rack is selling a gorgeous kendra scott necklace for and shopper get so many compliment openai ceo sam altman say he politically homeless in july post bashing democrat what to expect from boston scientifics next quarterly earnings report buttonwood financial advisor inc ha million holding in meta platform inc nasdaqmeta crown wealth group llc buy share of meta platform inc nasdaqmeta bankplus wealth management llc grows position in meta platform inc nasdaqmeta shilanski associate inc raise holding in meta platform inc nasdaqmeta amalgamated bank acquires share of meta platform inc nasdaqmeta monument capital management buy share of meta platform inc nasdaqmeta best car insurance company of july risk remains of uschina trade truce breakdown capital economics say ups make drastic change it never done before in year history a part of major overhaul the secret to great grilled kabob it all in the cut prediction this magnificent artificial intelligence ai stock will skyrocket to new high in july bitcoin price on the brink a congress introduces a new groundbreaking crypto bill forbes veraltos quarterly earnings preview what you need to know oppo pad se india launch check variant spec price breakdown sofi stock skyrocket in a year how high can it go in consolidated lithium metal announces exposure of a new libearing pegmatite at it preissac project and close financing bmo announces special cash distribution for etf series unit of bmo money market fund consolidated lithium metal announces exposure of a new libearing pegmatite at it preissac project and close financing niurstour i utboi rikisbrefa riks is trader joes open on the th of july best podcast headphone of auction result of treasury bond riks rtx corporation q earnings what to expect how to fix lenovo fingerprint scanner issue fast quick easy guide what to expect from dover q earnings report what you need to know ahead of erie indemnity earnings release petrovictory energy corp and azevedo travassos energia sa sign binding memorandum of understanding petrovictory energy corp and azevedo travassos energia sa sign binding memorandum of understanding sakana ai treequest deploy multimodel team that outperform individual llm by sony break exclusivity helldivers land on xbox this august tesla ha a problem and it not just the elon musk backlash bloombergcom eu stick with timeline for ai rule reuters lot of speculation is swirling around the sumy front wildfire cripple alberta oil production this is why tesla robotaxi launch needed human babysitter what to expect from raymond james financials q earnings report which store are open and closed on independence day kusacom btc hit k why pro trader arent fully confident yet the fiscal treadmill is speeding up and washington keep jogging after year of grinding i have million but am burned out what are my option these catalyst could lift micron stock higher in and beyond costco stock analysis buy sell or hold every breath you take affect how you move here how to fix both my smartest dividend stock to buy today earnings preview what to expect from globe life report here what to expect from ameriprise financials next earnings report key headwind facing usdc cme group quarterly earnings preview what you need to know is subway open on the fourth of july west fargo new herbz and spicez store offer customer allnatural alternative be resilient by accepting adversity and learning from it why black unemployment just rose to it highest level since january littleknown item in trump big agenda bill riley gaines ha been one of lia thomas most vocal critic she just scored two major win in her antitrans effort who the coolest person at your july barbecue they got six thing goin on according to a new study construction start on beacon at princeton hill at s dixie hwy homestead fl i visited universal studio and people were on their phone everywhereeven rollercoasters that habit is really hard to break expert say company in the new york city metro area that are great place to work the strategy that will make your sale call more successful editorial today we celebrate the real no king holiday how glen powell condiment brand made more than million in it first month azi announces receipt of minimum bid price notice from nasdaq fourth of july weekend lotterycom and sportscom driver revved up for midohio challenge stoneform launch a tokenized real estate platform to open up investment opportunity northwest copper announces closing of oversubscribed private placement bybit tradfi x crypto report regulatory tailwind drive coinbase outperformance despite premium valuation stoneform launch a tokenized real estate platform to open up investment opportunity esg hitgen release it inaugural sustainability report is chickfila closed on july northwest copper announces closing of oversubscribed private placement china using tiktok a a pawn to squeeze trump in trade talk source net zero now clear key milestone on acre energy campus accelerating alberta lowcarbon data center infrastructure build out whats open whats closed on july th what grocery store are open walmart costco target more alcom u future slide after trump say hell start sending tariff letter today setting levy up to musk back sen paul criticism of trump megabill in first comment since it passed cf cfrp market worth billion in exclusive report by marketsandmarketstm cf cfrp market worth billion in exclusive report by marketsandmarketstm trump vietnam pact take aim at china but it raise more question than answer cnbc new york state teacher retirement system sell share of avery dennison corporation nyseavy ameritas advisory service llc buy share of ulta beauty inc nasdaqulta these were the bestperforming stock in the dow jones industrial average in june hot dog eating contest host share prediction for this year winner partner value investment lp announces tenforone unit split xrp and ozak ai price prediction which token ha the clearer path to massive gain american flight diverts after nosy passenger cause bomb scare one mile at a time trump bill secures billion for u arctic surge six new icebreaker to counter russian and chinese dominance ethereum is powering wall street future the crypto scene at cannes show how far it come apex group appoints wang a chief ai and data science officer kinterra score small win in new world copper takeover fight new york state teacher retirement system reduces position in oge energy corporation nyseoge u patriotism among democrat crash a marxist demand grow louder birdie for charity in the final stretch to reach m milestone what oracle meta platform and nvidia stock investor should know about recent ai update amber international raise m to enhance m crypto ecosystem reserve best horror game that test your morality marsden launch workplace saving with charity pledge for first business in today gop there is no choice at all multiple suspect charged in separate drug dealing case in billing the secret to great grilled kabob it all in the cut is central asia the next target of russian aggression opinion congress making big mistake with energy tax credit what the justice department push to bring denaturalization case mean what the justice department push to bring denaturalization case mean what the justice department push to bring denaturalization case mean what the justice department push to bring denaturalization case mean what the justice department push to bring denaturalization case mean what the justice department push to bring denaturalization case mean what the justice department push to bring denaturalization case mean what the justice department push to bring denaturalization case mean the house just did our patriotic duty to deliver tax relief and uphold our value what the justice department push to bring denaturalization case mean what the justice department push to bring denaturalization case mean controversy a staggering amount of usmexico border is now militarized what is trump new realism in foreign policy to celebrate july fully consider the context of the declaration of independence selfevident truth every breath you take affect how you move here how to fix both my smartest dividend stock to buy today army experiment with integrating attack drone into artillery formation trump admin to adjust national park fee to prioritize american family over foreign tourist flooding in texas cause multiple fatality a guadalupe river surge to record level jocko willink in a sea of imperfect voice i heard the anthem and the spirit of a nation this july th a family wait american hostage father pleads for son freedom from hamas terrorist opinion bill lueders reason to celebrate july th why black unemployment just rose to it highest level since january littleknown item in trump big agenda bill riley gaines ha been one of lia thomas most vocal critic she just scored two major win in her antitrans effort guest opinion bj and brecken jones u supreme court got it right on parental right and education who the coolest person at your july barbecue they got six thing goin on according to a new study trump ha big plan for america next birthday historian have question trump to sign big beautiful bill in july fourth ceremony at white house editorial after year righteousness and truth must prevail letter to the editor county should be compensated for iris field honoring superintendent extraordinary service trump crowning moment is ammo for dems in america nonstop birthday party watt happening tonis weekly energy highlight hot dog eating contest host share prediction for this year winner opinion supreme court unitary executive theory threatens our balance of power trump concedes he made no progress on achieving top campaign promise democratic rep katherine clark discusses gop megabill heading for trump signature president trump take victory lap after congress pass tax cut and policy bill elote churrasco and churros alligator alcatraz worker fed by miami food truck scientist issue warning after detecting concerning surge in infection in domestic cat should be closely monitored chef who feed penn state student make summer shift helping family with meal are the worst of the storm behind u hateful trump trashed over fking disgusting line about half the country for th of july the allamerican director you dont know by name katy perry and orlando bloom confirm split what we know about the death of liverpool soccer star diogo jota and his brother la activist indicted after handing out face shield to antiice protester president trump to honor iran strike flight team at the white house glenn eden who is chicago greatest ambassador you editorial on july of all day a naturalized citizen is not less than a u citizen editorial america is soon to turn remember the warmth of the bicentennial heidi stevens on long list of thing being cut art may seem inconsequential it not zohran mamdani ha big housing plan here what stand in the way letter what july fourth mean to me a an ahmadi muslim american rep bob morgan what patriotism mean to me three year after the highland park mass shooting this artist hope to be chosen to make a sculpture for trump garden of american hero how ice raid turned part of los angeles into ghost town maggie mulqueen what doe summer mean for my family and me the beach and book a declaration of independence for these time trump pardon cost at least billion in restitution tax hike in december is helping local library raise worker wage and restore lost position ny official react to passage of big beautiful bill through congress impending signature into law who broke george washington walking stick at the sc statehouse yankee rebel an exgovernor hegseth halted weapon for ukraine despite military analysis that the aid wouldnt jeopardize u readiness legislature should act on the pernicious effect of cellphone in school trump success rate in the court so far letter budget cut harmful for health nutrition letter budget cut harmful for health nutrition think youre smarter than a slate associate writer find out with this week news quiz editorial cartoon for july world share are mostly down a trump tariff deadline loom while u stock set record trump pitch plan allowing farmer to vouch for illegal immigrant worker facing deportation blaze engulfs four home in la amid active firework a strike by air traffic controller is disrupting travel to from and over france trump ag secretary ha irony meter exploding left right and center with beyond parody spin trump decision to end taxfree loophole for lowvalue good from china lead to a sharp decline in air cargo shipment cyber school facing wrongful death suit say it unreasonable for teacher to see student weekly opinion blockbuster made me do it questionable advice from big summer movie pa republican gamble on rural health care a megabill push through cumberland county official optimistic that new memo will improve coordination with library system galasso look forward to tomorrow expectantly beyond current circumstance joey chestnut return to coney island expected to dominate hot dog eating contest trump proposes ufc fight at white house to celebrate year of independence will new england sky stay clear for friday night big firework show u colombia announce recall of envoy amid diplomatic rift lucas trump should demand the unconditional surrender of the democrat party food hygiene rating handed to four doncaster establishment one need major improvement elephant kill two female tourist from the uk and new zealand in zambian national park many missouri law restricting abortion blocked again by state judge iredell county name rodney harris a the new deputy county manager iran try keeping new military commander a secret mossad offer guessing game confirms winner atlanta clogged road bring out the rage in motorist opinion challenge opportunity and bright future in ct for dairy farming trump tear into marxist lunatic mamdani honor american hero in bold rebuke play these p plus free game in july xrp hold market confidence while lightchain ai latejuly launch prepares to broaden investor option rosen nationally regarded investor counsel encourages reckitt benckiser group plc investor to secure counsel before important deadline in security class action rbgly robinhood want to redo wall street on the blockchain gizmodo why tempus ai stock soared in june japan brace for more quake authority dismiss doomsday hype opec plus agrees to pump more oil in august the new york time trump reportedly told iran it wa ok to strike back after u attack i said go ahead i understand poland blast trumpputin dialogue after drone strike escalation walmart is selling calvin klein eternity perfume for only and shopper say it an unbeatable deal ap business summarybrief at pm edt ap business summarybrief at pm edt ap business summarybrief at pm edt ap business summarybrief at pm edt the newest stock in the sp ha soared since it ipo and it a buy right now according to wall street the newest stock in the sp ha soared since it ipo and it a buy right now according to wall street were watching a brain drain in real time openai hit hard a top researcher defect to rival tech giant meta rude baguette the best amazon prime day deal under save on gear from blink anker samsung and others engadget nextgen ai and social startup backed by thrive capital and y combinator shaping were on the brink of another big consumer wave click like sugar gambling in a world of quick pleasure an addiction expert say it might be time for a dopamine fast a amazon double down on robotaxis is amzn stock a buy charlize theron is choosing to be single she told call her daddy that can be a sign of strength say relationship expert the future of ai selfdriving car mechanical weeding health care assistant and more patriotic parade at the park the market hidden current delivering fast gain top romantic drama on ott to watch this weekend daily habit that separate high achiever from everyone else best altcoins for next bull run blockdags m summer raffle roi feature alongside inj rndr tia a forgotten megatrend that could be key to the ai economy quality nonus stock to buy in simply staggering cnn correspondent describes floodwater impact in texas good stock still worth buying in this market matt mower after nato summit europe free ride is on the line archer aviation the bet that could take off sooner than you think oneofakind brewery taproom closing no bankruptcy oneofakind brewery taproom closing no bankruptcy trump hit with backlash over use of antisemitic slur at iowa rally stage almost over arctic pablos price hike imminent a myro and housecoin push forward shopper race to get off all item in major closing down sale after iconic activewear brand shuts store investor deadline robbins geller rudman dowd llp announces that sarepta therapeutic inc srpt investor with substantial loss have opportunity to lead class action lawsuit one big beautiful budget deficit opec to increase output by barrel a day in august what it mean for oil market btc miner cloud mining platform strives to offer stability security a bitcoin recently crossed k amazon prime day the best deal live right now plus everything else you need to know engadget an iowa law rolling back trans civil right protection in the state ha taken effect here what to know thinkcarebelieve week of america victory walmart is selling a sleek digital camera for and shopper say it look professional subaru launch killer legacy lease offer for july top short anime to watch this weekend odd taxi death parade more safeway strike end a albertsons and local union reach agreement colorado public radio headed for sentencing sean diddy comb lawyer aim to show he no longer a bad boy for life the average american family is a millionaire how you can join them your kid is </t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>stock buy less nordstrom rack selling gorgeous kendra scott necklace shopper compliment openai ceo sam altman politically homeless post bashing democrat expect boston scientifics next quarterly earnings report buttonwood financial advisor million meta platform nasdaqmeta crown wealth buy share meta platform nasdaqmeta bankplus wealth grows meta platform nasdaqmeta shilanski associate raise meta platform nasdaqmeta amalgamated bank acquires share meta platform nasdaqmeta monument buy share meta platform nasdaqmeta best car insurance company risk remains uschina trade truce breakdown economics ups drastic change never history part major overhaul secret great grilled kabob cut prediction magnificent artificial intelligence ai stock skyrocket new high bitcoin price brink congress introduces new groundbreaking crypto bill forbes veraltos quarterly earnings preview oppo pad se india launch variant spec price breakdown sofi stock skyrocket high consolidated lithium metal announces exposure new libearing pegmatite preissac project close financing bmo announces special cash distribution series unit bmo money market fund consolidated lithium metal announces exposure new libearing pegmatite preissac project close financing niurstour utboi rikisbrefa riks trader joes open best podcast headphone auction treasury bond riks rtx corporation q earnings expect fix lenovo fingerprint scanner issue fast quick easy guide expect dover q earnings report ahead erie indemnity earnings release petrovictory energy corp azevedo travassos energia sa sign binding memorandum understanding petrovictory energy corp azevedo travassos energia sa sign binding memorandum understanding sakana ai treequest deploy multimodel team outperform individual llm sony break exclusivity helldivers land xbox august tesla problem elon musk backlash bloombergcom eu stick timeline ai rule reuters lot speculation swirling around sumy front wildfire cripple alberta oil production tesla robotaxi launch needed human babysitter expect raymond james financials q earnings report store open closed independence kusacom btc hit k pro trader arent fully confident yet fiscal treadmill speeding washington jogging grinding million burned option catalyst lift micron stock higher beyond costco stock analysis buy sell breath take affect move fix smartest dividend stock buy earnings preview expect globe life report expect ameriprise financials next earnings report headwind facing usdc cme quarterly earnings preview subway open fourth west fargo new herbz spicez store offer customer allnatural alternative resilient accepting adversity learning black unemployment rose highest level since january littleknown item trump agenda bill riley gaines lia thomas vocal critic scored major antitrans effort coolest barbecue got six goin according new study construction start beacon princeton hill dixie hwy homestead fl visited universal studio people phone everywhereeven rollercoasters habit hard break expert company new york metro area great place work strategy sale call successful editorial celebrate real king holiday glen powell condiment brand million month azi announces receipt minimum bid price notice nasdaq fourth weekend lotterycom sportscom driver revved midohio challenge stoneform launch tokenized real estate platform open investment opportunity northwest copper announces closing oversubscribed private placement bybit tradfi x crypto report regulatory tailwind drive coinbase outperformance premium valuation stoneform launch tokenized real estate platform open investment opportunity esg hitgen release inaugural sustainability report chickfila closed northwest copper announces closing oversubscribed private placement china tiktok pawn squeeze trump trade source net zero milestone acre energy campus accelerating alberta lowcarbon data center infrastructure build whats open whats closed grocery store open walmart costco target alcom future slide trump hell start sending tariff setting levy musk sen paul criticism trump megabill since passed cf cfrp market worth billion exclusive report marketsandmarketstm cf cfrp market worth billion exclusive report marketsandmarketstm trump vietnam pact take aim china raise answer cnbc new york teacher retirement system sell share avery dennison corporation nyseavy ameritas advisory service buy share ulta beauty nasdaqulta bestperforming stock dow jones industrial average hot dog eating contest host share prediction winner partner value investment lp announces tenforone unit split xrp ozak ai price prediction token clearer path massive gain american flight diverts nosy passenger cause bomb scare mile trump bill secures billion arctic surge six new icebreaker counter russian chinese dominance ethereum powering wall street future crypto scene cannes far come apex appoints wang chief ai data science officer kinterra score small new world copper takeover fight new york teacher retirement system reduces oge energy corporation nyseoge patriotism among democrat crash marxist demand grow louder birdie charity final stretch reach milestone oracle meta platform nvidia stock investor recent ai update amber international raise enhance crypto ecosystem reserve best horror game test morality marsden launch workplace saving charity pledge business gop choice multiple suspect charged separate drug dealing billing secret great grilled kabob cut central asia next target russian aggression opinion congress making mistake energy tax credit justice department push denaturalization justice department push denaturalization justice department push denaturalization justice department push denaturalization justice department push denaturalization justice department push denaturalization justice department push denaturalization justice department push denaturalization house patriotic duty deliver tax relief uphold value justice department push denaturalization justice department push denaturalization controversy staggering amount usmexico border militarized trump new realism foreign policy celebrate fully consider declaration independence selfevident truth breath take affect move fix smartest dividend stock buy army experiment integrating attack drone artillery formation trump admin adjust national park fee prioritize american family foreign tourist flooding texas cause multiple fatality guadalupe river surge record level jocko willink sea imperfect voice heard anthem spirit nation family wait american hostage father pleads son freedom hamas terrorist opinion bill lueders celebrate black unemployment rose highest level since january littleknown item trump agenda bill riley gaines lia thomas vocal critic scored major antitrans effort guest opinion bj brecken jones supreme got parental education coolest barbecue got six goin according new study trump plan america next birthday historian trump sign bill fourth ceremony white house editorial righteousness truth must prevail editor county compensated iris field honoring superintendent extraordinary service trump crowning moment ammo dems america nonstop birthday party watt happening tonis weekly energy highlight hot dog eating contest host share prediction winner opinion supreme unitary executive theory threatens balance power trump concedes progress achieving campaign promise democratic rep katherine clark discusses gop megabill heading trump signature president trump take victory lap congress pas tax cut policy bill elote churrasco churros alligator alcatraz worker fed miami truck scientist issue warning detecting concerning surge infection domestic cat closely monitored chef feed penn student summer shift helping family meal worst storm behind hateful trump trashed fking disgusting line half country allamerican director dont name katy perry orlando bloom confirm split death liverpool soccer star diogo jota brother la activist indicted handing face shield antiice protester president trump honor iran strike flight team white house glenn eden chicago greatest ambassador editorial naturalized citizen less citizen editorial america soon turn remember warmth bicentennial heidi stevens list cut art seem inconsequential zohran mamdani housing plan stand fourth ahmadi muslim american rep bob morgan patriotism highland park mass shooting artist chosen sculpture trump garden american hero raid turned part los angeles ghost town maggie mulqueen doe summer family beach book declaration independence trump pardon cost least billion restitution tax hike december helping local library raise worker wage restore ny react passage bill congress impending signature broke george washington walking stick sc statehouse yankee rebel exgovernor hegseth halted weapon ukraine military analysis aid wouldnt jeopardize readiness legislature act pernicious effect cellphone school trump success rate far budget cut harmful health nutrition budget cut harmful health nutrition youre smarter slate associate writer find quiz editorial cartoon world share mostly trump tariff deadline loom stock set record trump pitch plan allowing farmer vouch illegal immigrant worker facing deportation blaze engulfs la amid active firework strike air traffic controller disrupting travel france trump ag secretary irony meter exploding left center beyond parody spin trump decision end taxfree loophole lowvalue good china lead sharp decline air cargo shipment cyber school facing wrongful death suit unreasonable teacher student weekly opinion blockbuster questionable advice summer movie pa republican gamble rural health care megabill push cumberland county optimistic new memo improve coordination library system galasso look forward tomorrow expectantly beyond circumstance joey chestnut coney island expected dominate hot dog eating contest trump proposes ufc fight white house celebrate independence new england sky stay friday night firework colombia announce recall envoy amid diplomatic rift lucas trump demand unconditional surrender democrat party hygiene rating handed doncaster establishment major improvement elephant kill female tourist uk new zealand zambian national park missouri restricting abortion blocked judge iredell county name rodney harris new deputy county manager iran try keeping new military commander secret mossad offer guessing game confirms winner atlanta clogged road rage motorist opinion challenge opportunity bright future ct dairy farming trump tear marxist lunatic mamdani honor american hero bold rebuke play p plus free game xrp market confidence lightchain ai latejuly launch prepares broaden investor option rosen nationally regarded investor counsel encourages reckitt benckiser plc investor secure counsel important deadline security class action rbgly robinhood redo wall street blockchain gizmodo tempus ai stock soared japan brace quake authority dismiss doomsday hype opec plus agrees pump oil august new york trump reportedly iran ok strike attack ahead understand poland blast trumpputin dialogue drone strike escalation walmart selling calvin klein eternity perfume shopper unbeatable deal business pm business pm business pm business pm newest stock sp soared since ipo buy according wall street newest stock sp soared since ipo buy according wall street watching brain drain real openai hit hard researcher defect rival tech giant meta rude baguette best amazon prime deal save gear blink anker samsung others engadget nextgen ai social startup backed thrive combinator shaping brink another consumer wave click sugar gambling world quick pleasure addiction expert dopamine fast amazon double robotaxis amzn stock buy charlize theron choosing single call daddy sign strength relationship expert future ai selfdriving car mechanical weeding health care assistant patriotic parade park market hidden delivering fast gain romantic drama ott watch weekend habit separate high achiever everyone else best altcoins next bull run blockdags summer raffle roi feature alongside inj rndr tia forgotten megatrend ai economy quality nonus stock buy simply staggering cnn correspondent describes floodwater impact texas good stock worth buying market matt mower nato summit europe free ride line archer aviation bet take sooner oneofakind brewery taproom closing bankruptcy oneofakind brewery taproom closing bankruptcy trump hit backlash antisemitic slur iowa rally stage almost arctic pablos price hike imminent myro housecoin push forward shopper race item major closing sale iconic activewear brand shuts store investor deadline robbins geller rudman dowd llp announces sarepta therapeutic srpt investor substantial loss opportunity lead class action lawsuit budget deficit opec increase output barrel august oil market btc miner cloud mining platform strives offer stability security bitcoin crossed k amazon prime best deal plus everything else engadget iowa rolling trans civil protection taken effect thinkcarebelieve america victory walmart selling sleek digital camera shopper look professional subaru launch killer legacy lease offer short anime watch weekend odd taxi death parade safeway strike end albertsons local union reach agreement colorado public radio headed sentencing sean diddy comb lawyer aim longer bad boy life average american family millionaire join kid getting trump account put money unstoppable growth stock next solar battery egypt south africa lower mortgage rate save california housing market lower mortgage rate save california housing market rep mark green resigns congress leaving speaker johnson narrower republican majority house council vote new fire chief monday direct payday loan lender globenewswire fbi sheriff office arrest motorcycle gang operation mongolian beef oasis hiatus uk crowd ecstatic band hit dave ramsey real estate outperform stock warned higer dont come free best cryptos buy longterm growth bdag hbar fil algo pipeline disruption slash ecuador output bpd life saver lawrence general paramedic blood accident scene smart founder build company run without excia advisor presentation suggests enter postdebt era without raising taxesthanks overlooked federal asset atsfriendly resume free ai tip trick chipotle customer uncovers receipt price changed decade new york post business business china legoland open visitor shanghai opec surprise oversized output hike jim cramer fight joby aviation jim cramer titan international cant jim cramer domino jim cramer danaher comeback jim cramer centene painful story jim cramer happy fargo jim cramer considers morgan stanley tremendous investment bank jim cramer call jpmorgan dog banking sector jim cramer call goldman sachs cramer fave jim cramer citigroup best yet cheapest stock jim cramer call bank america weakest jim cramer great jim cramer etsy franchise worth stock jim cramer palantir cant avoid buying another data center jim cramer procter gamble theyll able beat jim cramer whirlpool driver seat jim cramer kontoor brand story jim cramer levi decent story jim cramer williamssonomas ceo moved ton manufacturing vietnam shipping climate reckoning imo billion pivot uk foreign secretary visit syria easing sanction pepsi shockingly discontinuous name soda electric solar sailpowered catamaran modx columbia pay million settle lawsuit college ranking data xrp mining introduces allnew cloud mining app seamless profitable green crypto earning shiba inu price prediction shib surge soon japan brace quake authority dismiss doomsday hype sinaloas boxing scion arrest allegation cartel tie cause unease click sugar gambling world quick pleasure addiction expert dopamine fast president threatens take away freedom longer free civil war never ended trip america destroyed inevitable progress popular sovietera fighter used give nato nightmare american veteran injured grenade attack distributing aid gaza kamala harris skewered social medium somber post photo crop joe biden iran supreme resurfaces public simply staggering cnn correspondent describes floodwater impact texas kpop idol ultimate fashion trendsetter vote least people killed central texas flood apple rescue cupertinos transit project deports men asia latin america criminal record south sudan legal saga iowa rolling trans civil protection taken effect thinkcarebelieve america victory decency title x planned parenthood headed sentencing sean diddy comb lawyer aim longer bad boy life musk steve bannon prison deportation jab lifetime crime pay continue fall world university ranking bloated spending worst trump deports men asia latin america south sudan legal saga oasis hiatus uk crowd ecstatic band hit crypto mining next pfmcrypto launch new mobile cloud mining app earning harris newsom diverge polling democrat race wide open harris newsom diverge polling democrat race wide open harris newsom diverge polling democrat race wide open harris newsom diverge polling democrat race wide open voted budget cut cry alaska steve mann lodi native swimming shark bernie sander middle class shrinking hood america freedom clock winding northrop f getting new lease lifein iran simon davidson inka grill peruvian flavor charlottesville dream come ukraine zelensky latest call trump productive yet trump satisfied narrative butler assassination exposed jdwp interface lead crypto mining hpingbot target ssh ddos improperly thrown away firework lead garage fire fond du lac susan shelley scotus restores needed balance government susan shelley scotus restores needed balance government susan shelley scotus restores needed balance government susan shelley scotus restores needed balance government injured shooting north elm street greensboro remembering gloucester victory reader view stauber duplicitous regarding public radio tv measles surge record high since disease declared eliminated rich msnbc panel loses republican budget vote defense retreat constitution affront ronda rich summer leaf heartache photo suv crash pool cape cod editor parental good idea editor fight trump editor sleep come easy editor new add protection editor failing meet goal editor abortion equitable editor compassion editor unhappy parade change california trial lawyer racket end california trial lawyer racket end california trial lawyer racket end california trial lawyer racket end amid terror smashandgrab mob retail theft never regret coming amid israel devastating strike iran woman traveling solo find larry wilson mamdani democratic party larry wilson mamdani democratic party larry wilson mamdani democratic party larry wilson mamdani democratic party protester midtown sound alarm trump bill land xi jinpings surprise noshow brics summit fuel speculation china global standing sensationalized headline brain plastic undermining trust safe sustainable material next megabill congress worry housing funding cut illinois budget homelessness increase laura mccall new weather station honor charlottesville weather connoisseur marine getting rid fa hornet jetsfor new f housing funding cut illinois budget homelessness increase matt fleming lunacy socialism new york matt fleming lunacy socialism new york matt fleming lunacy socialism new york matt fleming lunacy socialism new york burcum im haunted minnesota shooter uncanny police impersonation class caring example koerth behind scene good fishing hole opinion supreme decision citizenship injunction divide american unity reader opinion terrible north carolina governor veto republicanled anti dei trans legislation battle public land loom selloff proposal fails battle public land loom selloff proposal fails battle public land loom selloff proposal fails battle public land loom selloff proposal fails battle public land loom selloff proposal fails battle public land loom selloff proposal fails turkey arrest opposition mayor protect tick yearround bitcoin mark cloud mining platform quid miner attracts covering hit dont wait amazon prime expert found deal worth shopping early trump bill china great iova deadline alert iovances iova promising cell therapy falter triggering ubs downgrade investor lawsuit hagens berman chevron cloud migration roi real walmart selling pair travel bag shopper call wonderful costcos ev charging developed spacex engineer low price usher new wave car buyer paid share opinion benefit paid survey bitcoins bull springboard diversifying altcoins sense shiba inu price prediction shib rally little pepe lilpepe overtake hit billion market cap codi deadline alert hagens berman alert compass diversified codi investor security class action accounting irregularity encourages investor loss contact firm edge eternity bonus sheet leak disappointing dud mtg rock ozzy osbourne reunites original black sabbath band farewell performance content marketing idea august zelenskys latest call trump productive ever couple unable pay bill social security slashed k recipient face cut hims investor alert kessler topaz meltzer llp urge hims investor loss contact firm gps defines good society man spends searching wallet hiding plain sight optical illusion trending hindustan hindustan gps tom friedman making sense middle east serafina open trattoria latest anagram apartment tower gps cant build nice dot miner trusted crypto cloud mining platform launch new mobile app gps expert trump transformation world order beer pioneer south africa black female brewery owner train new generation gps debate regime change iran business pm business pm business pm amazon prime found best deal shop sale officially kick yahoo rise bitcoin stock bond lyn alden investment strategy business people new brighton mayor kari niedfeldtthomas lead regional bbb treasury secretary country tariff boomerang april rate aug california urban housing development exempted ceqa game changer steve milloy president trump terminate green new scam tariff dealine fed watch summer buzz build blockdag launch summer raffle doge bnb lose momentum new sanction iran increase pressure iraq meet men searching body tragic texas flood watauga county road closed mount airy firm highway work tchir risk stock administration decides along tariff final lottery jackpot winner claim prize expires player floor winning slip asiapacific market set mixed open trump shift goalpost tariff harder look cnn panel reacts musk saying launching new political party ton surge uae golden visa crypto community reacts excitement doubt gov beshear trump domestic policy attack rural america full interview bessent tariff boomerang liberation level country dont deal full interview shiba inu price prediction shib wont reach hit xrps ath market cap best meme coin buy instead propane council texas offer safety reminder recent flooding absolutely devastating texas congressman deadly flood bessent tariff boomerang liberation level country fail negotiate deal close several trade deal bessent bitcoin worth billion moved since bought k techspot tariff european good threaten shake world largest trade relationship tariff european good threaten shake world largest trade relationship tariff european good threaten shake world largest trade relationship tariff european good threaten shake world largest trade relationship anthony scaramucci discus new party musk mark cuban offer ballot access aid tuesday investor deadline compass diversified investor substantial loss opportunity lead class action lawsuit codi tropical storm chantal landfall eye possible nyc path soundhound ai quietly building global ai empire motley fool dan ives predicts strong half tech ai stock buy soundhound ai quietly building global ai empire tariff european good threaten shake world largest trade relationship yearold texas restaurant chain close location chron robert kiyosaki easiest money ever tesla stock react elon musk form america party ev giant loses tax credit mining stock buy ai boom sp soaring nobrainer vanguard buy solaxys surge grab attention blockdags presale tool focus trader salmar q trading update sp soaring nobrainer vanguard buy davenport co cut stock intel corporation nasdaqintc urban automotive open hq phoenix luxury tuning market explosive device likely damaged greek tanker libya bessent tariff boomerang april level aug country without deal mindmachine merge braincomputer interface transform everything musk form new political party split trump president signature tax cut tesla robotaxi hit parked car recorded accident pcmag social security tax message trump bill raise eyebrow russia report ammonia leak leningrad ustluga seaport expert revea</t>
+          <t>employer added surprising job month uncertainty economic policy canada trade deficit narrow export drop millionaire renter surge nyc high earner opt luxury lease report trader pare bet fed rate cut job report lindsell train global equity fund nintendo co ltd ntdoy stock market dow sp nasdaq future advance strong payroll data trump tax spending bill face vote marketwatch online casino canada reddit user leading real money online casino tcl csot exclusively supply display xiaomi mix flip xiaomi yu powering xiaomis beginning blowout payroll k job added smashing expectation unemployment rate drop avdx alert monsey firm wohl fruchter investigating fairness sale avidxchange tpg global corpay dune awakening drop massive update fix exploit rebalances pvp zone clearmind medicine announces irb approval phase clinical trial alcohol disorder tel aviv sourasky medical center stock bond market open eve close early trump world squeeze china starting vietnam application jobless aid fell layoff low application jobless aid fell layoff low application jobless aid fell layoff low application jobless aid fell layoff low application jobless aid fell layoff low application jobless aid fell layoff low application jobless aid fell layoff low trader pare bet fed rate cut job report yahoo finance application jobless aid fell layoff low application jobless aid fell layoff low application jobless aid fell layoff low application jobless aid fell layoff low parazero receives recurring bulk order safeair system australian distributor nyt strand serf sweet scoop icecream spangram half yearly report lvmhs liquidity contract oddo bhf sca half yearly report lvmhs liquidity contract oddo bhf sca fossil fuel stock rallied senate passed trump tax spending plan deep tristate layoff continuing jobless claim stuck highest since canada trade deficit narrow export rise fossil fuel stock rallied senate passed trump tax spending plan investor business ford jpmorgan amazon executive predict deep job cut ai advance weekly firsttime unemployment claim fewest since business application jobless aid fell layoff low application jobless aid fell layoff low review liquid death fire plus unique thc drink yet hog look close ahead holiday break cotton mixed early thursday trade corn pushing gain thursday morning trade cattle look round short wheat sneaking gain ahead threeday weekend soybean strength continuing thursday financial stock dump quarter house beat hidden venue sound emerging abu dhabi employer added surprising job month uncertainty economic policy employer added surprising job month uncertainty economic policy starbucks offer million stock bonus exec buy technical analysis fed rate cut less likely strongerthanforecast payroll data green science alliance established electric vehicle ev company utilizing next generation inwheel technology developed japanese engineer pioneered supercar ev named eliica ago economy add job unemployment rate dip percent stock market dow sp nasdaq future hit pause solid job report liveone synervoz partner nextgen voice experience employer added job strategy stock rise trading signal jobless claim fall lowest level since midmay sp build record high future rising strong job report barrons parent gifted economy add job expected popular restaurant chain close location bankruptcy application jobless aid fell layoff low application jobless aid fell layoff low application jobless aid fell layoff low trade deficit widens surpassing forecast previous figure job growth beat expectation celebrate independence wilmatm set aba practice free manual powerful patient relationship nike race billionaire bill ackman urge tired subdued andrew cuomo drop nyc mayoral race begrudgingly endorses eric adam payroll increased expected navitas semiconductor participate upcoming cjs security conference add k job beating expectation initial jobless claim dip expectation bolstering usd employer added job labor market resilience uncertainty trump economic policy employer added job labor market resilience uncertainty trump economic policy labor market stay afloat hiring forecastsagain employer added job labor market resilience uncertainty trump economic policy airline face investor strong cheaper holiday cnbc lamplight luxury rv park invite traveler discover perfect texas getaway holiday road rv park dsh hotel advisor close jacksonville fl candlewood suite sale hospitality market heat lamplight luxury rv park invite traveler discover perfect texas getaway holiday road rv park navitas semiconductor participate upcoming cjs security conference dsh hotel advisor close jacksonville fl candlewood suite sale hospitality market heat nonfarm payroll beat expectation indicating robust job market coinex research report bitcoin crossfire payroll increased expected cnbc etoro appoints sec commissioner laura unger wix cfo lior shemesh board beauty bear michael burry snub china smci stock price target bump price agf announces passing kevin mccreadie ceo cio coreweave cloud provider deploy nvidias latest ai chip kelly slater moved sustainable clothing brand la san diego kelly slater moved sustainable clothing brand la san diego kelly slater moved sustainable clothing brand la san diego kelly slater moved sustainable clothing brand la san diego kelly slater moved sustainable clothing brand la san diego kelly slater moved sustainable clothing brand la san diego kelly slater moved sustainable clothing brand la san diego california democrat require agent unmask id trump america wont tolerate nuclear threat james fitzpatrick trump america wont tolerate nuclear threat james fitzpatrick texas internet porn constitutional common sense prevails dallas morning texas internet porn constitutional common sense prevails dallas morning texas internet porn constitutional common sense prevails dallas morning trump america wont tolerate nuclear threat james fitzpatrick trump america wont tolerate nuclear threat james fitzpatrick texas internet porn constitutional common sense prevails dallas morning trump america wont tolerate nuclear threat james fitzpatrick texas internet porn constitutional common sense prevails dallas morning texas internet porn constitutional common sense prevails dallas morning trump america wont tolerate nuclear threat james fitzpatrick texas internet porn constitutional common sense prevails dallas morning texas internet porn constitutional common sense prevails dallas morning texas internet porn constitutional common sense prevails dallas morning trump america wont tolerate nuclear threat james fitzpatrick trump america wont tolerate nuclear threat james fitzpatrick trump america wont tolerate nuclear threat james fitzpatrick texas internet porn constitutional common sense prevails dallas morning congressional intern killed dc shooting scrum alliance ranked comparablys list best leadership team among small company judge strike trump policy deleted transgender page govt website house beat hidden venue sound emerging abu dhabi federal judge rule noncalifornia resident apply concealedcarry gun permit latest house rush final vote democrat floor maga american application jobless aid fell layoff low application jobless aid fell layoff low aclu sue block raid southern california alleging constitutional violation employer added job labor market resilience uncertainty trump economic policy employer added job labor market resilience uncertainty trump economic policy california boost film tv tax credit million preserve job attorney general tap politically connected billing lawyer judicial discipline panel dnrcs drought outlook montana grim hot dry summer attorney general tap politically connected billing lawyer judicial discipline panel attorney general tap politically connected billing lawyer judicial discipline panel double pentagon spread false ufo story skeptical trump megabill set house record longest vote history megarounds drop half biotech struggle worsening slump california school video immigration agent urinating public view homeland security investigating iran suspends cooperation un nuclear monitoring agency slider milestone heartfelt kershaws strikeout federal funding contraceptive access missouri nonprofit threemonth freeze dan walter california lawmaker finally achieve holy grail reform environmental jeffries u magic delay vote trump megabill settling trump cbs staffer fear come next education grant limbo used leftwing agenda trump administration education grant limbo used leftwing agenda trump administration education grant limbo used leftwing agenda trump administration education grant limbo used leftwing agenda trump administration education grant limbo used leftwing agenda trump administration education grant limbo used leftwing agenda trump administration education grant limbo used leftwing agenda trump administration education grant limbo used leftwing agenda trump administration education grant limbo used leftwing agenda trump administration education grant limbo used leftwing agenda trump administration education grant limbo used leftwing agenda trump administration family slain police officer krystal rivera shot fellow officer independent investigation vance boelter man charged minnesota lawmaker shooting due federal george washington america reluctant contrast frederic j fransen choosing war diplomacy increase danger elizabeth shackelford choosing war diplomacy increase danger elizabeth shackelford choosing war diplomacy increase danger elizabeth shackelford george washington america reluctant contrast frederic j fransen choosing war diplomacy increase danger elizabeth shackelford george washington america reluctant contrast frederic j fransen choosing war diplomacy increase danger elizabeth shackelford choosing war diplomacy increase danger elizabeth shackelford george washington america reluctant contrast frederic j fransen george washington america reluctant contrast frederic j fransen george washington america reluctant contrast frederic j fransen choosing war diplomacy increase danger elizabeth shackelford choosing war diplomacy increase danger elizabeth shackelford george washington america reluctant contrast frederic j fransen choosing war diplomacy increase danger elizabeth shackelford choosing war diplomacy increase danger elizabeth shackelford choosing war diplomacy increase danger elizabeth shackelford george washington america reluctant contrast frederic j fransen george washington america reluctant contrast frederic j fransen george washington america reluctant contrast frederic j fransen azerbaijan ally iran israel nova ukraine earns platinum seal transparency candid ukraine kill highestranking russian officer conflict federal budget megabill shift billion cost missouri taxpayer ups violates teamster national contract plan buyout chile cut red tape promise streamlined mining approval colorado education urge trump release million k school funding capitol walkway backed gov polis bridge nowhere lawmaker project face criticism colorado education urge trump release million k school funding capitol walkway backed gov polis bridge nowhere lawmaker project face criticism colorado education urge trump release million k school funding colorado education urge trump release million k school funding opinion pb national treasure worthy government support best american express credit card picked frequent traveler trump cut squeezing america popular national park peak season mental health study look christian college steven eng christian crisis across nation backyard united cut defense aid ukraine stock buy less nordstrom rack selling gorgeous kendra scott necklace shopper compliment openai ceo sam altman politically homeless post bashing democrat expect boston scientifics next quarterly earnings report buttonwood financial advisor million meta platform nasdaqmeta crown wealth buy meta platform nasdaqmeta bankplus wealth grows meta platform nasdaqmeta shilanski associate raise meta platform nasdaqmeta amalgamated bank acquires meta platform nasdaqmeta monument buy meta platform nasdaqmeta best car insurance company risk remains uschina trade truce breakdown economics ups drastic change never history part major overhaul secret great grilled kabob cut prediction magnificent artificial intelligence ai stock skyrocket high bitcoin price brink congress introduces groundbreaking crypto bill forbes veraltos quarterly earnings preview oppo pad se india launch variant spec price breakdown sofi stock skyrocket high consolidated lithium metal announces exposure libearing pegmatite preissac project close financing bmo announces special cash distribution series unit bmo money market fund consolidated lithium metal announces exposure libearing pegmatite preissac project close financing niurstour utboi rikisbrefa riks trader joes open best podcast headphone auction treasury bond riks rtx corporation q earnings expect fix lenovo fingerprint scanner issue fast quick easy guide expect dover q earnings report ahead erie indemnity earnings release petrovictory energy corp azevedo travassos energia sa sign binding memorandum understanding petrovictory energy corp azevedo travassos energia sa sign binding memorandum understanding sakana ai treequest deploy multimodel team outperform individual llm sony break exclusivity helldivers land xbox august tesla problem elon musk backlash bloombergcom eu stick timeline ai rule reuters lot speculation swirling around sumy front wildfire cripple alberta oil production tesla robotaxi launch needed human babysitter expect raymond james financials q earnings report store open closed independence kusacom btc hit k pro trader arent fully confident yet fiscal treadmill speeding washington jogging grinding million burned option catalyst lift micron stock higher beyond costco stock analysis buy sell breath take affect move fix smartest dividend stock buy earnings preview expect globe life report expect ameriprise financials next earnings report headwind facing usdc cme quarterly earnings preview subway open fourth west fargo herbz spicez store offer customer allnatural alternative resilient accepting adversity learning black unemployment rose highest level since january littleknown item trump agenda bill riley gaines lia thomas vocal critic scored major antitrans effort coolest barbecue got six goin according study construction start beacon princeton hill dixie hwy homestead fl visited universal studio people phone everywhereeven rollercoasters habit hard break expert company york metro area great place work strategy sale call successful editorial celebrate real king holiday glen powell condiment brand million month azi announces receipt minimum bid price notice nasdaq fourth weekend lotterycom sportscom driver revved midohio challenge stoneform launch tokenized real estate platform open investment opportunity northwest copper announces closing oversubscribed private placement bybit tradfi x crypto report regulatory tailwind drive coinbase outperformance premium valuation stoneform launch tokenized real estate platform open investment opportunity esg hitgen release inaugural sustainability report chickfila closed northwest copper announces closing oversubscribed private placement china tiktok pawn squeeze trump trade source net zero milestone acre energy campus accelerating alberta lowcarbon data center infrastructure build whats open whats closed grocery store open walmart costco target alcom future slide trump hell start sending tariff setting levy musk sen paul criticism trump megabill since passed cf cfrp market worth billion exclusive report marketsandmarketstm cf cfrp market worth billion exclusive report marketsandmarketstm trump vietnam pact take aim china raise answer cnbc york teacher retirement system sell avery dennison corporation nyseavy ameritas advisory service buy ulta beauty nasdaqulta bestperforming stock dow jones industrial average hot dog eating contest host prediction winner partner value investment lp announces tenforone unit split xrp ozak ai price prediction token clearer path massive gain american flight diverts nosy passenger cause bomb scare mile trump bill secures billion arctic surge six icebreaker counter russian chinese dominance ethereum powering wall street future crypto scene cannes far come apex appoints wang chief ai data science officer kinterra score small world copper takeover fight york teacher retirement system reduces oge energy corporation nyseoge patriotism among democrat crash marxist demand grow louder birdie charity final stretch reach milestone oracle meta platform nvidia stock investor recent ai update amber international raise enhance crypto ecosystem reserve best horror game test morality marsden launch workplace saving charity pledge business gop choice multiple suspect charged separate drug dealing billing secret great grilled kabob cut central asia next target russian aggression opinion congress making mistake energy tax credit justice department push denaturalization justice department push denaturalization justice department push denaturalization justice department push denaturalization justice department push denaturalization justice department push denaturalization justice department push denaturalization justice department push denaturalization house patriotic duty deliver tax relief uphold value justice department push denaturalization justice department push denaturalization controversy staggering amount usmexico border militarized trump realism foreign policy celebrate fully consider declaration independence selfevident truth breath take affect move fix smartest dividend stock buy army experiment integrating attack drone artillery formation trump admin adjust national park fee prioritize american family foreign tourist flooding texas cause multiple fatality guadalupe river surge record level jocko willink sea imperfect voice heard anthem spirit nation family wait american hostage father pleads son freedom hamas terrorist opinion bill lueders celebrate black unemployment rose highest level since january littleknown item trump agenda bill riley gaines lia thomas vocal critic scored major antitrans effort guest opinion bj brecken jones supreme got parental education coolest barbecue got six goin according study trump plan america next birthday historian trump sign bill fourth ceremony white house editorial righteousness truth must prevail editor county compensated iris field honoring superintendent extraordinary service trump crowning moment ammo dems america nonstop birthday party watt happening tonis weekly energy highlight hot dog eating contest host prediction winner opinion supreme unitary executive theory threatens balance power trump concedes progress achieving campaign promise democratic rep katherine clark discusses gop megabill heading trump signature president trump take victory lap congress pas tax cut policy bill elote churrasco churros alligator alcatraz worker fed miami truck scientist issue warning detecting concerning surge infection domestic cat closely monitored chef feed penn student summer shift helping family meal worst storm behind hateful trump trashed fking disgusting line half country allamerican director dont name katy perry orlando bloom confirm split death liverpool soccer star diogo jota brother la activist indicted handing face shield antiice protester president trump honor iran strike flight team white house glenn eden chicago greatest ambassador editorial naturalized citizen less citizen editorial america soon turn remember warmth bicentennial heidi stevens list cut art seem inconsequential zohran mamdani housing plan stand fourth ahmadi muslim american rep bob morgan patriotism highland park mass shooting artist chosen sculpture trump garden american hero raid turned part los angeles ghost town maggie mulqueen doe summer family beach book declaration independence trump pardon cost least billion restitution tax hike december helping local library raise worker wage restore ny react passage bill congress impending signature broke george washington walking stick sc statehouse yankee rebel exgovernor hegseth halted weapon ukraine military analysis aid wouldnt jeopardize readiness legislature act pernicious effect cellphone school trump success rate far budget cut harmful health nutrition budget cut harmful health nutrition youre smarter slate associate writer find quiz editorial cartoon world mostly trump tariff deadline loom stock set record trump pitch plan allowing farmer vouch illegal immigrant worker facing deportation blaze engulfs la amid active firework strike air traffic controller disrupting travel france trump ag secretary irony meter exploding left center beyond parody spin trump decision end taxfree loophole lowvalue good china lead sharp decline air cargo shipment cyber school facing wrongful death suit unreasonable teacher student weekly opinion blockbuster questionable advice summer movie pa republican gamble rural health care megabill push cumberland county optimistic memo improve coordination library system galasso look forward tomorrow expectantly beyond circumstance joey chestnut coney island expected dominate hot dog eating contest trump proposes ufc fight white house celebrate independence england sky stay friday night firework colombia announce recall envoy amid diplomatic rift lucas trump demand unconditional surrender democrat party hygiene rating handed doncaster establishment major improvement elephant kill female tourist uk zealand zambian national park missouri restricting abortion blocked judge iredell county name rodney harris deputy county manager iran try keeping military commander secret mossad offer guessing game confirms winner atlanta clogged road rage motorist opinion challenge opportunity bright future ct dairy farming trump tear marxist lunatic mamdani honor american hero bold rebuke play p plus free game xrp market confidence lightchain ai latejuly launch prepares broaden investor option rosen nationally regarded investor counsel encourages reckitt benckiser plc investor secure counsel important deadline security class action rbgly robinhood redo wall street blockchain gizmodo tempus ai stock soared japan brace quake authority dismiss doomsday hype opec plus agrees pump oil august york trump reportedly iran ok strike attack ahead understand poland blast trumpputin dialogue drone strike escalation walmart selling calvin klein eternity perfume shopper unbeatable deal business pm business pm business pm business pm newest stock sp soared since ipo buy according wall street newest stock sp soared since ipo buy according wall street watching brain drain real openai hit hard researcher defect rival tech giant meta rude baguette best amazon prime deal save gear blink anker samsung others engadget nextgen ai social startup backed thrive combinator shaping brink another consumer wave click sugar gambling world quick pleasure addiction expert dopamine fast amazon double robotaxis amzn stock buy charlize theron choosing single call daddy sign strength relationship expert future ai selfdriving car mechanical weeding health care assistant patriotic parade park market hidden delivering fast gain romantic drama ott watch weekend habit separate high achiever everyone else best altcoins next bull run blockdags summer raffle roi feature alongside inj rndr tia forgotten megatrend ai economy quality nonus stock buy simply staggering cnn correspondent describes floodwater impact texas good stock worth buying market matt mower nato summit europe free ride line archer aviation bet take sooner oneofakind brewery taproom closing bankruptcy oneofakind brewery taproom closing bankruptcy trump hit backlash antisemitic slur iowa rally stage almost arctic pablos price hike imminent myro housecoin push forward shopper race item major closing sale iconic activewear brand shuts store investor deadline robbins geller rudman dowd llp announces sarepta therapeutic srpt investor substantial loss opportunity lead class action lawsuit budget deficit opec increase output barrel august oil market btc miner cloud mining platform strives offer stability security bitcoin crossed k amazon prime best deal plus everything else engadget iowa rolling trans civil protection taken effect thinkcarebelieve america victory walmart selling sleek digital camera shopper look professional subaru launch killer legacy lease offer short anime watch weekend odd taxi death parade safeway strike end albertsons local union reach agreement colorado public radio headed sentencing sean diddy comb lawyer aim longer bad boy life average american family millionaire join kid</t>
         </is>
       </c>
     </row>
@@ -802,12 +798,12 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>medius now fully qualified yardi ecosystem partner cohen milstein seller toll pllc and bernstein litowitz berger grossmann llp announce pendency and proposed settlement of class action involving all person and entity who purchased or otherwise acquired the publicly traded common stock and preferred stock of silvergate capital corporation from november through march inclusive or in andor traceable to security offering during medius now fully qualified yardi ecosystem partner what you need to know ahead of live nation entertainment earnings release what you need to know ahead of live nation entertainment earnings release bloomberg law host ai symposium exploring the future of legal technology score prime day clothing deal on levi crocs spanx more starting at new york post thursday july evening cable news rating fillin host win the day ovation healthcare and ludi partner to streamline operational efficiency and financial health for rural hospital can micron stock hit in can micron stock hit in sealsq commences global deployment of it gsmaaccredited euicc with telco integrating a pioneering postquantum ready cryptographic security technology manulife investment management close third coinvestment fund at b surpassing predecessor by over m mitrex set guinness world record with largest bipv solar panel mural at sunrise residential longeveron announces u fda approval of ind application for a phase pivotal registration study evaluating laromestrocel a a treatment of pediatric dilated cardiomyopathy dcm saudi arabia crude oil export jumped by bpd in april substratelike pcb market size to hit usd billion by driven by demand for compact highperformance electronics research by sn insider application for delisting of sdrs from nasdaq stockholm what to expect from mondelez international q earnings report what to expect from mondelez international q earnings report amazon share form golden cross a prime day kick off national beverage credit lacroix marketing with q fiscal year growth world no magnus carlsen add to grand chess tour legacy with victory in zagreb at superunited rapid blitz croatia quanterix close m akoya deal after competing bid leading and lagging sector for july courtney caputo named chair of the national board of director at the epilepsy foundation of america optical imaging market to reach usd billion by fueled by rising demand for noninvasive diagnostic technology and octdriven clinical expansion sn insider courtney caputo named chair of the national board of director at the epilepsy foundation of america giant pigeon float through nyc for fifa club world cup what you need to know ahead of republic service earnings release what you need to know ahead of republic service earnings release column london metal exchange reaps the reward of tariff turmoil franklin resource quarterly earnings preview what you need to know franklin resource quarterly earnings preview what you need to know the salvation army to collect school supply at rochester walmart store elon musk fan took her first tesla robotaxi ride but then it made her get out and left her stranded cuz it wa about to rain unforgettable edible close after year on northwest side chile post steepest monthly price drop since ahead of rate decision what to expect from union pacific next quarterly earnings report what to expect from union pacific next quarterly earnings report the electric porsche macan is outselling the gas model but there more to the story motorcom the energy report so much for weak demand top company offering remote data science job why is penny stock prokidney stock trading higher on tuesday why is penny stock prokidney trading higher on tuesday robotics frenzy grip hong kong market and stock ride the hype is the rally sustainable goelzer investment management inc boost position in meta platform inc nasdaqmeta checchi capital adviser llc sell share of meta platform inc nasdaqmeta palisade capital management lp decrease stock holding in meta platform inc nasdaqmeta mountain capital investment advisor inc sell share of meta platform inc nasdaqmeta whimstay open platform to independent host for the first time netanyahu present trump with nomination for nobel peace prize a both downplay twostate solution cemtrexs vicon secures m followon order for county security infrastructure expansion cemtrexs vicon secures m followon order for county security infrastructure expansion barlow wealth partner inc acquires share of meta platform inc nasdaqmeta netsol technology appoints ian smith to it board of director aurora private wealth inc raise stock holding in meta platform inc nasdaqmeta netsol technology appoints ian smith to it board of director meta platform inc nasdaqmeta share acquired by sitrin capital management llc tkg advisor llc ha holding in meta platform inc nasdaqmeta ap business summarybrief at am edt at least may have killed themselves over uk post office wrongful conviction scandal why i always convert word to pdf now elon musk lash out at tesla bull dan ives over board proposal shut up how can large enterprise navigate tcpa compliance challenge percepta celebrates year of transforming automotive customer experience waymo offer teen account for driverless ride villa vie residence celebrates th visited port with summer celebration sale wednesday july evening cable news rating fox news stay no public record investment group buy ocean view apartment in norfolk k pure solution announces major strategic bleach distribution deal for the southwestern u mainly southern california u space force space system command selects rise for forge path to production contract inmorphis acquires servicenow practice of solugenix strengthening u market presence and expanding industryaligned offering in july and beyond honoring bebe moore campbell legacy u space force space system command selects rise for forge path to production contract deep dive into alcoa stock analyst perspective rating companion spine llc announces definitive agreement to acquire the business and asset of paradigm spine gmbh and the coflex and cofix spine implant from xtanttm medical holding inc what analyst are saying about edward lifesciences stock xsolis aidriven solution new feature evaluated in klas second look report what analyst rating have to say about kla petsmart name top catloving city tegna to host second quarter earnings conference call on thursday august startup raise m for universal flu vaccine made with mrna community bankshares inc revolutionizes access to capital and speed up loan closure for assessing enovis insight from financial analyst abbott laboratory stock a deep dive into analyst perspective rating is gaming and leisure prop gaining or losing market support whats driving the market sentiment around kbr breaking down agilent technology analyst share their view what to expect from norfolk southerns q earnings report what to expect from norfolk southerns q earnings report use this amex trick to save up to on amazon prime day locumtenenscom and march of dime partner to expand and scale maternal mental health training for clinician milliman analysis corporate pension funding improves in june to highest level since october milliman analysis corporate pension funding improves in june to highest level since october honor education secures m series a to reinvent digital learning experience outcome capital launch the first dedicated ophthalmology practice to address the world leading cause of disability can adobe stock hit in can adobe stock hit in instant legislation limit hoa enforcement in california swamp game at alligator alcatraz mamdanis socialist nightmare and more from fox news opinion hillsborough county target ruskin property for new sewer system vacuum lift station to boost environment and health south carolina gop urge trump supporter to give gavin newsom a huge southern welcome federal judge nix wisconsin judge bid to dismiss charge of helping illegal immigrant evade ice mona charen we need to remember the nobility of this nation trump extends federal hiring freeze until october use this amex trick to save up to on amazon prime day american kid have become increasingly unhealthy over nearly two decade new study find trump rip reporter for asking about epstein case a american doubt doj conclusion braille institute welcome distinguished tech executive roberto medrano to board of director northwestern energy adapts a demand evolve brian bird code for america unveils new government ai landscape assessment letter to the editor response to congressman downing sensorium therapeutic receives fda ind clearance for sntx a firstinclass rapidacting anxiolytic manatt enhances entertainment offering with leading film and tv partner montana conservation voter scorecard cut through noise kearstyn cook gov jim pillen sends nebraska urban searchandrescue team to help after texas flooding who had montana back the scorecard expose the record kearstyn cook who had montana back the scorecard expose the record kearstyn cook intention rise expectation fall the number of american planning to leave an inheritance go up a the number expecting to receive one go down find northwestern mutuals planning progress study jerome christenson closing the book on mailorder book club will we miss them big brother big sister of america appoints terrance williams of trustage a newest board member the u air force might send it retired b bomber to israel bad idea impactivize shareholder of company worth trillion vote overwhelmingly to defeat antidei proposal a a travel editor these are the amazon prime day deal id actually pack michelinstarred sushi aseat dinner vice president vance wrap up california visit someone using ai to impersonate marco rubio contacted at least five people including foreign minister cable say nyse content advisory premarket update trump announces new tariff on country trump slam russiaukraine war a bidencreated monster while unveiling new aid package ice raid derail southern california economy a worker go into hiding samsungs the frame make a gorgeous unique tv even better texas lawmaker want investigation into weather alert system and storm preparedness dr elseys reinforces it longstanding commitment to safer unscented cat litter presence of ice inside california hospital denounced by local leader immigration activist kinder and u soccer foundation launch goal of joy to inspire more active and joyful community through soccer the latest trump delay tariff implementation another month pastor who endorse political candidate shouldnt lose taxexempt status irs say in filing mob in rural india kill family accused of witchcraft iova notice iovance biotherapeutics shareholder are notified of the pending class action lawsuit contact bfa law by july court deadline nasdaqiova rich lowry dont blame donald trump for flood hims notice hims hers health inc shareholder are notified of the pending class action lawsuit contact bfa law by august court deadline nysehims aapl notice apple inc shareholder are notified of the pending class action lawsuit contact bfa law by august court deadline nasdaqaapl rddt notice reddit inc shareholder are notified of the pending class action lawsuit contact bfa law by august court deadline nyserddt ftre notice fortrea holding inc shareholder are notified of the pending class action lawsuit contact bfa law by august court deadline nasdaqftre i spent five week with the new roku ultra to see if you should upgrade video show deadly fire at cairo telecommunication building picking that bow back up northern cheyenne youth reconnect with archery letter to the editor independence day spark feeling ogn notice organon co shareholder are notified of the pending class action lawsuit contact bfa law by july court deadline nyseogn apple watch ultra review still the smartwatch to get horsemounted federal agent descend on los angeles park on video the google pixel watch finally delivers the big upgrade weve been waiting for lgs transparent oled tv just blew my mind at ce united by hatred vance rip mamdani expose the american left contradiction peace through power it electric injured after motorcycle strike deer on highway what if superman existed in a world like ours director james gunn on new superhero movie the best apple watch to buy in tested by expert trump outrage is hiding the real danger to america swiss village brace for possible alpine rockslide man dy at milan airport after being sucked into jet engine local medium report target of trump new tariff speak out the best sleep tracker in tested by editor tiger lsu purple and more it fig season here are tip to optimize your harvest letter to the editor wake up montana mississippi state university announces spring honor student rotary club of zachary present scholarship puretalk and allegiance flag supply honor veteran with americanmade flag nationwide zachary high school bronco explorer travel to japan ethel student named to washburn honor roll beta sigma phi member donate snack to eastside fire department letter denying global warning isnt cool held in texas immigration detention center shooting that wa planned ambush u attorney say the apple watch series is the smartwatch most people should buy kansa city chief heiress turn to scripture after yearold cousin killed in texas flood why the israeliran ceasefire feel like a strategic failure the best vacuum for pet hair in tried and tested why airtags are the ultimate travel companion this holiday season report accuses hamas of sexual violence i tried the latest version of the internetfamous bissell little green here my review sen ted cruz caught sightseeing in greece amid devastating flood in his home state a state attorney general say welcoming child of all race is illegal ideology opinion i really like the amazon kindle colorsoft but is color worth italy bergamo airport suspends flight after a person reportedly got sucked into engine the blink mini is a tiny camera that make your home a lot smarter a long hot summer day on the ground of st andrew conjures movie magic from yesteryear copy nurse practitioner kelsey st arnaud join north oak primary care in hammond joel boerkey named to the spring dean list at lincoln memorial university louisiana farm bureau elect officer during convention letter to the editor chinese communist party influence on american soil i cant stop using the ipad mini even though it a pretty boring update i tested this smart ipl device for athome hair removal and im never going to the salon again trial underway for ucla professor who refused to exercise compassion with racebased grading the google pixel tablet is a great slate that double a a smart display i tested the viral wavytalk thermal brush i didnt love it but here why you might egypt arrest famed belly dancer world focus the beijing olympics a pivotal moment for china key advisor called hunter bidens role on strategy call inappropriate after he overruled legal guidance letter to the editor dont pull plug on energy credit editorial cartoon for tuesday july</t>
+          <t>tribe property technology announces closing of best effort public offering of unit with full exercise of overallotment option for gross proceeds of approximately will recent event dent palantir technology stock growth sinopec launch new floating solar project with green hydrogen in play storen leading the future of home energy storage scottscott attorney at law llp file security class action against reckitt benckiser group plc otc rbgly chime financial first internetnative juggernaut focused on consumer banking say bullish analyst stock making big midday move tesla uber royal gold stellantis wns and more jeldwen expands cradle to cradle certification expanding portfolio of certified sustainable door energy demand optimism and houthi rebel attack on red sea shipping boost crude price nombase powered by bevnet launch new data hub a centralized resource for food beverage beer industry report iceland seafood international hf refinancing completed big beautiful bill may help some senior on social security but it doesnt eliminate tax on benefit noridian renews commitment to continuous improvement with the promotion of jeremiah mckay nvidias ai chip rival groq launch first european data center top ai growth stock to buy in july amazon prime day is here what it mean for the stock barrons fella it time to spice up your life with the help of lynks sexual wellness collection oneoncology appoints dr michael byrne a medical director for cellular therapy investing veteran see market pricing maseratis like ford tune in at noon workplace have embraced mindfulness and selfcompassionbut did capitalism hijack their true purpose google want to hit net zero by so it signed a massive deal with a bill gatesbacked startup thats still year away from making energy could amd and nvidia face new ai chip export restriction petco health and wellness company inc nasdaq woof shareholder alert bernstein liebhard llp reminds petco health and wellness company inc investor of upcoming deadline dhls german postal unit aim to increase use of parcel locker noridian renews commitment to continuous improvement with the promotion of jeremiah mckay rubis halfyear statement on rubis liquidity agreement with exane bnp paribas gtt monthly disclosure of the total number of voting right and share composing the share capital top trending meme coin breaking the internet arctic pablo freeze out the competition a fartboy and mubarak coin rise noridian renews commitment to continuous improvement with the promotion of jeremiah mckay kpn report on progress of m share buyback gtt halfyear liquidity contract statement asm share buyback update june july fnac darty disclosure of trading in own share june to july in french only this solanafocused etf by rexosprey offer a new way to earn from crypto wmo weather forecast for come true year early sarepta therapeutic inc nasdaq srpt shareholder alert bernstein liebhard llp reminds sarepta therapeutic inc investor of upcoming deadline thread is nearing x daily app user new data show techcrunch brazil to return to global bond market this year treasury secretary say planned parenthood sue trump administration over planned defunding gold price retreat to oneweek low on u tariff delay microstrategy paused it bitcoinbuying spree last week california bill seek to rein in debt settlement company that target mcas business loan borrower ageas report on the progress of share buyback programme luxury housing market no longer out of reach for some moveup buyer report homebuyers given new way to pay for a house after gamechanging policy switch and it not with cash up in a month should you buy plug power stock here yearold ran a one direction fan account a a teennow she run a medium brand with m follower including lorde and bella hadid i love my job rarely offered donut selling for off at krispy kreme on world chocolate day what will happen to the housing market during a baby dust taste radio one of the best trade show weve ever attended fancy that strait of hormuz in the spotlight forvia total number of voting right and share forming the share capital rite aid in ashland closing this summer gray and scripps to swap station and create more duopolies were booking profit in a topperforming bank stock in an extremely overbought market can trump run it hot plan trap the fed and jolt the bond market u child are much more likely to die than kid in similar country study find here how much invested in rtx year ago would be worth today best credit card for amazon of why everyones wrong about xrps real value a spacepay aim to become a top crypto payment solution weekly report share buyback from june to july weekly report share buyback from june to july historic yes could be better how to access perplexity ai free version fake image detection market is poised to expand beyond u million by say astute analytica uk fund invests million in carbon capture project hipgnosis founder talk new venture eye buying back catalog from blackstone the best amazon prime day deal under save on gear from samsung blink anker and others engadget lululemon v dupe texas flood live update death roll rise to a nw warns of more flooding trump say he will begin announcing trade deal and tariff rate at noon sinclair name narinder sahai evp and cfo sonar enhances oracle otm integration and launch shipper consortium for unmatched supply chain benchmarking palantir stock go warp speed but there a caveat walmart sam club and the walmart foundation commit up to to support texas flood relief effort explaining assessing the digital service tax dilemma gunman ambush border patrol agent in texas amid antiice rhetoric from democrat unmanned saildrones track russian shadow fleet during nato baltic sea operation jeldwen expands cradle to cradle certification expanding portfolio of certified sustainable door chase sapphire reserve lounge access in whats actually included tesla stock price fall after elon musk plan new political party micron meteoric rise can mu stock hit in ai is the new oil and america is laying the pipeline dow industrials intraday decline now exceeds point live update which worker will ai hurt most the young or the experienced the new york time will ai replace new hire or middle manager your job interviewer is not a person it ai catch up on your reading list this prime day with up to off kindles tesla trouble amplified by musk party politics etf on edge yemen houthi rebel say bulk carrier magic sea that they attacked sunday ha sunk starbucks launch new frappuccino kusacom hims hers navigates novo nordisk breakup and compounding lawsuit italy shipbuilder appoints new u chief trump administration move to terminate a form of humanitarian relief for nicaraguan and honduran in the u global wet chemical in semiconductor market forecast usd b by driven by advanced node manufacturing valuates report st elizabeth hospital and flight for life celebrate one year in fort morgan almonty industry applies for nasdaq listing elon musk realized too late how badly tesla will hurt from trump bill electrek ascendion win gold a the artificial intelligence service provider of the year in globee award borr drilling announces first settlement of the offering of common share brcevichelivjpg trump and netanyahu may take a victory lap on iran but the gaza war loom over their meeting alaskan lng the future of natural gas brcevichelivjpg brcevichelivjpg brcevichelivjpg brcevichelivjpg opinion reclaiming my time what in the hell happened bannon blast doj over epstein announcement daily beast try to use texas tragedy to attack ted cruz man killed after shooting at a u border patrol facility in southern texas u will make several trade announcement in next hour bessent hakeem jeffries roasted for obviously photoshopped instagram post a man ha been killed after opening fire at a u border patrol facility in texas authority say musk say he forming a new political party after split with trump over tax cut law strait of hormuz in the spotlight first look swapping beer for pisco sour see dive bar new life a madisonville restaurant society of st vincent de paul usa president john berry say work to protect the poor must go on after reconciliation bill passage liberal critic question why architect of failed biden foreign policy is advising project man killed after shooting at a u border patrol facility in southern texas american kid have become increasingly unhealthy over nearly two decade new study find patricia lopez ice doesnt need another billion surprise dems medium lie blame trump for storm death ken morris you may not be a diversified a you think rep carlos barron elected a state house minority whip tiktok user try to make texas flood all about race u child are much more likely to die than kid in similar country study find carnival cruise update rule critic cry racism trump threatens not to chicken out yet again over tariff democrat trying to field candidate slate to win first statewide race in year dccc target house republican over budget law impact on rural hospital dem lawmaker say their voter are threatening blood and violence over inability to hinder trump report dhs terminates temporary protected status for around k honduran nicaraguan migrant top maga voice stunned by trump administration debunking epstein theory jesse jackson jr explores a house comeback bid california expands automatic renewal law new requirement now in effect louisiana state police arrest woman in connection with motorcycle death of shreveport man gang burn down famous haitian hotel trump administration move to terminate a form of humanitarian relief for nicaraguan and honduran in the u leave bolsonaro alone trump furious a brazil exleader face coup trial mainer need to do what democracy demand letter maga influencers scream coverup following release of doj memo closing the book on jeffrey epstein case editorial chicago mourns with texas and the parent of the camp mystic girl schumer demand investigation of trump weather service vacancy in wake of texas flooding schumer demand investigation of trump weather service vacancy in wake of texas flooding schumer demand investigation of trump weather service vacancy in wake of texas flooding yemen houthi rebel say bulk carrier magic sea that they attacked sunday ha sunk schumer demand investigation of trump weather service vacancy in wake of texas flooding schumer demand investigation of trump weather service vacancy in wake of texas flooding schumer demand investigation of trump weather service vacancy in wake of texas flooding holy cross cattleman asks for permit to kill copper creek wolf u to revoke protected status for immigrant from honduras and nicaragua u chamber of commerce discusses how tariff will raise the cost of summer fun with yourupdatetv u cancel contract save million in day doge former librarian of congress fired by trump vow to improve public information in new mellon role former librarian of congress fired by trump vow to improve public information in new mellon role trump say he will visit texas probably on friday to tour flash flood damage mcafees summer shopping study reveals it prime time for smart shopping team technology an arlington capital partner portfolio company expands medical device manufacturing capability with acquisition of duke empirical inc trump th week in office set to include visit to texas devastated hill country third netanyahu meeting i dont use credit card point to shop for prime day here what i do instead this senator just sold up to k in unitedhealth group stock recent filing show that rep john rose sold over m worth of alphabet stock u lobby group urge tariff retaliation against australia socialised medicine face the nation stoltenberg panel wear it or resist anne hanson time to reboot lucy k wyman peacham th of july dave edward michael paul williams maga turn back the clock at uva proposed radio tower cynthia krieble abm announces new board of director and executive committee member threat to freedom of religion denise fontaine court release cctv footage shown during mushroom murder trial maine ban floating camp another big week for nepa new federal procedure and a big beautiful bill benefit the mindful minute by jon heydenreich my menu correction osisko development announces positive bulk tonnage ore sorting result for the project worldwide bolster indiasouth asia leadership with strategic appointment educator view throw a book at your kid to avoid summer slide jeffery epstein died by suicide and there no client list justice department say houston official fired over raciallytinged tiktok rant about search for missing girl man with rifle and tactical gear killed after exchange of fire with border patrol in texas prominent west bank sheikh face violent threat after proposing peace with israel zelenskyy spoke with trump on replacing kyivs envoy to u israel and hamas are inching toward a new ceasefire deal for gaza this is how it might look chrome day ivanti exploit macos stealer crypto heist and more russia exminister found dead hour after being fired in an apparent suicide official said don davis eye open north carolina senate seat white house asks american to pray after deadly texas flooding planned parenthood challenge gop reconciliation law north carolina also hit with lifethreatening flash flood governor murphy mansion tax modification breaking leo source report active shooter with rifle and tactical gear ambushed border patrol agent french gameshow contestant epic month winning streak finally end a reignited trumpmusk feud burn tesla investor share of ev company tumble a reignited trumpmusk feud burn tesla investor share of ev company tumble p miner launch the world first xrp liquid mining aidriven multiasset putting up the closed sign trump policy have cost vital u business b see what first responder are facing in texas a they search for victim airwavz solution appoints monte dube to market advisory board to strengthen healthcare wireless strategy hidden megabill clause hand taxpayer bill for huge gift to private jet owner church street closed for new sewer line trump administration revoke terrorism designation of new syrian leader group mayor adam hears community concern on housing ebikes education at bayside town hall flatbread barbecue and more best thing we ate this week in baton rouge and acadiana faimon robert how this la rural sheriff is remaking his office and redefining progressive the battle over the big beautiful bill move from capitol hill to the campaign trail global trade is back in limbo revealed white house email show desperate rush to punish university</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>medius fully qualified yardi ecosystem partner cohen milstein seller toll pllc bernstein litowitz berger grossmann llp announce pendency proposed settlement class action involving entity purchased otherwise acquired publicly traded common stock preferred stock silvergate corporation november march inclusive andor traceable security offering medius fully qualified yardi ecosystem partner ahead nation entertainment earnings release ahead nation entertainment earnings release bloomberg host ai symposium exploring future legal technology score prime clothing deal levi crocs spanx starting new york post thursday evening cable rating fillin host ovation healthcare ludi partner streamline operational efficiency financial health rural hospital micron stock hit micron stock hit sealsq commences global deployment gsmaaccredited euicc telco integrating pioneering postquantum ready cryptographic security technology manulife investment close third coinvestment fund b surpassing predecessor mitrex set guinness world record largest bipv solar panel mural sunrise residential longeveron announces fda approval ind application phase pivotal registration study evaluating laromestrocel treatment pediatric dilated cardiomyopathy dcm saudi arabia crude oil export jumped bpd april substratelike pcb market size hit usd billion driven demand compact highperformance electronics research sn insider application delisting sdrs nasdaq stockholm expect mondelez international q earnings report expect mondelez international q earnings report amazon share form golden cross prime kick national beverage credit lacroix marketing q fiscal growth world magnus carlsen add grand chess tour legacy victory zagreb superunited rapid blitz croatia quanterix close akoya deal competing bid leading lagging sector courtney caputo named chair national board director epilepsy foundation america optical imaging market reach usd billion fueled rising demand noninvasive diagnostic technology octdriven clinical expansion sn insider courtney caputo named chair national board director epilepsy foundation america giant pigeon float nyc fifa club world cup ahead republic service earnings release ahead republic service earnings release column london metal exchange reaps reward tariff turmoil franklin resource quarterly earnings preview franklin resource quarterly earnings preview salvation army collect school supply rochester walmart store elon musk fan took tesla robotaxi ride left stranded cuz rain unforgettable edible close northwest chile post steepest monthly price drop since ahead rate decision expect union pacific next quarterly earnings report expect union pacific next quarterly earnings report electric porsche macan outselling gas model story motorcom energy report weak demand company offering remote data science job penny stock prokidney stock trading higher tuesday penny stock prokidney trading higher tuesday robotics frenzy grip hong kong market stock ride hype rally sustainable goelzer investment boost meta platform nasdaqmeta checchi adviser sell share meta platform nasdaqmeta palisade lp decrease stock meta platform nasdaqmeta mountain investment advisor sell share meta platform nasdaqmeta whimstay open platform independent host netanyahu present trump nomination nobel peace prize downplay twostate solution cemtrexs vicon secures followon order county security infrastructure expansion cemtrexs vicon secures followon order county security infrastructure expansion barlow wealth partner acquires share meta platform nasdaqmeta netsol technology appoints ian smith board director aurora private wealth raise stock meta platform nasdaqmeta netsol technology appoints ian smith board director meta platform nasdaqmeta share acquired sitrin tkg advisor meta platform nasdaqmeta business least killed uk post office wrongful conviction scandal always convert word pdf elon musk lash tesla bull dan ives board proposal shut large enterprise navigate tcpa compliance challenge percepta celebrates transforming automotive customer experience waymo offer teen account driverless ride villa vie residence celebrates visited port summer celebration sale wednesday evening cable rating fox stay public record investment buy ocean view apartment norfolk k pure solution announces major strategic bleach distribution deal southwestern mainly southern california space force space system command selects rise forge path production contract inmorphis acquires servicenow practice solugenix strengthening market presence expanding industryaligned offering beyond honoring bebe moore campbell legacy space force space system command selects rise forge path production contract deep dive alcoa stock analyst perspective rating companion spine announces definitive agreement acquire business asset paradigm spine gmbh coflex cofix spine implant xtanttm medical analyst saying edward lifesciences stock xsolis aidriven solution new feature evaluated klas look report analyst rating kla petsmart name catloving tegna host quarter earnings conference call thursday august startup raise universal flu vaccine mrna community bankshares revolutionizes access speed loan closure assessing enovis insight financial analyst abbott laboratory stock deep dive analyst perspective rating gaming leisure prop gaining losing market support whats driving market sentiment around kbr breaking agilent technology analyst share view expect norfolk southerns q earnings report expect norfolk southerns q earnings report amex trick save amazon prime locumtenenscom march dime partner expand scale maternal mental health training clinician milliman analysis corporate pension funding improves highest level since october milliman analysis corporate pension funding improves highest level since october honor education secures series reinvent digital learning experience outcome launch dedicated ophthalmology practice address world leading cause disability adobe stock hit adobe stock hit instant legislation limit hoa enforcement california swamp game alligator alcatraz mamdanis socialist nightmare fox opinion hillsborough county target ruskin property new sewer system vacuum lift station boost environment health south carolina gop urge trump supporter give gavin newsom southern welcome federal judge nix wisconsin judge bid dismiss charge helping illegal immigrant evade mona charen remember nobility nation trump extends federal hiring freeze october amex trick save amazon prime american kid become increasingly unhealthy nearly decade new study find trump rip reporter asking epstein american doubt doj conclusion braille institute welcome distinguished tech executive roberto medrano board director northwestern energy adapts demand evolve brian code america unveils new government ai landscape assessment editor response congressman downing sensorium therapeutic receives fda ind clearance sntx firstinclass rapidacting anxiolytic manatt enhances entertainment offering leading film tv partner montana conservation voter scorecard cut noise kearstyn cook gov jim pillen sends nebraska urban searchandrescue team help texas flooding montana scorecard expose record kearstyn cook montana scorecard expose record kearstyn cook intention rise expectation fall american planning inheritance expecting receive find northwestern mutuals planning progress study jerome christenson closing book mailorder book club miss brother sister america appoints terrance williams trustage newest board air force send retired b bomber israel bad idea impactivize shareholder company worth trillion vote overwhelmingly defeat antidei proposal travel editor amazon prime deal id pack michelinstarred sushi aseat dinner vice president vance wrap california visit someone ai impersonate marco rubio contacted least five people foreign minister cable nyse content advisory premarket update trump announces new tariff country trump slam russiaukraine war bidencreated monster unveiling new aid package raid derail southern california economy worker hiding samsungs frame gorgeous unique tv better texas lawmaker investigation weather alert system storm preparedness dr elseys reinforces longstanding commitment safer unscented cat litter presence inside california hospital denounced local immigration activist kinder soccer foundation launch goal joy inspire active joyful community soccer latest trump delay tariff implementation another month pastor endorse political candidate shouldnt lose taxexempt status irs filing mob rural india kill family accused witchcraft iova notice iovance biotherapeutics shareholder notified pending class action lawsuit contact bfa deadline nasdaqiova rich lowry dont blame donald trump flood hims notice hims health shareholder notified pending class action lawsuit contact bfa august deadline nysehims aapl notice apple shareholder notified pending class action lawsuit contact bfa august deadline nasdaqaapl rddt notice reddit shareholder notified pending class action lawsuit contact bfa august deadline nyserddt ftre notice fortrea shareholder notified pending class action lawsuit contact bfa august deadline nasdaqftre spent five new roku ultra upgrade video deadly fire cairo telecommunication building picking bow northern cheyenne youth reconnect archery editor independence spark feeling ogn notice organon co shareholder notified pending class action lawsuit contact bfa deadline nyseogn apple watch ultra review smartwatch horsemounted federal agent descend los angeles park video google pixel watch finally delivers upgrade weve waiting lgs transparent oled tv blew mind ce united hatred vance rip mamdani expose american left contradiction peace power electric injured motorcycle strike deer highway superman existed world director james gunn new superhero movie best apple watch buy tested expert trump outrage hiding real danger america swiss village brace possible alpine rockslide man dy milan airport sucked jet engine local medium report target trump new tariff speak best sleep tracker tested editor tiger lsu purple fig season tip optimize harvest editor wake montana mississippi university announces spring honor student rotary club zachary present scholarship puretalk allegiance flag supply honor veteran americanmade flag nationwide zachary high school bronco explorer travel japan ethel student named washburn honor roll beta sigma phi donate snack eastside fire department denying global warning isnt cool texas immigration detention center shooting planned ambush attorney apple watch series smartwatch people buy kansa chief heiress turn scripture yearold cousin killed texas flood israeliran ceasefire feel strategic failure best vacuum pet hair tried tested airtags ultimate travel companion holiday season report accuses hamas sexual violence tried latest version internetfamous bissell little green review sen ted cruz caught sightseeing greece amid devastating flood attorney general welcoming child race illegal ideology opinion amazon kindle colorsoft color worth italy bergamo airport suspends flight reportedly got sucked engine blink mini tiny camera lot smarter hot summer ground st andrew conjures movie magic yesteryear copy nurse practitioner kelsey st arnaud join north oak primary care hammond joel boerkey named spring dean list lincoln memorial university louisiana bureau elect officer convention editor chinese communist party influence american soil cant stop ipad mini pretty boring update tested smart ipl device athome hair removal im never salon trial underway ucla professor refused exercise compassion racebased grading google pixel tablet great slate double smart display tested viral wavytalk thermal brush didnt love egypt arrest famed belly dancer world focus beijing olympics pivotal moment china advisor hunter bidens role strategy call inappropriate overruled legal guidance editor dont pull plug energy credit editorial cartoon tuesday</t>
+          <t>tribe property technology announces closing best effort public offering unit full exercise overallotment option gross proceeds approximately recent event dent palantir technology stock growth sinopec launch floating solar project green hydrogen play storen leading future energy storage scottscott attorney llp file security class action reckitt benckiser plc otc rbgly chime financial internetnative juggernaut focused consumer banking bullish analyst stock making midday move tesla uber royal gold stellantis wns jeldwen expands cradle cradle certification expanding portfolio certified sustainable door energy demand optimism houthi rebel attack red sea shipping boost crude price nombase powered bevnet launch data hub centralized resource beverage beer industry report iceland seafood international hf refinancing completed bill help senior social security doesnt eliminate tax benefit noridian renews commitment continuous improvement promotion jeremiah mckay nvidias ai chip rival groq launch european data center ai growth stock buy amazon prime stock barrons fella spice life help lynks sexual wellness collection oneoncology appoints dr michael byrne medical director cellular therapy investing veteran market pricing maseratis ford tune noon workplace embraced mindfulness selfcompassionbut capitalism hijack purpose google hit net zero signed massive deal bill gatesbacked startup thats away making energy amd nvidia face ai chip export restriction petco health wellness company nasdaq woof shareholder alert bernstein liebhard llp reminds petco health wellness company investor upcoming deadline dhls german postal unit aim increase parcel locker noridian renews commitment continuous improvement promotion jeremiah mckay rubis halfyear statement rubis liquidity agreement exane bnp paribas gtt monthly disclosure total voting composing trending meme coin breaking internet arctic pablo freeze competition fartboy mubarak coin rise noridian renews commitment continuous improvement promotion jeremiah mckay kpn report progress buyback gtt halfyear liquidity contract statement asm buyback update fnac darty disclosure trading french solanafocused rexosprey offer earn crypto wmo weather forecast come early sarepta therapeutic nasdaq srpt shareholder alert bernstein liebhard llp reminds sarepta therapeutic investor upcoming deadline thread nearing x app user data techcrunch brazil global bond market treasury secretary planned parenthood sue trump administration planned defunding gold price retreat oneweek low tariff delay microstrategy paused bitcoinbuying spree california bill seek rein debt settlement company target mcas business loan borrower ageas report progress buyback programme luxury housing market longer reach moveup buyer report homebuyers pay house gamechanging policy switch cash month buy plug power stock yearold ran direction fan account teennow run medium brand follower lorde bella hadid love job rarely offered donut selling krispy kreme world chocolate happen housing market baby dust taste radio best trade weve ever attended fancy strait hormuz spotlight forvia total voting forming rite aid ashland closing summer gray scripps swap station create duopolies booking profit topperforming bank stock extremely overbought market trump run hot plan trap fed jolt bond market child likely die kid similar country study find invested rtx ago worth best credit card amazon everyones xrps real value spacepay aim become crypto payment solution weekly report buyback weekly report buyback historic yes better access perplexity ai free version fake image detection market poised expand beyond million astute analytica uk fund invests million carbon capture project hipgnosis founder venture eye buying catalog blackstone best amazon prime deal save gear samsung blink anker others engadget lululemon v dupe texas flood update death roll rise nw warns flooding trump begin announcing trade deal tariff rate noon sinclair name narinder sahai evp cfo sonar enhances oracle otm integration launch shipper consortium unmatched supply chain benchmarking palantir stock warp speed caveat walmart sam club walmart foundation commit support texas flood relief effort explaining assessing digital service tax dilemma gunman ambush border patrol agent texas amid antiice rhetoric democrat unmanned saildrones track russian shadow fleet nato baltic sea operation jeldwen expands cradle cradle certification expanding portfolio certified sustainable door chase sapphire reserve lounge access whats included tesla stock price fall elon musk plan political party micron meteoric rise mu stock hit ai oil america laying pipeline dow industrials intraday decline exceeds update worker ai hurt young experienced york ai replace hire middle manager job interviewer ai catch reading list prime kindles tesla trouble amplified musk party politics edge yemen houthi rebel bulk carrier magic sea attacked sunday sunk starbucks launch frappuccino kusacom hims navigates novo nordisk breakup compounding lawsuit italy shipbuilder appoints chief trump administration move terminate form humanitarian relief nicaraguan honduran global wet chemical semiconductor market forecast usd b driven advanced node manufacturing valuates report st elizabeth hospital flight life celebrate fort morgan almonty industry applies nasdaq listing elon musk realized late badly tesla hurt trump bill electrek ascendion gold artificial intelligence service provider globee award borr drilling announces settlement offering common brcevichelivjpg trump netanyahu take victory lap iran gaza war loom meeting alaskan lng future natural gas brcevichelivjpg brcevichelivjpg brcevichelivjpg brcevichelivjpg opinion reclaiming hell happened bannon blast doj epstein announcement beast try texas tragedy attack ted cruz man killed shooting border patrol facility southern texas several trade announcement next hour bessent hakeem jeffries roasted obviously photoshopped instagram post man killed opening fire border patrol facility texas authority musk forming political party split trump tax cut strait hormuz spotlight look swapping beer pisco sour dive bar life madisonville restaurant society st vincent de paul usa president john berry work protect poor must reconciliation bill passage liberal critic architect failed biden foreign policy advising project man killed shooting border patrol facility southern texas american kid become increasingly unhealthy nearly decade study find patricia lopez doesnt another billion surprise dems medium lie blame trump storm death ken morris diversified rep carlos barron elected house minority whip tiktok user try texas flood race child likely die kid similar country study find carnival cruise update rule critic cry racism trump threatens chicken yet tariff democrat field candidate slate statewide race dccc target house republican budget impact rural hospital dem lawmaker voter threatening blood violence inability hinder trump report dhs terminates temporary protected status around k honduran nicaraguan migrant maga voice stunned trump administration debunking epstein theory jesse jackson jr explores house comeback bid california expands automatic renewal requirement effect louisiana police arrest woman connection motorcycle death shreveport man gang burn famous haitian hotel trump administration move terminate form humanitarian relief nicaraguan honduran bolsonaro alone trump furious brazil exleader face coup trial mainer democracy demand maga influencers scream coverup following release doj memo closing book jeffrey epstein editorial chicago mourns texas parent camp mystic girl schumer demand investigation trump weather service vacancy wake texas flooding schumer demand investigation trump weather service vacancy wake texas flooding schumer demand investigation trump weather service vacancy wake texas flooding yemen houthi rebel bulk carrier magic sea attacked sunday sunk schumer demand investigation trump weather service vacancy wake texas flooding schumer demand investigation trump weather service vacancy wake texas flooding schumer demand investigation trump weather service vacancy wake texas flooding holy cross cattleman asks permit kill copper creek wolf revoke protected status immigrant honduras nicaragua chamber commerce discusses tariff raise cost summer fun yourupdatetv cancel contract save million doge librarian congress fired trump vow improve public information mellon role librarian congress fired trump vow improve public information mellon role trump visit texas probably friday tour flash flood damage mcafees summer shopping study reveals prime smart shopping team technology arlington partner portfolio company expands medical device manufacturing capability acquisition duke empirical trump office set include visit texas devastated hill country third netanyahu meeting dont credit card shop prime instead senator k unitedhealth stock recent filing rep john rose worth alphabet stock lobby urge tariff retaliation australia socialised medicine face nation stoltenberg panel wear resist anne hanson reboot lucy k wyman peacham dave edward michael paul williams maga turn clock uva proposed radio tower cynthia krieble abm announces board director executive committee threat freedom religion denise fontaine release cctv footage shown mushroom murder trial maine ban floating camp another nepa federal procedure bill benefit mindful jon heydenreich menu correction osisko development announces positive bulk tonnage ore sorting project worldwide bolster indiasouth asia leadership strategic appointment educator view throw book kid avoid summer slide jeffery epstein died suicide client list justice department houston fired raciallytinged tiktok rant search missing girl man rifle tactical gear killed exchange fire border patrol texas prominent west bank sheikh face violent threat proposing peace israel zelenskyy spoke trump replacing kyivs envoy israel hamas inching ceasefire deal gaza look chrome ivanti exploit macos stealer crypto heist russia exminister found dead hour fired apparent suicide davis eye open north carolina senate seat white house asks american pray deadly texas flooding planned parenthood challenge gop reconciliation north carolina hit lifethreatening flash flood governor murphy mansion tax modification breaking leo source report active shooter rifle tactical gear ambushed border patrol agent french gameshow contestant epic month winning streak finally end reignited trumpmusk feud burn tesla investor ev company tumble reignited trumpmusk feud burn tesla investor ev company tumble p miner launch world xrp liquid mining aidriven multiasset putting closed sign trump policy cost vital business b responder facing texas search victim airwavz solution appoints monte dube market advisory board strengthen healthcare wireless strategy hidden megabill clause taxpayer bill gift private jet owner church street closed sewer line trump administration revoke terrorism designation syrian mayor adam hears community concern housing ebikes education bayside town hall flatbread barbecue best ate baton rouge acadiana faimon robert la rural sheriff remaking office redefining progressive battle bill move capitol hill campaign trail global trade limbo revealed white house email desperate rush punish university</t>
         </is>
       </c>
     </row>
@@ -838,12 +834,12 @@
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>what you need to know ahead of arch capital earnings release what really killed the mill reason to buy ethereum before what to expect from leidos holding q earnings report successful couple do these thing in the morning that little hello go a long way relationship expert say in a world of bull and bear be the tiger s ai launch agentic capability in latest molecular universe release to increase value proposition for rd a a service we found the best amazon prime day deal after shopping thousand of offer cnn most fed official see rate cut coming but opinion vary widely on how many minute show fury intercept m of lio at the ninaaskumuwin discovery incorporation of boerne in lawmaker will investigate response to flood covered call screener result for july th texas just passed quantum computing legislation how should you play ionq stock here homebuyers finally responded after mortgage rate hit lowest level in three month cnbc palantir technology ha been the sp s hottest stock over the past year and it not even close can it incredible rally continue cybersecurity stock you can buy and hold for the next decade business newsline july amazon extends prime day discount to day trump medium file for crypto blue chip etf vibe coding ha arrived for business wsj this bigname adviser say avoiding crypto is now a more speculative investment move than buying it marketwatch trump threatened to bomb the s out of moscow to deter putin cnn trump big beautiful bill promise no tax on tip and overtime but there a limitheres who qualifies droit launch explore mode on it adept platform h room for optimism risk for complacency aes freeportmcmoran verona pharma intel aehr penguin solution and more mover barrons michelle obama i learned this great parenting tip from my mom and dadthey did a beautiful job modeling it bmw v mercedes u sale race there a clear leader in linda yaccarino step down a ceo of elon musk x dax push higher a eu edge closer to tariff deal with u the prime day deal you can still get the verge eli manning say he no longer interested in buying a piece of the nfls giant it too expensive for me merck to acquire verona pharma expanding it portfolio to include ohtuvayre ensifentrine a firstinclass copd maintenance treatment for adult and expected to drive growth into the next decade merck to acquire verona pharma expanding it portfolio to include ohtuvayre ensifentrine a firstinclass copd maintenance treatment for adult and expected to drive growth into the next decade merckcom walmart is selling a fantastic chromebook laptop for just and shopper love the touchscreen feature these word help teach kid critical thinking say michelle obama and psychologist malaysian pm warns southeast asia that trade war is not a passing storm quadmotor rivians arrive with wild power and wilder price apple can it catch up in the ai race a rival turn up the heat boomer are buying the highestyielding dividend champion handoverfist a o smith corporation nyseaos share purchased by private trust co na elon musk grok ai chatbot denies that it praised hitler and made antisemitic comment daily vickers top insider pick for hudson edge investment partner inc ha million stock position in jpmorgan chase co nysejpm private trust co na ha stock holding in coterra energy inc nysectra rosalia is new balance newest brand ambassador russia launch another record drone attack on ukraine ukrainian official say beware of scam that promise good pay for completing easy online task beware of scam that promise good pay for completing easy online task today top money market account rate for july rate hit current heloc home equity loan rate july highyield saving account rate today july rate are steady beware of scam that promise good pay for completing easy online task ap news bank of england flag global debt pressure despite market stabilization goldman demand an oath from junior banker to fend off private equity poaching bloomberg court block rule that would let you cancel subscription easily sp future tick higher a investor shrug off trump tariff threat fomc minute on tap today mortgage refinance rate july rate increase mortgage rate today july rate move up cd rate today july rate rise uae say the oil market is thirsty for more opec barrel proposed clermont subdivision would redesign deadly lakeshore drive exact science announces medicare coverage for oncodetecttm molecular residual disease test in colorectal cancer fresh del monte produce inc to report second quarter financial result trump trade blitz produce few deal but lot of uncertainty trump trade blitz produce few deal but lot of uncertainty trump trade blitz produce few deal but lot of uncertainty trump trade blitz produce few deal but lot of uncertainty trump trade blitz produce few deal but lot of uncertainty trump trade blitz produce few deal but lot of uncertainty a new era of restaurant worker may earn sixfigure salary and benefit that no other industry can provide tesla board need ground rule for musk political activism analyst say samsung launch three new foldable smartphones a it fends off chinese rival trump tariff extension leaf bank fed in limbo hbo max is back prestige brand return to streaming corra group see rising demand from global investor for due diligence investigation market sputter after trump push tariff deadline xrp price forecast hit but insider are loading up on the new xrp that could go x auddia announces leadership change and special committee to evaluate business combination and restructuring a ai native holding company senate gop gear up for test on trump doge cut inside information orion upgrade fullyear outlook for social security sends million of american a misleading and blatantly political message see this shreveport director awardwinning screenplay red carpet premiere here how first atlantic nickel expands rpm zone awaruite nickelalloy nife discovery meter northern extension yield nickel concentrate over meter in dtr metallurgical recovery testing shreveport to kick off return of eleven store to louisiana more site planned two ragnarok ip title achieved top game ranking in taiwan hong kong and macau toast inc nysetost share acquired by da davidson co private trust co na ha stock holding in ge healthcare technology inc nasdaqgehc trump big beautiful bill slash cfpb funding what it mean for you davenport co llc sell share of fortive corporation nyseftv private trust co na acquires share of emcor group inc nyseeme you have less than month to claim the ev tax credit now is the time to buy say car expert this legend cross time zone with just pound of gear here are his favorite principal financial group inc increase stock position in zimmer biomet holding inc nysezbh mutual advisor llc buy share of trane technology plc nysett mutual advisor llc grows stock holding in decker outdoor corporation nysedeck first malaria drug for newborn and young infant expected to be approved in africa within week former rapid city anchor given suspended sentence in domestic assault case bank of england warns of high financial market risk despite easing tension kisti secures funding for national quantum center of excellence name ionq a primary quantum partner our opinion when the president punishes patriot wednesday letter a the world burn eye turn to diddy european court russia wa behind downing of mh watch popular podcaster discusses how kamala episode wa scrapped because she talked gibberish her own campaign wanted it canned fbi bust chinese national for multimillion dollar drug ring exploiting immigration system the president mean business trump admin sue california over transgender athlete policy other view state congressional delegation must fight cut to noaa burke county company say hildebran wont issue permit for train cabin business another voice buffalo garden vibrantly express a community soul trump admin subpoena harvard over foreign student misconduct campus radicalism george conway flag trump awkward new admission a fresh proof he a fool eu seek to finalize trade deal with trump by end of the month hawaii lawmaker demand immigration arrest briefing haleiwa development under council review state road usage charge begin for electric vehicle on july governor state budget veto trim public school maintenance hooser sbcd a travesty of process and policy senate gop gear up for test on trump doge cut senate gop gear up for test on trump doge cut jewish democrat in congress sound the alarm on mamdani tea party patriot to push lawmaker on noncitizen voting jewish democrat in congress sound the alarm on mamdani tea party patriot to push lawmaker on noncitizen voting senate gop gear up for test on trump doge cut larger fight rage on but trump racking up win against college tea party patriot to push lawmaker on noncitizen voting jewish democrat in congress sound the alarm on mamdani larger fight rage on but trump racking up win against college larger fight rage on but trump racking up win against college senate gop gear up for test on trump doge cut senate gop gear up for test on trump doge cut tea party patriot to push lawmaker on noncitizen voting jewish democrat in congress sound the alarm on mamdani tea party patriot to push lawmaker on noncitizen voting jewish democrat in congress sound the alarm on mamdani senate gop gear up for test on trump doge cut larger fight rage on but trump racking up win against college tea party patriot to push lawmaker on noncitizen voting larger fight rage on but trump racking up win against college jewish democrat in congress sound the alarm on mamdani larger fight rage on but trump racking up win against college candace cameron bure say son biblebased pep talk helped save her marriage antiviolence advocate why not hold gun manufacturer accountable for mass shooting like river north tragedy letter chicago allows people to be who they want to be trump trade blitz produce few deal but lot of uncertainty laura washington the art institute is slowly getting back to normal georgia police arrest farmworkers then get warrant from dhs firearm testing and ballistics unit could be open in september at county forensics lab former dc fire official want to cut tax increase police presence with city council bid my view trekking pole can lend some mountainclimber swagger steve corbin give me liberty or a tinpot dictator scare buying reported in rochester why should legislator favor legal pot business california focus why should legislator favor legal pot business california focus editorial cartoon for july this legend cross time zone with just pound of gear here are his favorite which u president had wife named ellen and edith first malaria drug for newborn and young infant expected to be approved in africa within week red bull team principal christian horner fired after year with team after month stuck in the south north korean go home letter billion not served by trump big bill letter billion not served by trump big bill supreme court reject shielding identity of police attending jan capitol rally trump slam democrat over inflation narrative say he cut cost more than any president in history red bull team principal christan horner sacked after year with team letter no one is voting after result are known letter no one is voting after result are known here everything to expect at this family fun day in colnes alkincoates park robinhood ceo tokenization is a major innovation in capital market here who will and wont qualify for the new car loan interest deduction allegheny county council approves innamorato choice for shuman advisory board pittsburgh city council pass further protection for lgbtq people elon musk grok remove politically incorrect instruction after it praise hitler wa the flash flooding in texas preventable trump say tariff on pharmaceutical import could increase to percent threetime mvp nikola jokic will delay signing extension with nugget this summer ap source say trump boast about threat to bomb the st out of moscow in leaked audio charles warns small boat crisis is a profound challenge a he host macron at state banquet ahead of migrant deal newsom go big on holy grail reform other view newsom go big on holy grail reform other view supreme court allows trump administration to resume mass federal layoff for now suit challenge government effort to deport supporter of propalestinian protest invest america act give to every u newborn investment account dell ceo call it futureproofing prosperity sam altman asks for more stuff like this reader speak why i say thank you to uconn health center off the rail trump ramble in the middle of cabinet meeting is karat nonsense wall street trump taco trade ha a chicken and an egg problem meet the new national police force mamdanis farleft ally want to primary hakeem jeffries and other nyc democrat reader speak american tragedy is that those who are in power are inhumane congressional democrat push for new watchdog to oversee trump white house american need to work together to fix education weve both done it before on opposite side the search for the old lady pony continues tariff are already squeezing corporate margin new survey find ai is changing the world faster than most realize fencing wa a chore that we enjoyed texas is relying on fema state leader said it should be cut letter trump usaid action are evil letter trump usaid action are evil microsoft patch vulnerability including critical flaw in spnego and sql server</t>
+          <t>medius now fully qualified yardi ecosystem partner cohen milstein seller toll pllc and bernstein litowitz berger grossmann llp announce pendency and proposed settlement of class action involving all person and entity who purchased or otherwise acquired the publicly traded common stock and preferred stock of silvergate capital corporation from november through march inclusive or in andor traceable to security offering during medius now fully qualified yardi ecosystem partner what you need to know ahead of live nation entertainment earnings release what you need to know ahead of live nation entertainment earnings release bloomberg law host ai symposium exploring the future of legal technology score prime day clothing deal on levi crocs spanx more starting at new york post thursday july evening cable news rating fillin host win the day ovation healthcare and ludi partner to streamline operational efficiency and financial health for rural hospital can micron stock hit in can micron stock hit in sealsq commences global deployment of it gsmaaccredited euicc with telco integrating a pioneering postquantum ready cryptographic security technology manulife investment management close third coinvestment fund at b surpassing predecessor by over m mitrex set guinness world record with largest bipv solar panel mural at sunrise residential longeveron announces u fda approval of ind application for a phase pivotal registration study evaluating laromestrocel a a treatment of pediatric dilated cardiomyopathy dcm saudi arabia crude oil export jumped by bpd in april substratelike pcb market size to hit usd billion by driven by demand for compact highperformance electronics research by sn insider application for delisting of sdrs from nasdaq stockholm what to expect from mondelez international q earnings report what to expect from mondelez international q earnings report amazon share form golden cross a prime day kick off national beverage credit lacroix marketing with q fiscal year growth world no magnus carlsen add to grand chess tour legacy with victory in zagreb at superunited rapid blitz croatia quanterix close m akoya deal after competing bid leading and lagging sector for july courtney caputo named chair of the national board of director at the epilepsy foundation of america optical imaging market to reach usd billion by fueled by rising demand for noninvasive diagnostic technology and octdriven clinical expansion sn insider courtney caputo named chair of the national board of director at the epilepsy foundation of america giant pigeon float through nyc for fifa club world cup what you need to know ahead of republic service earnings release what you need to know ahead of republic service earnings release column london metal exchange reaps the reward of tariff turmoil franklin resource quarterly earnings preview what you need to know franklin resource quarterly earnings preview what you need to know the salvation army to collect school supply at rochester walmart store elon musk fan took her first tesla robotaxi ride but then it made her get out and left her stranded cuz it wa about to rain unforgettable edible close after year on northwest side chile post steepest monthly price drop since ahead of rate decision what to expect from union pacific next quarterly earnings report what to expect from union pacific next quarterly earnings report the electric porsche macan is outselling the gas model but there more to the story motorcom the energy report so much for weak demand top company offering remote data science job why is penny stock prokidney stock trading higher on tuesday why is penny stock prokidney trading higher on tuesday robotics frenzy grip hong kong market and stock ride the hype is the rally sustainable goelzer investment management inc boost position in meta platform inc nasdaqmeta checchi capital adviser llc sell share of meta platform inc nasdaqmeta palisade capital management lp decrease stock holding in meta platform inc nasdaqmeta mountain capital investment advisor inc sell share of meta platform inc nasdaqmeta whimstay open platform to independent host for the first time netanyahu present trump with nomination for nobel peace prize a both downplay twostate solution cemtrexs vicon secures m followon order for county security infrastructure expansion cemtrexs vicon secures m followon order for county security infrastructure expansion barlow wealth partner inc acquires share of meta platform inc nasdaqmeta netsol technology appoints ian smith to it board of director aurora private wealth inc raise stock holding in meta platform inc nasdaqmeta netsol technology appoints ian smith to it board of director meta platform inc nasdaqmeta share acquired by sitrin capital management llc tkg advisor llc ha holding in meta platform inc nasdaqmeta ap business summarybrief at am edt at least may have killed themselves over uk post office wrongful conviction scandal why i always convert word to pdf now elon musk lash out at tesla bull dan ives over board proposal shut up how can large enterprise navigate tcpa compliance challenge percepta celebrates year of transforming automotive customer experience waymo offer teen account for driverless ride villa vie residence celebrates th visited port with summer celebration sale wednesday july evening cable news rating fox news stay no public record investment group buy ocean view apartment in norfolk k pure solution announces major strategic bleach distribution deal for the southwestern u mainly southern california u space force space system command selects rise for forge path to production contract inmorphis acquires servicenow practice of solugenix strengthening u market presence and expanding industryaligned offering in july and beyond honoring bebe moore campbell legacy u space force space system command selects rise for forge path to production contract deep dive into alcoa stock analyst perspective rating companion spine llc announces definitive agreement to acquire the business and asset of paradigm spine gmbh and the coflex and cofix spine implant from xtanttm medical holding inc what analyst are saying about edward lifesciences stock xsolis aidriven solution new feature evaluated in klas second look report what analyst rating have to say about kla petsmart name top catloving city tegna to host second quarter earnings conference call on thursday august startup raise m for universal flu vaccine made with mrna community bankshares inc revolutionizes access to capital and speed up loan closure for assessing enovis insight from financial analyst abbott laboratory stock a deep dive into analyst perspective rating is gaming and leisure prop gaining or losing market support whats driving the market sentiment around kbr breaking down agilent technology analyst share their view what to expect from norfolk southerns q earnings report what to expect from norfolk southerns q earnings report use this amex trick to save up to on amazon prime day locumtenenscom and march of dime partner to expand and scale maternal mental health training for clinician milliman analysis corporate pension funding improves in june to highest level since october milliman analysis corporate pension funding improves in june to highest level since october honor education secures m series a to reinvent digital learning experience outcome capital launch the first dedicated ophthalmology practice to address the world leading cause of disability can adobe stock hit in can adobe stock hit in instant legislation limit hoa enforcement in california swamp game at alligator alcatraz mamdanis socialist nightmare and more from fox news opinion hillsborough county target ruskin property for new sewer system vacuum lift station to boost environment and health south carolina gop urge trump supporter to give gavin newsom a huge southern welcome federal judge nix wisconsin judge bid to dismiss charge of helping illegal immigrant evade ice mona charen we need to remember the nobility of this nation trump extends federal hiring freeze until october use this amex trick to save up to on amazon prime day american kid have become increasingly unhealthy over nearly two decade new study find trump rip reporter for asking about epstein case a american doubt doj conclusion braille institute welcome distinguished tech executive roberto medrano to board of director northwestern energy adapts a demand evolve brian bird code for america unveils new government ai landscape assessment letter to the editor response to congressman downing sensorium therapeutic receives fda ind clearance for sntx a firstinclass rapidacting anxiolytic manatt enhances entertainment offering with leading film and tv partner montana conservation voter scorecard cut through noise kearstyn cook gov jim pillen sends nebraska urban searchandrescue team to help after texas flooding who had montana back the scorecard expose the record kearstyn cook who had montana back the scorecard expose the record kearstyn cook intention rise expectation fall the number of american planning to leave an inheritance go up a the number expecting to receive one go down find northwestern mutuals planning progress study jerome christenson closing the book on mailorder book club will we miss them big brother big sister of america appoints terrance williams of trustage a newest board member the u air force might send it retired b bomber to israel bad idea impactivize shareholder of company worth trillion vote overwhelmingly to defeat antidei proposal a a travel editor these are the amazon prime day deal id actually pack michelinstarred sushi aseat dinner vice president vance wrap up california visit someone using ai to impersonate marco rubio contacted at least five people including foreign minister cable say nyse content advisory premarket update trump announces new tariff on country trump slam russiaukraine war a bidencreated monster while unveiling new aid package ice raid derail southern california economy a worker go into hiding samsungs the frame make a gorgeous unique tv even better texas lawmaker want investigation into weather alert system and storm preparedness dr elseys reinforces it longstanding commitment to safer unscented cat litter presence of ice inside california hospital denounced by local leader immigration activist kinder and u soccer foundation launch goal of joy to inspire more active and joyful community through soccer the latest trump delay tariff implementation another month pastor who endorse political candidate shouldnt lose taxexempt status irs say in filing mob in rural india kill family accused of witchcraft iova notice iovance biotherapeutics shareholder are notified of the pending class action lawsuit contact bfa law by july court deadline nasdaqiova rich lowry dont blame donald trump for flood hims notice hims hers health inc shareholder are notified of the pending class action lawsuit contact bfa law by august court deadline nysehims aapl notice apple inc shareholder are notified of the pending class action lawsuit contact bfa law by august court deadline nasdaqaapl rddt notice reddit inc shareholder are notified of the pending class action lawsuit contact bfa law by august court deadline nyserddt ftre notice fortrea holding inc shareholder are notified of the pending class action lawsuit contact bfa law by august court deadline nasdaqftre i spent five week with the new roku ultra to see if you should upgrade video show deadly fire at cairo telecommunication building picking that bow back up northern cheyenne youth reconnect with archery letter to the editor independence day spark feeling ogn notice organon co shareholder are notified of the pending class action lawsuit contact bfa law by july court deadline nyseogn apple watch ultra review still the smartwatch to get horsemounted federal agent descend on los angeles park on video the google pixel watch finally delivers the big upgrade weve been waiting for lgs transparent oled tv just blew my mind at ce united by hatred vance rip mamdani expose the american left contradiction peace through power it electric injured after motorcycle strike deer on highway what if superman existed in a world like ours director james gunn on new superhero movie the best apple watch to buy in tested by expert trump outrage is hiding the real danger to america swiss village brace for possible alpine rockslide man dy at milan airport after being sucked into jet engine local medium report target of trump new tariff speak out the best sleep tracker in tested by editor tiger lsu purple and more it fig season here are tip to optimize your harvest letter to the editor wake up montana mississippi state university announces spring honor student rotary club of zachary present scholarship puretalk and allegiance flag supply honor veteran with americanmade flag nationwide zachary high school bronco explorer travel to japan ethel student named to washburn honor roll beta sigma phi member donate snack to eastside fire department letter denying global warning isnt cool held in texas immigration detention center shooting that wa planned ambush u attorney say the apple watch series is the smartwatch most people should buy kansa city chief heiress turn to scripture after yearold cousin killed in texas flood why the israeliran ceasefire feel like a strategic failure the best vacuum for pet hair in tried and tested why airtags are the ultimate travel companion this holiday season report accuses hamas of sexual violence i tried the latest version of the internetfamous bissell little green here my review sen ted cruz caught sightseeing in greece amid devastating flood in his home state a state attorney general say welcoming child of all race is illegal ideology opinion i really like the amazon kindle colorsoft but is color worth italy bergamo airport suspends flight after a person reportedly got sucked into engine the blink mini is a tiny camera that make your home a lot smarter a long hot summer day on the ground of st andrew conjures movie magic from yesteryear copy nurse practitioner kelsey st arnaud join north oak primary care in hammond joel boerkey named to the spring dean list at lincoln memorial university louisiana farm bureau elect officer during convention letter to the editor chinese communist party influence on american soil i cant stop using the ipad mini even though it a pretty boring update i tested this smart ipl device for athome hair removal and im never going to the salon again trial underway for ucla professor who refused to exercise compassion with racebased grading the google pixel tablet is a great slate that double a a smart display i tested the viral wavytalk thermal brush i didnt love it but here why you might egypt arrest famed belly dancer world focus the beijing olympics a pivotal moment for china key advisor called hunter bidens role on strategy call inappropriate after he overruled legal guidance letter to the editor dont pull plug on energy credit editorial cartoon for tuesday july</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>ahead arch earnings release killed mill buy ethereum expect leidos q earnings report successful couple morning little hello relationship expert world bull bear tiger ai launch agentic capability latest molecular universe release increase value proposition rd service found best amazon prime deal shopping thousand offer cnn fed rate cut coming opinion vary widely fury intercept lio ninaaskumuwin discovery incorporation boerne lawmaker investigate response flood covered call screener texas passed quantum computing legislation play ionq stock homebuyers finally responded mortgage rate hit lowest level month cnbc palantir technology sp hottest stock past close incredible rally continue cybersecurity stock buy next decade business newsline amazon extends prime discount trump medium file crypto blue chip vibe coding arrived business wsj bigname adviser avoiding crypto speculative investment move buying marketwatch trump threatened bomb moscow deter putin cnn trump bill promise tax tip overtime limitheres qualifies droit launch explore mode adept platform h room optimism risk complacency aes freeportmcmoran verona pharma intel aehr penguin solution mover barrons michelle obama learned great parenting tip mom dadthey job modeling bmw v mercedes sale race linda yaccarino step ceo elon musk x dax push higher eu edge closer tariff deal prime deal verge eli manning longer interested buying piece nfls giant expensive merck acquire verona pharma expanding portfolio include ohtuvayre ensifentrine firstinclass copd maintenance treatment adult expected drive growth next decade merck acquire verona pharma expanding portfolio include ohtuvayre ensifentrine firstinclass copd maintenance treatment adult expected drive growth next decade merckcom walmart selling fantastic chromebook laptop shopper love touchscreen feature word help teach kid critical thinking michelle obama psychologist malaysian pm warns southeast asia trade war passing storm quadmotor rivians arrive wild power wilder price apple catch ai race rival turn heat boomer buying highestyielding dividend champion handoverfist smith corporation nyseaos share purchased private trust co na elon musk grok ai chatbot denies praised hitler antisemitic vickers insider pick hudson edge investment partner million stock jpmorgan chase co nysejpm private trust co na stock coterra energy nysectra rosalia new balance newest brand ambassador russia launch another record drone attack ukraine ukrainian beware scam promise good pay completing easy online task beware scam promise good pay completing easy online task money market account rate rate hit heloc equity loan rate highyield saving account rate rate steady beware scam promise good pay completing easy online task bank england flag global debt pressure market stabilization goldman demand oath junior banker fend private equity poaching bloomberg block rule cancel subscription easily sp future tick higher investor shrug trump tariff threat fomc tap mortgage refinance rate rate increase mortgage rate rate move cd rate rate rise uae oil market thirsty opec barrel proposed clermont subdivision redesign deadly lakeshore drive exact science announces medicare coverage oncodetecttm molecular residual disease test colorectal cancer fresh del monte produce report quarter financial trump trade blitz produce deal lot uncertainty trump trade blitz produce deal lot uncertainty trump trade blitz produce deal lot uncertainty trump trade blitz produce deal lot uncertainty trump trade blitz produce deal lot uncertainty trump trade blitz produce deal lot uncertainty new era restaurant worker earn sixfigure salary benefit industry provide tesla board ground rule musk political activism analyst samsung launch new foldable smartphones fends chinese rival trump tariff extension leaf bank fed limbo hbo max prestige brand streaming corra rising demand global investor due diligence investigation market sputter trump push tariff deadline xrp price forecast hit insider loading new xrp x auddia announces leadership change special committee evaluate business combination restructuring ai native company senate gop gear test trump doge cut inside information orion upgrade fullyear outlook social security sends million american misleading blatantly political message shreveport director awardwinning screenplay red carpet premiere atlantic nickel expands rpm zone awaruite nickelalloy nife discovery meter northern extension yield nickel concentrate meter dtr metallurgical recovery testing shreveport kick eleven store louisiana site planned ragnarok ip title achieved game ranking taiwan hong kong macau toast nysetost share acquired da davidson co private trust co na stock ge healthcare technology nasdaqgehc trump bill slash cfpb funding davenport co sell share fortive corporation nyseftv private trust co na acquires share emcor nyseeme less month claim ev tax credit buy car expert legend cross zone pound gear favorite principal financial increase stock zimmer biomet nysezbh mutual advisor buy share trane technology plc nysett mutual advisor grows stock decker outdoor corporation nysedeck malaria drug newborn young infant expected approved africa rapid anchor suspended sentence domestic assault bank england warns high financial market risk easing tension kisti secures funding national quantum center excellence name ionq primary quantum partner opinion president punishes patriot wednesday world burn eye turn diddy european russia behind downing mh watch popular podcaster discusses kamala episode scrapped talked gibberish campaign wanted canned fbi bust chinese national multimillion dollar drug ring exploiting immigration system president business trump admin sue california transgender athlete policy view congressional delegation must fight cut noaa burke county company hildebran wont issue permit train cabin business another voice buffalo garden vibrantly express community soul trump admin subpoena harvard foreign student misconduct campus radicalism george conway flag trump awkward new admission fresh proof fool eu seek finalize trade deal trump end month hawaii lawmaker demand immigration arrest briefing haleiwa development council review road usage charge begin electric vehicle governor budget veto trim public school maintenance hooser sbcd travesty process policy senate gop gear test trump doge cut senate gop gear test trump doge cut jewish democrat congress sound alarm mamdani tea party patriot push lawmaker noncitizen voting jewish democrat congress sound alarm mamdani tea party patriot push lawmaker noncitizen voting senate gop gear test trump doge cut larger fight rage trump racking college tea party patriot push lawmaker noncitizen voting jewish democrat congress sound alarm mamdani larger fight rage trump racking college larger fight rage trump racking college senate gop gear test trump doge cut senate gop gear test trump doge cut tea party patriot push lawmaker noncitizen voting jewish democrat congress sound alarm mamdani tea party patriot push lawmaker noncitizen voting jewish democrat congress sound alarm mamdani senate gop gear test trump doge cut larger fight rage trump racking college tea party patriot push lawmaker noncitizen voting larger fight rage trump racking college jewish democrat congress sound alarm mamdani larger fight rage trump racking college candace cameron bure son biblebased pep helped save marriage antiviolence advocate gun manufacturer accountable mass shooting river north tragedy chicago allows people trump trade blitz produce deal lot uncertainty laura washington art institute slowly getting normal georgia police arrest farmworkers warrant dhs firearm testing ballistics unit open september county forensics lab dc fire cut tax increase police presence council bid view trekking pole lend mountainclimber swagger steve corbin give liberty tinpot dictator scare buying reported rochester legislator favor legal pot business california focus legislator favor legal pot business california focus editorial cartoon legend cross zone pound gear favorite president wife named ellen edith malaria drug newborn young infant expected approved africa red bull team principal christian horner fired team month stuck south north korean billion served trump bill billion served trump bill supreme reject shielding identity police attending jan capitol rally trump slam democrat inflation narrative cut cost president history red bull team principal christan horner sacked team voting known voting known everything expect family fun colnes alkincoates park robinhood ceo tokenization major innovation market wont qualify new car loan interest deduction allegheny county council approves innamorato choice shuman advisory board pittsburgh council pas protection lgbtq people elon musk grok remove politically incorrect instruction praise hitler flash flooding texas preventable trump tariff pharmaceutical import increase percent threetime mvp nikola jokic delay signing extension nugget summer source trump boast threat bomb st moscow leaked audio charles warns small boat crisis profound challenge host macron banquet ahead migrant deal newsom holy grail reform view newsom holy grail reform view supreme allows trump administration resume mass federal layoff suit challenge government effort deport supporter propalestinian protest invest america act give newborn investment account dell ceo call futureproofing prosperity sam altman asks stuff reader speak uconn health center rail trump ramble middle cabinet meeting karat nonsense wall street trump taco trade chicken egg problem meet new national police force mamdanis farleft ally primary hakeem jeffries nyc democrat reader speak american tragedy power inhumane congressional democrat push new watchdog oversee trump white house american work together fix education weve opposite search old lady pony continues tariff squeezing corporate margin new survey find ai changing world faster realize fencing chore enjoyed texas relying fema cut trump usaid action evil trump usaid action evil microsoft patch vulnerability critical flaw spnego sql server</t>
+          <t>medius fully qualified yardi ecosystem partner cohen milstein seller toll pllc bernstein litowitz berger grossmann llp announce pendency proposed settlement class action involving entity purchased otherwise acquired publicly traded common stock preferred stock silvergate corporation november march inclusive andor traceable security offering medius fully qualified yardi ecosystem partner ahead nation entertainment earnings release ahead nation entertainment earnings release bloomberg host ai symposium exploring future legal technology score prime clothing deal levi crocs spanx starting york post thursday evening cable rating fillin host ovation healthcare ludi partner streamline operational efficiency financial health rural hospital micron stock hit micron stock hit sealsq commences global deployment gsmaaccredited euicc telco integrating pioneering postquantum ready cryptographic security technology manulife investment close third coinvestment fund b surpassing predecessor mitrex set guinness world record largest bipv solar panel mural sunrise residential longeveron announces fda approval ind application phase pivotal registration study evaluating laromestrocel treatment pediatric dilated cardiomyopathy dcm saudi arabia crude oil export jumped bpd april substratelike pcb market size hit usd billion driven demand compact highperformance electronics research sn insider application delisting sdrs nasdaq stockholm expect mondelez international q earnings report expect mondelez international q earnings report amazon form golden cross prime kick national beverage credit lacroix marketing q fiscal growth world magnus carlsen add grand chess tour legacy victory zagreb superunited rapid blitz croatia quanterix close akoya deal competing bid leading lagging sector courtney caputo named chair national board director epilepsy foundation america optical imaging market reach usd billion fueled rising demand noninvasive diagnostic technology octdriven clinical expansion sn insider courtney caputo named chair national board director epilepsy foundation america giant pigeon float nyc fifa club world cup ahead republic service earnings release ahead republic service earnings release column london metal exchange reaps reward tariff turmoil franklin resource quarterly earnings preview franklin resource quarterly earnings preview salvation army collect school supply rochester walmart store elon musk fan took tesla robotaxi ride left stranded cuz rain unforgettable edible close northwest chile post steepest monthly price drop since ahead rate decision expect union pacific next quarterly earnings report expect union pacific next quarterly earnings report electric porsche macan outselling gas model story motorcom energy report weak demand company offering remote data science job penny stock prokidney stock trading higher tuesday penny stock prokidney trading higher tuesday robotics frenzy grip hong kong market stock ride hype rally sustainable goelzer investment boost meta platform nasdaqmeta checchi adviser sell meta platform nasdaqmeta palisade lp decrease stock meta platform nasdaqmeta mountain investment advisor sell meta platform nasdaqmeta whimstay open platform independent host netanyahu present trump nomination nobel peace prize downplay twostate solution cemtrexs vicon secures followon order county security infrastructure expansion cemtrexs vicon secures followon order county security infrastructure expansion barlow wealth partner acquires meta platform nasdaqmeta netsol technology appoints ian smith board director aurora private wealth raise stock meta platform nasdaqmeta netsol technology appoints ian smith board director meta platform nasdaqmeta acquired sitrin tkg advisor meta platform nasdaqmeta business least killed uk post office wrongful conviction scandal always convert word pdf elon musk lash tesla bull dan ives board proposal shut large enterprise navigate tcpa compliance challenge percepta celebrates transforming automotive customer experience waymo offer teen account driverless ride villa vie residence celebrates visited port summer celebration sale wednesday evening cable rating fox stay public record investment buy ocean view apartment norfolk k pure solution announces major strategic bleach distribution deal southwestern mainly southern california space force space system command selects rise forge path production contract inmorphis acquires servicenow practice solugenix strengthening market presence expanding industryaligned offering beyond honoring bebe moore campbell legacy space force space system command selects rise forge path production contract deep dive alcoa stock analyst perspective rating companion spine announces definitive agreement acquire business asset paradigm spine gmbh coflex cofix spine implant xtanttm medical analyst saying edward lifesciences stock xsolis aidriven solution feature evaluated klas look report analyst rating kla petsmart name catloving tegna host quarter earnings conference call thursday august startup raise universal flu vaccine mrna community bankshares revolutionizes access speed loan closure assessing enovis insight financial analyst abbott laboratory stock deep dive analyst perspective rating gaming leisure prop gaining losing market support whats driving market sentiment around kbr breaking agilent technology analyst view expect norfolk southerns q earnings report expect norfolk southerns q earnings report amex trick save amazon prime locumtenenscom march dime partner expand scale maternal mental health training clinician milliman analysis corporate pension funding improves highest level since october milliman analysis corporate pension funding improves highest level since october honor education secures series reinvent digital learning experience outcome launch dedicated ophthalmology practice address world leading cause disability adobe stock hit adobe stock hit instant legislation limit hoa enforcement california swamp game alligator alcatraz mamdanis socialist nightmare fox opinion hillsborough county target ruskin property sewer system vacuum lift station boost environment health south carolina gop urge trump supporter give gavin newsom southern welcome federal judge nix wisconsin judge bid dismiss charge helping illegal immigrant evade mona charen remember nobility nation trump extends federal hiring freeze october amex trick save amazon prime american kid become increasingly unhealthy nearly decade study find trump rip reporter asking epstein american doubt doj conclusion braille institute welcome distinguished tech executive roberto medrano board director northwestern energy adapts demand evolve brian code america unveils government ai landscape assessment editor response congressman downing sensorium therapeutic receives fda ind clearance sntx firstinclass rapidacting anxiolytic manatt enhances entertainment offering leading film tv partner montana conservation voter scorecard cut noise kearstyn cook gov jim pillen sends nebraska urban searchandrescue team help texas flooding montana scorecard expose record kearstyn cook montana scorecard expose record kearstyn cook intention rise expectation fall american planning inheritance expecting receive find northwestern mutuals planning progress study jerome christenson closing book mailorder book club miss brother sister america appoints terrance williams trustage newest board air force send retired b bomber israel bad idea impactivize shareholder company worth trillion vote overwhelmingly defeat antidei proposal travel editor amazon prime deal id pack michelinstarred sushi aseat dinner vice president vance wrap california visit someone ai impersonate marco rubio contacted least five people foreign minister cable nyse content advisory premarket update trump announces tariff country trump slam russiaukraine war bidencreated monster unveiling aid package raid derail southern california economy worker hiding samsungs frame gorgeous unique tv better texas lawmaker investigation weather alert system storm preparedness dr elseys reinforces longstanding commitment safer unscented cat litter presence inside california hospital denounced local immigration activist kinder soccer foundation launch goal joy inspire active joyful community soccer latest trump delay tariff implementation another month pastor endorse political candidate shouldnt lose taxexempt status irs filing mob rural india kill family accused witchcraft iova notice iovance biotherapeutics shareholder notified pending class action lawsuit contact bfa deadline nasdaqiova rich lowry dont blame donald trump flood hims notice hims health shareholder notified pending class action lawsuit contact bfa august deadline nysehims aapl notice apple shareholder notified pending class action lawsuit contact bfa august deadline nasdaqaapl rddt notice reddit shareholder notified pending class action lawsuit contact bfa august deadline nyserddt ftre notice fortrea shareholder notified pending class action lawsuit contact bfa august deadline nasdaqftre spent five roku ultra upgrade video deadly fire cairo telecommunication building picking bow northern cheyenne youth reconnect archery editor independence spark feeling ogn notice organon co shareholder notified pending class action lawsuit contact bfa deadline nyseogn apple watch ultra review smartwatch horsemounted federal agent descend los angeles park video google pixel watch finally delivers upgrade weve waiting lgs transparent oled tv blew mind ce united hatred vance rip mamdani expose american left contradiction peace power electric injured motorcycle strike deer highway superman existed world director james gunn superhero movie best apple watch buy tested expert trump outrage hiding real danger america swiss village brace possible alpine rockslide man dy milan airport sucked jet engine local medium report target trump tariff speak best sleep tracker tested editor tiger lsu purple fig season tip optimize harvest editor wake montana mississippi university announces spring honor student rotary club zachary present scholarship puretalk allegiance flag supply honor veteran americanmade flag nationwide zachary high school bronco explorer travel japan ethel student named washburn honor roll beta sigma phi donate snack eastside fire department denying global warning isnt cool texas immigration detention center shooting planned ambush attorney apple watch series smartwatch people buy kansa chief heiress turn scripture yearold cousin killed texas flood israeliran ceasefire feel strategic failure best vacuum pet hair tried tested airtags ultimate travel companion holiday season report accuses hamas sexual violence tried latest version internetfamous bissell little green review sen ted cruz caught sightseeing greece amid devastating flood attorney general welcoming child race illegal ideology opinion amazon kindle colorsoft color worth italy bergamo airport suspends flight reportedly got sucked engine blink mini tiny camera lot smarter hot summer ground st andrew conjures movie magic yesteryear copy nurse practitioner kelsey st arnaud join north oak primary care hammond joel boerkey named spring dean list lincoln memorial university louisiana bureau elect officer convention editor chinese communist party influence american soil cant stop ipad mini pretty boring update tested smart ipl device athome hair removal im never salon trial underway ucla professor refused exercise compassion racebased grading google pixel tablet great slate double smart display tested viral wavytalk thermal brush didnt love egypt arrest famed belly dancer world focus beijing olympics pivotal moment china advisor hunter bidens role strategy call inappropriate overruled legal guidance editor dont pull plug energy credit editorial cartoon tuesday</t>
         </is>
       </c>
     </row>
@@ -874,12 +870,12 @@
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>hot yield highlight energy midstream giant mplx advanced micro device earnings preview what to expect advanced micro device earnings preview what to expect vanguard smallcap value etf nysearcavbr share purchased by telos capital management inc kimberlyclark co nysekmb share acquired by telos capital management inc telos capital management inc make new million investment in te connectivity ltd nysetel stonebrook private inc purchase share of salesforce inc nysecrm telos capital management inc ha million stake in danaher corporation nysedhr cerity partner ocio llc buy share of ishares mb etf nasdaqmbb telos capital management inc ha million holding in deere company nysede keurig dr pepper inc nasdaqkdp share purchased by parr mcknight wealth management group llc stonebrook private inc purchase share of ishares core msci europe etf nysearcaieur capital insight partner llc lower holding in tractor supply company nasdaqtsco stonebrook private inc ha million stake in darden restaurant inc nysedri most u adult say child care cost are a major problem a new apnorc poll find sunrocket capital announces million financing for renewable energy project supporting ai and data center market united airline holding unusual option activity for july where comstock resource stand with analyst this is what whale are betting on palantir technology this is what whale are betting on celestica expert outlook associated banc through the eye of analyst olehenriksen launch peach glaze collection the juicy clinical result your skin craves application for jobless benefit fall to last week korean officer to receive imo highest bravery award for fishing vessel rescue nvidia ceo jensen huang could soon be richer than warren buffetthes worth billion now where federated hermes stand with analyst spotify technology nysespot is steadview capital management llcs th largest position marvell technology nasdaqmrvl now covered by the goldman sachs group applied material nasdaqamat coverage initiated by analyst at the goldman sachs group stryker corporation nysesyk share sold by aurdan capital management llc financial gravity asset management inc invests in ge aerospace nysege nvidia nasdaqnvda coverage initiated at the goldman sachs group applovin corporation nasdaqapp share sold by steadview capital management llc aurdan capital management llc trim stock position in stryker corporation nysesyk the analyst verdict molina healthcare in the eye of expert how kanava ai is bringing voice automation to industrial workflow an interview with smit dagli peering into borgwarners recent short interest what doe the market think about somnigroup international what analyst are saying about jdcom stock white house accuses powell of mismanaging federal reserve citing headquarters renovation what doe the market think about selective insurance gr wake up dead man a knife out mystery to open bfi london film festival beyond the number analyst discus verizon communication stock stock pressured by u trade policy uncertainty stock pressured by u trade policy uncertainty change in the supervisory and management board and audit committee of admiral market a trump loses appeal of million e jean carroll sexual abuse defamation verdict sun life u and dentaquest donate to support texas flooding relief effort spindrift partner with patricof co to welcome new wave of athlete investor brain monitoring market size to hit usd million by coherent market insight brain monitoring market size to hit usd million by coherent market insight ga telesis engine service gate usa spah launch leap engine quick turn service marking major capability expansion bigbank a extended the term of the supervisory board member hammond power solution announces second quarter financial result conference call and webcast notification china asean build new paradigm for regional cooperation temo inc achieved florida product approval for hurricaneresistant impact glass sunroom vixs premium with ad now available in directvs miespanol genre pack behavioral rehabilitation market surpasses usd billion in fueled by anxiety and substance abuse disorder hydroxyethyl cellulose market to surpass usd million by demand driven by expanding application in personal care construction and pharmaceutical oil price sink a iran and u resume nuclear talk research the gender wage gap tipping point hii to host second quarter earnings conference call and webcast on july packaging solution market valued at trillion and heading to trillion by spacelift raise m series c to redefine enterprise infrastructure automation consumer who sold real estate that wa listed on ml property information network and paid commission to a real estate agent may be affected by a settlement vishay intertechnology q result earnings call webcast detail exclusive nbcus super bowl ad now going for million helcim introduces it new smart terminal a faster sleeker smarter way to accept payment ine security launch enhanced emapt certification blockdags global launch release entry set it apart over bitcoin cash shiba inu american airline group announces webcast of secondquarter financial result consumer who sold real estate that wa listed on ml property information network and paid commission to a real estate agent may be affected by a settlement rapidscale start technology scholarship at wake tech proptech market to usd billion by owing to rising demand for digital real estate transaction and smart property solution report by sn insider trader weigh opec tariff and resilient demand change in the supervisory and management board and audit committee of admiral market a everyone know what broke in leverage ratio reform can fix it greenleaf trust grows holding in blackstone inc nysebx index fund advisor inc take position in servicenow inc nysenow axxcess wealth management llc ha million stock position in morgan stanley nysems parr mcknight wealth management group llc acquires share of vanguard total international bond etf nasdaqbndx peddock capital advisor llc ha million holding in thermo fisher scientific inc nysetmo index fund advisor inc make new million investment in vanguard total international stock etf nasdaqvxus financial review creditriskmonitorcom crmz versus it competitor parr mcknight wealth management group llc make new million investment in invesco bulletshares corporate bond etf nasdaqbscr this amd analyst turn bullish here are top upgrade for thursday dhls m expansion in uk and ireland novo nordisks quality testing site in china new mexico educational retirement board reduces stock position in copart inc nasdaqcprt axxcess wealth management llc lower stake in accenture plc nyseacn u capital wealth advisor llc ha million position in airbnb inc nasdaqabnb axxcess wealth management llc ha million position in philip morris international inc nysepm leavell investment management inc purchase share of caterpillar inc nysecat linden thomas advisory service llc acquires share of accenture plc nyseacn accenture plc nyseacn share sold by axxcess wealth management llc greenleaf trust sell share of norfolk southern corporation nysensc caterpillar inc nysecat share bought by leavell investment management inc hara capital llc sell share of united airline holding inc nasdaqual hara capital llc lower holding in or royalty inc nyseor abbvie nyseabbv v bayer aktiengesellschaft otcmktsbayry head to head contrast saba capital income opportunity fund ii nysesaba share sold by hara capital llc narus financial partner llc acquires new holding in decker outdoor corporation nysedeck cerity partner ocio llc trim holding in ishares year treasury bond etf nasdaqtlt parr mcknight wealth management group llc grows stake in salesforce inc nysecrm stonebrook private inc ha million stock position in best buy co inc nysebby stonebrook private inc boost stock position in darden restaurant inc nysedri albany veteran banned from boshart davis office sue iceblock criminal evasion tool or constitutionally protected speech iceblock criminal evasion tool or constitutionally protected speech iceblock criminal evasion tool or constitutionally protected speech gop sen thom tillis say hegseth is out of his depth a defense secretary defcon ai achieves major rd milestone with launch of advanced theater distribution planning tool for talisman sabre financial gravity asset management inc acquires share of solventum corporation nysesolv sweeping bipartisan bill would nationalize standard for student athlete pay wake up dead man a knife out mystery to open bfi london film festival drone nerd debut ndaacompliant wingtraray fixedwing drone judge weighs motion to dismiss charge against a north adam man accused of killing his wife america greatest threat come from within letter to the editor beware of halftruths around direct primary care medicaid cut in trump tax bill will devastate access to care in rural pennsylvania critic say iranian supreme leader appears in public for first time since war the washington post latest antitrump commentator is a literal clown on onon and the competition head to head contrast analyzing saker aviation service skas and it rival greenleaf trust sell share of norfolk southern corporation nysensc astra wealth partner llc increase stock position in dimensional international core equity etf batsdfic hara capital llc decrease stock position in invesco rafi u etf nysearcaprf hara capital llc sell share of gildan activewear inc nysegil hara capital llc invests in delta air line inc nysedal hara capital llc decrease holding in saba capital income opportunity fund ii nysesaba astra wealth partner llc purchase share of ishares sp midcap value etf nysearcaijj hara capital llc ha holding in franklin ftse south korea etf nysearcaflkr hara capital llc cut stake in zoom communication inc nasdaqzm bxm wealth llc ha stock position in visa inc nysev exclusive ice nabs two m ringleader in midwest raid after testifying before congress on antisemitism cal poly hosted all day for palestine hara capital llc trim stock holding in bank of america corporation nysebac parr mcknight wealth management group llc ha million stock holding in vanguard total bond market etf nasdaqbnd financial gravity asset management inc purchase share of baring bdc inc nysebbdc parr mcknight wealth management group llc acquires share of sp global inc nysespgi axxcess wealth management llc sell share of intuitive surgical inc nasdaqisrg people financial service corp trim stock position in mastercard incorporated nysema general motor company nysegm share bought by tru independence llc union pacific corporation nyseunp share purchased by axxcess wealth management llc hara capital llc sell share of japan smaller capitalization fund inc nysejof the estee lauder company inc nyseel share sold by vision capital management inc narus financial partner llc invests in marsh mclennan company inc nysemmc vision capital management inc sell share of f inc nasdaqffiv the clorox company nyseclx share purchased by vision capital management inc vision capital management inc boost stake in carmax inc nysekmx franklin resource inc nyseben position reduced by code waechter llc vision capital management inc sell share of schwab international equity etf nysearcaschf people bank oh cut stock position in broadcom inc nasdaqavgo vision capital management inc sell share of ishares esg aware msci usa etf nasdaqesgu people bank oh sell share of ishares msci eafe etf nysearcaefa stonebrook private inc ha stake in dexcom inc nasdaqdxcm realty income corporation plan aug dividend of nyseo website serving harvard undergrad woman minority and lgbtq student taken down crimson report moloney security asset management llc decrease holding in elevance health inc nyseelv nisa investment advisor llc decrease stake in marriott international inc nasdaqmar nisa investment advisor llc sell share of synopsys inc nasdaqsnps mainstreet investment advisor llc ha million stock holding in ameriprise financial inc nyseamp nisa investment advisor llc sell share of ameriprise financial inc nyseamp stratos investment management llc purchase new position in fiserv inc nysefi nisa investment advisor llc ha million position in paypal holding inc nasdaqpypl mt bank corp ha million stock position in marriott international inc nasdaqmar financial gravity asset management inc invests million in intuit inc nasdaqintu superman star nathan fillion staunchly defends his character extreme hairstyle i wa team bowl cut the whole way federal judge again block end to birthright citizenship doncasters planned number of new secondary school place will not meet demand jane birkins original hermes bag go on sale drunk and defiant a bar song tipsy top the chart froma harrop drunk and defiant a bar song tipsy top the chart froma harrop drunk and defiant a bar song tipsy top the chart froma harrop drunk and defiant a bar song tipsy top the chart froma harrop drunk and defiant a bar song tipsy top the chart froma harrop drunk and defiant a bar song tipsy top the chart froma harrop drunk and defiant a bar song tipsy top the chart froma harrop drunk and defiant a bar song tipsy top the chart froma harrop drunk and defiant a bar song tipsy top the chart froma harrop true vision mn llc make new investment in occidental petroleum corporation nyseoxy moloney security asset management llc sell share of northrop grumman corporation nysenoc trane technology plc nysett share sold by alpine wood capital investor llc alpine wood capital investor llc sell share of northrop grumman corporation nysenoc quotient wealth partner llc raise stake in trane technology plc nysett euna solution issue open letter introducing competition commitment to expand supplier participation for public procurement team deutsche bank aktiengesellschaft begin coverage on cinemark nysecnk share in shell plc unsponsored adr nyseshel purchased by pom investment strategy llc nxp semiconductor nasdaqnxpi and microchip technology nasdaqmchp critical analysis sekisui house skhsy and it rival critical comparison ishares sp smallcap growth etf nasdaqijt share acquired by code waechter llc financial comparison transocean nyserig and royale energy otcmktsroyl code waechter llc boost stock position in pacer u small cap cash cow etf batscalf analyzing zkh group nysezkh and taoping nasdaqtaop unitedhealth group incorporated nyseunh stake trimmed by code waechter llc northwest natural gas company nysenwn stock holding lessened by code waechter llc code waechter llc invests in the pnc financial service group inc nysepnc medtronic plc nysemdt position trimmed by code waechter llc dexterra group tsedxt set new year high time to buy mkango resource lonmka stock price down here why oracle power lonorcp share down here why</t>
+          <t>what you need to know ahead of arch capital earnings release what really killed the mill reason to buy ethereum before what to expect from leidos holding q earnings report successful couple do these thing in the morning that little hello go a long way relationship expert say in a world of bull and bear be the tiger s ai launch agentic capability in latest molecular universe release to increase value proposition for rd a a service we found the best amazon prime day deal after shopping thousand of offer cnn most fed official see rate cut coming but opinion vary widely on how many minute show fury intercept m of lio at the ninaaskumuwin discovery incorporation of boerne in lawmaker will investigate response to flood covered call screener result for july th texas just passed quantum computing legislation how should you play ionq stock here homebuyers finally responded after mortgage rate hit lowest level in three month cnbc palantir technology ha been the sp s hottest stock over the past year and it not even close can it incredible rally continue cybersecurity stock you can buy and hold for the next decade business newsline july amazon extends prime day discount to day trump medium file for crypto blue chip etf vibe coding ha arrived for business wsj this bigname adviser say avoiding crypto is now a more speculative investment move than buying it marketwatch trump threatened to bomb the s out of moscow to deter putin cnn trump big beautiful bill promise no tax on tip and overtime but there a limitheres who qualifies droit launch explore mode on it adept platform h room for optimism risk for complacency aes freeportmcmoran verona pharma intel aehr penguin solution and more mover barrons michelle obama i learned this great parenting tip from my mom and dadthey did a beautiful job modeling it bmw v mercedes u sale race there a clear leader in linda yaccarino step down a ceo of elon musk x dax push higher a eu edge closer to tariff deal with u the prime day deal you can still get the verge eli manning say he no longer interested in buying a piece of the nfls giant it too expensive for me merck to acquire verona pharma expanding it portfolio to include ohtuvayre ensifentrine a firstinclass copd maintenance treatment for adult and expected to drive growth into the next decade merck to acquire verona pharma expanding it portfolio to include ohtuvayre ensifentrine a firstinclass copd maintenance treatment for adult and expected to drive growth into the next decade merckcom walmart is selling a fantastic chromebook laptop for just and shopper love the touchscreen feature these word help teach kid critical thinking say michelle obama and psychologist malaysian pm warns southeast asia that trade war is not a passing storm quadmotor rivians arrive with wild power and wilder price apple can it catch up in the ai race a rival turn up the heat boomer are buying the highestyielding dividend champion handoverfist a o smith corporation nyseaos share purchased by private trust co na elon musk grok ai chatbot denies that it praised hitler and made antisemitic comment daily vickers top insider pick for hudson edge investment partner inc ha million stock position in jpmorgan chase co nysejpm private trust co na ha stock holding in coterra energy inc nysectra rosalia is new balance newest brand ambassador russia launch another record drone attack on ukraine ukrainian official say beware of scam that promise good pay for completing easy online task beware of scam that promise good pay for completing easy online task today top money market account rate for july rate hit current heloc home equity loan rate july highyield saving account rate today july rate are steady beware of scam that promise good pay for completing easy online task ap news bank of england flag global debt pressure despite market stabilization goldman demand an oath from junior banker to fend off private equity poaching bloomberg court block rule that would let you cancel subscription easily sp future tick higher a investor shrug off trump tariff threat fomc minute on tap today mortgage refinance rate july rate increase mortgage rate today july rate move up cd rate today july rate rise uae say the oil market is thirsty for more opec barrel proposed clermont subdivision would redesign deadly lakeshore drive exact science announces medicare coverage for oncodetecttm molecular residual disease test in colorectal cancer fresh del monte produce inc to report second quarter financial result trump trade blitz produce few deal but lot of uncertainty trump trade blitz produce few deal but lot of uncertainty trump trade blitz produce few deal but lot of uncertainty trump trade blitz produce few deal but lot of uncertainty trump trade blitz produce few deal but lot of uncertainty trump trade blitz produce few deal but lot of uncertainty a new era of restaurant worker may earn sixfigure salary and benefit that no other industry can provide tesla board need ground rule for musk political activism analyst say samsung launch three new foldable smartphones a it fends off chinese rival trump tariff extension leaf bank fed in limbo hbo max is back prestige brand return to streaming corra group see rising demand from global investor for due diligence investigation market sputter after trump push tariff deadline xrp price forecast hit but insider are loading up on the new xrp that could go x auddia announces leadership change and special committee to evaluate business combination and restructuring a ai native holding company senate gop gear up for test on trump doge cut inside information orion upgrade fullyear outlook for social security sends million of american a misleading and blatantly political message see this shreveport director awardwinning screenplay red carpet premiere here how first atlantic nickel expands rpm zone awaruite nickelalloy nife discovery meter northern extension yield nickel concentrate over meter in dtr metallurgical recovery testing shreveport to kick off return of eleven store to louisiana more site planned two ragnarok ip title achieved top game ranking in taiwan hong kong and macau toast inc nysetost share acquired by da davidson co private trust co na ha stock holding in ge healthcare technology inc nasdaqgehc trump big beautiful bill slash cfpb funding what it mean for you davenport co llc sell share of fortive corporation nyseftv private trust co na acquires share of emcor group inc nyseeme you have less than month to claim the ev tax credit now is the time to buy say car expert this legend cross time zone with just pound of gear here are his favorite principal financial group inc increase stock position in zimmer biomet holding inc nysezbh mutual advisor llc buy share of trane technology plc nysett mutual advisor llc grows stock holding in decker outdoor corporation nysedeck first malaria drug for newborn and young infant expected to be approved in africa within week former rapid city anchor given suspended sentence in domestic assault case bank of england warns of high financial market risk despite easing tension kisti secures funding for national quantum center of excellence name ionq a primary quantum partner our opinion when the president punishes patriot wednesday letter a the world burn eye turn to diddy european court russia wa behind downing of mh watch popular podcaster discusses how kamala episode wa scrapped because she talked gibberish her own campaign wanted it canned fbi bust chinese national for multimillion dollar drug ring exploiting immigration system the president mean business trump admin sue california over transgender athlete policy other view state congressional delegation must fight cut to noaa burke county company say hildebran wont issue permit for train cabin business another voice buffalo garden vibrantly express a community soul trump admin subpoena harvard over foreign student misconduct campus radicalism george conway flag trump awkward new admission a fresh proof he a fool eu seek to finalize trade deal with trump by end of the month hawaii lawmaker demand immigration arrest briefing haleiwa development under council review state road usage charge begin for electric vehicle on july governor state budget veto trim public school maintenance hooser sbcd a travesty of process and policy senate gop gear up for test on trump doge cut senate gop gear up for test on trump doge cut jewish democrat in congress sound the alarm on mamdani tea party patriot to push lawmaker on noncitizen voting jewish democrat in congress sound the alarm on mamdani tea party patriot to push lawmaker on noncitizen voting senate gop gear up for test on trump doge cut larger fight rage on but trump racking up win against college tea party patriot to push lawmaker on noncitizen voting jewish democrat in congress sound the alarm on mamdani larger fight rage on but trump racking up win against college larger fight rage on but trump racking up win against college senate gop gear up for test on trump doge cut senate gop gear up for test on trump doge cut tea party patriot to push lawmaker on noncitizen voting jewish democrat in congress sound the alarm on mamdani tea party patriot to push lawmaker on noncitizen voting jewish democrat in congress sound the alarm on mamdani senate gop gear up for test on trump doge cut larger fight rage on but trump racking up win against college tea party patriot to push lawmaker on noncitizen voting larger fight rage on but trump racking up win against college jewish democrat in congress sound the alarm on mamdani larger fight rage on but trump racking up win against college candace cameron bure say son biblebased pep talk helped save her marriage antiviolence advocate why not hold gun manufacturer accountable for mass shooting like river north tragedy letter chicago allows people to be who they want to be trump trade blitz produce few deal but lot of uncertainty laura washington the art institute is slowly getting back to normal georgia police arrest farmworkers then get warrant from dhs firearm testing and ballistics unit could be open in september at county forensics lab former dc fire official want to cut tax increase police presence with city council bid my view trekking pole can lend some mountainclimber swagger steve corbin give me liberty or a tinpot dictator scare buying reported in rochester why should legislator favor legal pot business california focus why should legislator favor legal pot business california focus editorial cartoon for july this legend cross time zone with just pound of gear here are his favorite which u president had wife named ellen and edith first malaria drug for newborn and young infant expected to be approved in africa within week red bull team principal christian horner fired after year with team after month stuck in the south north korean go home letter billion not served by trump big bill letter billion not served by trump big bill supreme court reject shielding identity of police attending jan capitol rally trump slam democrat over inflation narrative say he cut cost more than any president in history red bull team principal christan horner sacked after year with team letter no one is voting after result are known letter no one is voting after result are known here everything to expect at this family fun day in colnes alkincoates park robinhood ceo tokenization is a major innovation in capital market here who will and wont qualify for the new car loan interest deduction allegheny county council approves innamorato choice for shuman advisory board pittsburgh city council pass further protection for lgbtq people elon musk grok remove politically incorrect instruction after it praise hitler wa the flash flooding in texas preventable trump say tariff on pharmaceutical import could increase to percent threetime mvp nikola jokic will delay signing extension with nugget this summer ap source say trump boast about threat to bomb the st out of moscow in leaked audio charles warns small boat crisis is a profound challenge a he host macron at state banquet ahead of migrant deal newsom go big on holy grail reform other view newsom go big on holy grail reform other view supreme court allows trump administration to resume mass federal layoff for now suit challenge government effort to deport supporter of propalestinian protest invest america act give to every u newborn investment account dell ceo call it futureproofing prosperity sam altman asks for more stuff like this reader speak why i say thank you to uconn health center off the rail trump ramble in the middle of cabinet meeting is karat nonsense wall street trump taco trade ha a chicken and an egg problem meet the new national police force mamdanis farleft ally want to primary hakeem jeffries and other nyc democrat reader speak american tragedy is that those who are in power are inhumane congressional democrat push for new watchdog to oversee trump white house american need to work together to fix education weve both done it before on opposite side the search for the old lady pony continues tariff are already squeezing corporate margin new survey find ai is changing the world faster than most realize fencing wa a chore that we enjoyed texas is relying on fema state leader said it should be cut letter trump usaid action are evil letter trump usaid action are evil microsoft patch vulnerability including critical flaw in spnego and sql server</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>hot yield highlight energy midstream giant mplx advanced micro device earnings preview expect advanced micro device earnings preview expect vanguard smallcap value nysearcavbr share purchased telos kimberlyclark co nysekmb share acquired telos telos new million investment te connectivity ltd nysetel stonebrook private purchase share salesforce nysecrm telos million stake danaher corporation nysedhr cerity partner ocio buy share ishares mb nasdaqmbb telos million deere company nysede keurig dr pepper nasdaqkdp share purchased parr mcknight wealth stonebrook private purchase share ishares core msci europe nysearcaieur insight partner lower tractor supply company nasdaqtsco stonebrook private million stake darden restaurant nysedri adult child care cost major problem new apnorc poll find sunrocket announces million financing renewable energy project supporting ai data center market united airline unusual option activity comstock resource stand analyst whale betting palantir technology whale betting celestica expert outlook associated banc eye analyst olehenriksen launch peach glaze collection juicy clinical skin craves application jobless benefit fall korean officer receive imo highest bravery award fishing vessel rescue nvidia ceo jensen huang soon richer warren buffetthes worth billion federated hermes stand analyst spotify technology nysespot steadview llcs largest marvell technology nasdaqmrvl covered goldman sachs applied material nasdaqamat coverage initiated analyst goldman sachs stryker corporation nysesyk share aurdan financial gravity asset invests ge aerospace nysege nvidia nasdaqnvda coverage initiated goldman sachs applovin corporation nasdaqapp share steadview aurdan trim stock stryker corporation nysesyk analyst verdict molina healthcare eye expert kanava ai bringing voice automation industrial interview smit dagli peering borgwarners recent short interest doe market somnigroup international analyst saying jdcom stock white house accuses powell mismanaging federal reserve citing renovation doe market selective insurance gr wake dead man knife mystery open bfi london film festival beyond analyst discus verizon communication stock stock pressured trade policy uncertainty stock pressured trade policy uncertainty change supervisory board audit committee admiral market trump loses appeal million e jean carroll sexual abuse defamation verdict sun life dentaquest donate support texas flooding relief effort spindrift partner patricof co welcome new wave athlete investor brain monitoring market size hit usd million coherent market insight brain monitoring market size hit usd million coherent market insight ga telesis engine service gate usa spah launch leap engine quick turn service marking major capability expansion bigbank extended term supervisory board hammond power solution announces quarter financial conference call webcast notification china asean build new paradigm regional cooperation temo achieved florida product approval hurricaneresistant impact glass sunroom vixs premium ad available directvs miespanol genre pack behavioral rehabilitation market surpasses usd billion fueled anxiety substance abuse disorder hydroxyethyl cellulose market surpass usd million demand driven expanding application personal care construction pharmaceutical oil price sink iran resume nuclear research gender wage gap tipping hii host quarter earnings conference call webcast packaging solution market valued trillion heading trillion spacelift raise series c redefine enterprise infrastructure automation consumer real estate listed ml property information network paid commission real estate agent affected settlement vishay intertechnology q earnings call webcast detail exclusive nbcus super bowl ad million helcim introduces new smart terminal faster sleeker smarter accept payment ine security launch enhanced emapt certification blockdags global launch release entry set apart bitcoin cash shiba inu american airline announces webcast secondquarter financial consumer real estate listed ml property information network paid commission real estate agent affected settlement rapidscale start technology scholarship wake tech proptech market usd billion owing rising demand digital real estate transaction smart property solution report sn insider trader weigh opec tariff resilient demand change supervisory board audit committee admiral market everyone broke leverage ratio reform fix greenleaf trust grows blackstone nysebx index fund advisor take servicenow nysenow axxcess wealth million stock morgan stanley nysems parr mcknight wealth acquires share vanguard total international bond nasdaqbndx peddock advisor million thermo fisher scientific nysetmo index fund advisor new million investment vanguard total international stock nasdaqvxus financial review creditriskmonitorcom crmz versus competitor parr mcknight wealth new million investment invesco bulletshares corporate bond nasdaqbscr amd analyst turn bullish upgrade thursday dhls expansion uk ireland novo nordisks quality testing site china new mexico educational retirement board reduces stock copart nasdaqcprt axxcess wealth lower stake accenture plc nyseacn wealth advisor million airbnb nasdaqabnb axxcess wealth million philip morris international nysepm leavell investment purchase share caterpillar nysecat linden thomas advisory service acquires share accenture plc nyseacn accenture plc nyseacn share axxcess wealth greenleaf trust sell share norfolk southern corporation nysensc caterpillar nysecat share bought leavell investment hara sell share united airline nasdaqual hara lower royalty nyseor abbvie nyseabbv v bayer aktiengesellschaft otcmktsbayry head head contrast saba income opportunity fund ii nysesaba share hara narus financial partner acquires new decker outdoor corporation nysedeck cerity partner ocio trim ishares treasury bond nasdaqtlt parr mcknight wealth grows stake salesforce nysecrm stonebrook private million stock best buy co nysebby stonebrook private boost stock darden restaurant nysedri albany veteran banned boshart davis office sue iceblock criminal evasion tool constitutionally protected speech iceblock criminal evasion tool constitutionally protected speech iceblock criminal evasion tool constitutionally protected speech gop sen thom tillis hegseth depth defense secretary defcon ai achieves major rd milestone launch advanced theater distribution planning tool talisman sabre financial gravity asset acquires share solventum corporation nysesolv sweeping bipartisan bill nationalize student athlete pay wake dead man knife mystery open bfi london film festival drone nerd debut ndaacompliant wingtraray fixedwing drone judge weighs motion dismiss charge north adam man accused killing wife america greatest threat come editor beware halftruths around direct primary care medicaid cut trump tax bill devastate access care rural pennsylvania critic iranian supreme public since war washington post latest antitrump commentator literal clown onon competition head head contrast analyzing saker aviation service skas rival greenleaf trust sell share norfolk southern corporation nysensc astra wealth partner increase stock dimensional international core equity batsdfic hara decrease stock invesco rafi nysearcaprf hara sell share gildan activewear nysegil hara invests delta air line nysedal hara decrease saba income opportunity fund ii nysesaba astra wealth partner purchase share ishares sp midcap value nysearcaijj hara franklin ftse south korea nysearcaflkr hara cut stake zoom communication nasdaqzm bxm wealth stock visa nysev exclusive nabs ringleader midwest raid testifying congress antisemitism cal poly hosted palestine hara trim stock bank america corporation nysebac parr mcknight wealth million stock vanguard total bond market nasdaqbnd financial gravity asset purchase share baring bdc nysebbdc parr mcknight wealth acquires share sp global nysespgi axxcess wealth sell share intuitive surgical nasdaqisrg people financial service corp trim stock mastercard incorporated nysema general company nysegm share bought tru independence union pacific corporation nyseunp share purchased axxcess wealth hara sell share japan smaller capitalization fund nysejof estee company nyseel share vision narus financial partner invests marsh mclennan company nysemmc vision sell share f nasdaqffiv clorox company nyseclx share purchased vision vision boost stake carmax nysekmx franklin resource nyseben reduced code waechter vision sell share schwab international equity nysearcaschf people bank oh cut stock broadcom nasdaqavgo vision sell share ishares esg aware msci usa nasdaqesgu people bank oh sell share ishares msci eafe nysearcaefa stonebrook private stake dexcom nasdaqdxcm realty income corporation plan aug dividend nyseo website serving harvard undergrad woman minority lgbtq student taken crimson report moloney security asset decrease elevance health nyseelv nisa investment advisor decrease stake marriott international nasdaqmar nisa investment advisor sell share synopsys nasdaqsnps mainstreet investment advisor million stock ameriprise financial nyseamp nisa investment advisor sell share ameriprise financial nyseamp stratos investment purchase new fiserv nysefi nisa investment advisor million paypal nasdaqpypl mt bank corp million stock marriott international nasdaqmar financial gravity asset invests million intuit nasdaqintu superman star nathan fillion staunchly defends character extreme hairstyle team bowl cut federal judge block end birthright citizenship doncasters planned new secondary school place meet demand jane birkins original hermes bag sale drunk defiant bar song tipsy chart froma harrop drunk defiant bar song tipsy chart froma harrop drunk defiant bar song tipsy chart froma harrop drunk defiant bar song tipsy chart froma harrop drunk defiant bar song tipsy chart froma harrop drunk defiant bar song tipsy chart froma harrop drunk defiant bar song tipsy chart froma harrop drunk defiant bar song tipsy chart froma harrop drunk defiant bar song tipsy chart froma harrop vision mn new investment occidental petroleum corporation nyseoxy moloney security asset sell share northrop grumman corporation nysenoc trane technology plc nysett share alpine wood investor alpine wood investor sell share northrop grumman corporation nysenoc quotient wealth partner raise stake trane technology plc nysett euna solution issue open introducing competition commitment expand supplier participation public procurement team deutsche bank aktiengesellschaft begin coverage cinemark nysecnk share shell plc unsponsored adr nyseshel purchased pom investment strategy nxp semiconductor nasdaqnxpi microchip technology nasdaqmchp critical analysis sekisui house skhsy rival critical comparison ishares sp smallcap growth nasdaqijt share acquired code waechter financial comparison transocean nyserig royale energy otcmktsroyl code waechter boost stock pacer small cap cash cow batscalf analyzing zkh nysezkh taoping nasdaqtaop unitedhealth incorporated nyseunh stake trimmed code waechter northwest natural gas company nysenwn stock lessened code waechter code waechter invests pnc financial service nysepnc medtronic plc nysemdt trimmed code waechter dexterra tsedxt set new high buy mkango resource lonmka stock price oracle power lonorcp share</t>
+          <t>ahead arch earnings release killed mill buy ethereum expect leidos q earnings report successful couple morning little hello relationship expert world bull bear tiger ai launch agentic capability latest molecular universe release increase value proposition rd service found best amazon prime deal shopping thousand offer cnn fed rate cut coming opinion vary widely fury intercept lio ninaaskumuwin discovery incorporation boerne lawmaker investigate response flood covered call screener texas passed quantum computing legislation play ionq stock homebuyers finally responded mortgage rate hit lowest level month cnbc palantir technology sp hottest stock past close incredible rally continue cybersecurity stock buy next decade business newsline amazon extends prime discount trump medium file crypto blue chip vibe coding arrived business wsj bigname adviser avoiding crypto speculative investment move buying marketwatch trump threatened bomb moscow deter putin cnn trump bill promise tax tip overtime limitheres qualifies droit launch explore mode adept platform h room optimism risk complacency aes freeportmcmoran verona pharma intel aehr penguin solution mover barrons michelle obama learned great parenting tip mom dadthey job modeling bmw v mercedes sale race linda yaccarino step ceo elon musk x dax push higher eu edge closer tariff deal prime deal verge eli manning longer interested buying piece nfls giant expensive merck acquire verona pharma expanding portfolio include ohtuvayre ensifentrine firstinclass copd maintenance treatment adult expected drive growth next decade merck acquire verona pharma expanding portfolio include ohtuvayre ensifentrine firstinclass copd maintenance treatment adult expected drive growth next decade merckcom walmart selling fantastic chromebook laptop shopper love touchscreen feature word help teach kid critical thinking michelle obama psychologist malaysian pm warns southeast asia trade war passing storm quadmotor rivians arrive wild power wilder price apple catch ai race rival turn heat boomer buying highestyielding dividend champion handoverfist smith corporation nyseaos purchased private trust co na elon musk grok ai chatbot denies praised hitler antisemitic vickers insider pick hudson edge investment partner million stock jpmorgan chase co nysejpm private trust co na stock coterra energy nysectra rosalia balance newest brand ambassador russia launch another record drone attack ukraine ukrainian beware scam promise good pay completing easy online task beware scam promise good pay completing easy online task money market account rate rate hit heloc equity loan rate highyield saving account rate rate steady beware scam promise good pay completing easy online task bank england flag global debt pressure market stabilization goldman demand oath junior banker fend private equity poaching bloomberg block rule cancel subscription easily sp future tick higher investor shrug trump tariff threat fomc tap mortgage refinance rate rate increase mortgage rate rate move cd rate rate rise uae oil market thirsty opec barrel proposed clermont subdivision redesign deadly lakeshore drive exact science announces medicare coverage oncodetecttm molecular residual disease test colorectal cancer fresh del monte produce report quarter financial trump trade blitz produce deal lot uncertainty trump trade blitz produce deal lot uncertainty trump trade blitz produce deal lot uncertainty trump trade blitz produce deal lot uncertainty trump trade blitz produce deal lot uncertainty trump trade blitz produce deal lot uncertainty era restaurant worker earn sixfigure salary benefit industry provide tesla board ground rule musk political activism analyst samsung launch foldable smartphones fends chinese rival trump tariff extension leaf bank fed limbo hbo max prestige brand streaming corra rising demand global investor due diligence investigation market sputter trump push tariff deadline xrp price forecast hit insider loading xrp x auddia announces leadership change special committee evaluate business combination restructuring ai native company senate gop gear test trump doge cut inside information orion upgrade fullyear outlook social security sends million american misleading blatantly political message shreveport director awardwinning screenplay red carpet premiere atlantic nickel expands rpm zone awaruite nickelalloy nife discovery meter northern extension yield nickel concentrate meter dtr metallurgical recovery testing shreveport kick eleven store louisiana site planned ragnarok ip title achieved game ranking taiwan hong kong macau toast nysetost acquired da davidson co private trust co na stock ge healthcare technology nasdaqgehc trump bill slash cfpb funding davenport co sell fortive corporation nyseftv private trust co na acquires emcor nyseeme less month claim ev tax credit buy car expert legend cross zone pound gear favorite principal financial increase stock zimmer biomet nysezbh mutual advisor buy trane technology plc nysett mutual advisor grows stock decker outdoor corporation nysedeck malaria drug newborn young infant expected approved africa rapid anchor suspended sentence domestic assault bank england warns high financial market risk easing tension kisti secures funding national quantum center excellence name ionq primary quantum partner opinion president punishes patriot wednesday world burn eye turn diddy european russia behind downing mh watch popular podcaster discusses kamala episode scrapped talked gibberish campaign wanted canned fbi bust chinese national multimillion dollar drug ring exploiting immigration system president business trump admin sue california transgender athlete policy view congressional delegation must fight cut noaa burke county company hildebran wont issue permit train cabin business another voice buffalo garden vibrantly express community soul trump admin subpoena harvard foreign student misconduct campus radicalism george conway flag trump awkward admission fresh proof fool eu seek finalize trade deal trump end month hawaii lawmaker demand immigration arrest briefing haleiwa development council review road usage charge begin electric vehicle governor budget veto trim public school maintenance hooser sbcd travesty process policy senate gop gear test trump doge cut senate gop gear test trump doge cut jewish democrat congress sound alarm mamdani tea party patriot push lawmaker noncitizen voting jewish democrat congress sound alarm mamdani tea party patriot push lawmaker noncitizen voting senate gop gear test trump doge cut larger fight rage trump racking college tea party patriot push lawmaker noncitizen voting jewish democrat congress sound alarm mamdani larger fight rage trump racking college larger fight rage trump racking college senate gop gear test trump doge cut senate gop gear test trump doge cut tea party patriot push lawmaker noncitizen voting jewish democrat congress sound alarm mamdani tea party patriot push lawmaker noncitizen voting jewish democrat congress sound alarm mamdani senate gop gear test trump doge cut larger fight rage trump racking college tea party patriot push lawmaker noncitizen voting larger fight rage trump racking college jewish democrat congress sound alarm mamdani larger fight rage trump racking college candace cameron bure son biblebased pep helped save marriage antiviolence advocate gun manufacturer accountable mass shooting river north tragedy chicago allows people trump trade blitz produce deal lot uncertainty laura washington art institute slowly getting normal georgia police arrest farmworkers warrant dhs firearm testing ballistics unit open september county forensics lab dc fire cut tax increase police presence council bid view trekking pole lend mountainclimber swagger steve corbin give liberty tinpot dictator scare buying reported rochester legislator favor legal pot business california focus legislator favor legal pot business california focus editorial cartoon legend cross zone pound gear favorite president wife named ellen edith malaria drug newborn young infant expected approved africa red bull team principal christian horner fired team month stuck south north korean billion served trump bill billion served trump bill supreme reject shielding identity police attending jan capitol rally trump slam democrat inflation narrative cut cost president history red bull team principal christan horner sacked team voting known voting known everything expect family fun colnes alkincoates park robinhood ceo tokenization major innovation market wont qualify car loan interest deduction allegheny county council approves innamorato choice shuman advisory board pittsburgh council pas protection lgbtq people elon musk grok remove politically incorrect instruction praise hitler flash flooding texas preventable trump tariff pharmaceutical import increase percent threetime mvp nikola jokic delay signing extension nugget summer source trump boast threat bomb st moscow leaked audio charles warns small boat crisis profound challenge host macron banquet ahead migrant deal newsom holy grail reform view newsom holy grail reform view supreme allows trump administration resume mass federal layoff suit challenge government effort deport supporter propalestinian protest invest america act give newborn investment account dell ceo call futureproofing prosperity sam altman asks stuff reader speak uconn health center rail trump ramble middle cabinet meeting karat nonsense wall street trump taco trade chicken egg problem meet national police force mamdanis farleft ally primary hakeem jeffries nyc democrat reader speak american tragedy power inhumane congressional democrat push watchdog oversee trump white house american work together fix education weve opposite search old lady pony continues tariff squeezing corporate margin survey find ai changing world faster realize fencing chore enjoyed texas relying fema cut trump usaid action evil trump usaid action evil microsoft patch vulnerability critical flaw spnego sql server</t>
         </is>
       </c>
     </row>
@@ -910,12 +906,12 @@
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>time run out for nearly centuryold michigan clock company due to tariff other factor ap news sage rhino capital llc sell share of shell plc unsponsored adr nyseshel vanguard total stock market etf nysearcavti position increased by seamount financial group inc sage rhino capital llc acquires share of vanguard total stock market etf nysearcavti kesler norman wride llc boost stake in broadcom inc nasdaqavgo genus capital management inc invests million in ishares msci eafe etf nysearcaefa sage rhino capital llc buy share of broadcom inc nasdaqavgo vanguard total stock market etf nysearcavti is clarity wealth advisor llcs rd largest position seamount financial group inc buy share of vanguard dividend appreciation etf nysearcavig state of michigan retirement system ha million stock holding in chubb limited nysecb state of michigan retirement system ha million position in lam research corporation nasdaqlrcx clarity wealth advisor llc reduces holding in the walt disney company nysedis genus capital management inc make new investment in ishares msci eafe etf nysearcaefa kesler norman wride llc buy share of vanguard information technology etf nysearcavgt chubb limited nysecb share sold by state of michigan retirement system sage rhino capital llc purchase share of broadcom inc nasdaqavgo state of michigan retirement system decrease stake in lam research corporation nasdaqlrcx seamount financial group inc raise stock holding in vanguard dividend appreciation etf nysearcavig think quantum computing will be the next big thing these are the stock to buy today boss quietly veto devastating law that may pull the rug out on american and thousand would lose cash ford recall vehicle over fuel pump defect manufacturing layoff at pacira oak hill bios phase angelman data france launch criminal investigation into musk x over algorithm manipulation politicoeu trump million crypto mystery man reuters buy the dip win again for stock investor rockwell automation pharmasuite power sinteticas swiss drug production teledyne raymarine acquires maretron asset to boost marine automation cummins unveils new hydrogen turbocharger for european heavyduty engine dover techcon unveils new precision dispensing cartridge for key industry carrier global enhances aipowered abound app for proactive building management trane technology debut first u dynamic closed loop geothermal system in chicago school district johnson control sensormatic solution launch aipowered shopper tracking with privacyfirst reid technology goldman sachs mustbuy chip stock and a few you should forget honeywell explores sale of two division ahead of planned split raytheon from rtx demonstrates autonomous barracuda mine neutralization vehicle gmbacked energyx expands lithium holding in u smackover formation with pantera acquisition boeing win b space force contract for nextgen nuclear comms satellite penguin solution launch nextgen stratus ztc endurance for ultrahigh availability ai workload clarivate unveils enhanced g research innovation scorecard with expanded data ai insight xerox completes b lexmark acquisition support print market position globant suntory global spirit partner to deploy gen ai commercial insight agent concentrix half carbon emission target by detail progress in sustainability report dxc technology aipowered tendia solution slash bid writing time for ventia genpact launch aipowered ap suite to revolutionize account payable process kyndryl launch new aipowered service to accelerate mainframe migration to aws saic awarded m air force contract for rapid warfighting prototype development shopper can now buy a bjs membership for just a year in new deal it cheaper than rival sam club u bank set to post trading gain on trump tariff turmoil cognizant pledge to white house ai education initiative aim to train m by education department to resume interest accrual on million student loan borrower rtx corporation nysertx stake reduced by cfolife group llc fonville wealth management llc cut stake in costco wholesale corporation nasdaqcost kesler norman wride llc acquires share of invesco qqq nasdaqqqq bernardo wealth planning llc cut stock holding in alphabet inc nasdaqgoog nextera energy inc nysenee holding lifted by cerity partner llc leavell investment management inc reduces position in ishares core u aggregate bond etf nysearcaagg leavell investment management inc raise stake in uber technology inc nyseuber fonville wealth management llc sell share of southern company the nyseso cerity partner llc boost holding in invesco qqq nasdaqqqq capital insight partner llc raise stock holding in freeportmcmoran inc nysefcx kesler norman wride llc sell share of stryker corporation nysesyk costco wholesale corporation nasdaqcost share sold by alp advisor inc fonville wealth management llc increase stake in vanguard growth etf nysearcavug capital insight partner llc acquires share of freeportmcmoran inc nysefcx kesler norman wride llc increase stock holding in linde plc nasdaqlin phillips financial management llc sell share of schwab u largecap etf nysearcaschx financial gravity asset management inc purchase new position in costco wholesale corporation nasdaqcost kesler norman wride llc sell share of stryker corporation nysesyk parr mcknight wealth management group llc trim holding in spdr gold share nysearcagld cerity partner llc trim stock position in adobe inc nasdaqadbe uk business confidence plummet to threeyear low icaew walmart recall water bottle after two consumer suffer vision loss from ejecting lid walmart recall water bottle after two consumer suffer vision loss from ejecting lid walmart recall water bottle after two consumer suffer vision loss from ejecting lid walmart recall water bottle after two consumer suffer vision loss from ejecting lid wall street giant issue stark message on sp walmart recall water bottle after two consumer suffer vision loss from ejecting lid ap news nikki bella discusses wwe evolution looking at ge vernovas recent unusual option activity check out what whale are doing with citigroup analyzing broadcom in comparison to competitor in semiconductor semiconductor equipment industry chief executive officer of integral ad science holdi sold k in stock italianstyle villa in south minneapolis linden hill listed for m sell alert aaron yeon ho lee cash out m in acushnet holding stock sell alert kevin chang keun yoon cash out m in acushnet holding stock allworth financial lp raise holding in pepsico inc nasdaqpep state of michigan retirement system ha million holding in philip morris international inc nysepm state of michigan retirement system sell share of intuit inc nasdaqintu cisco system inc nasdaqcsco share sold by state of michigan retirement system state of michigan retirement system sell share of pepsico inc nasdaqpep leavell investment management inc sell share of merck co inc nysemrk mjp associate inc adv increase stake in invesco sp equal weight etf nysearcarsp state of michigan retirement system cut stake in merck co inc nysemrk state of michigan retirement system reduces holding in ishares core sp midcap etf nysearcaijh merck co inc nysemrk stake reduced by leavell investment management inc insider decision gene soo yoon yoon offloads m worth of acushnet holding stock lacroix announces new partnership with the dallas wing wnba team royal caribbean take delivery of world largest cruise ship insider decision tod e carpenter exercise option at donaldson for m evaluating apple against peer in technology hardware storage peripheral industry clarity wealth advisor llc sell share of the walt disney company nysedis state of michigan retirement system reduces stock holding in cme group inc nasdaqcme state of michigan retirement system ha million stock holding in palo alto network inc nasdaqpanw sage rhino capital llc cut position in vanguard ftse allworld exus etf nysearcaveu cfc planning co llc ha million stake in the walt disney company nysedis parr mcknight wealth management group llc sell share of spdr gold share nysearcagld kesler norman wride llc ha million position in fortinet inc nasdaqftnt round rock advisor llc purchase share of verizon communication inc nysevz financial gravity asset management inc buy share of costco wholesale corporation nasdaqcost phillips financial management llc sell share of schwab u largecap etf nysearcaschx round rock advisor llc ha stock holding in salesforce inc nysecrm kesler norman wride llc buy share of linde plc nasdaqlin omb director question powell over fed hq renovation spending perfektblue bluetooth vulnerability expose million of vehicle to remote code execution trump doing all the thing he said he would bondi or bongino bongino wont remain at fbi if bondi keep job source say u is selling weapon to nato ally to give to ukraine trump say ishares core sp midcap etf nysearcaijh share sold by state of michigan retirement system kla corporation nasdaqklac share bought by mjp associate inc adv state of michigan retirement system ha million stock position in merck co inc nysemrk veteran political reporter reveals what the medium missed about trump appeal to american in back to back barrie could the antisemitism plan be used to silence dissent podcast the special envoy plan is the latest push to weaponise antisemitism a a relentless campaign pay off louise adler albanese must be careful that tackling antisemitism doesnt curb free speech tom mcilroy virginia rep john mcguire bought over k worth of meta platform stock here what you should know congressional trading report rep susie lee sold over k in full house resort stock state right to sue over medical privacy state right to sue over medical privacy state right to sue over medical privacy california rep gilbert ray cisneros sold over k worth of springworks therapeutic inc ordinary share stock here what you should know laurel libby stood strong in the face of tyranny letter beth claybourn interior trump new front in the war on drug the bank the u air force want million to double production of the aim missile new themed playground equipment officially open for use in two lake charles park steve mann more on the aftermath of magees time in san bruno new england professional planning group inc reduces holding in international business machine corporation nyseibm pfizer inc nysepfe share sold by new england professional planning group inc diversify wealth management llc buy share of cocacola company the nyseko bipartisan legislation aim to legalize adultuse cannabis in pennsylvania cerity partner llc boost holding in mcdonalds corporation nysemcd mjp associate inc adv raise stock position in mcdonalds corporation nysemcd mcdonalds corporation nysemcd share purchased by freedom day solution llc moloney security asset management llc buy share of vanguard total bond market etf nasdaqbnd benny blanco ha made so much music he ha to shazam his own tune elv deadline today rosen leading trial attorney encourages elevance health inc investor epstein conspiracy just isnt there teacher union reveals true color and more from fox news opinion stratos wealth advisor llc trim stock position in the goldman sachs group inc nysegs freedom day solution llc decrease stock holding in amgen inc nasdaqamgn lbp am sa sell share of visa inc nysev the mindful minute by jon heydenreich that martini and megaburger u is selling weapon to nato ally to give to ukraine trump say u is selling weapon to nato ally to give to ukraine trump say u is selling weapon to nato ally to give to ukraine trump say u is selling weapon to nato ally to give to ukraine trump say u is selling weapon to nato ally to give to ukraine trump say greater midwest financial group llc purchase share of vanguard sp etf nysearcavoo barry investment advisor llc sell share of vanguard ftse emerging market etf nysearcavwo state department is firing over employee under trump administration plan rubio and wang stress cooperation after talk in malaysia a uschina tension simmer diversify wealth management llc buy share of ishares u treasury bond etf batsgovt cromwell holding llc decrease stake in micron technology inc nasdaqmu vanguard value etf nysearcavtv share sold by ade llc chevron corporation nysecvx share purchased by diversify wealth management llc cromwell holding llc raise stake in monolithic power system inc nasdaqmpwr church street road closure extended in brattleboro u is selling weapon to nato ally to give to ukraine trump say noqualifyjpg bill to clarify st louis sheriff duty stall in committee strategist flag very unusual trump admin loyalty test on cnn fidelis capital partner llc ha million stake in thermo fisher scientific inc nysetmo pkk fighter pile up their weapon in arm amnesty in northern iraq brazil vow retaliatory tariff against u if trump follows through on import tax new pac form to back mamdani nyc mayoral bid a business community rally to defeat him history program highlight the map and stone wall of dummerson financial gravity asset management inc buy new position in ishares tip bond etf nysearcatip phillips financial management llc increase holding in vanguard ftse developed market etf nysearcavea trump plan to hike tariff on canadian good to trump plan to tour texas flood damage a the scope of the disaster test his pledge to shutter fema trump plan to hike tariff on canadian good to ishares msci emerging market etf nysearcaeem share sold by ramsay stattman vela price inc burford brother inc raise position in the sherwinwilliams company nyseshw spdr dow jones industrial average etf trust nysearcadia position lifted by christopher j hasenberg inc genus capital management inc invests million in the sherwinwilliams company nyseshw state department to axe employee state of michigan retirement system boost stock position in prologis inc nysepld advanced micro device inc nasdaqamd share purchased by clarity wealth advisor llc seamount financial group inc sell share of vanguard total world stock etf nysearcavt share in vaneck gold miner etf nysearcagdx acquired by sage rhino capital llc vestia personal wealth advisor increase position in dimensional u marketwide value etf nysearcadfuv milwaukee remove fonzie statue amid reckoning with greaser past noqualifyingjpg exxon mobil corporation nysexom share sold by pineridge advisor llc cfolife group llc buy share of ge aerospace nysege stonebrook private inc buy share of vanguard total stock market etf nysearcavti allworth financial lp grows position in united parcel service inc nyseups cerity partner llc sell share of adobe inc nasdaqadbe adobe inc nasdaqadbe holding lowered by xponance inc honeywell international inc nasdaqhon share bought by kesler norman wride llc amphenol corporation nyseaph position boosted by cerity partner llc</t>
+          <t>hot yield highlight energy midstream giant mplx advanced micro device earnings preview what to expect advanced micro device earnings preview what to expect vanguard smallcap value etf nysearcavbr share purchased by telos capital management inc kimberlyclark co nysekmb share acquired by telos capital management inc telos capital management inc make new million investment in te connectivity ltd nysetel stonebrook private inc purchase share of salesforce inc nysecrm telos capital management inc ha million stake in danaher corporation nysedhr cerity partner ocio llc buy share of ishares mb etf nasdaqmbb telos capital management inc ha million holding in deere company nysede keurig dr pepper inc nasdaqkdp share purchased by parr mcknight wealth management group llc stonebrook private inc purchase share of ishares core msci europe etf nysearcaieur capital insight partner llc lower holding in tractor supply company nasdaqtsco stonebrook private inc ha million stake in darden restaurant inc nysedri most u adult say child care cost are a major problem a new apnorc poll find sunrocket capital announces million financing for renewable energy project supporting ai and data center market united airline holding unusual option activity for july where comstock resource stand with analyst this is what whale are betting on palantir technology this is what whale are betting on celestica expert outlook associated banc through the eye of analyst olehenriksen launch peach glaze collection the juicy clinical result your skin craves application for jobless benefit fall to last week korean officer to receive imo highest bravery award for fishing vessel rescue nvidia ceo jensen huang could soon be richer than warren buffetthes worth billion now where federated hermes stand with analyst spotify technology nysespot is steadview capital management llcs th largest position marvell technology nasdaqmrvl now covered by the goldman sachs group applied material nasdaqamat coverage initiated by analyst at the goldman sachs group stryker corporation nysesyk share sold by aurdan capital management llc financial gravity asset management inc invests in ge aerospace nysege nvidia nasdaqnvda coverage initiated at the goldman sachs group applovin corporation nasdaqapp share sold by steadview capital management llc aurdan capital management llc trim stock position in stryker corporation nysesyk the analyst verdict molina healthcare in the eye of expert how kanava ai is bringing voice automation to industrial workflow an interview with smit dagli peering into borgwarners recent short interest what doe the market think about somnigroup international what analyst are saying about jdcom stock white house accuses powell of mismanaging federal reserve citing headquarters renovation what doe the market think about selective insurance gr wake up dead man a knife out mystery to open bfi london film festival beyond the number analyst discus verizon communication stock stock pressured by u trade policy uncertainty stock pressured by u trade policy uncertainty change in the supervisory and management board and audit committee of admiral market a trump loses appeal of million e jean carroll sexual abuse defamation verdict sun life u and dentaquest donate to support texas flooding relief effort spindrift partner with patricof co to welcome new wave of athlete investor brain monitoring market size to hit usd million by coherent market insight brain monitoring market size to hit usd million by coherent market insight ga telesis engine service gate usa spah launch leap engine quick turn service marking major capability expansion bigbank a extended the term of the supervisory board member hammond power solution announces second quarter financial result conference call and webcast notification china asean build new paradigm for regional cooperation temo inc achieved florida product approval for hurricaneresistant impact glass sunroom vixs premium with ad now available in directvs miespanol genre pack behavioral rehabilitation market surpasses usd billion in fueled by anxiety and substance abuse disorder hydroxyethyl cellulose market to surpass usd million by demand driven by expanding application in personal care construction and pharmaceutical oil price sink a iran and u resume nuclear talk research the gender wage gap tipping point hii to host second quarter earnings conference call and webcast on july packaging solution market valued at trillion and heading to trillion by spacelift raise m series c to redefine enterprise infrastructure automation consumer who sold real estate that wa listed on ml property information network and paid commission to a real estate agent may be affected by a settlement vishay intertechnology q result earnings call webcast detail exclusive nbcus super bowl ad now going for million helcim introduces it new smart terminal a faster sleeker smarter way to accept payment ine security launch enhanced emapt certification blockdags global launch release entry set it apart over bitcoin cash shiba inu american airline group announces webcast of secondquarter financial result consumer who sold real estate that wa listed on ml property information network and paid commission to a real estate agent may be affected by a settlement rapidscale start technology scholarship at wake tech proptech market to usd billion by owing to rising demand for digital real estate transaction and smart property solution report by sn insider trader weigh opec tariff and resilient demand change in the supervisory and management board and audit committee of admiral market a everyone know what broke in leverage ratio reform can fix it greenleaf trust grows holding in blackstone inc nysebx index fund advisor inc take position in servicenow inc nysenow axxcess wealth management llc ha million stock position in morgan stanley nysems parr mcknight wealth management group llc acquires share of vanguard total international bond etf nasdaqbndx peddock capital advisor llc ha million holding in thermo fisher scientific inc nysetmo index fund advisor inc make new million investment in vanguard total international stock etf nasdaqvxus financial review creditriskmonitorcom crmz versus it competitor parr mcknight wealth management group llc make new million investment in invesco bulletshares corporate bond etf nasdaqbscr this amd analyst turn bullish here are top upgrade for thursday dhls m expansion in uk and ireland novo nordisks quality testing site in china new mexico educational retirement board reduces stock position in copart inc nasdaqcprt axxcess wealth management llc lower stake in accenture plc nyseacn u capital wealth advisor llc ha million position in airbnb inc nasdaqabnb axxcess wealth management llc ha million position in philip morris international inc nysepm leavell investment management inc purchase share of caterpillar inc nysecat linden thomas advisory service llc acquires share of accenture plc nyseacn accenture plc nyseacn share sold by axxcess wealth management llc greenleaf trust sell share of norfolk southern corporation nysensc caterpillar inc nysecat share bought by leavell investment management inc hara capital llc sell share of united airline holding inc nasdaqual hara capital llc lower holding in or royalty inc nyseor abbvie nyseabbv v bayer aktiengesellschaft otcmktsbayry head to head contrast saba capital income opportunity fund ii nysesaba share sold by hara capital llc narus financial partner llc acquires new holding in decker outdoor corporation nysedeck cerity partner ocio llc trim holding in ishares year treasury bond etf nasdaqtlt parr mcknight wealth management group llc grows stake in salesforce inc nysecrm stonebrook private inc ha million stock position in best buy co inc nysebby stonebrook private inc boost stock position in darden restaurant inc nysedri albany veteran banned from boshart davis office sue iceblock criminal evasion tool or constitutionally protected speech iceblock criminal evasion tool or constitutionally protected speech iceblock criminal evasion tool or constitutionally protected speech gop sen thom tillis say hegseth is out of his depth a defense secretary defcon ai achieves major rd milestone with launch of advanced theater distribution planning tool for talisman sabre financial gravity asset management inc acquires share of solventum corporation nysesolv sweeping bipartisan bill would nationalize standard for student athlete pay wake up dead man a knife out mystery to open bfi london film festival drone nerd debut ndaacompliant wingtraray fixedwing drone judge weighs motion to dismiss charge against a north adam man accused of killing his wife america greatest threat come from within letter to the editor beware of halftruths around direct primary care medicaid cut in trump tax bill will devastate access to care in rural pennsylvania critic say iranian supreme leader appears in public for first time since war the washington post latest antitrump commentator is a literal clown on onon and the competition head to head contrast analyzing saker aviation service skas and it rival greenleaf trust sell share of norfolk southern corporation nysensc astra wealth partner llc increase stock position in dimensional international core equity etf batsdfic hara capital llc decrease stock position in invesco rafi u etf nysearcaprf hara capital llc sell share of gildan activewear inc nysegil hara capital llc invests in delta air line inc nysedal hara capital llc decrease holding in saba capital income opportunity fund ii nysesaba astra wealth partner llc purchase share of ishares sp midcap value etf nysearcaijj hara capital llc ha holding in franklin ftse south korea etf nysearcaflkr hara capital llc cut stake in zoom communication inc nasdaqzm bxm wealth llc ha stock position in visa inc nysev exclusive ice nabs two m ringleader in midwest raid after testifying before congress on antisemitism cal poly hosted all day for palestine hara capital llc trim stock holding in bank of america corporation nysebac parr mcknight wealth management group llc ha million stock holding in vanguard total bond market etf nasdaqbnd financial gravity asset management inc purchase share of baring bdc inc nysebbdc parr mcknight wealth management group llc acquires share of sp global inc nysespgi axxcess wealth management llc sell share of intuitive surgical inc nasdaqisrg people financial service corp trim stock position in mastercard incorporated nysema general motor company nysegm share bought by tru independence llc union pacific corporation nyseunp share purchased by axxcess wealth management llc hara capital llc sell share of japan smaller capitalization fund inc nysejof the estee lauder company inc nyseel share sold by vision capital management inc narus financial partner llc invests in marsh mclennan company inc nysemmc vision capital management inc sell share of f inc nasdaqffiv the clorox company nyseclx share purchased by vision capital management inc vision capital management inc boost stake in carmax inc nysekmx franklin resource inc nyseben position reduced by code waechter llc vision capital management inc sell share of schwab international equity etf nysearcaschf people bank oh cut stock position in broadcom inc nasdaqavgo vision capital management inc sell share of ishares esg aware msci usa etf nasdaqesgu people bank oh sell share of ishares msci eafe etf nysearcaefa stonebrook private inc ha stake in dexcom inc nasdaqdxcm realty income corporation plan aug dividend of nyseo website serving harvard undergrad woman minority and lgbtq student taken down crimson report moloney security asset management llc decrease holding in elevance health inc nyseelv nisa investment advisor llc decrease stake in marriott international inc nasdaqmar nisa investment advisor llc sell share of synopsys inc nasdaqsnps mainstreet investment advisor llc ha million stock holding in ameriprise financial inc nyseamp nisa investment advisor llc sell share of ameriprise financial inc nyseamp stratos investment management llc purchase new position in fiserv inc nysefi nisa investment advisor llc ha million position in paypal holding inc nasdaqpypl mt bank corp ha million stock position in marriott international inc nasdaqmar financial gravity asset management inc invests million in intuit inc nasdaqintu superman star nathan fillion staunchly defends his character extreme hairstyle i wa team bowl cut the whole way federal judge again block end to birthright citizenship doncasters planned number of new secondary school place will not meet demand jane birkins original hermes bag go on sale drunk and defiant a bar song tipsy top the chart froma harrop drunk and defiant a bar song tipsy top the chart froma harrop drunk and defiant a bar song tipsy top the chart froma harrop drunk and defiant a bar song tipsy top the chart froma harrop drunk and defiant a bar song tipsy top the chart froma harrop drunk and defiant a bar song tipsy top the chart froma harrop drunk and defiant a bar song tipsy top the chart froma harrop drunk and defiant a bar song tipsy top the chart froma harrop drunk and defiant a bar song tipsy top the chart froma harrop true vision mn llc make new investment in occidental petroleum corporation nyseoxy moloney security asset management llc sell share of northrop grumman corporation nysenoc trane technology plc nysett share sold by alpine wood capital investor llc alpine wood capital investor llc sell share of northrop grumman corporation nysenoc quotient wealth partner llc raise stake in trane technology plc nysett euna solution issue open letter introducing competition commitment to expand supplier participation for public procurement team deutsche bank aktiengesellschaft begin coverage on cinemark nysecnk share in shell plc unsponsored adr nyseshel purchased by pom investment strategy llc nxp semiconductor nasdaqnxpi and microchip technology nasdaqmchp critical analysis sekisui house skhsy and it rival critical comparison ishares sp smallcap growth etf nasdaqijt share acquired by code waechter llc financial comparison transocean nyserig and royale energy otcmktsroyl code waechter llc boost stock position in pacer u small cap cash cow etf batscalf analyzing zkh group nysezkh and taoping nasdaqtaop unitedhealth group incorporated nyseunh stake trimmed by code waechter llc northwest natural gas company nysenwn stock holding lessened by code waechter llc code waechter llc invests in the pnc financial service group inc nysepnc medtronic plc nysemdt position trimmed by code waechter llc dexterra group tsedxt set new year high time to buy mkango resource lonmka stock price down here why oracle power lonorcp share down here why</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>run nearly centuryold michigan clock company due tariff factor sage rhino sell share shell plc unsponsored adr nyseshel vanguard total stock market nysearcavti increased seamount financial sage rhino acquires share vanguard total stock market nysearcavti kesler norman wride boost stake broadcom nasdaqavgo genus invests million ishares msci eafe nysearcaefa sage rhino buy share broadcom nasdaqavgo vanguard total stock market nysearcavti clarity wealth advisor llcs rd largest seamount financial buy share vanguard dividend appreciation nysearcavig michigan retirement system million stock chubb limited nysecb michigan retirement system million lam research corporation nasdaqlrcx clarity wealth advisor reduces walt disney company nysedis genus new investment ishares msci eafe nysearcaefa kesler norman wride buy share vanguard information technology nysearcavgt chubb limited nysecb share michigan retirement system sage rhino purchase share broadcom nasdaqavgo michigan retirement system decrease stake lam research corporation nasdaqlrcx seamount financial raise stock vanguard dividend appreciation nysearcavig quantum computing next stock buy bos quietly veto devastating pull rug american thousand lose cash ford recall vehicle fuel pump defect manufacturing layoff pacira oak hill bios phase angelman data france launch criminal investigation musk x algorithm manipulation politicoeu trump million crypto mystery man reuters buy dip stock investor rockwell automation pharmasuite power sinteticas swiss drug production teledyne raymarine acquires maretron asset boost marine automation cummins unveils new hydrogen turbocharger european heavyduty engine dover techcon unveils new precision dispensing cartridge industry carrier global enhances aipowered abound app proactive building trane technology debut dynamic closed loop geothermal system chicago school district johnson control sensormatic solution launch aipowered shopper tracking privacyfirst reid technology goldman sachs mustbuy chip stock forget honeywell explores sale division ahead planned split raytheon rtx demonstrates autonomous barracuda mine neutralization vehicle gmbacked energyx expands lithium smackover formation pantera acquisition boeing b space force contract nextgen nuclear comms satellite penguin solution launch nextgen stratus ztc endurance ultrahigh availability ai workload clarivate unveils enhanced g research innovation scorecard expanded data ai insight xerox completes b lexmark acquisition support print market globant suntory global spirit partner deploy gen ai commercial insight agent concentrix half carbon emission target detail progress sustainability report dxc technology aipowered tendia solution slash bid writing ventia genpact launch aipowered suite revolutionize account payable process kyndryl launch new aipowered service accelerate mainframe migration aws saic awarded air force contract rapid warfighting prototype development shopper buy bjs membership new deal cheaper rival sam club bank set post trading gain trump tariff turmoil cognizant pledge white house ai education initiative aim train education department resume interest accrual million student loan borrower rtx corporation nysertx stake reduced cfolife fonville wealth cut stake costco wholesale corporation nasdaqcost kesler norman wride acquires share invesco qqq nasdaqqqq bernardo wealth planning cut stock alphabet nasdaqgoog nextera energy nysenee lifted cerity partner leavell investment reduces ishares core aggregate bond nysearcaagg leavell investment raise stake uber technology nyseuber fonville wealth sell share southern company nyseso cerity partner boost invesco qqq nasdaqqqq insight partner raise stock freeportmcmoran nysefcx kesler norman wride sell share stryker corporation nysesyk costco wholesale corporation nasdaqcost share alp advisor fonville wealth increase stake vanguard growth nysearcavug insight partner acquires share freeportmcmoran nysefcx kesler norman wride increase stock linde plc nasdaqlin phillips financial sell share schwab largecap nysearcaschx financial gravity asset purchase new costco wholesale corporation nasdaqcost kesler norman wride sell share stryker corporation nysesyk parr mcknight wealth trim spdr gold share nysearcagld cerity partner trim stock adobe nasdaqadbe uk business confidence plummet threeyear low icaew walmart recall water bottle consumer suffer vision loss ejecting lid walmart recall water bottle consumer suffer vision loss ejecting lid walmart recall water bottle consumer suffer vision loss ejecting lid walmart recall water bottle consumer suffer vision loss ejecting lid wall street giant issue stark message sp walmart recall water bottle consumer suffer vision loss ejecting lid nikki bella discusses wwe evolution ge vernovas recent unusual option activity whale citigroup analyzing broadcom comparison competitor semiconductor semiconductor equipment industry chief executive officer integral ad science holdi k stock italianstyle villa south minneapolis linden hill listed sell alert aaron yeon ho lee cash acushnet stock sell alert kevin chang keun yoon cash acushnet stock allworth financial lp raise pepsico nasdaqpep michigan retirement system million philip morris international nysepm michigan retirement system sell share intuit nasdaqintu cisco system nasdaqcsco share michigan retirement system michigan retirement system sell share pepsico nasdaqpep leavell investment sell share merck co nysemrk mjp associate adv increase stake invesco sp equal weight nysearcarsp michigan retirement system cut stake merck co nysemrk michigan retirement system reduces ishares core sp midcap nysearcaijh merck co nysemrk stake reduced leavell investment insider decision gene soo yoon yoon offloads worth acushnet stock lacroix announces new partnership dallas wing wnba team royal caribbean take delivery world largest cruise ship insider decision tod e carpenter exercise option donaldson evaluating apple peer technology hardware storage peripheral industry clarity wealth advisor sell share walt disney company nysedis michigan retirement system reduces stock cme nasdaqcme michigan retirement system million stock palo alto network nasdaqpanw sage rhino cut vanguard ftse allworld exus nysearcaveu cfc planning co million stake walt disney company nysedis parr mcknight wealth sell share spdr gold share nysearcagld kesler norman wride million fortinet nasdaqftnt round rock advisor purchase share verizon communication nysevz financial gravity asset buy share costco wholesale corporation nasdaqcost phillips financial sell share schwab largecap nysearcaschx round rock advisor stock salesforce nysecrm kesler norman wride buy share linde plc nasdaqlin omb director powell fed hq renovation spending perfektblue bluetooth vulnerability expose million vehicle remote code execution trump bondi bongino bongino wont fbi bondi job source selling weapon nato ally give ukraine trump ishares core sp midcap nysearcaijh share michigan retirement system kla corporation nasdaqklac share bought mjp associate adv michigan retirement system million stock merck co nysemrk veteran political reporter reveals medium missed trump appeal american barrie antisemitism plan used silence dissent podcast special envoy plan latest push weaponise antisemitism relentless campaign pay louise adler albanese must careful tackling antisemitism doesnt curb free speech tom mcilroy virginia rep john mcguire bought k worth meta platform stock congressional trading report rep susie lee k full house resort stock sue medical privacy sue medical privacy sue medical privacy california rep gilbert ray cisneros k worth springworks therapeutic ordinary share stock laurel libby stood strong face tyranny beth claybourn interior trump new front war drug bank air force million double production aim missile new themed playground equipment officially open lake charles park steve mann aftermath magees san bruno new england professional planning reduces international business machine corporation nyseibm pfizer nysepfe share new england professional planning diversify wealth buy share cocacola company nyseko bipartisan legislation aim legalize adultuse cannabis pennsylvania cerity partner boost mcdonalds corporation nysemcd mjp associate adv raise stock mcdonalds corporation nysemcd mcdonalds corporation nysemcd share purchased freedom solution moloney security asset buy share vanguard total bond market nasdaqbnd benny blanco music shazam tune elv deadline rosen leading trial attorney encourages elevance health investor epstein conspiracy isnt teacher union reveals color fox opinion stratos wealth advisor trim stock goldman sachs nysegs freedom solution decrease stock amgen nasdaqamgn lbp sa sell share visa nysev mindful jon heydenreich martini megaburger selling weapon nato ally give ukraine trump selling weapon nato ally give ukraine trump selling weapon nato ally give ukraine trump selling weapon nato ally give ukraine trump selling weapon nato ally give ukraine trump greater midwest financial purchase share vanguard sp nysearcavoo barry investment advisor sell share vanguard ftse emerging market nysearcavwo department firing employee trump administration plan rubio wang stress cooperation malaysia uschina tension simmer diversify wealth buy share ishares treasury bond batsgovt cromwell decrease stake micron technology nasdaqmu vanguard value nysearcavtv share ade chevron corporation nysecvx share purchased diversify wealth cromwell raise stake monolithic power system nasdaqmpwr church street road closure extended brattleboro selling weapon nato ally give ukraine trump noqualifyjpg bill clarify st louis sheriff duty stall committee strategist flag unusual trump admin loyalty test cnn fidelis partner million stake thermo fisher scientific nysetmo pkk fighter pile weapon arm amnesty northern iraq brazil vow retaliatory tariff trump follows import tax new pac form mamdani nyc mayoral bid business community rally defeat history program highlight map stone wall dummerson financial gravity asset buy new ishares tip bond nysearcatip phillips financial increase vanguard ftse developed market nysearcavea trump plan hike tariff canadian good trump plan tour texas flood damage scope disaster test pledge shutter fema trump plan hike tariff canadian good ishares msci emerging market nysearcaeem share ramsay stattman vela price burford brother raise sherwinwilliams company nyseshw spdr dow jones industrial average trust nysearcadia lifted christopher j hasenberg genus invests million sherwinwilliams company nyseshw department axe employee michigan retirement system boost stock prologis nysepld advanced micro device nasdaqamd share purchased clarity wealth advisor seamount financial sell share vanguard total world stock nysearcavt share vaneck gold miner nysearcagdx acquired sage rhino vestia personal wealth advisor increase dimensional marketwide value nysearcadfuv milwaukee remove fonzie statue amid reckoning greaser past noqualifyingjpg exxon mobil corporation nysexom share pineridge advisor cfolife buy share ge aerospace nysege stonebrook private buy share vanguard total stock market nysearcavti allworth financial lp grows united parcel service nyseups cerity partner sell share adobe nasdaqadbe adobe nasdaqadbe lowered xponance honeywell international nasdaqhon share bought kesler norman wride amphenol corporation nyseaph boosted cerity partner</t>
+          <t>hot yield highlight energy midstream giant mplx advanced micro device earnings preview expect advanced micro device earnings preview expect vanguard smallcap value nysearcavbr purchased telos kimberlyclark co nysekmb acquired telos telos million investment te connectivity ltd nysetel stonebrook private purchase salesforce nysecrm telos million stake danaher corporation nysedhr cerity partner ocio buy ishares mb nasdaqmbb telos million deere company nysede keurig dr pepper nasdaqkdp purchased parr mcknight wealth stonebrook private purchase ishares core msci europe nysearcaieur insight partner lower tractor supply company nasdaqtsco stonebrook private million stake darden restaurant nysedri adult child care cost major problem apnorc poll find sunrocket announces million financing renewable energy project supporting ai data center market united airline unusual option activity comstock resource stand analyst whale betting palantir technology whale betting celestica expert outlook associated banc eye analyst olehenriksen launch peach glaze collection juicy clinical skin craves application jobless benefit fall korean officer receive imo highest bravery award fishing vessel rescue nvidia ceo jensen huang soon richer warren buffetthes worth billion federated hermes stand analyst spotify technology nysespot steadview llcs largest marvell technology nasdaqmrvl covered goldman sachs applied material nasdaqamat coverage initiated analyst goldman sachs stryker corporation nysesyk aurdan financial gravity asset invests ge aerospace nysege nvidia nasdaqnvda coverage initiated goldman sachs applovin corporation nasdaqapp steadview aurdan trim stock stryker corporation nysesyk analyst verdict molina healthcare eye expert kanava ai bringing voice automation industrial interview smit dagli peering borgwarners recent short interest doe market somnigroup international analyst saying jdcom stock white house accuses powell mismanaging federal reserve citing renovation doe market selective insurance gr wake dead man knife mystery open bfi london film festival beyond analyst discus verizon communication stock stock pressured trade policy uncertainty stock pressured trade policy uncertainty change supervisory board audit committee admiral market trump loses appeal million e jean carroll sexual abuse defamation verdict sun life dentaquest donate support texas flooding relief effort spindrift partner patricof co welcome wave athlete investor brain monitoring market size hit usd million coherent market insight brain monitoring market size hit usd million coherent market insight ga telesis engine service gate usa spah launch leap engine quick turn service marking major capability expansion bigbank extended term supervisory board hammond power solution announces quarter financial conference call webcast notification china asean build paradigm regional cooperation temo achieved florida product approval hurricaneresistant impact glass sunroom vixs premium ad available directvs miespanol genre pack behavioral rehabilitation market surpasses usd billion fueled anxiety substance abuse disorder hydroxyethyl cellulose market surpass usd million demand driven expanding application personal care construction pharmaceutical oil price sink iran resume nuclear research gender wage gap tipping hii host quarter earnings conference call webcast packaging solution market valued trillion heading trillion spacelift raise series c redefine enterprise infrastructure automation consumer real estate listed ml property information network paid commission real estate agent affected settlement vishay intertechnology q earnings call webcast detail exclusive nbcus super bowl ad million helcim introduces smart terminal faster sleeker smarter accept payment ine security launch enhanced emapt certification blockdags global launch release entry set apart bitcoin cash shiba inu american airline announces webcast secondquarter financial consumer real estate listed ml property information network paid commission real estate agent affected settlement rapidscale start technology scholarship wake tech proptech market usd billion owing rising demand digital real estate transaction smart property solution report sn insider trader weigh opec tariff resilient demand change supervisory board audit committee admiral market everyone broke leverage ratio reform fix greenleaf trust grows blackstone nysebx index fund advisor take servicenow nysenow axxcess wealth million stock morgan stanley nysems parr mcknight wealth acquires vanguard total international bond nasdaqbndx peddock advisor million thermo fisher scientific nysetmo index fund advisor million investment vanguard total international stock nasdaqvxus financial review creditriskmonitorcom crmz versus competitor parr mcknight wealth million investment invesco bulletshares corporate bond nasdaqbscr amd analyst turn bullish upgrade thursday dhls expansion uk ireland novo nordisks quality testing site china mexico educational retirement board reduces stock copart nasdaqcprt axxcess wealth lower stake accenture plc nyseacn wealth advisor million airbnb nasdaqabnb axxcess wealth million philip morris international nysepm leavell investment purchase caterpillar nysecat linden thomas advisory service acquires accenture plc nyseacn accenture plc nyseacn axxcess wealth greenleaf trust sell norfolk southern corporation nysensc caterpillar nysecat bought leavell investment hara sell united airline nasdaqual hara lower royalty nyseor abbvie nyseabbv v bayer aktiengesellschaft otcmktsbayry head head contrast saba income opportunity fund ii nysesaba hara narus financial partner acquires decker outdoor corporation nysedeck cerity partner ocio trim ishares treasury bond nasdaqtlt parr mcknight wealth grows stake salesforce nysecrm stonebrook private million stock best buy co nysebby stonebrook private boost stock darden restaurant nysedri albany veteran banned boshart davis office sue iceblock criminal evasion tool constitutionally protected speech iceblock criminal evasion tool constitutionally protected speech iceblock criminal evasion tool constitutionally protected speech gop sen thom tillis hegseth depth defense secretary defcon ai achieves major rd milestone launch advanced theater distribution planning tool talisman sabre financial gravity asset acquires solventum corporation nysesolv sweeping bipartisan bill nationalize student athlete pay wake dead man knife mystery open bfi london film festival drone nerd debut ndaacompliant wingtraray fixedwing drone judge weighs motion dismiss charge north adam man accused killing wife america greatest threat come editor beware halftruths around direct primary care medicaid cut trump tax bill devastate access care rural pennsylvania critic iranian supreme public since war washington post latest antitrump commentator literal clown onon competition head head contrast analyzing saker aviation service skas rival greenleaf trust sell norfolk southern corporation nysensc astra wealth partner increase stock dimensional international core equity batsdfic hara decrease stock invesco rafi nysearcaprf hara sell gildan activewear nysegil hara invests delta air line nysedal hara decrease saba income opportunity fund ii nysesaba astra wealth partner purchase ishares sp midcap value nysearcaijj hara franklin ftse south korea nysearcaflkr hara cut stake zoom communication nasdaqzm bxm wealth stock visa nysev exclusive nabs ringleader midwest raid testifying congress antisemitism cal poly hosted palestine hara trim stock bank america corporation nysebac parr mcknight wealth million stock vanguard total bond market nasdaqbnd financial gravity asset purchase baring bdc nysebbdc parr mcknight wealth acquires sp global nysespgi axxcess wealth sell intuitive surgical nasdaqisrg people financial service corp trim stock mastercard incorporated nysema general company nysegm bought tru independence union pacific corporation nyseunp purchased axxcess wealth hara sell japan smaller capitalization fund nysejof company nyseel vision narus financial partner invests marsh mclennan company nysemmc vision sell f nasdaqffiv clorox company nyseclx purchased vision vision boost stake carmax nysekmx franklin resource nyseben reduced code waechter vision sell schwab international equity nysearcaschf people bank oh cut stock broadcom nasdaqavgo vision sell ishares esg aware msci usa nasdaqesgu people bank oh sell ishares msci eafe nysearcaefa stonebrook private stake dexcom nasdaqdxcm realty income corporation plan aug dividend nyseo website serving harvard undergrad woman minority lgbtq student taken crimson report moloney security asset decrease elevance health nyseelv nisa investment advisor decrease stake marriott international nasdaqmar nisa investment advisor sell synopsys nasdaqsnps mainstreet investment advisor million stock ameriprise financial nyseamp nisa investment advisor sell ameriprise financial nyseamp stratos investment purchase fiserv nysefi nisa investment advisor million paypal nasdaqpypl mt bank corp million stock marriott international nasdaqmar financial gravity asset invests million intuit nasdaqintu superman star nathan fillion staunchly defends character extreme hairstyle team bowl cut federal judge block end birthright citizenship doncasters planned secondary school place meet demand jane birkins original hermes bag sale drunk defiant bar song tipsy chart froma harrop drunk defiant bar song tipsy chart froma harrop drunk defiant bar song tipsy chart froma harrop drunk defiant bar song tipsy chart froma harrop drunk defiant bar song tipsy chart froma harrop drunk defiant bar song tipsy chart froma harrop drunk defiant bar song tipsy chart froma harrop drunk defiant bar song tipsy chart froma harrop drunk defiant bar song tipsy chart froma harrop vision mn investment occidental petroleum corporation nyseoxy moloney security asset sell northrop grumman corporation nysenoc trane technology plc nysett alpine wood investor alpine wood investor sell northrop grumman corporation nysenoc quotient wealth partner raise stake trane technology plc nysett euna solution issue open introducing competition commitment expand supplier participation public procurement team deutsche bank aktiengesellschaft begin coverage cinemark nysecnk shell plc unsponsored adr nyseshel purchased pom investment strategy nxp semiconductor nasdaqnxpi microchip technology nasdaqmchp critical analysis sekisui house skhsy rival critical comparison ishares sp smallcap growth nasdaqijt acquired code waechter financial comparison transocean nyserig royale energy otcmktsroyl code waechter boost stock pacer small cap cash cow batscalf analyzing zkh nysezkh taoping nasdaqtaop unitedhealth incorporated nyseunh stake trimmed code waechter northwest natural gas company nysenwn stock lessened code waechter code waechter invests pnc financial service nysepnc medtronic plc nysemdt trimmed code waechter dexterra tsedxt set high buy mkango resource lonmka stock price oracle power lonorcp</t>
         </is>
       </c>
     </row>
@@ -924,7 +920,7 @@
         <v>45852</v>
       </c>
       <c r="B14" t="n">
-        <v>6269.5498046875</v>
+        <v>6268.56005859375</v>
       </c>
       <c r="C14" t="n">
         <v>6273.31005859375</v>
@@ -936,22 +932,162 @@
         <v>6255.14990234375</v>
       </c>
       <c r="F14" t="n">
-        <v>2040375000</v>
+        <v>4722250000</v>
       </c>
       <c r="G14" t="n">
-        <v>0.0015655265286154</v>
+        <v>0.0014074138094573</v>
       </c>
       <c r="H14" t="n">
         <v>1</v>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>b t capital management dba alpha capital management make new investment in taiwan semiconductor manufacturing company ltd nysetsm vanguard midcap etf nysearcavo is beirne wealth consulting service llcs th largest position vanguard smallcap etf nysearcavb share sold by b t capital management dba alpha capital management walmart inc nysewmt position increased by fort sheridan advisor llc kathmere capital management llc buy share of vanguard smallcap etf nysearcavb kathmere capital management llc purchase share of walmart inc nysewmt ishares core sp smallcap etf nysearcaijr share sold by forum private client group llc kathmere capital management llc purchase share of vanguard smallcap etf nysearcavb b t capital management dba alpha capital management boost position in honeywell international inc nasdaqhon fort sheridan advisor llc boost stake in walmart inc nysewmt ifc advisor llc sell share of the home depot inc nysehd ifc advisor llc ha million holding in pepsico inc nasdaqpep quest wealth builder inc sell share of eli lilly and company nyselly caterpillar inc nysecat share sold by ifc advisor llc ballentine partner llc lower position in invesco qqq nasdaqqqq quest wealth builder inc sell share of pepsico inc nasdaqpep ballentine partner llc sell share of invesco qqq nasdaqqqq caterpillar inc nysecat share sold by ifc advisor llc eureka business weather economic uncertainty ap business summarybrief at pm edt ap business summarybrief at pm edt why share of the metal company skyrocketed in the first half of why share of the metal company skyrocketed in the first half of is circle internet stock a millionaire maker another large grocery chain follows kroger in closing store is circle internet stock a millionaire maker another large grocery chain follows kroger in closing store fulcrum equity management ha stake in broadcom inc nasdaqavgo why nvidia partner navitas semiconductor surged in the first half of why nvidia partner navitas semiconductor surged in the first half of a bitcoin matures volatility dropsso expect slower climb say expert decrypt crypto top gainer why blockdag solana pepe and render are leading in growth and utility how ai notetakers can become the black box of business the low altitude market could be worth trillion by according to morgan stanley this cathie wood stock is my top pick to dominate the opportunity hint it not archer aviation the low altitude market could be worth trillion by according to morgan stanley this cathie wood stock is my top pick to dominate the opportunity hint it not archer aviation iron ore price surge amid china industrial crackdown northwest capital management inc buy share of ishares core sp midcap etf nysearcaijh rational advisor inc invests million in mcdonalds corporation nysemcd superman smash box office expectation soaring towards million opening pam bondi fire doj staffer who worked on trump case amid chaos at agency nikulski financial inc buy share of lowes company inc nyselow mjp associate inc adv ha holding in blackstone inc nysebx cerity partner llc grows stock position in palantir technology inc nasdaqpltr trump to impose tariff on eu mexico starting aug trump to impose eu tariff on aug trumnp to impose eu tariff on august trump announces tariff on import from mexico eu eu say it still want u trade deal will defend interest tucker carlson reveals who he think funded jeffrey epstein crime focused wealth management inc increase stock position in merck co inc nysemrk roger wittlin investment advisory llc acquires share of vanguard sp etf nysearcavoo family firm inc ha million stock holding in ishares russell etf nysearcaiwm schwab u smallcap etf nysearcascha share sold by family firm inc roger wittlin investment advisory llc purchase share of vanguard sp etf nysearcavoo quest wealth builder inc ha stock holding in parkerhannifin corporation nyseph share in vanguard high dividend yield etf nysearcavym acquired by stillwater wealth management group ishares russell etf nysearcaiwm share sold by family firm inc well fargo company nysewfc share sold by family firm inc bank of america corporation nysebac share acquired by fortem financial group llc fortem financial group llc boost stock position in att inc nyset unitedhealth down is the dividend still safe netflix inc nasdaqnflx share acquired by martin capital advisor llp vanguard ftse developed market etf nysearcavea share purchased by bridge generation wealth management llc riversedge advisor llc grows holding in vanguard ftse emerging market etf nysearcavwo american financial advisor llc reduces stock holding in ge vernova inc nysegev crowdstrike nasdaqcrwd share acquired by american financial advisor llc riversedge advisor llc purchase share of alphabet inc nasdaqgoog vanguard value etf nysearcavtv share purchased by riversedge advisor llc vanguard value etf nysearcavtv share purchased by riversedge advisor llc crowdstrike nasdaqcrwd share bought by american financial advisor llc tesla inc nasdaqtsla share bought by riversedge advisor llc riversedge advisor llc ha holding in salesforce inc nysecrm american financial advisor llc ha million position in ishares core sp etf nysearcaivv vanguard ftse developed market etf nysearcavea position decreased by riversedge advisor llc grant grossmendelsohn llc ha holding in vanguard ftse developed market etf nysearcavea dogecoins doge holder are shifting to ruvi ai ruvi passed audit and early entry bonus make it the smarter bet auour investment llc ha million stake in ishares core msci eafe etf batsiefa fort sheridan advisor llc raise stock holding in abbott laboratory nyseabt beirne wealth consulting service llc increase stock position in ishares core msci eafe etf batsiefa b t capital management dba alpha capital management buy share of schwab u largecap growth etf nysearcaschg b t capital management dba alpha capital management purchase share of schwab u largecap growth etf nysearcaschg quest wealth builder inc cut stock position in walmart inc nysewmt ifc advisor llc reduces position in vanguard midcap etf nysearcavo spdr gold share nysearcagld share purchased by acorn wealth advisor llc ballentine partner llc increase position in chevron corporation nysecvx acorn wealth advisor llc sell share of ishares core sp smallcap etf nysearcaijr acorn wealth advisor llc ha stock position in vanguard midcap etf nysearcavo acorn wealth advisor llc reduces stock position in ishares core sp smallcap etf nysearcaijr ballentine partner llc acquires share of walmart inc nysewmt history say these stock could be big winner in the second half history say these stock could be big winner in the second half alp advisor inc ha million stock position in kkr co inc nysekkr eli lilly and company nyselly share sold by wealthtrust asset management llc eli lilly and company nyselly is harmony asset management llcs th largest position the home depot inc nysehd share purchased by lane associate llc fulcrum equity management lower stock holding in eli lilly and company nyselly fulcrum equity management sell share of eli lilly and company nyselly servicenow inc nysenow share acquired by steelpeak wealth llc trump target mexico eu with tariff hartford bakery inc voluntarily recall hundred of loaf of artisanal bread sold in state cbs news reader view we can all reduce greenhouse gas shes great trump back bondi want top official to end conflict over epstein ishares core sp smallcap etf nysearcaijr share sold by forum private client group llc chevron corporation nysecvx share acquired by b t capital management dba alpha capital management forum private client group llc ha million position in vanguard midcap etf nysearcavo b t capital management dba alpha capital management increase stake in honeywell international inc nasdaqhon beirne wealth consulting service llc acquires share of vanguard smallcap etf nysearcavb ifc advisor llc boost holding in kkr co inc nysekkr ballentine partner llc grows holding in eli lilly and company nyselly young democrat have called for a rebrand theyre vying to replace the party old guard temperance in cabinetry climate change helped fuel heavy rain that led to devastating texas flood former pentagon insider could trump big beautiful bill finally unlock america longforgotten resource archaeolgists find largestever ceremony hall weapon hoard the democratic party is missing an opportunity to engage christian voter northwest capital management inc purchase share of ishares core sp midcap etf nysearcaijh rational advisor inc take position in mcdonalds corporation nysemcd superman smash box office expectation soaring towards million opening pam bondi fire doj staffer who worked on trump case amid chaos at agency nikulski financial inc acquires share of lowes company inc nyselow parkerhannifin corporation nyseph share sold by quest wealth builder inc family firm inc lower stock holding in schwab u smallcap etf nysearcascha family firm inc reduces stock holding in well fargo company nysewfc stillwater wealth management group invests in vanguard high dividend yield etf nysearcavym extrump lawyer dershowitz claim knowledge of epstein client list i know the name but im bound by confidentiality grant grossmendelsohn llc purchase share of vanguard ftse developed market etf nysearcavea riversedge advisor llc cut stake in vanguard ftse developed market etf nysearcavea piper sandler issue positive forecast for netflix nasdaqnflx stock price riversedge advisor llc ha holding in salesforce inc nysecrm american financial advisor llc ha million stake in ishares core sp etf nysearcaivv riversedge advisor llc increase stake in ishares core sp etf nysearcaivv start exploring cloud mining for free from the new winnermining app and get visible daily reward forum private client group llc trim position in vanguard growth etf nysearcavug fort sheridan advisor llc buy share of vanguard growth etf nysearcavug the big beautiful bill and mlp qualifying income acorn wealth advisor llc lower holding in chevron corporation nysecvx ballentine partner llc buy share of walmart inc nysewmt ballentine partner llc sell share of ishares core sp smallcap etf nysearcaijr lane associate llc sell share of eli lilly and company nyselly harmony asset management llc ha million holding in the home depot inc nysehd steelpeak wealth llc ha million stake in the progressive corporation nysepgr servicenow inc nysenow share acquired by steelpeak wealth llc trump threatens rosie odonnells citizenship she is a threat to humanity annual new london to new brighton antique car run to take place aug coyle financial counsel llc invests in qualcomm incorporated nasdaqqcom broadcom inc nasdaqavgo share sold by skyoak wealth llc forum private client group llc take position in elevance health inc nyseelv a major red flag for republican a trump policy threatens their future fbi director kash patel responds to controversy surrounding epstein file stillwater wealth management group grows position in amgen inc nasdaqamgn riversedge advisor llc grows stake in tesla inc nasdaqtsla fort sheridan advisor llc ha position in kla corporation nasdaqklac kathmere capital management llc grows holding in vanguard value etf nysearcavtv nycs broken election system need far more than these bandaid fix ballentine partner llc ha million position in abbott laboratory nyseabt abbott laboratory nyseabt share acquired by ifc advisor llc trump post support for embattled attorney general pam bondi ma private wealth take position in bristol myers squibb company nysebmy parkerhannifin corporation nyseph share sold by lbp am sa harmony asset management llc reduces stock position in chevron corporation nysecvx bonus editorial cartoon for july federal employee bracing after supreme court greenlights widespread layoff federal employee bracing after supreme court greenlights widespread layoff federal employee bracing after supreme court greenlights widespread layoff lawmaker visit alligator alcatraz but some wonder how much theyll get to see man convicted of meredith kerchers murder facing trial for sexual assault federal employee bracing after supreme court greenlights widespread layoff federal employee bracing after supreme court greenlights widespread layoff federal employee bracing after supreme court greenlights widespread layoff focused wealth management inc ha million stake in walmart inc nysewmt berbice capital management llc grows position in kkr co inc nysekkr coyle financial counsel llc raise holding in invesco qqq nasdaqqqq meet china man in lima who jetted over to u to collect train donated by biden admin amazon prime day delivers record sale and saving in expanded fourday shopping event how new tax legislation impact clean energy tax credit the dalai lama is planning his succession a the ultimate protest against china the u army m vulcan air defense system wa a beast in the vietnam war the us john f kennedy fordclass carrier may miss it delivery date comcast corporation nasdaqcmcsa share sold by sage rhino capital llc kesler norman wride llc sell share of comcast corporation nasdaqcmcsa exchange capital management inc sell share of servicenow inc nysenow fukoku mutual life insurance co sell share of duke energy corporation nyseduk cerity partner llc buy share of asml holding nv nasdaqasml mjp associate inc adv take position in elevance health inc nyseelv fidelis capital partner llc boost stock position in elevance health inc nyseelv reader view u must invest in our independence candidate view localgovernment focus would benefit school board stillwater wealth management group reduces position in unitedhealth group incorporated nyseunh martin capital advisor llp sell share of oracle corporation nyseorcl park square financial group llc decrease stock position in ishares core sp midcap etf nysearcaijh fortem financial group llc purchase share of blackstone inc nysebx pya waltman capital llc ha million stake in mcdonalds corporation nysemcd massachusetts police officer shot by colleague victim of campaign to criminalize her lawyer horrified by alligator alcatraz letter coyle financial counsel llc ha million stake in ishares core sp etf nysearcaivv vanguard high dividend yield etf nysearcavym stock holding decreased by auour investment llc ifc advisor llc increase position in ishares russell etf nysearcaiwm forum private client group llc purchase new stake in cummins inc nysecmi fortem financial group llc grows holding in tesla inc nasdaqtsla vanguard ftse developed market etf nysearcavea share purchased by beirne wealth consulting service llc schear investment adviser llc buy share of tmobile u inc nasdaqtmus jrmc recognized for infection control rate wall street pro drop bold price target on circle stock bitcoin hit new alltime high above k a trader eye week uptrend cointelegraph cardinal strategic wealth guidance cut position in alphabet inc nasdaqgoog bradley co private wealth management llc reduces position in costco wholesale corporation nasdaqcost pointe capital management llc grows holding in the walt disney company nysedis westmount partner llc sell share of amgen inc nasdaqamgn westmount partner llc sell share of starbucks corporation nasdaqsbux westmount partner llc trim holding in lockheed martin corporation nyselmt q asset management buy share of williams company inc the nysewmb westmount partner llc trim holding in lockheed martin corporation nyselmt westmount partner llc trim stock position in amgen inc nasdaqamgn zullo investment group inc lower stock position in alphabet inc nasdaqgoog trunorth capital management llc acquires share of vanguard sp etf nysearcavoo pointe capital management llc boost holding in linde plc nasdaqlin ishares core u aggregate bond etf nysearcaagg share acquired by pointe capital management llc nextera energy inc nysenee share sold by pointe capital management llc bristol myers squibb company nysebmy stock holding lifted by prudent man advisor llc mqs management llc buy new position in nextera energy inc nysenee prudent man advisor llc acquires new position in blackrock nyseblk zullo investment group inc buy share of eli lilly and company nyselly zullo investment group inc acquires share of eli lilly and company nyselly zullo investment group inc cut stake in m company nysemmm prudent man advisor llc make new million investment in blackrock nyseblk mqs management llc take position in nextera energy inc nysenee ai financial service llc boost holding in eli lilly and company nyselly u tomato price could jump a soon a monday xrp break out near gain yet blockdags coin unlock chance at steal market focus top altcoins still lag while bitcoin stay strong promising outdoor stock to add to your watchlist july th kathmere capital management llc sell share of kimberlyclark co nysekmb citigroup inc nysec share purchased by ballentine partner llc cigna group nyseci share bought by ballentine partner llc ballentine partner llc purchase share of the sherwinwilliams company nyseshw arizona state retirement system purchase share of kimberlyclark co nysekmb bankplus trust department grows holding in ishares core sp smallcap etf nysearcaijr berkeley inc ha million holding in schwab u largecap etf nysearcaschx arizona state retirement system increase stake in kimberlyclark co nysekmb fdx advisor inc invests in medtronic plc nysemdt how trump latest tariff threat risk deeper damage to europe economy fort sheridan advisor llc increase stock position in cocacola company the nyseko fortem financial group llc sell share of conocophillips nysecop blackstone inc nysebx share bought by louisiana state employee retirement system eaton corporation plc nyseetn share sold by stephen inc ar taiwan semiconductor manufacturing company ltd nysetsm share sold by fulton breakefield broenniman llc why broadcoms avgo ai momentum ha goldman sachs backing the stock on gps nvidia ceo on the overwhelmingly positive effect of ai isthmus partner llc sell share of thermo fisher scientific inc nysetmo whitener capital management inc ha million stake in verizon communication inc nysevz share in thermo fisher scientific inc nysetmo purchased by eos management lp lowes company inc nyselow share acquired by zullo investment group inc eos management lp invests million in thermo fisher scientific inc nysetmo whitener capital management inc raise stock holding in lowes company inc nyselow on gps nvidia ceo on whether ai will lead to job loss rosen a topranked law firm encourages rocket pharmaceutical inc investor to secure counsel before important deadline in security class action rckt dem strategist on trump epstein blowback you wound this up you caused this reyes financial architecture inc boost position in advanced micro device inc nasdaqamd lri investment llc ha holding in danaher corporation nysedhr on gps nvidia ceo on the uschina ai race iconic mall retailer face second chapter bankruptcy closure nvidias huang say china military unlikely to use u ai chip bloomberg greatmark investment partner inc ha position in rtx corporation nysertx mark group wealth management inc grows position in honeywell international inc nasdaqhon pfizer inc nysepfe share acquired by secured retirement advisor llc cwm llc purchase share of jpmorgan ultrashort income etf nysearcajpst tfr capital llc purchase share of rtx corporation nysertx cwm llc ha million position in jpmorgan ultrashort income etf nysearcajpst share in texas instrument incorporated nasdaqtxn purchased by secured retirement advisor llc trunorth capital management llc purchase share of fiserv inc nysefi iron horse wealth management llc purchase share of vanguard ftse developed market etf nysearcavea trunorth capital management llc ha stock holding in att inc nyset fulton breakefield broenniman llc ha million stock holding in vanguard ftse developed market etf nysearcavea abbott laboratory nyseabt share purchased by dock street asset management inc workday wday just got downgradedheres why analyst are worried about ai target sends stern message to employee amid customer struggle target sends stern message to employee amid customer struggle thestreet prism advisor inc trim stock position in ishares core msci eafe etf batsiefa the home depot inc nysehd position reduced by sentinel trust co lba philip morris international inc nysepm share sold by legacy financial group inc philip morris international inc nysepm share sold by legacy financial group inc texas congressman call for accountability after flood we cant just allow girl to drown in the middle of the night greatmark investment partner inc grows position in general mill inc nysegis tfr capital llc purchase share of jpmorgan equity premium income etf nysearcajepi greatmark investment partner inc reduces holding in southern company the nyseso tfr capital llc acquires share of cisco system inc nasdaqcsco greatmark investment partner inc trim holding in cisco system inc nasdaqcsco hughes financial service llc take position in southern company the nyseso greatmark investment partner inc trim stock position in cisco system inc nasdaqcsco tfr capital llc ha million stock position in vertex pharmaceutical incorporated nasdaqvrtx hughes financial service llc take position in southern company the nyseso brn the impact of sport betting is complicated is the stock market underestimating president trump tariff cwm llc sell share of gilead science inc nasdaqgild isthmus partner llc purchase share of accenture plc nyseacn mark group wealth management inc buy share of chipotle mexican grill inc nysecmg secured retirement advisor llc take million position in comcast corporation nasdaqcmcsa legacy financial group inc lower position in stryker corporation nysesyk prudent man advisor llc ha million stake in labcorp holding inc nyselh left brain wealth management llc sell share of ge vernova inc nysegev schear investment adviser llc lower position in deere company nysede westmount partner llc sell share of the walt disney company nysedis zullo investment group inc trim stake in alphabet inc nasdaqgoog trunorth capital management llc purchase share of vanguard sp etf nysearcavoo pet lover demand leadership change at san jose animal shelter zullo investment group inc trim stake in m company nysemmm u tomato price could jump a soon a monday trump issue executive order targeting unreliable clean energy option kathmere capital management llc buy share of citigroup inc nysec berkeley inc decrease stock holding in schwab u largecap etf nysearcaschx hotel stock to follow today july th on gps nvidia ceo on the overwhelmingly positive effect of ai whitener capital management inc grows position in lowes company inc nyselow zullo investment group inc grows stock holding in lowes company inc nyselow on gps nvidia ceo on whether ai will lead to job loss dem strategist on trump epstein blowback you wound this up you caused this on gps nvidia ceo on the uschina ai race lri investment llc ha stock position in the goldman sachs group inc nysegs secured retirement advisor llc purchase new position in texas instrument incorporated nasdaqtxn mark group wealth management inc purchase share of copart inc nasdaqcprt tfr capital llc boost holding in rtx corporation nysertx att inc nyset position boosted by trunorth capital management llc fulton breakefield broenniman llc buy share of vanguard ftse developed market etf nysearcavea blame new york democrat not washington for new state budget crisis pepsico inc nasdaqpep stock holding cut by new york state common retirement fund the home depot inc nysehd share sold by sentinel trust co lba fdx advisor inc trim holding in the home depot inc nysehd a digitally enslaved generation cry for independence texas congressman call for accountability after flood we cant just allow girl to drown in the middle of the night tfr capital llc make new investment in marsh mclennan company inc nysemmc tfr capital llc acquires share of vertex pharmaceutical incorporated nasdaqvrtx greatmark investment partner inc decrease holding in cv health corporation nysecvs tfr capital llc make new investment in southern company the nyseso octa to host public input meeting on coastal rail trouble more talk around erosion planned trump to make unprecedented second state visit to uk in september left brain wealth management llc reduces stock position in unitedhealth group incorporated nyseunh left brain wealth management llc raise position in altria group inc nysemo isthmus partner llc sell share of the pnc financial service group inc nysepnc cwm llc ha million holding in comcast corporation nasdaqcmcsa what security leader need to know about ai governance for saas violent clash erupt between farright group and migrant in spanish town caterpillar inc nysecat share sold by asset dedication llc goalfusion wealth management llc ha million stock position in vanguard value etf nysearcavtv hughes financial service llc take position in vanguard value etf nysearcavtv rainey randall wealth advisor inc invests in zoetis inc nysezts hoag open new health center monday in san clemente oxbow advisor llc sell share of vanguard growth etf nysearcavug ishares tip bond etf nysearcatip share bought by hughes financial service llc schear investment adviser llc ha position in marathon petroleum corporation nysempc who is the most handsome waterbomb seoul star vote now maga faithful weigh in on epstein file debate prisoner in france escape in his cellmates bag homeowner and driver would pay for these scheme homeowner and driver would pay for these scheme homeowner and driver would pay for these scheme texas nw office had no warning coordination meteorologist during the flood did it make a difference caster semenyas sex eligibility battle ha confounded sport for yearsand still isnt over prudent man advisor llc boost stock position in deere company nysede prudent man advisor llc purchase share of costco wholesale corporation nasdaqcost mqs management llc buy share of lockheed martin corporation nyselmt prudent man advisor llc purchase share of alphabet inc nasdaqgoog ballentine partner llc increase stock holding in waste management inc nysewm promising outdoor stock to add to your watchlist july th kathmere capital management llc sell share of bristol myers squibb company nysebmy video game stock to follow now july th stephen inc ar increase position in walmart inc nysewmt schechter investment advisor llc ha million stock position in vanguard total international stock etf nasdaqvxus trump could potentially fire fed powell over building renovation hassett say learn how to can your own garden fresh produce mason investment advisory service inc ha stock position in procter gamble company the nysepg fulton breakefield broenniman llc purchase share of vanguard dividend appreciation etf nysearcavig fulton breakefield broenniman llc buy share of ishares core sp smallcap etf nysearcaijr prudent man advisor llc sell share of conocophillips nysecop sfs zero fatality goal crash into reality sfs zero fatality goal crash into reality sfs zero fatality goal crash into reality wilkinson global asset management llc buy share of parkerhannifin corporation nyseph reyes financial architecture inc purchase share of vanguard shortterm bond etf nysearcabsv lri investment llc purchase share of ishares u technology etf nysearcaiyw lri investment llc ha position in blackstone inc nysebx gopled state discussing plan to build prison like alligator alcatraz noem lri investment llc ha stake in danaher corporation nysedhr mark group wealth management inc acquires share of eaton corporation plc nyseetn dock street asset management inc acquires share of abbott laboratory nyseabt greatmark investment partner inc ha million stake in paychex inc nasdaqpayx oxbow advisor llc boost holding in jpmorgan ultrashort income etf nysearcajpst trunorth capital management llc purchase share of rtx corporation nysertx mutual of america capital management llc decrease stock holding in att inc nyset edge asset management lp boost holding in spdr portfolio emerging market etf nysearcaspem sen padilla ice is getting more aggressive more cruel more extreme child killed in albion hitandrun man charged legacy financial group inc cut stake in vanguard shortterm inflationprotected security etf nasdaqvtip ken morris be very careful what you do two year ago legacy financial group inc reduces stake in dimensional u core equity etf nysearcadfac left brain wealth management llc cut stock holding in applovin corporation nasdaqapp were going to litigate that order homan responds to judge restricting ice raid in la reyes financial architecture inc purchase share of ww grainger inc nysegww lri investment llc sell share of corning incorporated nyseglw kerntke otto mcglone wealth management group trim position in vanguard midcap etf nysearcavo one year after trump assassination attempt in butler change at secret service but question remain axecap investment llc sell share of apple inc nasdaqaapl fifth third bancorp sell share of apple inc nasdaqaapl sagace wealth management llc sell share of microsoft corporation nasdaqmsft microsoft corporation nasdaqmsft stake lowered by tran capital management lp define financial llc buy share of microsoft corporation nasdaqmsft sapient capital llc sell share of microsoft corporation nasdaqmsft teacher retirement system of texas sell share of safety insurance group inc nasdaqsaft teacher retirement system of texas sell share of organon co nyseogn teacher retirement system of texas cut stock holding in artisan partner asset management inc nyseapam teacher retirement system of texas buy new share in a o smith corporation nyseaos rev group inc nyserevg position trimmed by teacher retirement system of texas share in lamb weston nyselw acquired by teacher retirement system of texas bridgebio pharma inc nasdaqbbio share sold by teacher retirement system of texas two west capital advisor llc trim position in apple inc nasdaqaapl teacher retirement system of texas take million position in community health system inc nysecyh teacher retirement system of texas ha million position in portland general electric company nysepor teacher retirement system of texas buy share of ugi corporation nyseugi teacher retirement system of texas ha million stake in ziff davis inc nasdaqzd teacher retirement system of texas purchase new stake in the campbell company nasdaqcpb asian heat squeeze lng flow to europe borgwarner inc nysebwa share sold by cambridge investment research advisor inc teacher retirement system of texas ha million stake in madrigal pharmaceutical inc nasdaqmdgl exclusive interview the future belongs to nocodes with deep ai integration abhinav girdhar ceo founder appy pie european trade minister meet to forge strategy after trump surprise tariff european trade minister meet to forge strategy after trump surprise tariff european trade minister meet to forge strategy after trump surprise tariff relx nyserelx rating lowered to hold at wall street zen southside bancshares nysesbsi rating lowered to sell at wall street zen wall street zen downgrade vista energy nysevist to sell bank of america cut primo brand nyseprmb price target to silgan nyseslgn price target raised to stifel financial nysesf price target raised to ubiquitis ui buy rating reiterated at bw financial wall street zen upgrade rafael nyserfl to hold charles schwab nyseschw price target raised to sea nysese stock rating lowered by wall street zen sealed air nysesee price target raised to wall street zen upgrade te connectivity nysetel to buy telus digital nysetixt stock rating upgraded by wall street zen sealed air nysesee price target raised to telephone and data system nysetds stock rating upgraded by wall street zen synovus financial nysesnv price target raised to truist financial cut sonoco product nyseson price target to att nyset price target raised to wec energy group nysewec rating lowered to sell at wall street zen exxon mobil nysexom price target raised to at scotiabank truist financial raise webster financial nysewbs price target to top ai stock to buy this week the place report surge in company relocation driving demand for flexible office space in dubai and riyadh rockfire resource lonrock stock price up still a buy rockfire resource lonrock trading up should you buy new zealand energy cvenz trading down here what happened argentina lithium energy cvelit share down should you sell silver spruce resource cvesse share down here what happened silver spruce resource cvesse trading down time to sell new zealand energy cvenz trading down should you sell argentina lithium energy cvelit stock price down here why geomega resource cvegma stock price up whats next geomega resource cvegma trading higher still a buy geomega reso</t>
+          <t>time run out for nearly centuryold michigan clock company due to tariff other factor ap news sage rhino capital llc sell share of shell plc unsponsored adr nyseshel vanguard total stock market etf nysearcavti position increased by seamount financial group inc sage rhino capital llc acquires share of vanguard total stock market etf nysearcavti kesler norman wride llc boost stake in broadcom inc nasdaqavgo genus capital management inc invests million in ishares msci eafe etf nysearcaefa sage rhino capital llc buy share of broadcom inc nasdaqavgo vanguard total stock market etf nysearcavti is clarity wealth advisor llcs rd largest position seamount financial group inc buy share of vanguard dividend appreciation etf nysearcavig state of michigan retirement system ha million stock holding in chubb limited nysecb state of michigan retirement system ha million position in lam research corporation nasdaqlrcx clarity wealth advisor llc reduces holding in the walt disney company nysedis genus capital management inc make new investment in ishares msci eafe etf nysearcaefa kesler norman wride llc buy share of vanguard information technology etf nysearcavgt chubb limited nysecb share sold by state of michigan retirement system sage rhino capital llc purchase share of broadcom inc nasdaqavgo state of michigan retirement system decrease stake in lam research corporation nasdaqlrcx seamount financial group inc raise stock holding in vanguard dividend appreciation etf nysearcavig think quantum computing will be the next big thing these are the stock to buy today boss quietly veto devastating law that may pull the rug out on american and thousand would lose cash ford recall vehicle over fuel pump defect manufacturing layoff at pacira oak hill bios phase angelman data france launch criminal investigation into musk x over algorithm manipulation politicoeu trump million crypto mystery man reuters buy the dip win again for stock investor rockwell automation pharmasuite power sinteticas swiss drug production teledyne raymarine acquires maretron asset to boost marine automation cummins unveils new hydrogen turbocharger for european heavyduty engine dover techcon unveils new precision dispensing cartridge for key industry carrier global enhances aipowered abound app for proactive building management trane technology debut first u dynamic closed loop geothermal system in chicago school district johnson control sensormatic solution launch aipowered shopper tracking with privacyfirst reid technology goldman sachs mustbuy chip stock and a few you should forget honeywell explores sale of two division ahead of planned split raytheon from rtx demonstrates autonomous barracuda mine neutralization vehicle gmbacked energyx expands lithium holding in u smackover formation with pantera acquisition boeing win b space force contract for nextgen nuclear comms satellite penguin solution launch nextgen stratus ztc endurance for ultrahigh availability ai workload clarivate unveils enhanced g research innovation scorecard with expanded data ai insight xerox completes b lexmark acquisition support print market position globant suntory global spirit partner to deploy gen ai commercial insight agent concentrix half carbon emission target by detail progress in sustainability report dxc technology aipowered tendia solution slash bid writing time for ventia genpact launch aipowered ap suite to revolutionize account payable process kyndryl launch new aipowered service to accelerate mainframe migration to aws saic awarded m air force contract for rapid warfighting prototype development shopper can now buy a bjs membership for just a year in new deal it cheaper than rival sam club u bank set to post trading gain on trump tariff turmoil cognizant pledge to white house ai education initiative aim to train m by education department to resume interest accrual on million student loan borrower rtx corporation nysertx stake reduced by cfolife group llc fonville wealth management llc cut stake in costco wholesale corporation nasdaqcost kesler norman wride llc acquires share of invesco qqq nasdaqqqq bernardo wealth planning llc cut stock holding in alphabet inc nasdaqgoog nextera energy inc nysenee holding lifted by cerity partner llc leavell investment management inc reduces position in ishares core u aggregate bond etf nysearcaagg leavell investment management inc raise stake in uber technology inc nyseuber fonville wealth management llc sell share of southern company the nyseso cerity partner llc boost holding in invesco qqq nasdaqqqq capital insight partner llc raise stock holding in freeportmcmoran inc nysefcx kesler norman wride llc sell share of stryker corporation nysesyk costco wholesale corporation nasdaqcost share sold by alp advisor inc fonville wealth management llc increase stake in vanguard growth etf nysearcavug capital insight partner llc acquires share of freeportmcmoran inc nysefcx kesler norman wride llc increase stock holding in linde plc nasdaqlin phillips financial management llc sell share of schwab u largecap etf nysearcaschx financial gravity asset management inc purchase new position in costco wholesale corporation nasdaqcost kesler norman wride llc sell share of stryker corporation nysesyk parr mcknight wealth management group llc trim holding in spdr gold share nysearcagld cerity partner llc trim stock position in adobe inc nasdaqadbe uk business confidence plummet to threeyear low icaew walmart recall water bottle after two consumer suffer vision loss from ejecting lid walmart recall water bottle after two consumer suffer vision loss from ejecting lid walmart recall water bottle after two consumer suffer vision loss from ejecting lid walmart recall water bottle after two consumer suffer vision loss from ejecting lid wall street giant issue stark message on sp walmart recall water bottle after two consumer suffer vision loss from ejecting lid ap news nikki bella discusses wwe evolution looking at ge vernovas recent unusual option activity check out what whale are doing with citigroup analyzing broadcom in comparison to competitor in semiconductor semiconductor equipment industry chief executive officer of integral ad science holdi sold k in stock italianstyle villa in south minneapolis linden hill listed for m sell alert aaron yeon ho lee cash out m in acushnet holding stock sell alert kevin chang keun yoon cash out m in acushnet holding stock allworth financial lp raise holding in pepsico inc nasdaqpep state of michigan retirement system ha million holding in philip morris international inc nysepm state of michigan retirement system sell share of intuit inc nasdaqintu cisco system inc nasdaqcsco share sold by state of michigan retirement system state of michigan retirement system sell share of pepsico inc nasdaqpep leavell investment management inc sell share of merck co inc nysemrk mjp associate inc adv increase stake in invesco sp equal weight etf nysearcarsp state of michigan retirement system cut stake in merck co inc nysemrk state of michigan retirement system reduces holding in ishares core sp midcap etf nysearcaijh merck co inc nysemrk stake reduced by leavell investment management inc insider decision gene soo yoon yoon offloads m worth of acushnet holding stock lacroix announces new partnership with the dallas wing wnba team royal caribbean take delivery of world largest cruise ship insider decision tod e carpenter exercise option at donaldson for m evaluating apple against peer in technology hardware storage peripheral industry clarity wealth advisor llc sell share of the walt disney company nysedis state of michigan retirement system reduces stock holding in cme group inc nasdaqcme state of michigan retirement system ha million stock holding in palo alto network inc nasdaqpanw sage rhino capital llc cut position in vanguard ftse allworld exus etf nysearcaveu cfc planning co llc ha million stake in the walt disney company nysedis parr mcknight wealth management group llc sell share of spdr gold share nysearcagld kesler norman wride llc ha million position in fortinet inc nasdaqftnt round rock advisor llc purchase share of verizon communication inc nysevz financial gravity asset management inc buy share of costco wholesale corporation nasdaqcost phillips financial management llc sell share of schwab u largecap etf nysearcaschx round rock advisor llc ha stock holding in salesforce inc nysecrm kesler norman wride llc buy share of linde plc nasdaqlin omb director question powell over fed hq renovation spending perfektblue bluetooth vulnerability expose million of vehicle to remote code execution trump doing all the thing he said he would bondi or bongino bongino wont remain at fbi if bondi keep job source say u is selling weapon to nato ally to give to ukraine trump say ishares core sp midcap etf nysearcaijh share sold by state of michigan retirement system kla corporation nasdaqklac share bought by mjp associate inc adv state of michigan retirement system ha million stock position in merck co inc nysemrk veteran political reporter reveals what the medium missed about trump appeal to american in back to back barrie could the antisemitism plan be used to silence dissent podcast the special envoy plan is the latest push to weaponise antisemitism a a relentless campaign pay off louise adler albanese must be careful that tackling antisemitism doesnt curb free speech tom mcilroy virginia rep john mcguire bought over k worth of meta platform stock here what you should know congressional trading report rep susie lee sold over k in full house resort stock state right to sue over medical privacy state right to sue over medical privacy state right to sue over medical privacy california rep gilbert ray cisneros sold over k worth of springworks therapeutic inc ordinary share stock here what you should know laurel libby stood strong in the face of tyranny letter beth claybourn interior trump new front in the war on drug the bank the u air force want million to double production of the aim missile new themed playground equipment officially open for use in two lake charles park steve mann more on the aftermath of magees time in san bruno new england professional planning group inc reduces holding in international business machine corporation nyseibm pfizer inc nysepfe share sold by new england professional planning group inc diversify wealth management llc buy share of cocacola company the nyseko bipartisan legislation aim to legalize adultuse cannabis in pennsylvania cerity partner llc boost holding in mcdonalds corporation nysemcd mjp associate inc adv raise stock position in mcdonalds corporation nysemcd mcdonalds corporation nysemcd share purchased by freedom day solution llc moloney security asset management llc buy share of vanguard total bond market etf nasdaqbnd benny blanco ha made so much music he ha to shazam his own tune elv deadline today rosen leading trial attorney encourages elevance health inc investor epstein conspiracy just isnt there teacher union reveals true color and more from fox news opinion stratos wealth advisor llc trim stock position in the goldman sachs group inc nysegs freedom day solution llc decrease stock holding in amgen inc nasdaqamgn lbp am sa sell share of visa inc nysev the mindful minute by jon heydenreich that martini and megaburger u is selling weapon to nato ally to give to ukraine trump say u is selling weapon to nato ally to give to ukraine trump say u is selling weapon to nato ally to give to ukraine trump say u is selling weapon to nato ally to give to ukraine trump say u is selling weapon to nato ally to give to ukraine trump say greater midwest financial group llc purchase share of vanguard sp etf nysearcavoo barry investment advisor llc sell share of vanguard ftse emerging market etf nysearcavwo state department is firing over employee under trump administration plan rubio and wang stress cooperation after talk in malaysia a uschina tension simmer diversify wealth management llc buy share of ishares u treasury bond etf batsgovt cromwell holding llc decrease stake in micron technology inc nasdaqmu vanguard value etf nysearcavtv share sold by ade llc chevron corporation nysecvx share purchased by diversify wealth management llc cromwell holding llc raise stake in monolithic power system inc nasdaqmpwr church street road closure extended in brattleboro u is selling weapon to nato ally to give to ukraine trump say noqualifyjpg bill to clarify st louis sheriff duty stall in committee strategist flag very unusual trump admin loyalty test on cnn fidelis capital partner llc ha million stake in thermo fisher scientific inc nysetmo pkk fighter pile up their weapon in arm amnesty in northern iraq brazil vow retaliatory tariff against u if trump follows through on import tax new pac form to back mamdani nyc mayoral bid a business community rally to defeat him history program highlight the map and stone wall of dummerson financial gravity asset management inc buy new position in ishares tip bond etf nysearcatip phillips financial management llc increase holding in vanguard ftse developed market etf nysearcavea trump plan to hike tariff on canadian good to trump plan to tour texas flood damage a the scope of the disaster test his pledge to shutter fema trump plan to hike tariff on canadian good to ishares msci emerging market etf nysearcaeem share sold by ramsay stattman vela price inc burford brother inc raise position in the sherwinwilliams company nyseshw spdr dow jones industrial average etf trust nysearcadia position lifted by christopher j hasenberg inc genus capital management inc invests million in the sherwinwilliams company nyseshw state department to axe employee state of michigan retirement system boost stock position in prologis inc nysepld advanced micro device inc nasdaqamd share purchased by clarity wealth advisor llc seamount financial group inc sell share of vanguard total world stock etf nysearcavt share in vaneck gold miner etf nysearcagdx acquired by sage rhino capital llc vestia personal wealth advisor increase position in dimensional u marketwide value etf nysearcadfuv milwaukee remove fonzie statue amid reckoning with greaser past noqualifyingjpg exxon mobil corporation nysexom share sold by pineridge advisor llc cfolife group llc buy share of ge aerospace nysege stonebrook private inc buy share of vanguard total stock market etf nysearcavti allworth financial lp grows position in united parcel service inc nyseups cerity partner llc sell share of adobe inc nasdaqadbe adobe inc nasdaqadbe holding lowered by xponance inc honeywell international inc nasdaqhon share bought by kesler norman wride llc amphenol corporation nyseaph position boosted by cerity partner llc b t capital management dba alpha capital management make new investment in taiwan semiconductor manufacturing company ltd nysetsm vanguard midcap etf nysearcavo is beirne wealth consulting service llcs th largest position vanguard smallcap etf nysearcavb share sold by b t capital management dba alpha capital management walmart inc nysewmt position increased by fort sheridan advisor llc kathmere capital management llc buy share of vanguard smallcap etf nysearcavb kathmere capital management llc purchase share of walmart inc nysewmt ishares core sp smallcap etf nysearcaijr share sold by forum private client group llc kathmere capital management llc purchase share of vanguard smallcap etf nysearcavb b t capital management dba alpha capital management boost position in honeywell international inc nasdaqhon fort sheridan advisor llc boost stake in walmart inc nysewmt ifc advisor llc sell share of the home depot inc nysehd ifc advisor llc ha million holding in pepsico inc nasdaqpep quest wealth builder inc sell share of eli lilly and company nyselly caterpillar inc nysecat share sold by ifc advisor llc ballentine partner llc lower position in invesco qqq nasdaqqqq quest wealth builder inc sell share of pepsico inc nasdaqpep ballentine partner llc sell share of invesco qqq nasdaqqqq caterpillar inc nysecat share sold by ifc advisor llc eureka business weather economic uncertainty ap business summarybrief at pm edt ap business summarybrief at pm edt why share of the metal company skyrocketed in the first half of why share of the metal company skyrocketed in the first half of is circle internet stock a millionaire maker another large grocery chain follows kroger in closing store is circle internet stock a millionaire maker another large grocery chain follows kroger in closing store fulcrum equity management ha stake in broadcom inc nasdaqavgo why nvidia partner navitas semiconductor surged in the first half of why nvidia partner navitas semiconductor surged in the first half of a bitcoin matures volatility dropsso expect slower climb say expert decrypt crypto top gainer why blockdag solana pepe and render are leading in growth and utility how ai notetakers can become the black box of business the low altitude market could be worth trillion by according to morgan stanley this cathie wood stock is my top pick to dominate the opportunity hint it not archer aviation the low altitude market could be worth trillion by according to morgan stanley this cathie wood stock is my top pick to dominate the opportunity hint it not archer aviation iron ore price surge amid china industrial crackdown northwest capital management inc buy share of ishares core sp midcap etf nysearcaijh rational advisor inc invests million in mcdonalds corporation nysemcd superman smash box office expectation soaring towards million opening pam bondi fire doj staffer who worked on trump case amid chaos at agency nikulski financial inc buy share of lowes company inc nyselow mjp associate inc adv ha holding in blackstone inc nysebx cerity partner llc grows stock position in palantir technology inc nasdaqpltr trump to impose tariff on eu mexico starting aug trump to impose eu tariff on aug trumnp to impose eu tariff on august trump announces tariff on import from mexico eu eu say it still want u trade deal will defend interest tucker carlson reveals who he think funded jeffrey epstein crime focused wealth management inc increase stock position in merck co inc nysemrk roger wittlin investment advisory llc acquires share of vanguard sp etf nysearcavoo family firm inc ha million stock holding in ishares russell etf nysearcaiwm schwab u smallcap etf nysearcascha share sold by family firm inc roger wittlin investment advisory llc purchase share of vanguard sp etf nysearcavoo quest wealth builder inc ha stock holding in parkerhannifin corporation nyseph share in vanguard high dividend yield etf nysearcavym acquired by stillwater wealth management group ishares russell etf nysearcaiwm share sold by family firm inc well fargo company nysewfc share sold by family firm inc bank of america corporation nysebac share acquired by fortem financial group llc fortem financial group llc boost stock position in att inc nyset unitedhealth down is the dividend still safe netflix inc nasdaqnflx share acquired by martin capital advisor llp vanguard ftse developed market etf nysearcavea share purchased by bridge generation wealth management llc riversedge advisor llc grows holding in vanguard ftse emerging market etf nysearcavwo american financial advisor llc reduces stock holding in ge vernova inc nysegev crowdstrike nasdaqcrwd share acquired by american financial advisor llc riversedge advisor llc purchase share of alphabet inc nasdaqgoog vanguard value etf nysearcavtv share purchased by riversedge advisor llc vanguard value etf nysearcavtv share purchased by riversedge advisor llc crowdstrike nasdaqcrwd share bought by american financial advisor llc tesla inc nasdaqtsla share bought by riversedge advisor llc riversedge advisor llc ha holding in salesforce inc nysecrm american financial advisor llc ha million position in ishares core sp etf nysearcaivv vanguard ftse developed market etf nysearcavea position decreased by riversedge advisor llc grant grossmendelsohn llc ha holding in vanguard ftse developed market etf nysearcavea dogecoins doge holder are shifting to ruvi ai ruvi passed audit and early entry bonus make it the smarter bet auour investment llc ha million stake in ishares core msci eafe etf batsiefa fort sheridan advisor llc raise stock holding in abbott laboratory nyseabt beirne wealth consulting service llc increase stock position in ishares core msci eafe etf batsiefa b t capital management dba alpha capital management buy share of schwab u largecap growth etf nysearcaschg b t capital management dba alpha capital management purchase share of schwab u largecap growth etf nysearcaschg quest wealth builder inc cut stock position in walmart inc nysewmt ifc advisor llc reduces position in vanguard midcap etf nysearcavo spdr gold share nysearcagld share purchased by acorn wealth advisor llc ballentine partner llc increase position in chevron corporation nysecvx acorn wealth advisor llc sell share of ishares core sp smallcap etf nysearcaijr acorn wealth advisor llc ha stock position in vanguard midcap etf nysearcavo acorn wealth advisor llc reduces stock position in ishares core sp smallcap etf nysearcaijr ballentine partner llc acquires share of walmart inc nysewmt history say these stock could be big winner in the second half history say these stock could be big winner in the second half alp advisor inc ha million stock position in kkr co inc nysekkr eli lilly and company nyselly share sold by wealthtrust asset management llc eli lilly and company nyselly is harmony asset management llcs th largest position the home depot inc nysehd share purchased by lane associate llc fulcrum equity management lower stock holding in eli lilly and company nyselly fulcrum equity management sell share of eli lilly and company nyselly servicenow inc nysenow share acquired by steelpeak wealth llc trump target mexico eu with tariff hartford bakery inc voluntarily recall hundred of loaf of artisanal bread sold in state cbs news reader view we can all reduce greenhouse gas shes great trump back bondi want top official to end conflict over epstein ishares core sp smallcap etf nysearcaijr share sold by forum private client group llc chevron corporation nysecvx share acquired by b t capital management dba alpha capital management forum private client group llc ha million position in vanguard midcap etf nysearcavo b t capital management dba alpha capital management increase stake in honeywell international inc nasdaqhon beirne wealth consulting service llc acquires share of vanguard smallcap etf nysearcavb ifc advisor llc boost holding in kkr co inc nysekkr ballentine partner llc grows holding in eli lilly and company nyselly young democrat have called for a rebrand theyre vying to replace the party old guard temperance in cabinetry climate change helped fuel heavy rain that led to devastating texas flood former pentagon insider could trump big beautiful bill finally unlock america longforgotten resource archaeolgists find largestever ceremony hall weapon hoard the democratic party is missing an opportunity to engage christian voter northwest capital management inc purchase share of ishares core sp midcap etf nysearcaijh rational advisor inc take position in mcdonalds corporation nysemcd superman smash box office expectation soaring towards million opening pam bondi fire doj staffer who worked on trump case amid chaos at agency nikulski financial inc acquires share of lowes company inc nyselow parkerhannifin corporation nyseph share sold by quest wealth builder inc family firm inc lower stock holding in schwab u smallcap etf nysearcascha family firm inc reduces stock holding in well fargo company nysewfc stillwater wealth management group invests in vanguard high dividend yield etf nysearcavym extrump lawyer dershowitz claim knowledge of epstein client list i know the name but im bound by confidentiality grant grossmendelsohn llc purchase share of vanguard ftse developed market etf nysearcavea riversedge advisor llc cut stake in vanguard ftse developed market etf nysearcavea piper sandler issue positive forecast for netflix nasdaqnflx stock price riversedge advisor llc ha holding in salesforce inc nysecrm american financial advisor llc ha million stake in ishares core sp etf nysearcaivv riversedge advisor llc increase stake in ishares core sp etf nysearcaivv start exploring cloud mining for free from the new winnermining app and get visible daily reward forum private client group llc trim position in vanguard growth etf nysearcavug fort sheridan advisor llc buy share of vanguard growth etf nysearcavug the big beautiful bill and mlp qualifying income acorn wealth advisor llc lower holding in chevron corporation nysecvx ballentine partner llc buy share of walmart inc nysewmt ballentine partner llc sell share of ishares core sp smallcap etf nysearcaijr lane associate llc sell share of eli lilly and company nyselly harmony asset management llc ha million holding in the home depot inc nysehd steelpeak wealth llc ha million stake in the progressive corporation nysepgr servicenow inc nysenow share acquired by steelpeak wealth llc trump threatens rosie odonnells citizenship she is a threat to humanity annual new london to new brighton antique car run to take place aug coyle financial counsel llc invests in qualcomm incorporated nasdaqqcom broadcom inc nasdaqavgo share sold by skyoak wealth llc forum private client group llc take position in elevance health inc nyseelv a major red flag for republican a trump policy threatens their future fbi director kash patel responds to controversy surrounding epstein file stillwater wealth management group grows position in amgen inc nasdaqamgn riversedge advisor llc grows stake in tesla inc nasdaqtsla fort sheridan advisor llc ha position in kla corporation nasdaqklac kathmere capital management llc grows holding in vanguard value etf nysearcavtv nycs broken election system need far more than these bandaid fix ballentine partner llc ha million position in abbott laboratory nyseabt abbott laboratory nyseabt share acquired by ifc advisor llc trump post support for embattled attorney general pam bondi ma private wealth take position in bristol myers squibb company nysebmy parkerhannifin corporation nyseph share sold by lbp am sa harmony asset management llc reduces stock position in chevron corporation nysecvx bonus editorial cartoon for july federal employee bracing after supreme court greenlights widespread layoff federal employee bracing after supreme court greenlights widespread layoff federal employee bracing after supreme court greenlights widespread layoff lawmaker visit alligator alcatraz but some wonder how much theyll get to see man convicted of meredith kerchers murder facing trial for sexual assault federal employee bracing after supreme court greenlights widespread layoff federal employee bracing after supreme court greenlights widespread layoff federal employee bracing after supreme court greenlights widespread layoff focused wealth management inc ha million stake in walmart inc nysewmt berbice capital management llc grows position in kkr co inc nysekkr coyle financial counsel llc raise holding in invesco qqq nasdaqqqq meet china man in lima who jetted over to u to collect train donated by biden admin amazon prime day delivers record sale and saving in expanded fourday shopping event how new tax legislation impact clean energy tax credit the dalai lama is planning his succession a the ultimate protest against china the u army m vulcan air defense system wa a beast in the vietnam war the us john f kennedy fordclass carrier may miss it delivery date comcast corporation nasdaqcmcsa share sold by sage rhino capital llc kesler norman wride llc sell share of comcast corporation nasdaqcmcsa exchange capital management inc sell share of servicenow inc nysenow fukoku mutual life insurance co sell share of duke energy corporation nyseduk cerity partner llc buy share of asml holding nv nasdaqasml mjp associate inc adv take position in elevance health inc nyseelv fidelis capital partner llc boost stock position in elevance health inc nyseelv reader view u must invest in our independence candidate view localgovernment focus would benefit school board stillwater wealth management group reduces position in unitedhealth group incorporated nyseunh martin capital advisor llp sell share of oracle corporation nyseorcl park square financial group llc decrease stock position in ishares core sp midcap etf nysearcaijh fortem financial group llc purchase share of blackstone inc nysebx pya waltman capital llc ha million stake in mcdonalds corporation nysemcd massachusetts police officer shot by colleague victim of campaign to criminalize her lawyer horrified by alligator alcatraz letter coyle financial counsel llc ha million stake in ishares core sp etf nysearcaivv vanguard high dividend yield etf nysearcavym stock holding decreased by auour investment llc ifc advisor llc increase position in ishares russell etf nysearcaiwm forum private client group llc purchase new stake in cummins inc nysecmi fortem financial group llc grows holding in tesla inc nasdaqtsla vanguard ftse developed market etf nysearcavea share purchased by beirne wealth consulting service llc schear investment adviser llc buy share of tmobile u inc nasdaqtmus jrmc recognized for infection control rate wall street pro drop bold price target on circle stock bitcoin hit new alltime high above k a trader eye week uptrend cointelegraph cardinal strategic wealth guidance cut position in alphabet inc nasdaqgoog bradley co private wealth management llc reduces position in costco wholesale corporation nasdaqcost pointe capital management llc grows holding in the walt disney company nysedis westmount partner llc sell share of amgen inc nasdaqamgn westmount partner llc sell share of starbucks corporation nasdaqsbux westmount partner llc trim holding in lockheed martin corporation nyselmt q asset management buy share of williams company inc the nysewmb westmount partner llc trim holding in lockheed martin corporation nyselmt westmount partner llc trim stock position in amgen inc nasdaqamgn zullo investment group inc lower stock position in alphabet inc nasdaqgoog trunorth capital management llc acquires share of vanguard sp etf nysearcavoo pointe capital management llc boost holding in linde plc nasdaqlin ishares core u aggregate bond etf nysearcaagg share acquired by pointe capital management llc nextera energy inc nysenee share sold by pointe capital management llc bristol myers squibb company nysebmy stock holding lifted by prudent man advisor llc mqs management llc buy new position in nextera energy inc nysenee prudent man advisor llc acquires new position in blackrock nyseblk zullo investment group inc buy share of eli lilly and company nyselly zullo investment group inc acquires share of eli lilly and company nyselly zullo investment group inc cut stake in m company nysemmm prudent man advisor llc make new million investment in blackrock nyseblk mqs management llc take position in nextera energy inc nysenee ai financial service llc boost holding in eli lilly and company nyselly u tomato price could jump a soon a monday xrp break out near gain yet blockdags coin unlock chance at steal market focus top altcoins still lag while bitcoin stay strong promising outdoor stock to add to your watchlist july th kathmere capital management llc sell share of kimberlyclark co nysekmb citigroup inc nysec share purchased by ballentine partner llc cigna group nyseci share bought by ballentine partner llc ballentine partner llc purchase share of the sherwinwilliams company nyseshw arizona state retirement system purchase share of kimberlyclark co nysekmb bankplus trust department grows holding in ishares core sp smallcap etf nysearcaijr berkeley inc ha million holding in schwab u largecap etf nysearcaschx arizona state retirement system increase stake in kimberlyclark co nysekmb fdx advisor inc invests in medtronic plc nysemdt how trump latest tariff threat risk deeper damage to europe economy fort sheridan advisor llc increase stock position in cocacola company the nyseko fortem financial group llc sell share of conocophillips nysecop blackstone inc nysebx share bought by louisiana state employee retirement system eaton corporation plc nyseetn share sold by stephen inc ar taiwan semiconductor manufacturing company ltd nysetsm share sold by fulton breakefield broenniman llc why broadcoms avgo ai momentum ha goldman sachs backing the stock on gps nvidia ceo on the overwhelmingly positive effect of ai isthmus partner llc sell share of thermo fisher scientific inc nysetmo whitener ca</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>b dba alpha new investment taiwan semiconductor manufacturing company ltd nysetsm vanguard midcap nysearcavo beirne wealth consulting service llcs largest vanguard smallcap nysearcavb share b dba alpha walmart nysewmt increased fort sheridan advisor kathmere buy share vanguard smallcap nysearcavb kathmere purchase share walmart nysewmt ishares core sp smallcap nysearcaijr share forum private client kathmere purchase share vanguard smallcap nysearcavb b dba alpha boost honeywell international nasdaqhon fort sheridan advisor boost stake walmart nysewmt ifc advisor sell share depot nysehd ifc advisor million pepsico nasdaqpep quest wealth builder sell share eli lilly company nyselly caterpillar nysecat share ifc advisor ballentine partner lower invesco qqq nasdaqqqq quest wealth builder sell share pepsico nasdaqpep ballentine partner sell share invesco qqq nasdaqqqq caterpillar nysecat share ifc advisor eureka business weather economic uncertainty business pm business pm share metal company skyrocketed half share metal company skyrocketed half circle internet stock millionaire maker another large grocery chain follows kroger closing store circle internet stock millionaire maker another large grocery chain follows kroger closing store fulcrum equity stake broadcom nasdaqavgo nvidia partner navitas semiconductor surged half nvidia partner navitas semiconductor surged half bitcoin matures volatility dropsso expect slower climb expert decrypt crypto gainer blockdag solana pepe render leading growth utility ai notetakers become black box business low altitude market worth trillion according morgan stanley cathie wood stock pick dominate opportunity hint archer aviation low altitude market worth trillion according morgan stanley cathie wood stock pick dominate opportunity hint archer aviation iron ore price surge amid china industrial crackdown northwest buy share ishares core sp midcap nysearcaijh rational advisor invests million mcdonalds corporation nysemcd superman smash box office expectation soaring towards million opening pam bondi fire doj staffer worked trump amid chaos agency nikulski financial buy share lowes company nyselow mjp associate adv blackstone nysebx cerity partner grows stock palantir technology nasdaqpltr trump impose tariff eu mexico starting aug trump impose eu tariff aug trumnp impose eu tariff august trump announces tariff import mexico eu eu trade deal defend interest tucker carlson reveals funded jeffrey epstein crime focused wealth increase stock merck co nysemrk roger wittlin investment advisory acquires share vanguard sp nysearcavoo family firm million stock ishares russell nysearcaiwm schwab smallcap nysearcascha share family firm roger wittlin investment advisory purchase share vanguard sp nysearcavoo quest wealth builder stock parkerhannifin corporation nyseph share vanguard high dividend yield nysearcavym acquired stillwater wealth ishares russell nysearcaiwm share family firm fargo company nysewfc share family firm bank america corporation nysebac share acquired fortem financial fortem financial boost stock att nyset unitedhealth dividend safe netflix nasdaqnflx share acquired martin advisor llp vanguard ftse developed market nysearcavea share purchased bridge generation wealth riversedge advisor grows vanguard ftse emerging market nysearcavwo american financial advisor reduces stock ge vernova nysegev crowdstrike nasdaqcrwd share acquired american financial advisor riversedge advisor purchase share alphabet nasdaqgoog vanguard value nysearcavtv share purchased riversedge advisor vanguard value nysearcavtv share purchased riversedge advisor crowdstrike nasdaqcrwd share bought american financial advisor tesla nasdaqtsla share bought riversedge advisor riversedge advisor salesforce nysecrm american financial advisor million ishares core sp nysearcaivv vanguard ftse developed market nysearcavea decreased riversedge advisor grant grossmendelsohn vanguard ftse developed market nysearcavea dogecoins doge holder shifting ruvi ai ruvi passed audit early entry bonus smarter bet auour investment million stake ishares core msci eafe batsiefa fort sheridan advisor raise stock abbott laboratory nyseabt beirne wealth consulting service increase stock ishares core msci eafe batsiefa b dba alpha buy share schwab largecap growth nysearcaschg b dba alpha purchase share schwab largecap growth nysearcaschg quest wealth builder cut stock walmart nysewmt ifc advisor reduces vanguard midcap nysearcavo spdr gold share nysearcagld share purchased acorn wealth advisor ballentine partner increase chevron corporation nysecvx acorn wealth advisor sell share ishares core sp smallcap nysearcaijr acorn wealth advisor stock vanguard midcap nysearcavo acorn wealth advisor reduces stock ishares core sp smallcap nysearcaijr ballentine partner acquires share walmart nysewmt history stock winner half history stock winner half alp advisor million stock kkr co nysekkr eli lilly company nyselly share wealthtrust asset eli lilly company nyselly harmony asset llcs largest depot nysehd share purchased lane associate fulcrum equity lower stock eli lilly company nyselly fulcrum equity sell share eli lilly company nyselly servicenow nysenow share acquired steelpeak wealth trump target mexico eu tariff hartford bakery voluntarily recall hundred loaf artisanal bread cbs reader view reduce greenhouse gas shes great trump bondi end conflict epstein ishares core sp smallcap nysearcaijr share forum private client chevron corporation nysecvx share acquired b dba alpha forum private client million vanguard midcap nysearcavo b dba alpha increase stake honeywell international nasdaqhon beirne wealth consulting service acquires share vanguard smallcap nysearcavb ifc advisor boost kkr co nysekkr ballentine partner grows eli lilly company nyselly young democrat rebrand theyre vying replace party old guard temperance cabinetry climate change helped fuel heavy rain led devastating texas flood pentagon insider trump bill finally unlock america longforgotten resource archaeolgists find largestever ceremony hall weapon hoard democratic party missing opportunity engage christian voter northwest purchase share ishares core sp midcap nysearcaijh rational advisor take mcdonalds corporation nysemcd superman smash box office expectation soaring towards million opening pam bondi fire doj staffer worked trump amid chaos agency nikulski financial acquires share lowes company nyselow parkerhannifin corporation nyseph share quest wealth builder family firm lower stock schwab smallcap nysearcascha family firm reduces stock fargo company nysewfc stillwater wealth invests vanguard high dividend yield nysearcavym extrump lawyer dershowitz claim knowledge epstein client list name im bound confidentiality grant grossmendelsohn purchase share vanguard ftse developed market nysearcavea riversedge advisor cut stake vanguard ftse developed market nysearcavea piper sandler issue positive forecast netflix nasdaqnflx stock price riversedge advisor salesforce nysecrm american financial advisor million stake ishares core sp nysearcaivv riversedge advisor increase stake ishares core sp nysearcaivv start exploring cloud mining free new winnermining app visible reward forum private client trim vanguard growth nysearcavug fort sheridan advisor buy share vanguard growth nysearcavug bill mlp qualifying income acorn wealth advisor lower chevron corporation nysecvx ballentine partner buy share walmart nysewmt ballentine partner sell share ishares core sp smallcap nysearcaijr lane associate sell share eli lilly company nyselly harmony asset million depot nysehd steelpeak wealth million stake progressive corporation nysepgr servicenow nysenow share acquired steelpeak wealth trump threatens rosie odonnells citizenship threat humanity annual new london new brighton antique car run take place aug coyle financial counsel invests qualcomm incorporated nasdaqqcom broadcom nasdaqavgo share skyoak wealth forum private client take elevance health nyseelv major red flag republican trump policy threatens future fbi director kash patel responds controversy surrounding epstein file stillwater wealth grows amgen nasdaqamgn riversedge advisor grows stake tesla nasdaqtsla fort sheridan advisor kla corporation nasdaqklac kathmere grows vanguard value nysearcavtv nycs broken election system far bandaid fix ballentine partner million abbott laboratory nyseabt abbott laboratory nyseabt share acquired ifc advisor trump post support embattled attorney general pam bondi private wealth take bristol myers squibb company nysebmy parkerhannifin corporation nyseph share lbp sa harmony asset reduces stock chevron corporation nysecvx bonus editorial cartoon federal employee bracing supreme greenlights widespread layoff federal employee bracing supreme greenlights widespread layoff federal employee bracing supreme greenlights widespread layoff lawmaker visit alligator alcatraz wonder theyll man convicted meredith kerchers murder facing trial sexual assault federal employee bracing supreme greenlights widespread layoff federal employee bracing supreme greenlights widespread layoff federal employee bracing supreme greenlights widespread layoff focused wealth million stake walmart nysewmt berbice grows kkr co nysekkr coyle financial counsel raise invesco qqq nasdaqqqq meet china man lima jetted collect train donated biden admin amazon prime delivers record sale saving expanded fourday shopping event new tax legislation impact clean energy tax credit dalai lama planning succession ultimate protest china army vulcan air defense system beast vietnam war u john f kennedy fordclass carrier miss delivery date comcast corporation nasdaqcmcsa share sage rhino kesler norman wride sell share comcast corporation nasdaqcmcsa exchange sell share servicenow nysenow fukoku mutual life insurance co sell share duke energy corporation nyseduk cerity partner buy share asml nv nasdaqasml mjp associate adv take elevance health nyseelv fidelis partner boost stock elevance health nyseelv reader view must invest independence candidate view localgovernment focus benefit school board stillwater wealth reduces unitedhealth incorporated nyseunh martin advisor llp sell share oracle corporation nyseorcl park square financial decrease stock ishares core sp midcap nysearcaijh fortem financial purchase share blackstone nysebx pya waltman million stake mcdonalds corporation nysemcd massachusetts police officer shot colleague victim campaign criminalize lawyer horrified alligator alcatraz coyle financial counsel million stake ishares core sp nysearcaivv vanguard high dividend yield nysearcavym stock decreased auour investment ifc advisor increase ishares russell nysearcaiwm forum private client purchase new stake cummins nysecmi fortem financial grows tesla nasdaqtsla vanguard ftse developed market nysearcavea share purchased beirne wealth consulting service schear investment adviser buy share tmobile nasdaqtmus jrmc recognized infection control rate wall street pro drop bold price target circle stock bitcoin hit new alltime high k trader eye uptrend cointelegraph cardinal strategic wealth guidance cut alphabet nasdaqgoog bradley co private wealth reduces costco wholesale corporation nasdaqcost pointe grows walt disney company nysedis westmount partner sell share amgen nasdaqamgn westmount partner sell share starbucks corporation nasdaqsbux westmount partner trim lockheed martin corporation nyselmt q asset buy share williams company nysewmb westmount partner trim lockheed martin corporation nyselmt westmount partner trim stock amgen nasdaqamgn zullo investment lower stock alphabet nasdaqgoog trunorth acquires share vanguard sp nysearcavoo pointe boost linde plc nasdaqlin ishares core aggregate bond nysearcaagg share acquired pointe nextera energy nysenee share pointe bristol myers squibb company nysebmy stock lifted prudent man advisor mqs buy new nextera energy nysenee prudent man advisor acquires new blackrock nyseblk zullo investment buy share eli lilly company nyselly zullo investment acquires share eli lilly company nyselly zullo investment cut stake company nysemmm prudent man advisor new million investment blackrock nyseblk mqs take nextera energy nysenee ai financial service boost eli lilly company nyselly tomato price jump soon monday xrp break near gain yet blockdags coin unlock chance steal market focus altcoins lag bitcoin stay strong promising outdoor stock add watchlist kathmere sell share kimberlyclark co nysekmb citigroup nysec share purchased ballentine partner cigna nyseci share bought ballentine partner ballentine partner purchase share sherwinwilliams company nyseshw arizona retirement system purchase share kimberlyclark co nysekmb bankplus trust department grows ishares core sp smallcap nysearcaijr berkeley million schwab largecap nysearcaschx arizona retirement system increase stake kimberlyclark co nysekmb fdx advisor invests medtronic plc nysemdt trump latest tariff threat risk deeper damage europe economy fort sheridan advisor increase stock cocacola company nyseko fortem financial sell share conocophillips nysecop blackstone nysebx share bought louisiana employee retirement system eaton corporation plc nyseetn share stephen ar taiwan semiconductor manufacturing company ltd nysetsm share fulton breakefield broenniman broadcoms avgo ai momentum goldman sachs backing stock gps nvidia ceo overwhelmingly positive effect ai isthmus partner sell share thermo fisher scientific nysetmo whitener million stake verizon communication nysevz share thermo fisher scientific nysetmo purchased eos lp lowes company nyselow share acquired zullo investment eos lp invests million thermo fisher scientific nysetmo whitener raise stock lowes company nyselow gps nvidia ceo ai lead job loss rosen topranked firm encourages rocket pharmaceutical investor secure counsel important deadline security class action rckt dem strategist trump epstein blowback wound caused reyes financial architecture boost advanced micro device nasdaqamd lri investment danaher corporation nysedhr gps nvidia ceo uschina ai race iconic mall retailer face chapter bankruptcy closure nvidias huang china military unlikely ai chip bloomberg greatmark investment partner rtx corporation nysertx mark wealth grows honeywell international nasdaqhon pfizer nysepfe share acquired secured retirement advisor cwm purchase share jpmorgan ultrashort income nysearcajpst tfr purchase share rtx corporation nysertx cwm million jpmorgan ultrashort income nysearcajpst share texas instrument incorporated nasdaqtxn purchased secured retirement advisor trunorth purchase share fiserv nysefi iron horse wealth purchase share vanguard ftse developed market nysearcavea trunorth stock att nyset fulton breakefield broenniman million stock vanguard ftse developed market nysearcavea abbott laboratory nyseabt share purchased dock street asset workday wday got downgradedheres analyst worried ai target sends stern message employee amid customer struggle target sends stern message employee amid customer struggle thestreet prism advisor trim stock ishares core msci eafe batsiefa depot nysehd reduced sentinel trust co lba philip morris international nysepm share legacy financial philip morris international nysepm share legacy financial texas congressman call accountability flood cant allow girl drown middle night greatmark investment partner grows general mill nysegis tfr purchase share jpmorgan equity premium income nysearcajepi greatmark investment partner reduces southern company nyseso tfr acquires share cisco system nasdaqcsco greatmark investment partner trim cisco system nasdaqcsco hughes financial service take southern company nyseso greatmark investment partner trim stock cisco system nasdaqcsco tfr million stock vertex pharmaceutical incorporated nasdaqvrtx hughes financial service take southern company nyseso brn impact sport betting complicated stock market underestimating president trump tariff cwm sell share gilead science nasdaqgild isthmus partner purchase share accenture plc nyseacn mark wealth buy share chipotle mexican grill nysecmg secured retirement advisor take million comcast corporation nasdaqcmcsa legacy financial lower stryker corporation nysesyk prudent man advisor million stake labcorp nyselh left brain wealth sell share ge vernova nysegev schear investment adviser lower deere company nysede westmount partner sell share walt disney company nysedis zullo investment trim stake alphabet nasdaqgoog trunorth purchase share vanguard sp nysearcavoo pet lover demand leadership change san jose animal shelter zullo investment trim stake company nysemmm tomato price jump soon monday trump issue executive order targeting unreliable clean energy option kathmere buy share citigroup nysec berkeley decrease stock schwab largecap nysearcaschx hotel stock follow gps nvidia ceo overwhelmingly positive effect ai whitener grows lowes company nyselow zullo investment grows stock lowes company nyselow gps nvidia ceo ai lead job loss dem strategist trump epstein blowback wound caused gps nvidia ceo uschina ai race lri investment stock goldman sachs nysegs secured retirement advisor purchase new texas instrument incorporated nasdaqtxn mark wealth purchase share copart nasdaqcprt tfr boost rtx corporation nysertx att nyset boosted trunorth fulton breakefield broenniman buy share vanguard ftse developed market nysearcavea blame new york democrat washington new budget crisis pepsico nasdaqpep stock cut new york common retirement fund depot nysehd share sentinel trust co lba fdx advisor trim depot nysehd digitally enslaved generation cry independence texas congressman call accountability flood cant allow girl drown middle night tfr new investment marsh mclennan company nysemmc tfr acquires share vertex pharmaceutical incorporated nasdaqvrtx greatmark investment partner decrease cv health corporation nysecvs tfr new investment southern company nyseso octa host public input meeting coastal rail trouble around erosion planned trump unprecedented visit uk september left brain wealth reduces stock unitedhealth incorporated nyseunh left brain wealth raise altria nysemo isthmus partner sell share pnc financial service nysepnc cwm million comcast corporation nasdaqcmcsa security ai governance saas violent clash erupt farright migrant spanish town caterpillar nysecat share asset dedication goalfusion wealth million stock vanguard value nysearcavtv hughes financial service take vanguard value nysearcavtv rainey randall wealth advisor invests zoetis nysezts hoag open new health center monday san clemente oxbow advisor sell share vanguard growth nysearcavug ishares tip bond nysearcatip share bought hughes financial service schear investment adviser marathon petroleum corporation nysempc handsome waterbomb seoul star vote maga faithful weigh epstein file debate prisoner france escape cellmates bag homeowner driver pay scheme homeowner driver pay scheme homeowner driver pay scheme texas nw office warning coordination meteorologist flood difference caster semenyas sex eligibility battle confounded sport yearsand isnt prudent man advisor boost stock deere company nysede prudent man advisor purchase share costco wholesale corporation nasdaqcost mqs buy share lockheed martin corporation nyselmt prudent man advisor purchase share alphabet nasdaqgoog ballentine partner increase stock waste nysewm promising outdoor stock add watchlist kathmere sell share bristol myers squibb company nysebmy video game stock follow stephen ar increase walmart nysewmt schechter investment advisor million stock vanguard total international stock nasdaqvxus trump potentially fire fed powell building renovation hassett learn garden fresh produce mason investment advisory service stock procter gamble company nysepg fulton breakefield broenniman purchase share vanguard dividend appreciation nysearcavig fulton breakefield broenniman buy share ishares core sp smallcap nysearcaijr prudent man advisor sell share conocophillips nysecop sfs zero fatality goal crash reality sfs zero fatality goal crash reality sfs zero fatality goal crash reality wilkinson global asset buy share parkerhannifin corporation nyseph reyes financial architecture purchase share vanguard shortterm bond nysearcabsv lri investment purchase share ishares technology nysearcaiyw lri investment blackstone nysebx gopled discussing plan build prison alligator alcatraz noem lri investment stake danaher corporation nysedhr mark wealth acquires share eaton corporation plc nyseetn dock street asset acquires share abbott laboratory nyseabt greatmark investment partner million stake paychex nasdaqpayx oxbow advisor boost jpmorgan ultrashort income nysearcajpst trunorth purchase share rtx corporation nysertx mutual america decrease stock att nyset edge asset lp boost spdr portfolio emerging market nysearcaspem sen padilla getting aggressive cruel extreme child killed albion hitandrun man charged legacy financial cut stake vanguard shortterm inflationprotected security nasdaqvtip ken morris careful ago legacy financial reduces stake dimensional core equity nysearcadfac left brain wealth cut stock applovin corporation nasdaqapp litigate order homan responds judge restricting raid la reyes financial architecture purchase share ww grainger nysegww lri investment sell share corning incorporated nyseglw kerntke otto mcglone wealth trim vanguard midcap nysearcavo trump assassination attempt butler change secret service axecap investment sell share apple nasdaqaapl fifth third bancorp sell share apple nasdaqaapl sagace wealth sell share microsoft corporation nasdaqmsft microsoft corporation nasdaqmsft stake lowered tran lp define financial buy share microsoft corporation nasdaqmsft sapient sell share microsoft corporation nasdaqmsft teacher retirement system texas sell share safety insurance nasdaqsaft teacher retirement system texas sell share organon co nyseogn teacher retirement system texas cut stock artisan partner asset nyseapam teacher retirement system texas buy new share smith corporation nyseaos rev nyserevg trimmed teacher retirement system texas share lamb weston nyselw acquired teacher retirement system texas bridgebio pharma nasdaqbbio share teacher retirement system texas west advisor trim apple nasdaqaapl teacher retirement system texas take million community health system nysecyh teacher retirement system texas million portland general electric company nysepor teacher retirement system texas buy share ugi corporation nyseugi teacher retirement system texas million stake ziff davis nasdaqzd teacher retirement system texas purchase new stake campbell company nasdaqcpb asian heat squeeze lng flow europe borgwarner nysebwa share cambridge investment research advisor teacher retirement system texas million stake madrigal pharmaceutical nasdaqmdgl exclusive interview future belongs nocodes deep ai integration abhinav girdhar ceo founder appy pie european trade minister meet forge strategy trump surprise tariff european trade minister meet forge strategy trump surprise tariff european trade minister meet forge strategy trump surprise tariff relx nyserelx rating lowered wall street zen southside bancshares nysesbsi rating lowered sell wall street zen wall street zen downgrade vista energy nysevist sell bank america cut primo brand nyseprmb price target silgan nyseslgn price target raised stifel financial nysesf price target raised ubiquitis ui buy rating reiterated bw financial wall street zen upgrade rafael nyserfl charles schwab nyseschw price target raised sea nysese stock rating lowered wall street zen sealed air nysesee price target raised wall street zen upgrade te connectivity nysetel buy telus digital nysetixt stock rating upgraded wall street zen sealed air nysesee price target raised telephone data system nysetds stock rating upgraded wall street zen synovus financial nysesnv price target raised truist financial cut sonoco product nyseson price target att nyset price target raised wec energy nysewec rating lowered sell wall street zen exxon mobil nysexom price target raised scotiabank truist financial raise webster financial nysewbs price target ai stock buy place report surge company relocation driving demand flexible office space dubai riyadh rockfire resource lonrock stock price buy rockfire resource lonrock trading buy new zealand energy cvenz trading happened argentina lithium energy cvelit share sell silver spruce resource cvesse share happened silver spruce resource cvesse trading sell new zealand energy cvenz trading sell argentina lithium energy cvelit stock price geomega resource cvegma stock price whats next geomega resource cvegma trading higher buy geomega reso</t>
+          <t>run nearly centuryold michigan clock company due tariff factor sage rhino sell shell plc unsponsored adr nyseshel vanguard total stock market nysearcavti increased seamount financial sage rhino acquires vanguard total stock market nysearcavti kesler norman wride boost stake broadcom nasdaqavgo genus invests million ishares msci eafe nysearcaefa sage rhino buy broadcom nasdaqavgo vanguard total stock market nysearcavti clarity wealth advisor llcs rd largest seamount financial buy vanguard dividend appreciation nysearcavig michigan retirement system million stock chubb limited nysecb michigan retirement system million lam research corporation nasdaqlrcx clarity wealth advisor reduces walt disney company nysedis genus investment ishares msci eafe nysearcaefa kesler norman wride buy vanguard information technology nysearcavgt chubb limited nysecb michigan retirement system sage rhino purchase broadcom nasdaqavgo michigan retirement system decrease stake lam research corporation nasdaqlrcx seamount financial raise stock vanguard dividend appreciation nysearcavig quantum computing next stock buy bos quietly veto devastating pull rug american thousand lose cash ford recall vehicle fuel pump defect manufacturing layoff pacira oak hill bios phase angelman data france launch criminal investigation musk x algorithm manipulation politicoeu trump million crypto mystery man reuters buy dip stock investor rockwell automation pharmasuite power sinteticas swiss drug production teledyne raymarine acquires maretron asset boost marine automation cummins unveils hydrogen turbocharger european heavyduty engine dover techcon unveils precision dispensing cartridge industry carrier global enhances aipowered abound app proactive building trane technology debut dynamic closed loop geothermal system chicago school district johnson control sensormatic solution launch aipowered shopper tracking privacyfirst reid technology goldman sachs mustbuy chip stock forget honeywell explores sale division ahead planned split raytheon rtx demonstrates autonomous barracuda mine neutralization vehicle gmbacked energyx expands lithium smackover formation pantera acquisition boeing b space force contract nextgen nuclear comms satellite penguin solution launch nextgen stratus ztc endurance ultrahigh availability ai workload clarivate unveils enhanced g research innovation scorecard expanded data ai insight xerox completes b lexmark acquisition support print market globant suntory global spirit partner deploy gen ai commercial insight agent concentrix half carbon emission target detail progress sustainability report dxc technology aipowered tendia solution slash bid writing ventia genpact launch aipowered suite revolutionize account payable process kyndryl launch aipowered service accelerate mainframe migration aws saic awarded air force contract rapid warfighting prototype development shopper buy bjs membership deal cheaper rival sam club bank set post trading gain trump tariff turmoil cognizant pledge white house ai education initiative aim train education department resume interest accrual million student loan borrower rtx corporation nysertx stake reduced cfolife fonville wealth cut stake costco wholesale corporation nasdaqcost kesler norman wride acquires invesco qqq nasdaqqqq bernardo wealth planning cut stock alphabet nasdaqgoog nextera energy nysenee lifted cerity partner leavell investment reduces ishares core aggregate bond nysearcaagg leavell investment raise stake uber technology nyseuber fonville wealth sell southern company nyseso cerity partner boost invesco qqq nasdaqqqq insight partner raise stock freeportmcmoran nysefcx kesler norman wride sell stryker corporation nysesyk costco wholesale corporation nasdaqcost alp advisor fonville wealth increase stake vanguard growth nysearcavug insight partner acquires freeportmcmoran nysefcx kesler norman wride increase stock linde plc nasdaqlin phillips financial sell schwab largecap nysearcaschx financial gravity asset purchase costco wholesale corporation nasdaqcost kesler norman wride sell stryker corporation nysesyk parr mcknight wealth trim spdr gold nysearcagld cerity partner trim stock adobe nasdaqadbe uk business confidence plummet threeyear low icaew walmart recall water bottle consumer suffer vision loss ejecting lid walmart recall water bottle consumer suffer vision loss ejecting lid walmart recall water bottle consumer suffer vision loss ejecting lid walmart recall water bottle consumer suffer vision loss ejecting lid wall street giant issue stark message sp walmart recall water bottle consumer suffer vision loss ejecting lid nikki bella discusses wwe evolution ge vernovas recent unusual option activity whale citigroup analyzing broadcom comparison competitor semiconductor semiconductor equipment industry chief executive officer integral ad science holdi k stock italianstyle villa south minneapolis linden hill listed sell alert aaron yeon ho lee cash acushnet stock sell alert kevin chang keun yoon cash acushnet stock allworth financial lp raise pepsico nasdaqpep michigan retirement system million philip morris international nysepm michigan retirement system sell intuit nasdaqintu cisco system nasdaqcsco michigan retirement system michigan retirement system sell pepsico nasdaqpep leavell investment sell merck co nysemrk mjp associate adv increase stake invesco sp equal weight nysearcarsp michigan retirement system cut stake merck co nysemrk michigan retirement system reduces ishares core sp midcap nysearcaijh merck co nysemrk stake reduced leavell investment insider decision gene soo yoon yoon offloads worth acushnet stock lacroix announces partnership dallas wing wnba team royal caribbean take delivery world largest cruise ship insider decision tod e carpenter exercise option donaldson evaluating apple peer technology hardware storage peripheral industry clarity wealth advisor sell walt disney company nysedis michigan retirement system reduces stock cme nasdaqcme michigan retirement system million stock palo alto network nasdaqpanw sage rhino cut vanguard ftse allworld exus nysearcaveu cfc planning co million stake walt disney company nysedis parr mcknight wealth sell spdr gold nysearcagld kesler norman wride million fortinet nasdaqftnt round rock advisor purchase verizon communication nysevz financial gravity asset buy costco wholesale corporation nasdaqcost phillips financial sell schwab largecap nysearcaschx round rock advisor stock salesforce nysecrm kesler norman wride buy linde plc nasdaqlin omb director powell fed hq renovation spending perfektblue bluetooth vulnerability expose million vehicle remote code execution trump bondi bongino bongino wont fbi bondi job source selling weapon nato ally give ukraine trump ishares core sp midcap nysearcaijh michigan retirement system kla corporation nasdaqklac bought mjp associate adv michigan retirement system million stock merck co nysemrk veteran political reporter reveals medium missed trump appeal american barrie antisemitism plan used silence dissent podcast special envoy plan latest push weaponise antisemitism relentless campaign pay louise adler albanese must careful tackling antisemitism doesnt curb free speech tom mcilroy virginia rep john mcguire bought k worth meta platform stock congressional trading report rep susie lee k full house resort stock sue medical privacy sue medical privacy sue medical privacy california rep gilbert ray cisneros k worth springworks therapeutic ordinary stock laurel libby stood strong face tyranny beth claybourn interior trump front war drug bank air force million double production aim missile themed playground equipment officially open lake charles park steve mann aftermath magees san bruno england professional planning reduces international business machine corporation nyseibm pfizer nysepfe england professional planning diversify wealth buy cocacola company nyseko bipartisan legislation aim legalize adultuse cannabis pennsylvania cerity partner boost mcdonalds corporation nysemcd mjp associate adv raise stock mcdonalds corporation nysemcd mcdonalds corporation nysemcd purchased freedom solution moloney security asset buy vanguard total bond market nasdaqbnd benny blanco music shazam tune elv deadline rosen leading trial attorney encourages elevance health investor epstein conspiracy isnt teacher union reveals color fox opinion stratos wealth advisor trim stock goldman sachs nysegs freedom solution decrease stock amgen nasdaqamgn lbp sa sell visa nysev mindful jon heydenreich martini megaburger selling weapon nato ally give ukraine trump selling weapon nato ally give ukraine trump selling weapon nato ally give ukraine trump selling weapon nato ally give ukraine trump selling weapon nato ally give ukraine trump greater midwest financial purchase vanguard sp nysearcavoo barry investment advisor sell vanguard ftse emerging market nysearcavwo department firing employee trump administration plan rubio wang stress cooperation malaysia uschina tension simmer diversify wealth buy ishares treasury bond batsgovt cromwell decrease stake micron technology nasdaqmu vanguard value nysearcavtv ade chevron corporation nysecvx purchased diversify wealth cromwell raise stake monolithic power system nasdaqmpwr church street road closure extended brattleboro selling weapon nato ally give ukraine trump noqualifyjpg bill clarify st louis sheriff duty stall committee strategist flag unusual trump admin loyalty test cnn fidelis partner million stake thermo fisher scientific nysetmo pkk fighter pile weapon arm amnesty northern iraq brazil vow retaliatory tariff trump follows import tax pac form mamdani nyc mayoral bid business community rally defeat history program highlight map stone wall dummerson financial gravity asset buy ishares tip bond nysearcatip phillips financial increase vanguard ftse developed market nysearcavea trump plan hike tariff canadian good trump plan tour texas flood damage scope disaster test pledge shutter fema trump plan hike tariff canadian good ishares msci emerging market nysearcaeem ramsay stattman vela price burford brother raise sherwinwilliams company nyseshw spdr dow jones industrial average trust nysearcadia lifted christopher j hasenberg genus invests million sherwinwilliams company nyseshw department axe employee michigan retirement system boost stock prologis nysepld advanced micro device nasdaqamd purchased clarity wealth advisor seamount financial sell vanguard total world stock nysearcavt vaneck gold miner nysearcagdx acquired sage rhino vestia personal wealth advisor increase dimensional marketwide value nysearcadfuv milwaukee remove fonzie statue amid reckoning greaser past noqualifyingjpg exxon mobil corporation nysexom pineridge advisor cfolife buy ge aerospace nysege stonebrook private buy vanguard total stock market nysearcavti allworth financial lp grows united parcel service nyseups cerity partner sell adobe nasdaqadbe adobe nasdaqadbe lowered xponance honeywell international nasdaqhon bought kesler norman wride amphenol corporation nyseaph boosted cerity partner b dba alpha investment taiwan semiconductor manufacturing company ltd nysetsm vanguard midcap nysearcavo beirne wealth consulting service llcs largest vanguard smallcap nysearcavb b dba alpha walmart nysewmt increased fort sheridan advisor kathmere buy vanguard smallcap nysearcavb kathmere purchase walmart nysewmt ishares core sp smallcap nysearcaijr forum private client kathmere purchase vanguard smallcap nysearcavb b dba alpha boost honeywell international nasdaqhon fort sheridan advisor boost stake walmart nysewmt ifc advisor sell depot nysehd ifc advisor million pepsico nasdaqpep quest wealth builder sell eli lilly company nyselly caterpillar nysecat ifc advisor ballentine partner lower invesco qqq nasdaqqqq quest wealth builder sell pepsico nasdaqpep ballentine partner sell invesco qqq nasdaqqqq caterpillar nysecat ifc advisor eureka business weather economic uncertainty business pm business pm metal company skyrocketed half metal company skyrocketed half circle internet stock millionaire maker another large grocery chain follows kroger closing store circle internet stock millionaire maker another large grocery chain follows kroger closing store fulcrum equity stake broadcom nasdaqavgo nvidia partner navitas semiconductor surged half nvidia partner navitas semiconductor surged half bitcoin matures volatility dropsso expect slower climb expert decrypt crypto gainer blockdag solana pepe render leading growth utility ai notetakers become black box business low altitude market worth trillion according morgan stanley cathie wood stock pick dominate opportunity hint archer aviation low altitude market worth trillion according morgan stanley cathie wood stock pick dominate opportunity hint archer aviation iron ore price surge amid china industrial crackdown northwest buy ishares core sp midcap nysearcaijh rational advisor invests million mcdonalds corporation nysemcd superman smash box office expectation soaring towards million opening pam bondi fire doj staffer worked trump amid chaos agency nikulski financial buy lowes company nyselow mjp associate adv blackstone nysebx cerity partner grows stock palantir technology nasdaqpltr trump impose tariff eu mexico starting aug trump impose eu tariff aug trumnp impose eu tariff august trump announces tariff import mexico eu eu trade deal defend interest tucker carlson reveals funded jeffrey epstein crime focused wealth increase stock merck co nysemrk roger wittlin investment advisory acquires vanguard sp nysearcavoo family firm million stock ishares russell nysearcaiwm schwab smallcap nysearcascha family firm roger wittlin investment advisory purchase vanguard sp nysearcavoo quest wealth builder stock parkerhannifin corporation nyseph vanguard high dividend yield nysearcavym acquired stillwater wealth ishares russell nysearcaiwm family firm fargo company nysewfc family firm bank america corporation nysebac acquired fortem financial fortem financial boost stock att nyset unitedhealth dividend safe netflix nasdaqnflx acquired martin advisor llp vanguard ftse developed market nysearcavea purchased bridge generation wealth riversedge advisor grows vanguard ftse emerging market nysearcavwo american financial advisor reduces stock ge vernova nysegev crowdstrike nasdaqcrwd acquired american financial advisor riversedge advisor purchase alphabet nasdaqgoog vanguard value nysearcavtv purchased riversedge advisor vanguard value nysearcavtv purchased riversedge advisor crowdstrike nasdaqcrwd bought american financial advisor tesla nasdaqtsla bought riversedge advisor riversedge advisor salesforce nysecrm american financial advisor million ishares core sp nysearcaivv vanguard ftse developed market nysearcavea decreased riversedge advisor grant grossmendelsohn vanguard ftse developed market nysearcavea dogecoins doge holder shifting ruvi ai ruvi passed audit early entry bonus smarter bet auour investment million stake ishares core msci eafe batsiefa fort sheridan advisor raise stock abbott laboratory nyseabt beirne wealth consulting service increase stock ishares core msci eafe batsiefa b dba alpha buy schwab largecap growth nysearcaschg b dba alpha purchase schwab largecap growth nysearcaschg quest wealth builder cut stock walmart nysewmt ifc advisor reduces vanguard midcap nysearcavo spdr gold nysearcagld purchased acorn wealth advisor ballentine partner increase chevron corporation nysecvx acorn wealth advisor sell ishares core sp smallcap nysearcaijr acorn wealth advisor stock vanguard midcap nysearcavo acorn wealth advisor reduces stock ishares core sp smallcap nysearcaijr ballentine partner acquires walmart nysewmt history stock winner half history stock winner half alp advisor million stock kkr co nysekkr eli lilly company nyselly wealthtrust asset eli lilly company nyselly harmony asset llcs largest depot nysehd purchased lane associate fulcrum equity lower stock eli lilly company nyselly fulcrum equity sell eli lilly company nyselly servicenow nysenow acquired steelpeak wealth trump target mexico eu tariff hartford bakery voluntarily recall hundred loaf artisanal bread cbs reader view reduce greenhouse gas shes great trump bondi end conflict epstein ishares core sp smallcap nysearcaijr forum private client chevron corporation nysecvx acquired b dba alpha forum private client million vanguard midcap nysearcavo b dba alpha increase stake honeywell international nasdaqhon beirne wealth consulting service acquires vanguard smallcap nysearcavb ifc advisor boost kkr co nysekkr ballentine partner grows eli lilly company nyselly young democrat rebrand theyre vying replace party old guard temperance cabinetry climate change helped fuel heavy rain led devastating texas flood pentagon insider trump bill finally unlock america longforgotten resource archaeolgists find largestever ceremony hall weapon hoard democratic party missing opportunity engage christian voter northwest purchase ishares core sp midcap nysearcaijh rational advisor take mcdonalds corporation nysemcd superman smash box office expectation soaring towards million opening pam bondi fire doj staffer worked trump amid chaos agency nikulski financial acquires lowes company nyselow parkerhannifin corporation nyseph quest wealth builder family firm lower stock schwab smallcap nysearcascha family firm reduces stock fargo company nysewfc stillwater wealth invests vanguard high dividend yield nysearcavym extrump lawyer dershowitz claim knowledge epstein client list name im bound confidentiality grant grossmendelsohn purchase vanguard ftse developed market nysearcavea riversedge advisor cut stake vanguard ftse developed market nysearcavea piper sandler issue positive forecast netflix nasdaqnflx stock price riversedge advisor salesforce nysecrm american financial advisor million stake ishares core sp nysearcaivv riversedge advisor increase stake ishares core sp nysearcaivv start exploring cloud mining free winnermining app visible reward forum private client trim vanguard growth nysearcavug fort sheridan advisor buy vanguard growth nysearcavug bill mlp qualifying income acorn wealth advisor lower chevron corporation nysecvx ballentine partner buy walmart nysewmt ballentine partner sell ishares core sp smallcap nysearcaijr lane associate sell eli lilly company nyselly harmony asset million depot nysehd steelpeak wealth million stake progressive corporation nysepgr servicenow nysenow acquired steelpeak wealth trump threatens rosie odonnells citizenship threat humanity annual london brighton antique car run take place aug coyle financial counsel invests qualcomm incorporated nasdaqqcom broadcom nasdaqavgo skyoak wealth forum private client take elevance health nyseelv major red flag republican trump policy threatens future fbi director kash patel responds controversy surrounding epstein file stillwater wealth grows amgen nasdaqamgn riversedge advisor grows stake tesla nasdaqtsla fort sheridan advisor kla corporation nasdaqklac kathmere grows vanguard value nysearcavtv nycs broken election system far bandaid fix ballentine partner million abbott laboratory nyseabt abbott laboratory nyseabt acquired ifc advisor trump post support embattled attorney general pam bondi private wealth take bristol myers squibb company nysebmy parkerhannifin corporation nyseph lbp sa harmony asset reduces stock chevron corporation nysecvx bonus editorial cartoon federal employee bracing supreme greenlights widespread layoff federal employee bracing supreme greenlights widespread layoff federal employee bracing supreme greenlights widespread layoff lawmaker visit alligator alcatraz wonder theyll man convicted meredith kerchers murder facing trial sexual assault federal employee bracing supreme greenlights widespread layoff federal employee bracing supreme greenlights widespread layoff federal employee bracing supreme greenlights widespread layoff focused wealth million stake walmart nysewmt berbice grows kkr co nysekkr coyle financial counsel raise invesco qqq nasdaqqqq meet china man lima jetted collect train donated biden admin amazon prime delivers record sale saving expanded fourday shopping event tax legislation impact clean energy tax credit dalai lama planning succession ultimate protest china army vulcan air defense system beast vietnam war u john f kennedy fordclass carrier miss delivery date comcast corporation nasdaqcmcsa sage rhino kesler norman wride sell comcast corporation nasdaqcmcsa exchange sell servicenow nysenow fukoku mutual life insurance co sell duke energy corporation nyseduk cerity partner buy asml nv nasdaqasml mjp associate adv take elevance health nyseelv fidelis partner boost stock elevance health nyseelv reader view must invest independence candidate view localgovernment focus benefit school board stillwater wealth reduces unitedhealth incorporated nyseunh martin advisor llp sell oracle corporation nyseorcl park square financial decrease stock ishares core sp midcap nysearcaijh fortem financial purchase blackstone nysebx pya waltman million stake mcdonalds corporation nysemcd massachusetts police officer shot colleague victim campaign criminalize lawyer horrified alligator alcatraz coyle financial counsel million stake ishares core sp nysearcaivv vanguard high dividend yield nysearcavym stock decreased auour investment ifc advisor increase ishares russell nysearcaiwm forum private client purchase stake cummins nysecmi fortem financial grows tesla nasdaqtsla vanguard ftse developed market nysearcavea purchased beirne wealth consulting service schear investment adviser buy tmobile nasdaqtmus jrmc recognized infection control rate wall street pro drop bold price target circle stock bitcoin hit alltime high k trader eye uptrend cointelegraph cardinal strategic wealth guidance cut alphabet nasdaqgoog bradley co private wealth reduces costco wholesale corporation nasdaqcost pointe grows walt disney company nysedis westmount partner sell amgen nasdaqamgn westmount partner sell starbucks corporation nasdaqsbux westmount partner trim lockheed martin corporation nyselmt q asset buy williams company nysewmb westmount partner trim lockheed martin corporation nyselmt westmount partner trim stock amgen nasdaqamgn zullo investment lower stock alphabet nasdaqgoog trunorth acquires vanguard sp nysearcavoo pointe boost linde plc nasdaqlin ishares core aggregate bond nysearcaagg acquired pointe nextera energy nysenee pointe bristol myers squibb company nysebmy stock lifted prudent man advisor mqs buy nextera energy nysenee prudent man advisor acquires blackrock nyseblk zullo investment buy eli lilly company nyselly zullo investment acquires eli lilly company nyselly zullo investment cut stake company nysemmm prudent man advisor million investment blackrock nyseblk mqs take nextera energy nysenee ai financial service boost eli lilly company nyselly tomato price jump soon monday xrp break near gain yet blockdags coin unlock chance steal market focus altcoins lag bitcoin stay strong promising outdoor stock add watchlist kathmere sell kimberlyclark co nysekmb citigroup nysec purchased ballentine partner cigna nyseci bought ballentine partner ballentine partner purchase sherwinwilliams company nyseshw arizona retirement system purchase kimberlyclark co nysekmb bankplus trust department grows ishares core sp smallcap nysearcaijr berkeley million schwab largecap nysearcaschx arizona retirement system increase stake kimberlyclark co nysekmb fdx advisor invests medtronic plc nysemdt trump latest tariff threat risk deeper damage europe economy fort sheridan advisor increase stock cocacola company nyseko fortem financial sell conocophillips nysecop blackstone nysebx bought louisiana employee retirement system eaton corporation plc nyseetn stephen ar taiwan semiconductor manufacturing company ltd nysetsm fulton breakefield broenniman broadcoms avgo ai momentum goldman sachs backing stock gps nvidia ceo overwhelmingly positive effect ai isthmus partner sell thermo fisher scientific nysetmo whitener ca</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="2" t="n">
+        <v>45853</v>
+      </c>
+      <c r="B15" t="n">
+        <v>6243.759765625</v>
+      </c>
+      <c r="C15" t="n">
+        <v>6302.0400390625</v>
+      </c>
+      <c r="D15" t="n">
+        <v>6241.68017578125</v>
+      </c>
+      <c r="E15" t="n">
+        <v>6295.2900390625</v>
+      </c>
+      <c r="F15" t="n">
+        <v>5133670000</v>
+      </c>
+      <c r="G15" t="n">
+        <v>-0.0039562982147312</v>
+      </c>
+      <c r="H15" t="n">
+        <v>-1</v>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>axecap investment llc sell share of apple inc nasdaqaapl fifth third bancorp sell share of apple inc nasdaqaapl sagace wealth management llc sell share of microsoft corporation nasdaqmsft microsoft corporation nasdaqmsft stake lowered by tran capital management lp define financial llc buy share of microsoft corporation nasdaqmsft sapient capital llc sell share of microsoft corporation nasdaqmsft teacher retirement system of texas sell share of safety insurance group inc nasdaqsaft teacher retirement system of texas sell share of organon co nyseogn teacher retirement system of texas cut stock holding in artisan partner asset management inc nyseapam teacher retirement system of texas buy new share in a o smith corporation nyseaos rev group inc nyserevg position trimmed by teacher retirement system of texas share in lamb weston nyselw acquired by teacher retirement system of texas bridgebio pharma inc nasdaqbbio share sold by teacher retirement system of texas two west capital advisor llc trim position in apple inc nasdaqaapl teacher retirement system of texas take million position in community health system inc nysecyh teacher retirement system of texas ha million position in portland general electric company nysepor teacher retirement system of texas buy share of ugi corporation nyseugi teacher retirement system of texas ha million stake in ziff davis inc nasdaqzd teacher retirement system of texas purchase new stake in the campbell company nasdaqcpb asian heat squeeze lng flow to europe borgwarner inc nysebwa share sold by cambridge investment research advisor inc teacher retirement system of texas ha million stake in madrigal pharmaceutical inc nasdaqmdgl exclusive interview the future belongs to nocodes with deep ai integration abhinav girdhar ceo founder appy pie european trade minister meet to forge strategy after trump surprise tariff european trade minister meet to forge strategy after trump surprise tariff european trade minister meet to forge strategy after trump surprise tariff relx nyserelx rating lowered to hold at wall street zen southside bancshares nysesbsi rating lowered to sell at wall street zen wall street zen downgrade vista energy nysevist to sell bank of america cut primo brand nyseprmb price target to silgan nyseslgn price target raised to stifel financial nysesf price target raised to ubiquitis ui buy rating reiterated at bw financial wall street zen upgrade rafael nyserfl to hold charles schwab nyseschw price target raised to sea nysese stock rating lowered by wall street zen sealed air nysesee price target raised to wall street zen upgrade te connectivity nysetel to buy telus digital nysetixt stock rating upgraded by wall street zen sealed air nysesee price target raised to telephone and data system nysetds stock rating upgraded by wall street zen synovus financial nysesnv price target raised to truist financial cut sonoco product nyseson price target to att nyset price target raised to wec energy group nysewec rating lowered to sell at wall street zen exxon mobil nysexom price target raised to at scotiabank truist financial raise webster financial nysewbs price target to top ai stock to buy this week the place report surge in company relocation driving demand for flexible office space in dubai and riyadh rockfire resource lonrock stock price up still a buy rockfire resource lonrock trading up should you buy new zealand energy cvenz trading down here what happened argentina lithium energy cvelit share down should you sell silver spruce resource cvesse share down here what happened silver spruce resource cvesse trading down time to sell new zealand energy cvenz trading down should you sell argentina lithium energy cvelit stock price down here why geomega resource cvegma stock price up whats next geomega resource cvegma trading higher still a buy geomega resource cvegma stock price up here what happened geomega resource cvegma share up time to buy geomega resource cvegma trading higher should you buy form eptriricardo plc advanced drainage system inc nysewms share bought by teacher retirement system of texas teacher retirement system of texas purchase share of lxp industrial trust nyselxp teacher retirement system of texas purchase new stake in exact science corporation nasdaqexas teacher retirement system of texas raise holding in advanced drainage system inc nysewms amentum holding inc nyseamtm share sold by teacher retirement system of texas teacher retirement system of texas boost stock position in sprinklr inc nysecxm teacher retirement system of texas acquires share of lxp industrial trust nyselxp ola electric share rise to r a market reacts to q update aktietilbagekbsprogram uge share buyback programme week bunge global earnings preview what to expect robinhood eu wont retaliate to trump tariff countermeasure on hold until august avis budget group car v it peer head to head analysis contrasting cps technology cpsh the competition head to head analysis better home finance betr and it peer analyzing greif bros gefb the competition head to head review better home finance betr the competition cps technology cpsh it competitor head to head survey avis budget group car it peer financial comparison how doe nvidias reaching trillion in market cap impact the sp nasdaq and dow jones marc benioff dismisses ai panic say whitecollar workforce wont be wiped out market week ahead strong bank earnings sticky inflation could jolt summer lull china exporter rush to beat trump next big tariff deadline bp nysebp stock price expected to rise scotiabank analyst say ladenburg thalmsh sh initiate coverage on kala bio nasdaqkala franklin resource nyseben given new price target at well fargo company kkrs quarterly earnings preview what you need to know wall street zen upgrade wintrust financial nasdaqwtfc to hold botswana diamond lonbod trading higher still a buy botswana diamond lonbod share up here what happened botswana diamond lonbod trading higher whats next majestic ideal holding refiled mjid plan to raise million in july th ipo tower resource cvetwr trading up here what happened tower resource cvetwr trading up here why botswana diamond lonbod share up here what happened tower resource cvetwr trading up time to buy trump envoy meet with ukraine zelenskyy a u pledge more patriot missile for kyiv trump threatens russia with tariff and boost u weapon for ukraine trump envoy arrives in kyiv a u pledge more patriot missile to ukraine trump threatens russia with tariff and boost u weapon for ukraine trump envoy arrives in kyiv a u pledge more patriot missile to ukraine trump threatens russia with tariff and boost u weapon for ukraine trump threatens russia with tariff if war on ukraine isnt resolved within day trump envoy meet with ukraine zelenskyy a u weighs next step on russia invasion trump envoy meet with ukraine zelenskyy a u weighs next step on russia invasion trump threatens russia with tariff if war on ukraine isnt resolved within day trump threatens russia with tariff if war on ukraine isnt resolved within day spin cycle theyre throwing spaghetti at the wall bbc dump masterchef host over sex misconduct report eu want no trade war a trade minister mull new u tariff threat new review ordered into nh murdersuicide case amid criticism of shooter bail morning brief the epstein firestorm ice raid riot california v trump aquestive therapeutic inc nasdaqaqst given consensus recommendation of buy by analyst astera lab inc nasdaqalab receives consensus target price from analyst mplx lp nysemplx receives consensus recommendation of moderate buy from analyst brokerage set altria group inc nysemo price target at kornit digital ltd nasdaqkrnt receives average price target from brokerage exwhite house aide reveals why trump panicking right now brokerage set triple flag precious metal corp nysetfpm price target at lionsgate studio corp nyselion receives average price target from brokerage agnico eagle mine limited tseaem receives c consensus pt from analyst democrat already lining up for presidential race in early voting state these state are america best for quality of life in letter for monday july a bitcoin rush past k whats next for ether xrp dogecoin elkem asa elkef to release earnings on tuesday america movil amx expected to announce quarterly earnings on tuesday nikki wegner understanding big beautiful bill impact on long term care in nd why not hold gun manufacturer accountable for mass shooting boston herald will democrat reembrace musk now that he feuding with trump guest view bipartisan push to strengthen pa disability care system must succeed house debate pentagon spending crypto a rescission head to senate hancock whitney hwc projected to post quarterly earnings on tuesday omnicom group omc expected to announce quarterly earnings on tuesday what is bastille day what to know about the french holiday and why it is celebrated insider buying schroders plc lonsdr insider purchase share of stock cv group plc loncvsg insider buy in stock crest nicholson holding plc loncrst insider acquires in stock nextdecade nasdaqnext hit new month high on analyst upgrade trump mark anniversary of assassination attempt at the fifa club world cup final historic grand canyon lodge destroyed a wildfire force evacuation in northern arizona today in history july the storming of the bastille invisible rural homelessness grows in the shadow of a maine tourism mecca education notebook bond result child nutrition change and federal consultation orrington trash plant at risk of permanent closure if judge freeze funding susan collins start lining up money for maine that may not actually arrive hungary oldest library is fighting to save book from a beetle infestation trump to meet nato secretarygeneral a plan take shape for ukraine weapon sale chris christie say trump not pam bondi pulled the plug on epstein memo when you start the fire sometimes you cant put it out iyo sue former engineer after io founder tang yew tan admits to receiving trade secret from him poll show support for immigration is rising in u amid president trump crackdown trial will be very difficult for sen nicole mitchell to win minneapolis attorney say who got next democrat already lining up for presidential race in early voting state who got next democrat already lining up for presidential race in early voting state who got next democrat already lining up for presidential race in early voting state a nicotine pouch popularity soar theyre also responsible for more poisoning in young kid study find the biden doj tried to imprison a trump supporter over meme now he fighting back gop infighting over trump doge cut to take center stage a deadline loom how much trump big beautiful bill could raise electricity cost in every u state over the next year claudia istel ken barnes budget ayotte signed is designed to perpetuate inequality letter to the editor response to a response william hinkle eversource customer deserve more stable electric bill letter to the editor resident deserve more information about data center a look at a new poll showing support for immigration is rising in the u bitcoin top for the first time peter schiff give trump tariff threat on mexico eu a reality check america relies on deficit to make up for excess debt and consumption trump say he spoke to bongino amid report of infighting over epstein file trump reflects on surviving pennsylvania rally shooting year on god alone saved me one year after trump assassination attempt change at secret service but question remain jim chalmers insists labor can meet target of m new home despite department warning trump to meet nato secretary general a plan take shape for ukraine weapon sale tragedy in fall river read the full press release on sunday deadly fire amd warns of new transient scheduler attack impacting a wide range of cpu cambodia khmer rouge torture site added to unesco heritage list cant contain debris then forget about starbase dont allow hidden tax on energy producer hydrogen is a pipe dream dont be fooled the epstein list still remain relevant immigrant in overcapacity ice detention say theyre hungry raise food quality concern miranda devine shocking new poll reveals majority of deluded dems still believe the russia collusion hoax wa real live update trump threatens russia with tariff if war on ukraine isnt resolved dhs secretary kristi noem say trump want fema remade not dismantled homicide investigation underway after stabbing in southeast portland trump to announce aggressive ukraine weapon plan houston astros select lsus ethan frey in the third round of the mlb draft here when trump say american spirit triumph over force of evil on anniversary of butler assassination attempt trump brazil tariff imposed because they jail insurrectionist say economist your next coffee come with an insurrection infusion fee christie say trump benefited from epstein conspiracy theory boston red sox select lsus anthony eyanson in third round of mlb draft here when biden say he had to use autopen because he simply granted too many pardon company cast party biden defends frequent autopen use at end of term alex jose padilla say trump is to blame for violence against ice carried out by dems foot soldier fulltime mayor is unnecessary appendage an lsu baseball signee ha been picked by the tampa bay ray in the mlb draft here who portland police seize pound of cannabis in traffic stop florida financial advisor llc grows position in spdr sp small cap value etf nysearcaslyv share in united therapeutic corporation nasdaquthr bought by aurora investment counsel aurora investment counsel take million position in globe life inc nysegl florida financial advisor llc acquires share of spdr sp mid cap growth etf nysearcamdyg bhk investment advisor llc ha stake in eli lilly and company nyselly bleakley financial group llc boost stock position in bank of america corporation nysebac bleakley financial group llc sell share of ishares silver trust nysearcaslv rice hall james associate llc boost holding in green brick partner inc nasdaqgrbk jpmorgan betabuilders u equity etf batsbbus is florida financial advisor llcs rd largest position securian asset management inc sell share of servicenow inc nysenow florida financial advisor llc acquires new holding in ishares core high dividend etf nysearcahdv bleakley financial group llc sell share of ishares year treasury bond etf nasdaqshy securian asset management inc ha million stock holding in merck co inc nysemrk florida financial advisor llc buy share of ishares core high dividend etf nysearcahdv focused investor llc decrease stock holding in the home depot inc nysehd the pnc financial service group inc nysepnc share sold by bhk investment advisor llc rice hall james associate llc sell share of griffon corporation nysegff florida financial advisor llc sell share of fidelity msci information technology index etf nysearcaftec bleakley financial group llc buy share of vanguard total world stock etf nysearcavt charity fraud alert how to donate safely to texas flood victim charity fraud alert how to donate safely to texas flood victim tight oil market shrug off supply surge heartland advisor value plus fund q investor letter boy girl club program threatened by trump grant freeze serve thousand of family sun pharma announces launch of leqselvitm deuruxolitinib in the united state for the treatment of severe alopecia areata texas roadhouse inc nasdaqtxrh given consensus recommendation of moderate buy by analyst mqs management llc make new investment in rli corp nyserli stephen investment management group llc buy share of autodesk inc nasdaqadsk lri investment llc acquires share of newmont corporation nysenem lri investment llc sell share of teledyne technology incorporated nysetdy lri investment llc take position in spdr portfolio sp growth etf nysearcaspyg mqs management llc invests in centene corporation nysecnc eaton corporation plc nyseetn stock position lowered by lri investment llc stephen investment management group llc increase position in roper technology inc nyserop mtm investment management llc ha holding in ishares russell midcap etf nysearcaiwr lri investment llc acquires share of union pacific corporation nyseunp lri investment llc sell share of ameriprise financial inc nyseamp mtm investment management llc sell share of kinder morgan inc nysekmi mtm investment management llc buy share of vanguard sp etf nysearcavoo stephen inc ar boost stock position in hp inc nysehpq church dwight co inc nysechd share acquired by key financial inc lri investment llc reduces holding in kenvue inc nysekvue lri investment llc reduces position in ferrari nv nyserace lri investment llc buy share of spdr portfolio sp growth etf nysearcaspyg prudent man advisor llc sell share of vanguard intermediateterm bond etf nysearcabiv cme group inc nasdaqcme share purchased by key financial inc eaton corporation plc nyseetn share sold by lri investment llc mqs management llc buy new position in astrazeneca plc nasdaqazn kinder morgan inc nysekmi is mtm investment management llcs th largest position analyst set regeneron pharmaceutical inc nasdaqregn pt at catalyst financial partner llc grows stock position in linde plc nasdaqlin evergreen private wealth llc boost stock position in zoetis inc nysezts schwab u largecap etf nysearcaschx share sold by slow capital inc catalyst financial partner llc buy share of att inc nyset catalyst financial partner llc raise position in lowes company inc nyselow shore capital reiterates house stock rating for touchstone exploration lontxp cohen capital management inc sell share of ishares europe etf nysearcaiev vanguard ftse allworld exus etf nysearcaveu share sold by slow capital inc signaturefd llc reduces holding in rollins inc nyserol braime group lonbmt announces quarterly earnings result catalyst financial partner llc ha stock holding in sp global inc nysespgi beeks financial cloud group lonbks receives buy rating from canaccord genuity group catalyst financial partner llc increase holding in att inc nyset slow capital inc sell share of jpmorgan ultrashort municipal etf batsjmst catalyst financial partner llc ha stock position in intuitive surgical inc nasdaqisrg creightons loncrl trading higher still a buy dewhurst group londwha announces earnings result signaturefd llc boost stake in cisco system inc nasdaqcsco beeks financial cloud group lonbks receives buy rating from canaccord genuity group dunelm group londnlm receives buy rating from deutsche bank aktiengesellschaft catalyst financial partner llc ha position in capital group global growth equity etf nysearcacggo ariana resource lonaau trading up whats next simec atlantis energy lonsae trading down time to sell creightons loncrl trading higher still a buy what make uber technology uber a great business to invest in nearly half of u child are without summer learning program a cost rise study say world chess lonchss stock price down time to sell catalyst financial partner llc ha holding in the tjx company inc nysetjx a tariff on europe would effectively knock out transatlantic trade say eu trade chief promising cybersecurity stock to keep an eye on july th stratos wealth partner ltd sell share of universal display corporation nasdaqoled ge vernova inc nysegev share sold by mutual of america capital management llc bleakley financial group llc acquires share of marsh mclennan company inc nysemmc owen corning inc nyseoc given average recommendation of moderate buy by brokerage schechter investment advisor llc sell share of morgan stanley nysems corrado advisor llc raise stock position in vici property inc nysevici new york state common retirement fund trim position in ansys inc nasdaqanss arizona state retirement system sell share of raymond james financial inc nyserjf new york state common retirement fund sell share of mondelez international inc nasdaqmdlz diversify wealth management llc raise stock position in appfolio inc nasdaqappf emerald adviser llc decrease stock position in lharris technology inc nyselhx stephen inc ar boost stock position in automatic data processing inc nasdaqadp m mmm hold c rating reaffirmed at weiss rating weatherly asset management l p take position in chubb limited nysecb emerald adviser llc ha stock position in msci inc nysemsci bleakley financial group llc acquires share of marsh mclennan company inc nysemmc arizona state retirement system reduces stock position in ansys inc nasdaqanss fortinet inc nasdaqftnt share sold by new york state common retirement fund new york state common retirement fund sell share of cognizant technology solution corporation nasdaqctsh key financial inc increase stock position in kinsale capital group inc nyseknsl focused investor llc sell share of the home depot inc nysehd aurora investment counsel take position in elf beauty nyseelf bleakley financial group llc purchase share of vanguard total world stock etf nysearcavt trump adviser say this is how the president could certainly fire powell regeneron pharmaceutical inc nasdaqregn given average recommendation of moderate buy by brokerage mtm investment management llc acquires new position in american electric power company inc nasdaqaep lri investment llc trim stock position in kenvue inc nysekvue key financial inc purchase share of kla corporation nasdaqklac alp advisor inc purchase share of global payment inc nysegpn lri investment llc reduces stock position in ferrari nv nyserace cme group inc nasdaqcme share purchased by key financial inc mtm investment management llc ha position in hershey company the nysehsy signaturefd llc raise stock position in ishares msci usa value factor etf batsvlue slow capital inc sell share of jpmorgan ultrashort municipal etf batsjmst catalyst financial partner llc boost stock position in intuitive surgical inc nasdaqisrg pulsar group lonpuls post quarterly earnings result evergreen private wealth llc ha million position in vaneck long muni etf batsmln world chess lonchss stock price down time to sell rockfire resource lonrock trading up still a buy catalyst financial partner llc ha holding in capital group global growth equity etf nysearcacggo catalyst financial partner llc purchase share of deere company nysede dunelm group londnlm receives buy rating from deutsche bank aktiengesellschaft a tariff on europe would effectively knock out transatlantic trade say eu trade chief kathmere capital management llc cut stake in ge vernova inc nysegev arthur j gallagher co nyseajg share purchased by new york state common retirement fund analyst set wex inc nysewex target price at corrado advisor llc sell share of corning incorporated nyseglw dominion energy inc nysed share acquired by new york state common retirement fund kathmere capital management llc trim holding in dell technology inc nysedell new york state common retirement fund sell share of nike inc nysenke new york state common retirement fund sell share of marvell technology inc nasdaqmrvl kinsale capital group inc nyseknsl given consensus rating of hold by brokerage emerald adviser llc sell share of xpo inc nysexpo emerald adviser llc ha stake in burlington store inc nyseburl invmun incom oia to go exdividend on july th doubleline yield opportunity fund plan monthly dividend of nysedly inv vk invt ny announces monthly dividend of nysevtn gladstone land co announces monthly dividend of nasdaqlandp regency center co declares quarterly dividend of nasdaqregcp thor exploration lonthx given buy rating at canaccord genuity group berenberg bank issue positive forecast for volex lonvlx stock price gladstone commercial co nasdaqgoodn plan monthly dividend trump give russia a day deadline on ukraine signaturefd llc ha million stock position in ishares msci acwi ex u etf nasdaqacwx signaturefd llc buy share of toyota motor corporation nysetm cheems cheemspet cheems price hit on exchange reviewing cyclo therapeutic nasdaqcyth sorrento therapeutic nasdaqsrne financial contrast cemtrex nasdaqcetx versus omron otcmktsomrny empower self reported market capitalization top thousand mpwr animecoin anime hit day volume of million dignity gold digau trading higher over last day share in howmet aerospace inc nysehwm bought by florida financial advisor llc florida financial advisor llc sell share of unitedhealth group incorporated nyseunh aercap holding nv nyseaer stake cut by check capital management inc ca headtohead contrast insight enterprise nasdaqnsit v flowerscom nasdaqflws slow capital inc sell share of ishares global consumer staple etf nysearcakxi fidelity national information service inc nysefis position boosted by isthmus partner llc gould asset management llc ca reduces stock holding in ishares select dividend etf nasdaqdvy abbvie inc nyseabbv share sold by florida financial advisor llc slow capital inc cut stake in ishares global comm service etf nysearcaixp top renewable energy stock to research july th gould asset management llc ca lower position in ishares msci acwi low carbon target etf nysearcacrbn alta foundation donates k toward texas flood relief trump envoy arrives in kyiv a u pledge more patriot missile to ukraine trump envoy arrives in kyiv a u pledge more patriot missile to ukraine trump envoy arrives in kyiv a u pledge more patriot missile to ukraine trump envoy arrives in kyiv a u pledge more patriot missile to ukraine trump envoy arrives in kyiv a u pledge more patriot missile to ukraine trump envoy arrives in kyiv a u pledge more patriot missile to ukraine trump envoy arrives in kyiv a u pledge more patriot missile to ukraine trump envoy arrives in kyiv a u pledge more patriot missile to ukraine trump envoy arrives in kyiv a u pledge more patriot missile to ukraine trump envoy arrives in kyiv a u pledge more patriot missile to ukraine trump envoy arrives in kyiv a u pledge more patriot missile to ukraine rice hall james associate llc lower stock position in lantheus holding inc nasdaqlnth aurora investment counsel buy share of euronet worldwide inc nasdaqeeft slow capital inc raise stock position in cadence design system inc nasdaqcdns moody corporation nysemco share purchased by slow capital inc corteva inc nysectva share sold by lri investment llc top fintech stock to keep an eye on july th first bancorp nysefbp share bought by edgestream partner lp revolution medicine inc nasdaqrvmd share acquired by edgestream partner lp rithm capital corp nyseritm share bought by edgestream partner lp edgestream partner lp raise holding in ncino inc nasdaqncno antisemitic post appear on elmos x account after hack bleakley financial group llc purchase share of schwab u smallcap etf nysearcascha bleakley financial group llc boost stock holding in dimensional u small cap etf nysearcadfas edgestream partner lp acquires share of simpson manufacturing company inc nysessd edgestream partner lp ha million stake in nmi holding inc nasdaqnmih edgestream partner lp make new investment in exlservice holding inc nasdaqexls hartford schroders taxaware bond etf nysearcahtab share acquired by leelyn smith llc edgestream partner lp increase stock holding in cno financial group inc nysecno invesco sp high dividend low volatility etf nysearcasphd share sold by leelyn smith llc edgestream partner lp buy new position in bentley system incorporated nasdaqbsy fortress financial solution llc decrease holding in avantis emerging market equity etf nysearcaavem share in ishares future ai tech etf nysearcaarty acquired by mitchell mcleod pugh williams inc eu trade minister meet in brussels after u announces percent tariff private capital advisor inc take position in relay therapeutic inc nasdaqrlay mutual of america capital management llc ha million holding in ametek inc nyseame mitchell mcleod pugh williams inc purchase share of becton dickinson and company nysebdx</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>axecap investment sell apple nasdaqaapl fifth third bancorp sell apple nasdaqaapl sagace wealth sell microsoft corporation nasdaqmsft microsoft corporation nasdaqmsft stake lowered tran lp define financial buy microsoft corporation nasdaqmsft sapient sell microsoft corporation nasdaqmsft teacher retirement system texas sell safety insurance nasdaqsaft teacher retirement system texas sell organon co nyseogn teacher retirement system texas cut stock artisan partner asset nyseapam teacher retirement system texas buy smith corporation nyseaos rev nyserevg trimmed teacher retirement system texas lamb weston nyselw acquired teacher retirement system texas bridgebio pharma nasdaqbbio teacher retirement system texas west advisor trim apple nasdaqaapl teacher retirement system texas take million community health system nysecyh teacher retirement system texas million portland general electric company nysepor teacher retirement system texas buy ugi corporation nyseugi teacher retirement system texas million stake ziff davis nasdaqzd teacher retirement system texas purchase stake campbell company nasdaqcpb asian heat squeeze lng flow europe borgwarner nysebwa cambridge investment research advisor teacher retirement system texas million stake madrigal pharmaceutical nasdaqmdgl exclusive interview future belongs nocodes deep ai integration abhinav girdhar ceo founder appy pie european trade minister meet forge strategy trump surprise tariff european trade minister meet forge strategy trump surprise tariff european trade minister meet forge strategy trump surprise tariff relx nyserelx rating lowered wall street zen southside bancshares nysesbsi rating lowered sell wall street zen wall street zen downgrade vista energy nysevist sell bank america cut primo brand nyseprmb price target silgan nyseslgn price target raised stifel financial nysesf price target raised ubiquitis ui buy rating reiterated bw financial wall street zen upgrade rafael nyserfl charles schwab nyseschw price target raised sea nysese stock rating lowered wall street zen sealed air nysesee price target raised wall street zen upgrade te connectivity nysetel buy telus digital nysetixt stock rating upgraded wall street zen sealed air nysesee price target raised telephone data system nysetds stock rating upgraded wall street zen synovus financial nysesnv price target raised truist financial cut sonoco product nyseson price target att nyset price target raised wec energy nysewec rating lowered sell wall street zen exxon mobil nysexom price target raised scotiabank truist financial raise webster financial nysewbs price target ai stock buy place report surge company relocation driving demand flexible office space dubai riyadh rockfire resource lonrock stock price buy rockfire resource lonrock trading buy zealand energy cvenz trading happened argentina lithium energy cvelit sell silver spruce resource cvesse happened silver spruce resource cvesse trading sell zealand energy cvenz trading sell argentina lithium energy cvelit stock price geomega resource cvegma stock price whats next geomega resource cvegma trading higher buy geomega resource cvegma stock price happened geomega resource cvegma buy geomega resource cvegma trading higher buy form eptriricardo plc advanced drainage system nysewms bought teacher retirement system texas teacher retirement system texas purchase lxp industrial trust nyselxp teacher retirement system texas purchase stake exact science corporation nasdaqexas teacher retirement system texas raise advanced drainage system nysewms amentum nyseamtm teacher retirement system texas teacher retirement system texas boost stock sprinklr nysecxm teacher retirement system texas acquires lxp industrial trust nyselxp ola electric rise r market reacts q update aktietilbagekbsprogram uge buyback programme bunge global earnings preview expect robinhood eu wont retaliate trump tariff countermeasure august avis budget car v peer head head analysis contrasting cps technology cpsh competition head head analysis better finance betr peer analyzing greif bros gefb competition head head review better finance betr competition cps technology cpsh competitor head head survey avis budget car peer financial comparison doe nvidias reaching trillion market cap impact sp nasdaq dow jones marc benioff dismisses ai panic whitecollar workforce wont wiped market ahead strong bank earnings sticky inflation jolt summer lull china exporter rush beat trump next tariff deadline bp nysebp stock price expected rise scotiabank analyst ladenburg thalmsh sh initiate coverage kala bio nasdaqkala franklin resource nyseben price target fargo company kkrs quarterly earnings preview wall street zen upgrade wintrust financial nasdaqwtfc botswana diamond lonbod trading higher buy botswana diamond lonbod happened botswana diamond lonbod trading higher whats next majestic ideal refiled mjid plan raise million ipo tower resource cvetwr trading happened tower resource cvetwr trading botswana diamond lonbod happened tower resource cvetwr trading buy trump envoy meet ukraine zelenskyy pledge patriot missile kyiv trump threatens russia tariff boost weapon ukraine trump envoy arrives kyiv pledge patriot missile ukraine trump threatens russia tariff boost weapon ukraine trump envoy arrives kyiv pledge patriot missile ukraine trump threatens russia tariff boost weapon ukraine trump threatens russia tariff war ukraine isnt resolved trump envoy meet ukraine zelenskyy weighs next step russia invasion trump envoy meet ukraine zelenskyy weighs next step russia invasion trump threatens russia tariff war ukraine isnt resolved trump threatens russia tariff war ukraine isnt resolved spin cycle theyre throwing spaghetti wall bbc dump masterchef host sex misconduct report eu trade war trade minister mull tariff threat review ordered nh murdersuicide amid criticism shooter bail morning brief epstein firestorm raid riot california v trump aquestive therapeutic nasdaqaqst consensus recommendation buy analyst astera lab nasdaqalab receives consensus target price analyst mplx lp nysemplx receives consensus recommendation moderate buy analyst brokerage set altria nysemo price target kornit digital ltd nasdaqkrnt receives average price target brokerage exwhite house aide reveals trump panicking brokerage set triple flag precious metal corp nysetfpm price target lionsgate studio corp nyselion receives average price target brokerage agnico eagle mine limited tseaem receives c consensus pt analyst democrat lining presidential race early voting america best quality life monday bitcoin rush past k whats next ether xrp dogecoin elkem asa elkef release earnings tuesday america movil amx expected announce quarterly earnings tuesday nikki wegner understanding bill impact term care nd gun manufacturer accountable mass shooting boston herald democrat reembrace musk feuding trump guest view bipartisan push strengthen pa disability care system must succeed house debate pentagon spending crypto rescission head senate hancock whitney hwc projected post quarterly earnings tuesday omnicom omc expected announce quarterly earnings tuesday bastille french holiday celebrated insider buying schroders plc lonsdr insider purchase stock cv plc loncvsg insider buy stock crest nicholson plc loncrst insider acquires stock nextdecade nasdaqnext hit month high analyst upgrade trump mark anniversary assassination attempt fifa club world cup final historic grand canyon lodge destroyed wildfire force evacuation northern arizona history storming bastille invisible rural homelessness grows shadow maine tourism mecca education notebook bond child nutrition change federal consultation orrington trash plant risk permanent closure judge freeze funding susan collins start lining money maine arrive hungary oldest library fighting save book beetle infestation trump meet nato secretarygeneral plan take shape ukraine weapon sale chris christie trump pam bondi pulled plug epstein memo start fire sometimes cant put iyo sue engineer io founder tang yew tan admits receiving trade secret poll support immigration rising amid president trump crackdown trial difficult sen nicole mitchell minneapolis attorney got next democrat lining presidential race early voting got next democrat lining presidential race early voting got next democrat lining presidential race early voting nicotine pouch popularity soar theyre responsible poisoning young kid study find biden doj tried imprison trump supporter meme fighting gop infighting trump doge cut take center stage deadline loom trump bill raise electricity cost next claudia istel ken barnes budget ayotte signed designed perpetuate inequality editor response response william hinkle eversource customer deserve stable electric bill editor resident deserve information data center look poll showing support immigration rising bitcoin peter schiff give trump tariff threat mexico eu reality america relies deficit excess debt consumption trump spoke bongino amid report infighting epstein file trump reflects surviving pennsylvania rally shooting god alone saved trump assassination attempt change secret service jim chalmers insists labor meet target department warning trump meet nato secretary general plan take shape ukraine weapon sale tragedy fall river full press release sunday deadly fire amd warns transient scheduler attack impacting wide range cpu cambodia khmer rouge torture site added unesco heritage list cant contain debris forget starbase dont allow hidden tax energy producer hydrogen pipe dream dont fooled epstein list relevant immigrant overcapacity detention theyre hungry raise quality concern miranda devine shocking poll reveals majority deluded dems believe russia collusion hoax real update trump threatens russia tariff war ukraine isnt resolved dhs secretary kristi noem trump fema remade dismantled homicide investigation underway stabbing southeast portland trump announce aggressive ukraine weapon plan houston astros select lsus ethan frey third round mlb draft trump american spirit triumph force evil anniversary butler assassination attempt trump brazil tariff imposed jail insurrectionist economist next coffee come insurrection infusion fee christie trump benefited epstein conspiracy theory boston red sox select lsus anthony eyanson third round mlb draft biden autopen simply granted pardon company cast party biden defends frequent autopen end term alex jose padilla trump blame violence carried dems foot soldier fulltime mayor unnecessary appendage lsu baseball signee picked tampa bay ray mlb draft portland police seize pound cannabis traffic stop florida financial advisor grows spdr sp small cap value nysearcaslyv united therapeutic corporation nasdaquthr bought aurora investment counsel aurora investment counsel take million globe life nysegl florida financial advisor acquires spdr sp mid cap growth nysearcamdyg bhk investment advisor stake eli lilly company nyselly bleakley financial boost stock bank america corporation nysebac bleakley financial sell ishares silver trust nysearcaslv rice hall james associate boost green brick partner nasdaqgrbk jpmorgan betabuilders equity batsbbus florida financial advisor llcs rd largest securian asset sell servicenow nysenow florida financial advisor acquires ishares core high dividend nysearcahdv bleakley financial sell ishares treasury bond nasdaqshy securian asset million stock merck co nysemrk florida financial advisor buy ishares core high dividend nysearcahdv focused investor decrease stock depot nysehd pnc financial service nysepnc bhk investment advisor rice hall james associate sell griffon corporation nysegff florida financial advisor sell fidelity msci information technology index nysearcaftec bleakley financial buy vanguard total world stock nysearcavt charity fraud alert donate safely texas flood victim charity fraud alert donate safely texas flood victim tight oil market shrug supply surge heartland advisor value plus fund q investor boy girl club program threatened trump grant freeze thousand family sun pharma announces launch leqselvitm deuruxolitinib united treatment severe alopecia areata texas roadhouse nasdaqtxrh consensus recommendation moderate buy analyst mqs investment rli corp nyserli stephen investment buy autodesk nasdaqadsk lri investment acquires newmont corporation nysenem lri investment sell teledyne technology incorporated nysetdy lri investment take spdr portfolio sp growth nysearcaspyg mqs invests centene corporation nysecnc eaton corporation plc nyseetn stock lowered lri investment stephen investment increase roper technology nyserop mtm investment ishares russell midcap nysearcaiwr lri investment acquires union pacific corporation nyseunp lri investment sell ameriprise financial nyseamp mtm investment sell kinder morgan nysekmi mtm investment buy vanguard sp nysearcavoo stephen ar boost stock hp nysehpq church dwight co nysechd acquired financial lri investment reduces kenvue nysekvue lri investment reduces ferrari nv nyserace lri investment buy spdr portfolio sp growth nysearcaspyg prudent man advisor sell vanguard intermediateterm bond nysearcabiv cme nasdaqcme purchased financial eaton corporation plc nyseetn lri investment mqs buy astrazeneca plc nasdaqazn kinder morgan nysekmi mtm investment llcs largest analyst set regeneron pharmaceutical nasdaqregn pt catalyst financial partner grows stock linde plc nasdaqlin evergreen private wealth boost stock zoetis nysezts schwab largecap nysearcaschx slow catalyst financial partner buy att nyset catalyst financial partner raise lowes company nyselow shore reiterates house stock rating touchstone exploration lontxp cohen sell ishares europe nysearcaiev vanguard ftse allworld exus nysearcaveu slow signaturefd reduces rollins nyserol braime lonbmt announces quarterly earnings catalyst financial partner stock sp global nysespgi beeks financial cloud lonbks receives buy rating canaccord genuity catalyst financial partner increase att nyset slow sell jpmorgan ultrashort municipal batsjmst catalyst financial partner stock intuitive surgical nasdaqisrg creightons loncrl trading higher buy dewhurst londwha announces earnings signaturefd boost stake cisco system nasdaqcsco beeks financial cloud lonbks receives buy rating canaccord genuity dunelm londnlm receives buy rating deutsche bank aktiengesellschaft catalyst financial partner global growth equity nysearcacggo ariana resource lonaau trading whats next simec atlantis energy lonsae trading sell creightons loncrl trading higher buy uber technology uber great business invest nearly half child without summer learning program cost rise study world chess lonchss stock price sell catalyst financial partner tjx company nysetjx tariff europe effectively knock transatlantic trade eu trade chief promising cybersecurity stock eye stratos wealth partner ltd sell universal display corporation nasdaqoled ge vernova nysegev mutual america bleakley financial acquires marsh mclennan company nysemmc owen corning nyseoc average recommendation moderate buy brokerage schechter investment advisor sell morgan stanley nysems corrado advisor raise stock vici property nysevici york common retirement fund trim ansys nasdaqanss arizona retirement system sell raymond james financial nyserjf york common retirement fund sell mondelez international nasdaqmdlz diversify wealth raise stock appfolio nasdaqappf emerald adviser decrease stock lharris technology nyselhx stephen ar boost stock automatic data processing nasdaqadp mmm c rating reaffirmed weiss rating weatherly asset l p take chubb limited nysecb emerald adviser stock msci nysemsci bleakley financial acquires marsh mclennan company nysemmc arizona retirement system reduces stock ansys nasdaqanss fortinet nasdaqftnt york common retirement fund york common retirement fund sell cognizant technology solution corporation nasdaqctsh financial increase stock kinsale nyseknsl focused investor sell depot nysehd aurora investment counsel take elf beauty nyseelf bleakley financial purchase vanguard total world stock nysearcavt trump adviser president certainly fire powell regeneron pharmaceutical nasdaqregn average recommendation moderate buy brokerage mtm investment acquires american electric power company nasdaqaep lri investment trim stock kenvue nysekvue financial purchase kla corporation nasdaqklac alp advisor purchase global payment nysegpn lri investment reduces stock ferrari nv nyserace cme nasdaqcme purchased financial mtm investment hershey company nysehsy signaturefd raise stock ishares msci usa value factor batsvlue slow sell jpmorgan ultrashort municipal batsjmst catalyst financial partner boost stock intuitive surgical nasdaqisrg pulsar lonpuls post quarterly earnings evergreen private wealth million vaneck muni batsmln world chess lonchss stock price sell rockfire resource lonrock trading buy catalyst financial partner global growth equity nysearcacggo catalyst financial partner purchase deere company nysede dunelm londnlm receives buy rating deutsche bank aktiengesellschaft tariff europe effectively knock transatlantic trade eu trade chief kathmere cut stake ge vernova nysegev arthur j gallagher co nyseajg purchased york common retirement fund analyst set wex nysewex target price corrado advisor sell corning incorporated nyseglw dominion energy nysed acquired york common retirement fund kathmere trim dell technology nysedell york common retirement fund sell nike nysenke york common retirement fund sell marvell technology nasdaqmrvl kinsale nyseknsl consensus rating brokerage emerald adviser sell xpo nysexpo emerald adviser stake burlington store nyseburl invmun incom oia exdividend doubleline yield opportunity fund plan monthly dividend nysedly inv vk invt ny announces monthly dividend nysevtn gladstone land co announces monthly dividend nasdaqlandp regency center co declares quarterly dividend nasdaqregcp thor exploration lonthx buy rating canaccord genuity berenberg bank issue positive forecast volex lonvlx stock price gladstone commercial co nasdaqgoodn plan monthly dividend trump give russia deadline ukraine signaturefd million stock ishares msci acwi ex nasdaqacwx signaturefd buy toyota corporation nysetm cheems cheemspet cheems price hit exchange reviewing cyclo therapeutic nasdaqcyth sorrento therapeutic nasdaqsrne financial contrast cemtrex nasdaqcetx versus omron otcmktsomrny empower self reported market capitalization thousand mpwr animecoin anime hit volume million dignity gold digau trading higher howmet aerospace nysehwm bought florida financial advisor florida financial advisor sell unitedhealth incorporated nyseunh aercap nv nyseaer stake cut ca headtohead contrast insight enterprise nasdaqnsit v flowerscom nasdaqflws slow sell ishares global consumer staple nysearcakxi fidelity national information service nysefis boosted isthmus partner gould asset ca reduces stock ishares select dividend nasdaqdvy abbvie nyseabbv florida financial advisor slow cut stake ishares global comm service nysearcaixp renewable energy stock research gould asset ca lower ishares msci acwi low carbon target nysearcacrbn alta foundation donates k texas flood relief trump envoy arrives kyiv pledge patriot missile ukraine trump envoy arrives kyiv pledge patriot missile ukraine trump envoy arrives kyiv pledge patriot missile ukraine trump envoy arrives kyiv pledge patriot missile ukraine trump envoy arrives kyiv pledge patriot missile ukraine trump envoy arrives kyiv pledge patriot missile ukraine trump envoy arrives kyiv pledge patriot missile ukraine trump envoy arrives kyiv pledge patriot missile ukraine trump envoy arrives kyiv pledge patriot missile ukraine trump envoy arrives kyiv pledge patriot missile ukraine trump envoy arrives kyiv pledge patriot missile ukraine rice hall james associate lower stock lantheus nasdaqlnth aurora investment counsel buy euronet worldwide nasdaqeeft slow raise stock cadence design system nasdaqcdns moody corporation nysemco purchased slow corteva nysectva lri investment fintech stock eye bancorp nysefbp bought edgestream partner lp revolution medicine nasdaqrvmd acquired edgestream partner lp rithm corp nyseritm bought edgestream partner lp edgestream partner lp raise ncino nasdaqncno antisemitic post appear elmos x account hack bleakley financial purchase schwab smallcap nysearcascha bleakley financial boost stock dimensional small cap nysearcadfas edgestream partner lp acquires simpson manufacturing company nysessd edgestream partner lp million stake nmi nasdaqnmih edgestream partner lp investment exlservice nasdaqexls hartford schroders taxaware bond nysearcahtab acquired leelyn smith edgestream partner lp increase stock cno financial nysecno invesco sp high dividend low volatility nysearcasphd leelyn smith edgestream partner lp buy bentley system incorporated nasdaqbsy fortress financial solution decrease avantis emerging market equity nysearcaavem ishares future ai tech nysearcaarty acquired mitchell mcleod pugh williams eu trade minister meet brussels announces percent tariff private advisor take relay therapeutic nasdaqrlay mutual america million ametek nyseame mitchell mcleod pugh williams purchase becton dickinson company nysebdx</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="2" t="n">
+        <v>45854</v>
+      </c>
+      <c r="B16" t="n">
+        <v>6263.7001953125</v>
+      </c>
+      <c r="C16" t="n">
+        <v>6268.1201171875</v>
+      </c>
+      <c r="D16" t="n">
+        <v>6201.58984375</v>
+      </c>
+      <c r="E16" t="n">
+        <v>6254.5</v>
+      </c>
+      <c r="F16" t="n">
+        <v>5177460000</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0.0031936574173276</v>
+      </c>
+      <c r="H16" t="n">
+        <v>1</v>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>modelop appoints exstrategy executive alex rice a director of partnership modelop appoints exstrategy executive alex rice a director of partnership precision scissors five type designed for specific task first mining announces upsized million public offering for a total offering of up to million massachusetts financial service co ma acquires share of cdw corporation nasdaqcdw leo wealth llc sell share of bank of america corporation nysebac dakota wealth management buy share of spdr sp midcap etf trust nysearcamdy stratum wealth advisor llc sell share of costco wholesale corporation nasdaqcost dominion energy inc nysed stock position cut by dakota wealth management dakota wealth management acquires share of intercontinental exchange inc nyseice oversea chinese banking corp ltd cut stock holding in essential property realty trust inc nyseeprt dakota wealth management sell share of schwab u largecap growth etf nysearcaschg massachusetts financial service co ma reduces stock position in veeva system inc nyseveev sumitomo life insurance co sell share of shopify inc nyseshop dakota wealth management reduces holding in hershey company the nysehsy dakota wealth management take position in incyte corporation nasdaqincy newmont corporation nysenem stock position raised by dakota wealth management top tech news today oneplus ai assistant samsung f launch gta v p in saudi trump cyber plan grok ai companion intel corporation nasdaqintc position reduced by dakota wealth management timessquare capital management llc cut stock holding in synaptics incorporated nasdaqsyna sumitomo life insurance co lower stock holding in costar group inc nasdaqcsgp dakota wealth management raise stake in resmed inc nysermd oversea chinese banking corp ltd raise stock position in shopify inc nyseshop timessquare capital management llc boost stock position in clean harbor inc nyseclh dakota wealth management buy share of rollins inc nyserol leo wealth llc acquires share of shopify inc nyseshop gartner inc nyseit share sold by sumitomo life insurance co leo wealth llc trim stock holding in grayscale bitcoin trust etf nysearcagbtc coterra energy inc nysectra share sold by cornercap investment counsel inc massachusetts financial service co ma sell share of nike inc nysenke port of long beach break ground on million terminal expansion project bitcoin whale move btc is a billion dump coming crea cut forecast again but say home sale are rebounding from chaotic start fiserv fi fell on concern over declining payment volume fiserv fi fell on concern over declining payment volume jpmorgan post strong second quarter number though dimon warns of tariff geopolitical risk jpmorgan post strong second quarter number though dimon warns of tariff geopolitical risk jpmorgan post strong second quarter number though dimon warns of tariff geopolitical risk jpmorgan post strong second quarter number though dimon warns of tariff geopolitical risk jpmorgan post strong second quarter number though dimon warns of tariff geopolitical risk jpmorgan post strong second quarter number though dimon warns of tariff geopolitical risk jpmorgan post strong second quarter number though dimon warns of tariff geopolitical risk jpmorgan post strong second quarter number though dimon warns of tariff geopolitical risk jpmorgan post strong second quarter number though dimon warns of tariff geopolitical risk jpmorgan post strong second quarter number though dimon warns of tariff geopolitical risk jpmorgan post strong second quarter number though dimon warns of tariff geopolitical risk jpmorgan post strong second quarter number though dimon warns of tariff geopolitical risk jpmorgan post strong second quarter number though dimon warns of tariff geopolitical risk jpmorgan post strong second quarter number though dimon warns of tariff geopolitical risk jpmorgan post strong second quarter number though dimon warns of tariff geopolitical risk jpmorgan post strong second quarter number though dimon warns of tariff geopolitical risk jpmorgan post strong second quarter number though dimon warns of tariff geopolitical risk jpmorgan post strong second quarter number though dimon warns of tariff geopolitical risk jpmorgan post strong second quarter number though dimon warns of tariff geopolitical risk jpmorgan post strong second quarter number though dimon warns of tariff geopolitical risk popular yogurt recalled could contain sharp plastic piece apple invests m in pentagonbacked mp material dolores catania team up with advanced herbal from the maker of dramamine to launch the dish on glps content series and tackle one of the most common complaint from glp user nausea tiktok denies viral rumor about new u app head to head contrast china bak battery nasdaqcbat v alaska power telephone otcmktsaptl made scientific and sentinel biotherapeutics announce strategic manufacturing partnership to advance ph iii allogeneic epp encapsulated cell therapy program techprecision tpcs v it rival head to head survey head to head analysis ucloudlink group nasdaqucl and intertek gp otcmktsiktsy analyzing irobot nasdaqirbt and fanuc otcmktsfanuy bridgewater advisor inc purchase share of marriott international inc nasdaqmar bridgewater advisor inc take position in sp global inc nysespgi bryn mawr capital management llc grows position in ssc technology holding inc nasdaqssnc xcel energy inc nasdaqxel stake boosted by midwest professional planner ltd insig ai loninsg stock price up still a buy iconic mineral cveicm trading up here why ocean power technology nasdaqoptt v spine injury solution otcmktsspin financial analysis sonoro energy cvesnv trading down whats next andretti acquisition corp ii nasdaqpole share sold by wealthspring capital llc champion bear resource cvecba trading down should you sell montauk renewables mntk it competitor financial contrast sonoro energy cvesnv stock price down should you sell bryn mawr capital management llc decrease stock position in vanguard sp etf nysearcavoo bridgewater advisor inc purchase new share in thermo fisher scientific inc nysetmo dogwood therapeutic dwtx versus the competition head to head comparison reviewing oriental land otcmktsolcly h world group nasdaqhtht qep otcmktsqepc issue quarterly earnings result sonoro energy cvesnv trading down whats next paul mueller muel and the competition critical survey contrasting montauk renewables mntk and it rival wealthspring capital llc trim stock position in andretti acquisition corp ii nasdaqpole clearsign technology nasdaqclir ashtead group otcmktsashty head to head analysis linkedins city on the rise see location to grow your career here what to expect from idexx laboratory next earnings report do you believe in the upside potential of icon plc iclr here what to expect from idexx laboratory next earnings report china economy grows steadily despite trump tariff the new york time u banking giant reap gain from dealmaking rebound june cpi signal tariff impact what the expert say plug named exclusive wholesale partner for recurrents ev selling platform bryn mawr capital management llc trim holding in oracle corporation nyseorcl hager investment management service llc sell share of waste management inc nysewm apollon wealth management llc acquires share of apollo global management inc nyseapo schrum private wealth management llc take position in roper technology inc nyserop sbi security co ltd sell share of cintas corporation nasdaqctas hager investment management service llc ha holding in canadian pacific kansa city limited nysecp massachusetts financial service co ma buy share of atlassian corporation plc nasdaqteam share in ryman hospitality property inc nyserhp purchased by oversea chinese banking corp ltd poehling capital management inc invests in howard hughes holding inc nysehhh massachusetts financial service co ma decrease holding in nike inc nysenke share in veeva system inc nyseveev bought by sumitomo life insurance co dakota wealth management sell share of global payment inc nysegpn dakota wealth management purchase share of rollins inc nyserol clearsign technology nasdaqclir and ashtead group otcmktsashty critical analysis headtohead analysis paul mueller muel v the competition oriental land otcmktsolcly v h world group nasdaqhtht headtohead survey kane biotech cvekne share down here what happened midwest professional planner ltd acquires share of torm plc nasdaqtrmd qep otcmktsqepc issue quarterly earnings result mesa royalty trust mtr v it rival financial review hegseth yank u military participant from globalist security forum gcm resource longcm share up still a buy schrum private wealth management llc ha position in cisco system inc nasdaqcsco accenture plc nyseacn share sold by schrum private wealth management llc poehling capital management inc ha million stock holding in marathon petroleum corporation nysempc poehling capital management inc increase stock position in british american tobacco plc nysebti the home depot inc nysehd share sold by provident trust co gcm resource longcm stock price up here what happened hager investment management service llc decrease stock holding in chipotle mexican grill inc nysecmg hager investment management service llc decrease stock holding in toll brother inc nysetol schrum private wealth management llc take position in cigna group nyseci what on earth are elon musk and greg abbott emailing about proposed cut to nasa science would be disastrous bridgewater advisor inc make new investment in coinbase global inc nasdaqcoin amcor plc nyseamcr share sold by oversea chinese banking corp ltd sim acquisition corp i nasdaqsima is wealthspring capital llcs th largest position silverbox corp iv nysesbxd share bought by wealthspring capital llc bridgewater advisor inc make new million investment in netflix inc nasdaqnflx wealthspring capital llc invests in newbury street ii acquisition corp class a ordinary share nasdaqntwo illinois tool work inc nyseitw share acquired by apollon wealth management llc a year later many rome resident still grapple with tornado impact bridgewater advisor inc purchase new stake in eli lilly and company nyselly bogart wealth llc increase holding in well fargo company nysewfc the walt disney company nysedis stock holding increased by apollon wealth management llc signaturefd llc acquires share of kimberlyclark co nysekmb hohimer wealth management llc ha stock holding in mueller industry inc nysemli catalyst financial partner llc invests in schlumberger limited nyseslb midwest professional planner ltd purchase share of nxp semiconductor nv nasdaqnxpi uc berkeley marketing professor killed by gunman in greece in broad daylight in wake of crash india order look at boeings fuel switch scam artist trump demand justice after doj criminal referral target adam schiff ice cream giant commit to nix artificial dye by federal health official say u ice cream maker say theyll stop using artificial dye by u ice cream maker say theyll stop using artificial dye by grant street asset management inc cut stock position in ft vest u equity enhance moderate buffer etf december batsxdec midwest professional planner ltd ha million holding in arista network inc nyseanet albertsons company nyseaci post quarterly earnings result beat expectation by eps tectonic advisor llc decrease stock holding in loews corporation nysel tectonic advisor llc cut holding in cbre group inc nysecbre parthenon llc ha million stock position in water corporation nysewat tectonic advisor llc acquires share of sunopta inc nasdaqstkl northern oil and gas inc nysenog share purchased by midwest professional planner ltd parthenon llc ha million position in turning point brand inc nysetpb mitchell mcleod pugh williams inc make new investment in tractor supply company nasdaqtsco florida financial advisor llc grows stake in royal caribbean cruise ltd nysercl securian asset management inc ha million stock position in exxon mobil corporation nysexom bleakley financial group llc purchase share of exxon mobil corporation nysexom bleakley financial group llc sell share of cadence design system inc nasdaqcdns tectonic advisor llc sell share of goldman sachs access treasury year etf nysearcagbil securian asset management inc sell share of the allstate corporation nyseall bleakley financial group llc sell share of danaher corporation nysedhr vanguard ftse allworld exus smallcap etf nysearcavss share purchased by tectonic advisor llc mitchell mcleod pugh williams inc raise stake in johnson johnson nysejnj securian asset management inc cut position in cadence design system inc nasdaqcdns gould asset management llc ca buy share of exxon mobil corporation nysexom reflecting on the new format of the expanded fifa club world cup tectonic advisor llc ha million holding in western midstream partner lp nysewes hr block inc nysehrb share bought by tectonic advisor llc lri investment llc reduces stock holding in ansys inc nasdaqanss stack financial management inc decrease holding in stryker corporation nysesyk tectonic advisor llc sell share of lkq corporation nasdaqlkq tectonic advisor llc increase stake in enbridge inc nyseenb exclusive state department roll out profamily exemption to hiring freeze west family investment inc boost position in chubb limited nysecb whittier trust co purchase share of topbuild corp nysebld landaas co wi adv purchase share of capital group international focus equity etf nysearcacgxu grant street asset management inc sell share of ft vest u equity buffer etf february batsffeb stack financial management inc sell share of centerpoint energy inc nysecnp corteva inc nysectva stock position raised by first business financial service inc txo partner nysetxo hess midstream partner nysehesm headtohead comparison rtx corporation nysertx share bought by mosaic family wealth partner llc fortress wealth management inc cut holding in proshares investment grade interest rate hedged batsighg kornitzer capital management inc k decrease stake in chart industry inc nysegtls saba closedend fund etf batscefs share sold by fortress wealth management inc fortress wealth management inc invests in bondbloxx private credit clo etf nasdaqpcmm stack financial management inc ha million position in conocophillips nysecop fortress wealth management inc sell share of principal active high yield etf nysearcayld fortress wealth management inc purchase share of cohen steer quality income realty fund inc nyserqi kaye capital management ha million position in ishares global etf nysearcaioo mizuho financial group inc nysemfg share sold by west family investment inc mine arao wealth creation management llc sell share of caterpillar inc nysecat doubleline opportunistic bond etf nysearcadbnd share sold by landmark wealth management llc landmark wealth management llc raise position in western asset bond etf nasdaqwabf pinkerton retirement specialist llc invests in franconevada corporation nysefnv landmark wealth management llc increase stock position in vanguard russell etf nasdaqvone ishares core u reit etf nysearcausrt share acquired by landmark wealth management llc</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>modelop appoints exstrategy executive alex rice director partnership modelop appoints exstrategy executive alex rice director partnership precision scissors five type designed specific task mining announces upsized million public offering total offering million massachusetts financial service co acquires cdw corporation nasdaqcdw leo wealth sell bank america corporation nysebac dakota wealth buy spdr sp midcap trust nysearcamdy stratum wealth advisor sell costco wholesale corporation nasdaqcost dominion energy nysed stock cut dakota wealth dakota wealth acquires intercontinental exchange nyseice oversea chinese banking corp ltd cut stock essential property realty trust nyseeprt dakota wealth sell schwab largecap growth nysearcaschg massachusetts financial service co reduces stock veeva system nyseveev sumitomo life insurance co sell shopify nyseshop dakota wealth reduces hershey company nysehsy dakota wealth take incyte corporation nasdaqincy newmont corporation nysenem stock raised dakota wealth tech oneplus ai assistant samsung f launch gta v p saudi trump cyber plan grok ai companion intel corporation nasdaqintc reduced dakota wealth timessquare cut stock synaptics incorporated nasdaqsyna sumitomo life insurance co lower stock costar nasdaqcsgp dakota wealth raise stake resmed nysermd oversea chinese banking corp ltd raise stock shopify nyseshop timessquare boost stock clean harbor nyseclh dakota wealth buy rollins nyserol leo wealth acquires shopify nyseshop gartner nyseit sumitomo life insurance co leo wealth trim stock grayscale bitcoin trust nysearcagbtc coterra energy nysectra cornercap investment counsel massachusetts financial service co sell nike nysenke port beach break ground million terminal expansion project bitcoin whale move btc billion dump coming crea cut forecast sale rebounding chaotic start fiserv fi fell concern declining payment volume fiserv fi fell concern declining payment volume jpmorgan post strong quarter dimon warns tariff geopolitical risk jpmorgan post strong quarter dimon warns tariff geopolitical risk jpmorgan post strong quarter dimon warns tariff geopolitical risk jpmorgan post strong quarter dimon warns tariff geopolitical risk jpmorgan post strong quarter dimon warns tariff geopolitical risk jpmorgan post strong quarter dimon warns tariff geopolitical risk jpmorgan post strong quarter dimon warns tariff geopolitical risk jpmorgan post strong quarter dimon warns tariff geopolitical risk jpmorgan post strong quarter dimon warns tariff geopolitical risk jpmorgan post strong quarter dimon warns tariff geopolitical risk jpmorgan post strong quarter dimon warns tariff geopolitical risk jpmorgan post strong quarter dimon warns tariff geopolitical risk jpmorgan post strong quarter dimon warns tariff geopolitical risk jpmorgan post strong quarter dimon warns tariff geopolitical risk jpmorgan post strong quarter dimon warns tariff geopolitical risk jpmorgan post strong quarter dimon warns tariff geopolitical risk jpmorgan post strong quarter dimon warns tariff geopolitical risk jpmorgan post strong quarter dimon warns tariff geopolitical risk jpmorgan post strong quarter dimon warns tariff geopolitical risk jpmorgan post strong quarter dimon warns tariff geopolitical risk popular yogurt recalled contain sharp plastic piece apple invests pentagonbacked mp material dolores catania team advanced herbal maker dramamine launch dish glps content series tackle common complaint glp user nausea tiktok denies viral rumor app head head contrast china bak battery nasdaqcbat v alaska power telephone otcmktsaptl scientific sentinel biotherapeutics announce strategic manufacturing partnership advance ph iii allogeneic epp encapsulated cell therapy program techprecision tpcs v rival head head survey head head analysis ucloudlink nasdaqucl intertek gp otcmktsiktsy analyzing irobot nasdaqirbt fanuc otcmktsfanuy bridgewater advisor purchase marriott international nasdaqmar bridgewater advisor take sp global nysespgi bryn mawr grows ssc technology nasdaqssnc xcel energy nasdaqxel stake boosted midwest professional planner ltd insig ai loninsg stock price buy iconic mineral cveicm trading ocean power technology nasdaqoptt v spine injury solution otcmktsspin financial analysis sonoro energy cvesnv trading whats next andretti acquisition corp ii nasdaqpole wealthspring champion bear resource cvecba trading sell montauk renewables mntk competitor financial contrast sonoro energy cvesnv stock price sell bryn mawr decrease stock vanguard sp nysearcavoo bridgewater advisor purchase thermo fisher scientific nysetmo dogwood therapeutic dwtx versus competition head head comparison reviewing oriental land otcmktsolcly h world nasdaqhtht qep otcmktsqepc issue quarterly earnings sonoro energy cvesnv trading whats next paul mueller muel competition critical survey contrasting montauk renewables mntk rival wealthspring trim stock andretti acquisition corp ii nasdaqpole clearsign technology nasdaqclir ashtead otcmktsashty head head analysis linkedins rise location grow career expect idexx laboratory next earnings report believe upside potential icon plc iclr expect idexx laboratory next earnings report china economy grows steadily trump tariff york banking giant reap gain dealmaking rebound cpi signal tariff impact expert plug named exclusive wholesale partner recurrents ev selling platform bryn mawr trim oracle corporation nyseorcl hager investment service sell waste nysewm apollon wealth acquires apollo global nyseapo schrum private wealth take roper technology nyserop sbi security co ltd sell cintas corporation nasdaqctas hager investment service canadian pacific kansa limited nysecp massachusetts financial service co buy atlassian corporation plc nasdaqteam ryman hospitality property nyserhp purchased oversea chinese banking corp ltd poehling invests howard hughes nysehhh massachusetts financial service co decrease nike nysenke veeva system nyseveev bought sumitomo life insurance co dakota wealth sell global payment nysegpn dakota wealth purchase rollins nyserol clearsign technology nasdaqclir ashtead otcmktsashty critical analysis headtohead analysis paul mueller muel v competition oriental land otcmktsolcly v h world nasdaqhtht headtohead survey kane biotech cvekne happened midwest professional planner ltd acquires torm plc nasdaqtrmd qep otcmktsqepc issue quarterly earnings mesa royalty trust mtr v rival financial review hegseth yank military participant globalist security forum gcm resource longcm buy schrum private wealth cisco system nasdaqcsco accenture plc nyseacn schrum private wealth poehling million stock marathon petroleum corporation nysempc poehling increase stock british american tobacco plc nysebti depot nysehd provident trust co gcm resource longcm stock price happened hager investment service decrease stock chipotle mexican grill nysecmg hager investment service decrease stock toll brother nysetol schrum private wealth take cigna nyseci earth elon musk greg abbott emailing proposed cut nasa science disastrous bridgewater advisor investment coinbase global nasdaqcoin amcor plc nyseamcr oversea chinese banking corp ltd sim acquisition corp nasdaqsima wealthspring llcs largest silverbox corp iv nysesbxd bought wealthspring bridgewater advisor million investment netflix nasdaqnflx wealthspring invests newbury street ii acquisition corp class ordinary nasdaqntwo illinois tool work nyseitw acquired apollon wealth later rome resident grapple tornado impact bridgewater advisor purchase stake eli lilly company nyselly bogart wealth increase fargo company nysewfc walt disney company nysedis stock increased apollon wealth signaturefd acquires kimberlyclark co nysekmb hohimer wealth stock mueller industry nysemli catalyst financial partner invests schlumberger limited nyseslb midwest professional planner ltd purchase nxp semiconductor nv nasdaqnxpi uc berkeley marketing professor killed gunman greece broad daylight wake crash india order look boeings fuel switch scam artist trump demand justice doj criminal referral target adam schiff cream giant commit nix artificial dye federal health cream maker theyll stop artificial dye cream maker theyll stop artificial dye grant street asset cut stock ft vest equity enhance moderate buffer december batsxdec midwest professional planner ltd million arista network nyseanet albertsons company nyseaci post quarterly earnings beat expectation eps tectonic advisor decrease stock loews corporation nysel tectonic advisor cut cbre nysecbre parthenon million stock water corporation nysewat tectonic advisor acquires sunopta nasdaqstkl northern oil gas nysenog purchased midwest professional planner ltd parthenon million turning brand nysetpb mitchell mcleod pugh williams investment tractor supply company nasdaqtsco florida financial advisor grows stake royal caribbean cruise ltd nysercl securian asset million stock exxon mobil corporation nysexom bleakley financial purchase exxon mobil corporation nysexom bleakley financial sell cadence design system nasdaqcdns tectonic advisor sell goldman sachs access treasury nysearcagbil securian asset sell allstate corporation nyseall bleakley financial sell danaher corporation nysedhr vanguard ftse allworld exus smallcap nysearcavss purchased tectonic advisor mitchell mcleod pugh williams raise stake johnson johnson nysejnj securian asset cut cadence design system nasdaqcdns gould asset ca buy exxon mobil corporation nysexom reflecting format expanded fifa club world cup tectonic advisor million western midstream partner lp nysewes hr block nysehrb bought tectonic advisor lri investment reduces stock ansys nasdaqanss stack financial decrease stryker corporation nysesyk tectonic advisor sell lkq corporation nasdaqlkq tectonic advisor increase stake enbridge nyseenb exclusive department roll profamily exemption hiring freeze west family investment boost chubb limited nysecb whittier trust co purchase topbuild corp nysebld landaas co wi adv purchase international focus equity nysearcacgxu grant street asset sell ft vest equity buffer february batsffeb stack financial sell centerpoint energy nysecnp corteva nysectva stock raised business financial service txo partner nysetxo hess midstream partner nysehesm headtohead comparison rtx corporation nysertx bought mosaic family wealth partner fortress wealth cut proshares investment grade interest rate hedged batsighg kornitzer k decrease stake chart industry nysegtls saba closedend fund batscefs fortress wealth fortress wealth invests bondbloxx private credit clo nasdaqpcmm stack financial million conocophillips nysecop fortress wealth sell principal active high yield nysearcayld fortress wealth purchase cohen steer quality income realty fund nyserqi kaye million ishares global nysearcaioo mizuho financial nysemfg west family investment mine arao wealth creation sell caterpillar nysecat doubleline opportunistic bond nysearcadbnd landmark wealth landmark wealth raise western asset bond nasdaqwabf pinkerton retirement specialist invests franconevada corporation nysefnv landmark wealth increase stock vanguard russell nasdaqvone ishares core reit nysearcausrt acquired landmark wealth</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="2" t="n">
+        <v>45855</v>
+      </c>
+      <c r="B17" t="n">
+        <v>6297.35986328125</v>
+      </c>
+      <c r="C17" t="n">
+        <v>6304.68994140625</v>
+      </c>
+      <c r="D17" t="n">
+        <v>6262.27001953125</v>
+      </c>
+      <c r="E17" t="n">
+        <v>6263.39990234375</v>
+      </c>
+      <c r="F17" t="n">
+        <v>5512290000</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0.0053737674089093</v>
+      </c>
+      <c r="H17" t="n">
+        <v>1</v>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>american trust investment service serf a sole underwriter for ktech solution co ltd ipo american trust investment service serf a sole underwriter for ktech solution co ltd ipo henry samuel son of heidi klum and seal sign with next management get a head start on back to school shopping at amazon and save up to macomb county manufacturer urged to register for mfg day week to connect with local student deadline alert faruqi faruqi llp investigates claim on behalf of investor of doubleverify stifel rank no in jd power study for third straight year investor deadline next week robbins geller rudman dowd llp announces that red cat holding inc investor with substantial loss have opportunity to lead class action lawsuit rcat stevens capital partner trim position in ishares core msci eafe etf batsiefa wealthgarden f llc lower stock position in ishares russell etf nysearcaiwm vanguard smallcap value etf nysearcavbr share sold by theory financial llc donald trump slam backer who continue to talk about jeffrey epstein hoax i dont want their support anymore what happens if trump fire fed chair powell this would be a mess analyst warn newmont net m from selling greatland discovery silver stake deadline alert faruqi faruqi llp investigates claim on behalf of investor of petco video firsttime home buyer workshop u stock mixed bank of america earnings top view humankind list announced mechanic financial corp boost holding in altria group inc nysemo seabridge investment advisor llc sell share of deere company nysede qep co inc unveils stateoftheart robert adhesive manufacturing plant in dalton georgia mechanic financial corp buy new share in booking holding inc nasdaqbkng signaturefd llc sell share of ishares gold trust nysearcaiau the tjx company inc nysetjx stake boosted by mechanic financial corp share in booking holding inc nasdaqbkng bought by mechanic financial corp seabridge investment advisor llc grows stock holding in amgen inc nasdaqamgn altman advisor inc reduces position in the goldman sachs group inc nysegs danaher corporation nysedhr share acquired by sigma planning corp cable hill partner llc acquires share of accenture plc nyseacn caterpillar inc nysecat share acquired by cable hill partner llc equity investment corp sell share of cisco system inc nasdaqcsco seabridge investment advisor llc buy share of bank of america corporation nysebac pax financial group llc make new investment in the goldman sachs group inc nysegs sage mountain advisor llc raise stock holding in automatic data processing inc nasdaqadp automatic data processing inc nasdaqadp share bought by cable hill partner llc broadcom inc nasdaqavgo share sold by seabridge investment advisor llc altman advisor inc trim stake in the goldman sachs group inc nysegs sage mountain advisor llc buy new position in duke energy corporation nyseduk signaturefd llc purchase share of motorola solution inc nysemsi sage mountain advisor llc purchase share of gilead science inc nasdaqgild danaher corporation nysedhr share acquired by sage mountain advisor llc equity investment corp sell share of cisco system inc nasdaqcsco vanguard shortterm bond etf nysearcabsv share sold by stephen inc ar caterpillar inc nysecat share purchased by cable hill partner llc danaher corporation nysedhr share purchased by sigma planning corp pax financial group llc sell share of salesforce inc nysecrm share in verizon communication inc nysevz acquired by pax financial group llc barclays fined million for moneylaundering failure barclays fined million for moneylaundering failure the wall street journal seb collaborates with sp global market intelligence off the la vega strip restaurant close for bizarre reason great northern energy metal announces closing of private placement for gross proceeds of m why dogecoin is rising today analysisfrances plan to cull public holiday may not help the economy big buck for better bark gallant land m to bring gamechanging stem cell therapy to pet desantis tap state senator for florida highprofile cfo post gimme credit report warns of mounting headwind for u health insurer amid regulatory scrutiny and funding challenge deadline alert faruqi faruqi llp investigates claim on behalf of investor of fortrea holding duke football and basketball game security help needed investor deadline next week robbins geller rudman dowd llp announces that organon co investor with substantial loss have opportunity to lead class action lawsuit ogn congruence therapeutic announces oral presentation on mcr corrector development candidate cgx for earlyonset obesity at the rd annual obesity weight loss drug development summit invested in argenx year ago would be worth this much today power quality equipment market size expected to reach u billion by cagr of exclusive report by the insight partner life science lab signal shifting strategy amid new economic pressure according to survey of researcher power quality equipment market size expected to reach u billion by cagr of exclusive report by the insight partner welch forbes llc lower holding in cocacola company the nyseko summit x llc ha million stake in united parcel service inc nyseups shayne jacob llc take position in constellation brand inc nysestz welch forbes llc cut position in qualcomm incorporated nasdaqqcom altman advisor inc boost holding in lam research corporation nasdaqlrcx ine networking expertise essential a enterprise struggle with ai infrastructure ine networking expertise essential a enterprise struggle with ai infrastructure free flow inc fflo announces subsidiary contract to purchase real estate investment property finn partner introduces new aipowered crisis training platform to counter narrative manipulation and coordinated reputational attack in realtime ford share in decline a cost of largescale suv recall is disclosed olympus eume ultrasound processor for gi and pulmonary disease detection and diagnosis launch in u market summit x llc ha million position in invesco qqq nasdaqqqq parcion private wealth llc ha stake in ge aerospace nysege costco wholesale corporation nasdaqcost stock position raised by parcion private wealth llc cullen frost banker inc ha million position in costco wholesale corporation nasdaqcost cullen frost banker inc sell share of union pacific corporation nyseunp whittier trust co sell share of nike inc nysenke whittier trust co of nevada inc ha million holding in union pacific corporation nyseunp cullen frost banker inc ha million stake in walmart inc nysewmt costco wholesale corporation nasdaqcost share sold by cullen frost banker inc triasima portfolio management inc raise stock holding in arthur j gallagher co nyseajg vanguard ftse developed market etf nysearcavea stock holding lifted by seaside wealth management inc cullen frost banker inc sell share of alphabet inc nasdaqgoog parcion private wealth llc boost stock holding in eli lilly and company nyselly cullen frost banker inc sell share of the sherwinwilliams company nyseshw guardian wealth advisor llc sell share of vanguard sp etf nysearcavoo ishares sp growth etf nysearcaivw position decreased by guardian wealth advisor llc summit x llc ha million position in walmart inc nysewmt walmart inc nysewmt stock position lessened by summit x llc european commission will investigate umgs plan to buy downtown report sharplink gaming sbet share soar after becoming largest corporate ethereum holder nigeria inflation fall for third month in june chasing the potential of intelligent automation deadline alert faruqi faruqi llp investigates claim on behalf of investor of red cat holding fbs analyzes cryptocurrency market trend in h and outline key driver for h maine gop allegation of voter fraud arent true shenna bellow say rfk jr ousts two trump loyalist from hhs top rank ishares national muni bond etf nysearcamub share sold by wealthgarden f llc trump compare jeffrey epstein hoax to russiagate blast past supporter what is the annabelle doll and why are people so convinced it haunted mechanic financial corp take position in servicenow inc nysenow blue circle health expands type diabetes care program to louisiana grandfield dodd llc cut holding in booking holding inc nasdaqbkng altman advisor inc raise stock holding in att inc nyset sage mountain advisor llc invests in duke energy corporation nyseduk sigma planning corp buy share of cisco system inc nasdaqcsco pax financial group llc purchase share of republic service inc nysersg first command advisory service inc ha stock holding in danaher corporation nysedhr share in verizon communication inc nysevz purchased by pax financial group llc doj fire maurene comey daughter of exfbi director james comey live now trump participates in an official working visit with the crown prince of the kingdom of bahrain altman advisor inc increase stock position in lam research corporation nasdaqlrcx welch forbes llc decrease stake in qualcomm incorporated nasdaqqcom taiwan semiconductor manufacturing company ltd nysetsm position boosted by triasima portfolio management inc senate vote to move ahead with trump request for b in spending cut cullen frost banker inc acquires share of walmart inc nysewmt parcion private wealth llc boost position in abbott laboratory nyseabt cullen frost banker inc sell share of the sherwinwilliams company nyseshw guardian wealth advisor llc reduces position in vanguard sp etf nysearcavoo triasima portfolio management inc ha million position in arthur j gallagher co nyseajg parcion private wealth llc boost stock holding in blackrock nyseblk steve scalise recall near assassination on butler anniversary the left is getting more radical biden aide bernal is second witness to plead the fifth in probe of expresidents mental decline equity investment corp sell share of medtronic plc nysemdt share in southern company the nyseso bought by altman advisor inc welch forbes llc sell share of ishares core sp etf nysearcaivv shayne jacob llc ha million stake in kimberlyclark co nysekmb lmg wealth partner llc ha million stock holding in ishares russell midcap growth etf nysearcaiwp shayne jacob llc ha million stock position in philip morris international inc nysepm ishares core sp etf nysearcaivv share sold by shayne jacob llc trump blasted after admitting he used autopen day after attacking biden for same thing gov katie hobbs announces erasure of m in medical debt for arizonan armed service panel approves defense bill after marathon markup trump asked gop lawmaker if he should fire fed chair jerome powell source say colorado park and wildlife confirms new wolf pack ahead of commission meeting wishbone gold lonwsbn trading down whats next the latest trump welcome bahrain crown prince after signing nuclear energy deal summit x llc boost stock position in palo alto network inc nasdaqpanw first on fox red state investigating mm and skittle manufacturer for deceptive practice syrian anchor take cover from airstrike live on tv federal housing official submitted schiff criminal referral to doj over mortgage document trump slam his own supporter who are angered over how his team ha handled the epstein case trump slam his own supporter who are angered over how his team ha handled the epstein case trump slam his own supporter a weakling for falling for what he now call the epstein hoax rnc chair say big beautiful bill key part of gop strategy to win seat in midterm election in the shadow of the hiroshima blast the secret romance that bloomed in defiance of the white australia policy torres strait leader lost their landmark case how can government be held to account on climate rep rick allen ha bought up to k worth of intuit stock here what you should know push to end antisemitism is welcome but envoy plan raise concern australia race commissioner warns albaneses warm welcome in beijing show icy tension are a thing of the past at least for now tom mcilroy america b are in guam for resolute force pacific exercise north dakota tribe ask u supreme court to keep legislative district intact amid lawsuit state sue trump administration for cutting disaster prevention grant breaking news speaker raise a lot of money clergy view love is the answer vanguard intermediateterm treasury etf nasdaqvgit holding raised by private wealth management group llc welch forbes llc reduces stake in rtx corporation nysertx sage mountain advisor llc ha stock holding in chubb limited nysecb kornitzer capital management inc k sell share of corning incorporated nyseglw violich capital management inc purchase share of johnson johnson nysejnj kornitzer capital management inc k raise holding in citigroup inc nysec ishares esg aware msci usa etf nasdaqesgu stock position reduced by shared vision wealth group llc kinder morgan inc nysekmi share purchased by tectonic advisor llc kornitzer capital management inc k buy share of johnson johnson nysejnj lmg wealth partner llc ha million position in bristol myers squibb company nysebmy sky mountain capital management inc take position in marathon petroleum corporation nysempc israel bomb syrian capital despite u pressure to stand down rfk jr fire top aide appoints new acting chief of staff zohran mamdani brief house democrat on lesson from his campaign doctor responds to fresh donald trump picture and hint at significant health issue bogart wealth llc ha position in freeportmcmoran inc nysefcx pax financial group llc acquires share of conocophillips nysecop whittier trust co of nevada inc ha million holding in check point software technology ltd nasdaqchkp sage mountain advisor llc purchase share of boston scientific corporation nysebsx pax financial group llc take position in tmobile u inc nasdaqtmus pax financial group llc acquires share of borgwarner inc nysebwa seabridge investment advisor llc lower position in tmobile u inc nasdaqtmus supporter arrive early for vp vances visit to west pittston supporter arrive early for vp vances visit to west pittston cable hill partner llc acquires share of verizon communication inc nysevz vanguard shortterm bond etf nysearcabsv share bought by richmond brother inc altman advisor inc ha million stock position in gilead science inc nasdaqgild by the number wisconsin race for governor nyc mayor race mamdani camp say he had constructive meeting with big apple ceo ishares gold trust nysearcaiau share sold by altman advisor inc triasima portfolio management inc cut position in att inc nyset oreilly automotive inc nasdaqorly share acquired by summit x llc triasima portfolio management inc boost stake in shopify inc nyseshop live coverage noem say u electrical grid is vulnerable at hill nation summit live coverage noem say u electrical grid is vulnerable at hill nation summit live coverage noem say u electrical grid is vulnerable at hill nation summit live coverage noem say u electrical grid is vulnerable at hill nation summit live coverage noem say u electrical grid is vulnerable at hill nation summit live coverage noem say u electrical grid is vulnerable at hill nation summit summit x llc ha million stake in ishares core sp smallcap etf nysearcaijr</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>american trust investment service serf sole underwriter ktech solution co ltd ipo american trust investment service serf sole underwriter ktech solution co ltd ipo henry samuel son heidi klum seal sign next head start school shopping amazon save macomb county manufacturer urged register mfg connect local student deadline alert faruqi faruqi llp investigates claim behalf investor doubleverify stifel rank jd power study third straight investor deadline next robbins geller rudman dowd llp announces red cat investor substantial loss opportunity lead class action lawsuit rcat stevens partner trim ishares core msci eafe batsiefa wealthgarden f lower stock ishares russell nysearcaiwm vanguard smallcap value nysearcavbr theory financial donald trump slam backer continue jeffrey epstein hoax dont support anymore happens trump fire fed chair powell mess analyst warn newmont net selling greatland discovery silver stake deadline alert faruqi faruqi llp investigates claim behalf investor petco video firsttime buyer workshop stock mixed bank america earnings view humankind list announced mechanic financial corp boost altria nysemo seabridge investment advisor sell deere company nysede qep co unveils stateoftheart robert adhesive manufacturing plant dalton georgia mechanic financial corp buy booking nasdaqbkng signaturefd sell ishares gold trust nysearcaiau tjx company nysetjx stake boosted mechanic financial corp booking nasdaqbkng bought mechanic financial corp seabridge investment advisor grows stock amgen nasdaqamgn altman advisor reduces goldman sachs nysegs danaher corporation nysedhr acquired sigma planning corp cable hill partner acquires accenture plc nyseacn caterpillar nysecat acquired cable hill partner equity investment corp sell cisco system nasdaqcsco seabridge investment advisor buy bank america corporation nysebac pax financial investment goldman sachs nysegs sage mountain advisor raise stock automatic data processing nasdaqadp automatic data processing nasdaqadp bought cable hill partner broadcom nasdaqavgo seabridge investment advisor altman advisor trim stake goldman sachs nysegs sage mountain advisor buy duke energy corporation nyseduk signaturefd purchase motorola solution nysemsi sage mountain advisor purchase gilead science nasdaqgild danaher corporation nysedhr acquired sage mountain advisor equity investment corp sell cisco system nasdaqcsco vanguard shortterm bond nysearcabsv stephen ar caterpillar nysecat purchased cable hill partner danaher corporation nysedhr purchased sigma planning corp pax financial sell salesforce nysecrm verizon communication nysevz acquired pax financial barclays fined million moneylaundering failure barclays fined million moneylaundering failure wall street journal seb collaborates sp global market intelligence la vega strip restaurant close bizarre great northern energy metal announces closing private placement gross proceeds dogecoin rising analysisfrances plan cull public holiday help economy buck better bark gallant land gamechanging stem cell therapy pet desantis tap senator florida highprofile cfo post gim credit report warns mounting headwind health insurer amid regulatory scrutiny funding challenge deadline alert faruqi faruqi llp investigates claim behalf investor fortrea duke football basketball game security help needed investor deadline next robbins geller rudman dowd llp announces organon co investor substantial loss opportunity lead class action lawsuit ogn congruence therapeutic announces oral presentation mcr corrector development candidate cgx earlyonset obesity rd annual obesity weight loss drug development summit invested argenx ago worth power quality equipment market size expected reach billion cagr exclusive report insight partner life science lab signal shifting strategy amid economic pressure according survey researcher power quality equipment market size expected reach billion cagr exclusive report insight partner welch forbes lower cocacola company nyseko summit x million stake united parcel service nyseups shayne jacob take constellation brand nysestz welch forbes cut qualcomm incorporated nasdaqqcom altman advisor boost lam research corporation nasdaqlrcx ine networking expertise essential enterprise struggle ai infrastructure ine networking expertise essential enterprise struggle ai infrastructure free flow fflo announces subsidiary contract purchase real estate investment property finn partner introduces aipowered crisis training platform counter narrative manipulation coordinated reputational attack realtime ford decline cost largescale suv recall disclosed olympus eume ultrasound processor gi pulmonary disease detection diagnosis launch market summit x million invesco qqq nasdaqqqq parcion private wealth stake ge aerospace nysege costco wholesale corporation nasdaqcost stock raised parcion private wealth cullen frost banker million costco wholesale corporation nasdaqcost cullen frost banker sell union pacific corporation nyseunp whittier trust co sell nike nysenke whittier trust co nevada million union pacific corporation nyseunp cullen frost banker million stake walmart nysewmt costco wholesale corporation nasdaqcost cullen frost banker triasima portfolio raise stock arthur j gallagher co nyseajg vanguard ftse developed market nysearcavea stock lifted seaside wealth cullen frost banker sell alphabet nasdaqgoog parcion private wealth boost stock eli lilly company nyselly cullen frost banker sell sherwinwilliams company nyseshw guardian wealth advisor sell vanguard sp nysearcavoo ishares sp growth nysearcaivw decreased guardian wealth advisor summit x million walmart nysewmt walmart nysewmt stock lessened summit x european commission investigate umgs plan buy downtown report sharplink gaming sbet soar becoming largest corporate ethereum holder nigeria inflation fall third month chasing potential intelligent automation deadline alert faruqi faruqi llp investigates claim behalf investor red cat fbs analyzes cryptocurrency market trend h outline driver h maine gop allegation voter fraud arent shenna bellow rfk jr ousts trump loyalist hhs rank ishares national muni bond nysearcamub wealthgarden f trump compare jeffrey epstein hoax russiagate blast past supporter annabelle doll people convinced haunted mechanic financial corp take servicenow nysenow blue circle health expands type diabetes care program louisiana grandfield dodd cut booking nasdaqbkng altman advisor raise stock att nyset sage mountain advisor invests duke energy corporation nyseduk sigma planning corp buy cisco system nasdaqcsco pax financial purchase republic service nysersg command advisory service stock danaher corporation nysedhr verizon communication nysevz purchased pax financial doj fire maurene comey daughter exfbi director james comey trump participates working visit crown prince kingdom bahrain altman advisor increase stock lam research corporation nasdaqlrcx welch forbes decrease stake qualcomm incorporated nasdaqqcom taiwan semiconductor manufacturing company ltd nysetsm boosted triasima portfolio senate vote move ahead trump request b spending cut cullen frost banker acquires walmart nysewmt parcion private wealth boost abbott laboratory nyseabt cullen frost banker sell sherwinwilliams company nyseshw guardian wealth advisor reduces vanguard sp nysearcavoo triasima portfolio million arthur j gallagher co nyseajg parcion private wealth boost stock blackrock nyseblk steve scalise recall near assassination butler anniversary left getting radical biden aide bernal witness plead fifth probe expresidents mental decline equity investment corp sell medtronic plc nysemdt southern company nyseso bought altman advisor welch forbes sell ishares core sp nysearcaivv shayne jacob million stake kimberlyclark co nysekmb lmg wealth partner million stock ishares russell midcap growth nysearcaiwp shayne jacob million stock philip morris international nysepm ishares core sp nysearcaivv shayne jacob trump blasted admitting used autopen attacking biden gov katie hobbs announces erasure medical debt arizonan armed service panel approves defense bill marathon markup trump gop lawmaker fire fed chair jerome powell source colorado park wildlife confirms wolf pack ahead commission meeting wishbone gold lonwsbn trading whats next latest trump welcome bahrain crown prince signing nuclear energy deal summit x boost stock palo alto network nasdaqpanw fox red investigating mm skittle manufacturer deceptive practice syrian anchor take cover airstrike tv federal housing submitted schiff criminal referral doj mortgage document trump slam supporter angered team handled epstein trump slam supporter angered team handled epstein trump slam supporter weakling falling call epstein hoax rnc chair bill part gop strategy seat midterm election shadow hiroshima blast secret romance bloomed defiance white australia policy torres strait landmark government account climate rep rick allen bought k worth intuit stock push end antisemitism welcome envoy plan raise concern australia race commissioner warns albaneses warm welcome beijing icy tension past least tom mcilroy america b guam resolute force pacific exercise north dakota tribe supreme legislative district intact amid lawsuit sue trump administration cutting disaster prevention grant breaking speaker raise lot money clergy view love answer vanguard intermediateterm treasury nasdaqvgit raised private wealth welch forbes reduces stake rtx corporation nysertx sage mountain advisor stock chubb limited nysecb kornitzer k sell corning incorporated nyseglw violich purchase johnson johnson nysejnj kornitzer k raise citigroup nysec ishares esg aware msci usa nasdaqesgu stock reduced shared vision wealth kinder morgan nysekmi purchased tectonic advisor kornitzer k buy johnson johnson nysejnj lmg wealth partner million bristol myers squibb company nysebmy sky mountain take marathon petroleum corporation nysempc israel bomb syrian pressure stand rfk jr fire aide appoints acting chief staff zohran mamdani brief house democrat lesson campaign doctor responds fresh donald trump picture hint significant health issue bogart wealth freeportmcmoran nysefcx pax financial acquires conocophillips nysecop whittier trust co nevada million software technology ltd nasdaqchkp sage mountain advisor purchase boston scientific corporation nysebsx pax financial take tmobile nasdaqtmus pax financial acquires borgwarner nysebwa seabridge investment advisor lower tmobile nasdaqtmus supporter arrive early vp vances visit west pittston supporter arrive early vp vances visit west pittston cable hill partner acquires verizon communication nysevz vanguard shortterm bond nysearcabsv bought richmond brother altman advisor million stock gilead science nasdaqgild wisconsin race governor nyc mayor race mamdani camp constructive meeting apple ceo ishares gold trust nysearcaiau altman advisor triasima portfolio cut att nyset oreilly automotive nasdaqorly acquired summit x triasima portfolio boost stake shopify nyseshop coverage noem electrical grid vulnerable hill nation summit coverage noem electrical grid vulnerable hill nation summit coverage noem electrical grid vulnerable hill nation summit coverage noem electrical grid vulnerable hill nation summit coverage noem electrical grid vulnerable hill nation summit coverage noem electrical grid vulnerable hill nation summit summit x million stake ishares core sp smallcap nysearcaijr</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="2" t="n">
+        <v>45856</v>
+      </c>
+      <c r="B18" t="n">
+        <v>6296.7900390625</v>
+      </c>
+      <c r="C18" t="n">
+        <v>6315.60986328125</v>
+      </c>
+      <c r="D18" t="n">
+        <v>6285.27001953125</v>
+      </c>
+      <c r="E18" t="n">
+        <v>6312.9501953125</v>
+      </c>
+      <c r="F18" t="n">
+        <v>5184700000</v>
+      </c>
+      <c r="G18" t="n">
+        <v>-9.048620868445932e-05</v>
+      </c>
+      <c r="H18" t="n">
+        <v>-1</v>
+      </c>
+      <c r="I18" t="inlineStr"/>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>nan</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
chore: pin Streamlit Cloud to Python 3.10 for SciPy compatibility
</commit_message>
<xml_diff>
--- a/notebooks/Cleaned_Topic_Headlines.xlsx
+++ b/notebooks/Cleaned_Topic_Headlines.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J18"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1091,6 +1091,38 @@
         </is>
       </c>
     </row>
+    <row r="19">
+      <c r="A19" s="2" t="n">
+        <v>45859</v>
+      </c>
+      <c r="B19" t="n">
+        <v>6305.60009765625</v>
+      </c>
+      <c r="C19" t="n">
+        <v>6336.080078125</v>
+      </c>
+      <c r="D19" t="n">
+        <v>6303.7900390625</v>
+      </c>
+      <c r="E19" t="n">
+        <v>6304.740234375</v>
+      </c>
+      <c r="F19" t="n">
+        <v>5010840000</v>
+      </c>
+      <c r="G19" t="n">
+        <v>0.0013991348828683</v>
+      </c>
+      <c r="H19" t="n">
+        <v>1</v>
+      </c>
+      <c r="I19" t="inlineStr"/>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>